<commit_message>
Added US01 and Paired Prgm US08
</commit_message>
<xml_diff>
--- a/Team2Report.xlsx
+++ b/Team2Report.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10913"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ztyle\Documents\SSW 555\SSW_555_Project\Agile_Methods_Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Avaneesh/Desktop/CS 555/avaneeshSprint1/Agile_Methods_Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50B92CB9-1406-49F1-AC95-FF446115650C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{038DF635-DC4D-EA49-A9AB-04B6290C8E06}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="26940" yWindow="1980" windowWidth="33760" windowHeight="17480" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="606" uniqueCount="273">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="608" uniqueCount="274">
   <si>
     <t>Date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -894,6 +894,9 @@
   </si>
   <si>
     <t>Store date field</t>
+  </si>
+  <si>
+    <t>Completed</t>
   </si>
 </sst>
 </file>
@@ -1073,11 +1076,11 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="66">
@@ -1188,7 +1191,7 @@
             <c:numRef>
               <c:f>'Burndown README'!$B$15:$B$20</c:f>
               <c:numCache>
-                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:formatCode>m/d/yy</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>42632</c:v>
@@ -1259,7 +1262,7 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
+        <c:numFmt formatCode="m/d/yy" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1325,7 +1328,7 @@
             <c:numRef>
               <c:f>Burndown!$A$2:$A$7</c:f>
               <c:numCache>
-                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:formatCode>m/d/yy</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>42632</c:v>
@@ -1387,7 +1390,7 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
+        <c:numFmt formatCode="m/d/yy" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2249,16 +2252,16 @@
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.07421875" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="7.84375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.15234375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.4609375" customWidth="1"/>
-    <col min="4" max="4" width="22.84375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.4609375" customWidth="1"/>
+    <col min="1" max="1" width="7.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.5" customWidth="1"/>
+    <col min="4" max="4" width="22.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>19</v>
       </c>
@@ -2275,7 +2278,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>180</v>
       </c>
@@ -2292,7 +2295,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>196</v>
       </c>
@@ -2309,7 +2312,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>190</v>
       </c>
@@ -2326,7 +2329,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>181</v>
       </c>
@@ -2343,7 +2346,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>186</v>
       </c>
@@ -2360,7 +2363,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.15">
       <c r="D8" s="4" t="s">
         <v>34</v>
       </c>
@@ -2393,16 +2396,16 @@
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.07421875" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="6.84375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="29" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.4609375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.4609375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>29</v>
       </c>
@@ -2420,7 +2423,7 @@
       </c>
       <c r="G1" s="18"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2437,7 +2440,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A3">
         <v>1</v>
       </c>
@@ -2453,14 +2456,14 @@
       <c r="E3" s="17" t="s">
         <v>202</v>
       </c>
-      <c r="G3" s="20" t="s">
+      <c r="G3" s="21" t="s">
         <v>203</v>
       </c>
-      <c r="H3" s="20"/>
-      <c r="I3" s="20"/>
-      <c r="J3" s="20"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="H3" s="21"/>
+      <c r="I3" s="21"/>
+      <c r="J3" s="21"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A4">
         <v>1</v>
       </c>
@@ -2477,7 +2480,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A5">
         <v>1</v>
       </c>
@@ -2494,7 +2497,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A6">
         <v>1</v>
       </c>
@@ -2511,7 +2514,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A7">
         <v>1</v>
       </c>
@@ -2528,7 +2531,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A8">
         <v>1</v>
       </c>
@@ -2545,7 +2548,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A9">
         <v>1</v>
       </c>
@@ -2562,7 +2565,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A10">
         <v>1</v>
       </c>
@@ -2579,7 +2582,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A11">
         <v>1</v>
       </c>
@@ -2596,7 +2599,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A12">
         <v>2</v>
       </c>
@@ -2613,7 +2616,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A13">
         <v>2</v>
       </c>
@@ -2630,7 +2633,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A14">
         <v>2</v>
       </c>
@@ -2647,7 +2650,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A15">
         <v>2</v>
       </c>
@@ -2664,7 +2667,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A16">
         <v>2</v>
       </c>
@@ -2681,7 +2684,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A17">
         <v>2</v>
       </c>
@@ -2698,7 +2701,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A18">
         <v>2</v>
       </c>
@@ -2715,7 +2718,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A19">
         <v>2</v>
       </c>
@@ -2732,7 +2735,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A20">
         <v>2</v>
       </c>
@@ -2749,7 +2752,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A21">
         <v>2</v>
       </c>
@@ -2766,7 +2769,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A22">
         <v>3</v>
       </c>
@@ -2783,7 +2786,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A23">
         <v>3</v>
       </c>
@@ -2800,7 +2803,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A24">
         <v>3</v>
       </c>
@@ -2817,7 +2820,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A25">
         <v>3</v>
       </c>
@@ -2834,7 +2837,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A26">
         <v>3</v>
       </c>
@@ -2851,7 +2854,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A27">
         <v>3</v>
       </c>
@@ -2868,7 +2871,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A28">
         <v>3</v>
       </c>
@@ -2885,7 +2888,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A29">
         <v>3</v>
       </c>
@@ -2902,7 +2905,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A30">
         <v>3</v>
       </c>
@@ -2919,7 +2922,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A31">
         <v>3</v>
       </c>
@@ -2936,7 +2939,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A32">
         <v>4</v>
       </c>
@@ -2953,7 +2956,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A33">
         <v>4</v>
       </c>
@@ -2970,7 +2973,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A34">
         <v>4</v>
       </c>
@@ -2987,7 +2990,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A35">
         <v>4</v>
       </c>
@@ -3004,7 +3007,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A36">
         <v>4</v>
       </c>
@@ -3021,7 +3024,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A37">
         <v>4</v>
       </c>
@@ -3038,7 +3041,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A38">
         <v>4</v>
       </c>
@@ -3055,7 +3058,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A39">
         <v>4</v>
       </c>
@@ -3072,7 +3075,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A40">
         <v>4</v>
       </c>
@@ -3089,7 +3092,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A41">
         <v>4</v>
       </c>
@@ -3120,51 +3123,51 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="150" workbookViewId="0">
+    <sheetView topLeftCell="A8" zoomScale="150" workbookViewId="0">
       <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.07421875" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="10.84375" style="7"/>
-    <col min="2" max="2" width="10.23046875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.84375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.3046875" customWidth="1"/>
-    <col min="5" max="5" width="6.84375" customWidth="1"/>
-    <col min="6" max="6" width="12.4609375" style="9" customWidth="1"/>
+    <col min="1" max="1" width="10.83203125" style="7"/>
+    <col min="2" max="2" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.33203125" customWidth="1"/>
+    <col min="5" max="5" width="6.83203125" customWidth="1"/>
+    <col min="6" max="6" width="12.5" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A1" s="7" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A2" s="7" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A3" s="7" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A5" s="7" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A6" s="7" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A8" s="7" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A14" s="4" t="s">
         <v>161</v>
       </c>
@@ -3187,7 +3190,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
         <v>162</v>
       </c>
@@ -3203,7 +3206,7 @@
       <c r="F15" s="14"/>
       <c r="G15" s="9"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
         <v>163</v>
       </c>
@@ -3227,7 +3230,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A17" s="7" t="s">
         <v>164</v>
       </c>
@@ -3252,7 +3255,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A18" s="7" t="s">
         <v>165</v>
       </c>
@@ -3277,7 +3280,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A19" s="7" t="s">
         <v>166</v>
       </c>
@@ -3317,17 +3320,17 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.07421875" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="10.84375" style="2"/>
-    <col min="2" max="2" width="16.69140625" customWidth="1"/>
-    <col min="3" max="3" width="12.4609375" customWidth="1"/>
-    <col min="4" max="4" width="7.15234375" customWidth="1"/>
-    <col min="5" max="5" width="6.84375" customWidth="1"/>
-    <col min="6" max="6" width="12.4609375" style="9" customWidth="1"/>
+    <col min="1" max="1" width="10.83203125" style="2"/>
+    <col min="2" max="2" width="16.6640625" customWidth="1"/>
+    <col min="3" max="3" width="12.5" customWidth="1"/>
+    <col min="4" max="4" width="7.1640625" customWidth="1"/>
+    <col min="5" max="5" width="6.83203125" customWidth="1"/>
+    <col min="6" max="6" width="12.5" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -3347,7 +3350,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A2" s="13">
         <v>42632</v>
       </c>
@@ -3358,7 +3361,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A3" s="13">
         <v>42647</v>
       </c>
@@ -3380,17 +3383,17 @@
         <v>125.00000000000001</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A4" s="13">
         <v>42661</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A5" s="13">
         <v>42675</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A6" s="13">
         <v>42689</v>
       </c>
@@ -3407,23 +3410,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:I63"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="F53" sqref="F53"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.07421875" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="33.07421875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.4609375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.4609375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.3046875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.69140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.4609375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.3046875" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.33203125" style="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
@@ -3452,7 +3455,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>114</v>
       </c>
@@ -3471,8 +3474,17 @@
       <c r="F2">
         <v>60</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="G2">
+        <v>42</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A3" s="17" t="s">
         <v>204</v>
       </c>
@@ -3487,11 +3499,11 @@
       </c>
       <c r="I3" s="7"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A4" s="17" t="s">
         <v>205</v>
       </c>
-      <c r="B4" s="21" t="s">
+      <c r="B4" s="20" t="s">
         <v>272</v>
       </c>
       <c r="C4" s="17" t="s">
@@ -3502,7 +3514,7 @@
       </c>
       <c r="I4" s="7"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A5" s="17" t="s">
         <v>206</v>
       </c>
@@ -3517,7 +3529,7 @@
       </c>
       <c r="I5" s="7"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>115</v>
       </c>
@@ -3536,8 +3548,17 @@
       <c r="F6">
         <v>100</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="G6">
+        <v>43</v>
+      </c>
+      <c r="H6">
+        <v>1</v>
+      </c>
+      <c r="I6" s="7" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A7" s="17" t="s">
         <v>209</v>
       </c>
@@ -3552,7 +3573,7 @@
       </c>
       <c r="I7" s="7"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A8" s="17" t="s">
         <v>210</v>
       </c>
@@ -3567,7 +3588,7 @@
       </c>
       <c r="I8" s="7"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A9" s="17" t="s">
         <v>211</v>
       </c>
@@ -3582,7 +3603,7 @@
       </c>
       <c r="I9" s="7"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A10" s="17" t="s">
         <v>224</v>
       </c>
@@ -3597,7 +3618,7 @@
       </c>
       <c r="I10" s="7"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
         <v>116</v>
       </c>
@@ -3617,7 +3638,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A12" s="17" t="s">
         <v>215</v>
       </c>
@@ -3632,7 +3653,7 @@
       </c>
       <c r="I12" s="7"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A13" s="17" t="s">
         <v>216</v>
       </c>
@@ -3647,7 +3668,7 @@
       </c>
       <c r="I13" s="7"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A14" s="17" t="s">
         <v>217</v>
       </c>
@@ -3662,7 +3683,7 @@
       </c>
       <c r="I14" s="7"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A15" s="17" t="s">
         <v>236</v>
       </c>
@@ -3677,7 +3698,7 @@
       </c>
       <c r="I15" s="7"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
         <v>117</v>
       </c>
@@ -3697,7 +3718,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A17" s="17" t="s">
         <v>220</v>
       </c>
@@ -3712,7 +3733,7 @@
       </c>
       <c r="I17" s="7"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A18" s="17" t="s">
         <v>221</v>
       </c>
@@ -3727,7 +3748,7 @@
       </c>
       <c r="I18" s="7"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A19" s="17" t="s">
         <v>222</v>
       </c>
@@ -3742,7 +3763,7 @@
       </c>
       <c r="I19" s="7"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A20" s="17" t="s">
         <v>223</v>
       </c>
@@ -3757,7 +3778,7 @@
       </c>
       <c r="I20" s="7"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A21" s="17" t="s">
         <v>237</v>
       </c>
@@ -3772,7 +3793,7 @@
       </c>
       <c r="I21" s="7"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A22" t="s">
         <v>118</v>
       </c>
@@ -3792,7 +3813,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A23" s="17" t="s">
         <v>229</v>
       </c>
@@ -3807,7 +3828,7 @@
       </c>
       <c r="I23" s="7"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A24" s="17" t="s">
         <v>230</v>
       </c>
@@ -3822,7 +3843,7 @@
       </c>
       <c r="I24" s="7"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A25" s="17" t="s">
         <v>231</v>
       </c>
@@ -3837,7 +3858,7 @@
       </c>
       <c r="I25" s="7"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A26" s="17" t="s">
         <v>232</v>
       </c>
@@ -3852,7 +3873,7 @@
       </c>
       <c r="I26" s="7"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A27" s="17" t="s">
         <v>233</v>
       </c>
@@ -3867,7 +3888,7 @@
       </c>
       <c r="I27" s="7"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A28" t="s">
         <v>119</v>
       </c>
@@ -3887,7 +3908,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A29" s="17" t="s">
         <v>238</v>
       </c>
@@ -3902,7 +3923,7 @@
       </c>
       <c r="I29" s="7"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A30" s="17" t="s">
         <v>239</v>
       </c>
@@ -3917,7 +3938,7 @@
       </c>
       <c r="I30" s="7"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A31" s="17" t="s">
         <v>240</v>
       </c>
@@ -3932,7 +3953,7 @@
       </c>
       <c r="I31" s="7"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A32" s="17" t="s">
         <v>241</v>
       </c>
@@ -3947,7 +3968,7 @@
       </c>
       <c r="I32" s="7"/>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A33" s="17" t="s">
         <v>242</v>
       </c>
@@ -3962,7 +3983,7 @@
       </c>
       <c r="I33" s="7"/>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A34" t="s">
         <v>120</v>
       </c>
@@ -3982,7 +4003,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A35" s="17" t="s">
         <v>244</v>
       </c>
@@ -3997,7 +4018,7 @@
       </c>
       <c r="I35" s="7"/>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A36" s="17" t="s">
         <v>245</v>
       </c>
@@ -4012,7 +4033,7 @@
       </c>
       <c r="I36" s="7"/>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A37" s="17" t="s">
         <v>246</v>
       </c>
@@ -4027,7 +4048,7 @@
       </c>
       <c r="I37" s="7"/>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A38" s="17" t="s">
         <v>247</v>
       </c>
@@ -4042,7 +4063,7 @@
       </c>
       <c r="I38" s="7"/>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A39" s="17" t="s">
         <v>248</v>
       </c>
@@ -4057,7 +4078,7 @@
       </c>
       <c r="I39" s="7"/>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A40" s="17" t="s">
         <v>251</v>
       </c>
@@ -4072,7 +4093,7 @@
       </c>
       <c r="I40" s="7"/>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A41" t="s">
         <v>121</v>
       </c>
@@ -4092,7 +4113,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A42" s="17" t="s">
         <v>254</v>
       </c>
@@ -4107,7 +4128,7 @@
       </c>
       <c r="I42" s="7"/>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A43" s="17" t="s">
         <v>255</v>
       </c>
@@ -4122,7 +4143,7 @@
       </c>
       <c r="I43" s="7"/>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A44" s="17" t="s">
         <v>256</v>
       </c>
@@ -4137,7 +4158,7 @@
       </c>
       <c r="I44" s="7"/>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A45" t="s">
         <v>122</v>
       </c>
@@ -4157,7 +4178,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A46" s="17" t="s">
         <v>257</v>
       </c>
@@ -4172,7 +4193,7 @@
       </c>
       <c r="I46" s="7"/>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A47" s="17" t="s">
         <v>258</v>
       </c>
@@ -4187,7 +4208,7 @@
       </c>
       <c r="I47" s="7"/>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A48" s="17" t="s">
         <v>259</v>
       </c>
@@ -4202,7 +4223,7 @@
       </c>
       <c r="I48" s="7"/>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A49" s="17" t="s">
         <v>260</v>
       </c>
@@ -4217,7 +4238,7 @@
       </c>
       <c r="I49" s="7"/>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A50" t="s">
         <v>123</v>
       </c>
@@ -4237,11 +4258,11 @@
         <v>240</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A51" s="17" t="s">
         <v>264</v>
       </c>
-      <c r="B51" s="21" t="s">
+      <c r="B51" s="20" t="s">
         <v>265</v>
       </c>
       <c r="C51" s="17" t="s">
@@ -4251,11 +4272,11 @@
         <v>202</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A52" s="17" t="s">
         <v>266</v>
       </c>
-      <c r="B52" s="21" t="s">
+      <c r="B52" s="20" t="s">
         <v>213</v>
       </c>
       <c r="C52" s="17" t="s">
@@ -4266,11 +4287,11 @@
       </c>
       <c r="I52" s="7"/>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A53" s="17" t="s">
         <v>267</v>
       </c>
-      <c r="B53" s="21" t="s">
+      <c r="B53" s="20" t="s">
         <v>212</v>
       </c>
       <c r="C53" s="17" t="s">
@@ -4281,11 +4302,11 @@
       </c>
       <c r="I53" s="7"/>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A54" s="17" t="s">
         <v>268</v>
       </c>
-      <c r="B54" s="21" t="s">
+      <c r="B54" s="20" t="s">
         <v>269</v>
       </c>
       <c r="C54" s="17" t="s">
@@ -4295,11 +4316,11 @@
         <v>202</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A55" s="17" t="s">
         <v>270</v>
       </c>
-      <c r="B55" s="21" t="s">
+      <c r="B55" s="20" t="s">
         <v>271</v>
       </c>
       <c r="C55" s="17" t="s">
@@ -4310,25 +4331,25 @@
       </c>
       <c r="I55" s="7"/>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A56" s="17"/>
       <c r="I56" s="7"/>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="B57" s="5" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B58" s="5"/>
       <c r="I58" s="7"/>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="B59" s="5" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="B63" s="5" t="s">
         <v>32</v>
       </c>
@@ -4348,9 +4369,9 @@
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.07421875" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="28" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
@@ -4394,9 +4415,9 @@
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.07421875" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="28" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
@@ -4439,9 +4460,9 @@
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.07421875" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="28" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
@@ -4484,13 +4505,13 @@
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.07421875" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="2" max="2" width="28.15234375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="49.4609375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="28.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="49.5" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" s="4" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>113</v>
       </c>
@@ -4501,7 +4522,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>114</v>
       </c>
@@ -4512,7 +4533,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" ht="17" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>115</v>
       </c>
@@ -4523,7 +4544,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="17" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>116</v>
       </c>
@@ -4534,7 +4555,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>117</v>
       </c>
@@ -4545,7 +4566,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>118</v>
       </c>
@@ -4556,7 +4577,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" ht="17" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
         <v>119</v>
       </c>
@@ -4567,7 +4588,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="45" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" ht="51" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>120</v>
       </c>
@@ -4578,7 +4599,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
         <v>121</v>
       </c>
@@ -4589,7 +4610,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>122</v>
       </c>
@@ -4600,7 +4621,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" ht="51" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
         <v>123</v>
       </c>
@@ -4611,7 +4632,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
         <v>124</v>
       </c>
@@ -4622,7 +4643,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="45" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" ht="51" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
         <v>125</v>
       </c>
@@ -4633,7 +4654,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="45" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" ht="68" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
         <v>126</v>
       </c>
@@ -4644,7 +4665,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
         <v>127</v>
       </c>
@@ -4655,7 +4676,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" ht="17" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
         <v>128</v>
       </c>
@@ -4666,7 +4687,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
         <v>129</v>
       </c>
@@ -4677,7 +4698,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" ht="17" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
         <v>130</v>
       </c>
@@ -4688,7 +4709,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" ht="17" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
         <v>131</v>
       </c>
@@ -4699,7 +4720,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" ht="17" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
         <v>132</v>
       </c>
@@ -4710,7 +4731,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
         <v>133</v>
       </c>
@@ -4721,7 +4742,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A22" t="s">
         <v>134</v>
       </c>
@@ -4732,7 +4753,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A23" t="s">
         <v>135</v>
       </c>
@@ -4743,7 +4764,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A24" t="s">
         <v>136</v>
       </c>
@@ -4754,7 +4775,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="45" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" ht="51" x14ac:dyDescent="0.15">
       <c r="A25" t="s">
         <v>137</v>
       </c>
@@ -4765,7 +4786,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A26" t="s">
         <v>138</v>
       </c>
@@ -4776,7 +4797,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="105" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" ht="136" x14ac:dyDescent="0.15">
       <c r="A27" t="s">
         <v>139</v>
       </c>
@@ -4787,7 +4808,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A28" t="s">
         <v>140</v>
       </c>
@@ -4798,7 +4819,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A29" t="s">
         <v>141</v>
       </c>
@@ -4809,7 +4830,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" ht="17" x14ac:dyDescent="0.15">
       <c r="A30" t="s">
         <v>142</v>
       </c>
@@ -4820,7 +4841,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" ht="17" x14ac:dyDescent="0.15">
       <c r="A31" t="s">
         <v>143</v>
       </c>
@@ -4831,7 +4852,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A32" t="s">
         <v>144</v>
       </c>
@@ -4842,7 +4863,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" ht="17" x14ac:dyDescent="0.15">
       <c r="A33" t="s">
         <v>145</v>
       </c>
@@ -4853,7 +4874,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A34" t="s">
         <v>146</v>
       </c>
@@ -4864,7 +4885,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" ht="51" x14ac:dyDescent="0.15">
       <c r="A35" t="s">
         <v>147</v>
       </c>
@@ -4875,7 +4896,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A36" t="s">
         <v>148</v>
       </c>
@@ -4886,7 +4907,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A37" t="s">
         <v>149</v>
       </c>
@@ -4897,7 +4918,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A38" t="s">
         <v>150</v>
       </c>
@@ -4908,7 +4929,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A39" t="s">
         <v>151</v>
       </c>
@@ -4919,7 +4940,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A40" t="s">
         <v>152</v>
       </c>
@@ -4930,7 +4951,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A41" t="s">
         <v>153</v>
       </c>
@@ -4941,7 +4962,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A42" t="s">
         <v>154</v>
       </c>
@@ -4952,7 +4973,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A43" t="s">
         <v>155</v>
       </c>

</xml_diff>

<commit_message>
Added updates to US 02, 07 and 08
Added updates to User Story 02, 07 and 08
</commit_message>
<xml_diff>
--- a/Team2Report.xlsx
+++ b/Team2Report.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10913"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10914"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Avaneesh/Desktop/CS 555/avaneeshSprint1/Agile_Methods_Project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/srikanth/Documenta/StevensInstitute/SoftwareEngg/SSW-555/Sprint1/Agile_Methods_Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{038DF635-DC4D-EA49-A9AB-04B6290C8E06}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39E29418-2CF0-D24E-956B-114A8A6FE7AC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="26940" yWindow="1980" windowWidth="33760" windowHeight="17480" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1340" yWindow="1700" windowWidth="33760" windowHeight="17480" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -23,19 +23,10 @@
     <sheet name="Sprint4" sheetId="6" r:id="rId8"/>
     <sheet name="Stories" sheetId="11" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -45,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="608" uniqueCount="274">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="630" uniqueCount="276">
   <si>
     <t>Date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -897,6 +888,12 @@
   </si>
   <si>
     <t>Completed</t>
+  </si>
+  <si>
+    <t>60 mins</t>
+  </si>
+  <si>
+    <t>90 mins</t>
   </si>
 </sst>
 </file>
@@ -1045,7 +1042,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1081,6 +1078,12 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="66">
@@ -2372,7 +2375,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D4">
+  <sortState ref="A2:D4">
     <sortCondition ref="C2:C4"/>
   </sortState>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -3410,8 +3413,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:I63"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="I60" sqref="I60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -3477,10 +3480,10 @@
       <c r="G2">
         <v>42</v>
       </c>
-      <c r="H2">
-        <v>1</v>
-      </c>
-      <c r="I2" s="6" t="s">
+      <c r="H2" s="22" t="s">
+        <v>274</v>
+      </c>
+      <c r="I2" s="23" t="s">
         <v>273</v>
       </c>
     </row>
@@ -3497,7 +3500,9 @@
       <c r="D3" s="17" t="s">
         <v>202</v>
       </c>
-      <c r="I3" s="7"/>
+      <c r="I3" s="23" t="s">
+        <v>273</v>
+      </c>
     </row>
     <row r="4" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A4" s="17" t="s">
@@ -3512,7 +3517,9 @@
       <c r="D4" s="17" t="s">
         <v>202</v>
       </c>
-      <c r="I4" s="7"/>
+      <c r="I4" s="23" t="s">
+        <v>273</v>
+      </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A5" s="17" t="s">
@@ -3527,7 +3534,9 @@
       <c r="D5" s="17" t="s">
         <v>202</v>
       </c>
-      <c r="I5" s="7"/>
+      <c r="I5" s="23" t="s">
+        <v>273</v>
+      </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
@@ -3549,12 +3558,12 @@
         <v>100</v>
       </c>
       <c r="G6">
-        <v>43</v>
-      </c>
-      <c r="H6">
-        <v>1</v>
-      </c>
-      <c r="I6" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="H6" s="22" t="s">
+        <v>275</v>
+      </c>
+      <c r="I6" s="23" t="s">
         <v>273</v>
       </c>
     </row>
@@ -3571,7 +3580,9 @@
       <c r="D7" s="17" t="s">
         <v>202</v>
       </c>
-      <c r="I7" s="7"/>
+      <c r="I7" s="23" t="s">
+        <v>273</v>
+      </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A8" s="17" t="s">
@@ -3586,7 +3597,9 @@
       <c r="D8" s="17" t="s">
         <v>202</v>
       </c>
-      <c r="I8" s="7"/>
+      <c r="I8" s="23" t="s">
+        <v>273</v>
+      </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A9" s="17" t="s">
@@ -3601,7 +3614,9 @@
       <c r="D9" s="17" t="s">
         <v>202</v>
       </c>
-      <c r="I9" s="7"/>
+      <c r="I9" s="23" t="s">
+        <v>273</v>
+      </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A10" s="17" t="s">
@@ -3616,7 +3631,9 @@
       <c r="D10" s="17" t="s">
         <v>202</v>
       </c>
-      <c r="I10" s="7"/>
+      <c r="I10" s="23" t="s">
+        <v>273</v>
+      </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
@@ -3637,6 +3654,7 @@
       <c r="F11">
         <v>100</v>
       </c>
+      <c r="I11" s="23"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A12" s="17" t="s">
@@ -3651,7 +3669,7 @@
       <c r="D12" s="17" t="s">
         <v>202</v>
       </c>
-      <c r="I12" s="7"/>
+      <c r="I12" s="23"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A13" s="17" t="s">
@@ -3666,7 +3684,7 @@
       <c r="D13" s="17" t="s">
         <v>202</v>
       </c>
-      <c r="I13" s="7"/>
+      <c r="I13" s="23"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A14" s="17" t="s">
@@ -3681,7 +3699,7 @@
       <c r="D14" s="17" t="s">
         <v>202</v>
       </c>
-      <c r="I14" s="7"/>
+      <c r="I14" s="23"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A15" s="17" t="s">
@@ -3696,7 +3714,7 @@
       <c r="D15" s="17" t="s">
         <v>202</v>
       </c>
-      <c r="I15" s="7"/>
+      <c r="I15" s="23"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
@@ -3717,6 +3735,7 @@
       <c r="F16">
         <v>140</v>
       </c>
+      <c r="I16" s="23"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A17" s="17" t="s">
@@ -3731,7 +3750,7 @@
       <c r="D17" s="17" t="s">
         <v>202</v>
       </c>
-      <c r="I17" s="7"/>
+      <c r="I17" s="23"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A18" s="17" t="s">
@@ -3746,7 +3765,7 @@
       <c r="D18" s="17" t="s">
         <v>202</v>
       </c>
-      <c r="I18" s="7"/>
+      <c r="I18" s="23"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A19" s="17" t="s">
@@ -3761,7 +3780,7 @@
       <c r="D19" s="17" t="s">
         <v>202</v>
       </c>
-      <c r="I19" s="7"/>
+      <c r="I19" s="23"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A20" s="17" t="s">
@@ -3776,7 +3795,7 @@
       <c r="D20" s="17" t="s">
         <v>202</v>
       </c>
-      <c r="I20" s="7"/>
+      <c r="I20" s="23"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A21" s="17" t="s">
@@ -3791,7 +3810,7 @@
       <c r="D21" s="17" t="s">
         <v>202</v>
       </c>
-      <c r="I21" s="7"/>
+      <c r="I21" s="23"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A22" t="s">
@@ -3812,6 +3831,7 @@
       <c r="F22">
         <v>140</v>
       </c>
+      <c r="I22" s="23"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A23" s="17" t="s">
@@ -3826,7 +3846,7 @@
       <c r="D23" s="17" t="s">
         <v>202</v>
       </c>
-      <c r="I23" s="7"/>
+      <c r="I23" s="23"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A24" s="17" t="s">
@@ -3841,7 +3861,7 @@
       <c r="D24" s="17" t="s">
         <v>202</v>
       </c>
-      <c r="I24" s="7"/>
+      <c r="I24" s="23"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A25" s="17" t="s">
@@ -3856,7 +3876,7 @@
       <c r="D25" s="17" t="s">
         <v>202</v>
       </c>
-      <c r="I25" s="7"/>
+      <c r="I25" s="23"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A26" s="17" t="s">
@@ -3871,7 +3891,7 @@
       <c r="D26" s="17" t="s">
         <v>202</v>
       </c>
-      <c r="I26" s="7"/>
+      <c r="I26" s="23"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A27" s="17" t="s">
@@ -3886,7 +3906,7 @@
       <c r="D27" s="17" t="s">
         <v>202</v>
       </c>
-      <c r="I27" s="7"/>
+      <c r="I27" s="23"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A28" t="s">
@@ -3907,6 +3927,7 @@
       <c r="F28">
         <v>140</v>
       </c>
+      <c r="I28" s="23"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A29" s="17" t="s">
@@ -3921,7 +3942,7 @@
       <c r="D29" s="17" t="s">
         <v>202</v>
       </c>
-      <c r="I29" s="7"/>
+      <c r="I29" s="23"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A30" s="17" t="s">
@@ -3936,7 +3957,7 @@
       <c r="D30" s="17" t="s">
         <v>202</v>
       </c>
-      <c r="I30" s="7"/>
+      <c r="I30" s="23"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A31" s="17" t="s">
@@ -3951,7 +3972,7 @@
       <c r="D31" s="17" t="s">
         <v>202</v>
       </c>
-      <c r="I31" s="7"/>
+      <c r="I31" s="23"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A32" s="17" t="s">
@@ -3966,7 +3987,7 @@
       <c r="D32" s="17" t="s">
         <v>202</v>
       </c>
-      <c r="I32" s="7"/>
+      <c r="I32" s="23"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A33" s="17" t="s">
@@ -3981,7 +4002,7 @@
       <c r="D33" s="17" t="s">
         <v>202</v>
       </c>
-      <c r="I33" s="7"/>
+      <c r="I33" s="23"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A34" t="s">
@@ -4002,6 +4023,15 @@
       <c r="F34">
         <v>180</v>
       </c>
+      <c r="G34">
+        <v>34</v>
+      </c>
+      <c r="H34" s="22" t="s">
+        <v>274</v>
+      </c>
+      <c r="I34" s="23" t="s">
+        <v>273</v>
+      </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A35" s="17" t="s">
@@ -4016,7 +4046,9 @@
       <c r="D35" s="17" t="s">
         <v>202</v>
       </c>
-      <c r="I35" s="7"/>
+      <c r="I35" s="23" t="s">
+        <v>273</v>
+      </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A36" s="17" t="s">
@@ -4031,7 +4063,9 @@
       <c r="D36" s="17" t="s">
         <v>202</v>
       </c>
-      <c r="I36" s="7"/>
+      <c r="I36" s="23" t="s">
+        <v>273</v>
+      </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A37" s="17" t="s">
@@ -4046,7 +4080,9 @@
       <c r="D37" s="17" t="s">
         <v>202</v>
       </c>
-      <c r="I37" s="7"/>
+      <c r="I37" s="23" t="s">
+        <v>273</v>
+      </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A38" s="17" t="s">
@@ -4061,7 +4097,9 @@
       <c r="D38" s="17" t="s">
         <v>202</v>
       </c>
-      <c r="I38" s="7"/>
+      <c r="I38" s="23" t="s">
+        <v>273</v>
+      </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A39" s="17" t="s">
@@ -4076,7 +4114,9 @@
       <c r="D39" s="17" t="s">
         <v>202</v>
       </c>
-      <c r="I39" s="7"/>
+      <c r="I39" s="23" t="s">
+        <v>273</v>
+      </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A40" s="17" t="s">
@@ -4091,7 +4131,9 @@
       <c r="D40" s="17" t="s">
         <v>202</v>
       </c>
-      <c r="I40" s="7"/>
+      <c r="I40" s="23" t="s">
+        <v>273</v>
+      </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A41" t="s">
@@ -4112,6 +4154,15 @@
       <c r="F41">
         <v>60</v>
       </c>
+      <c r="G41">
+        <v>44</v>
+      </c>
+      <c r="H41" s="22" t="s">
+        <v>275</v>
+      </c>
+      <c r="I41" s="23" t="s">
+        <v>273</v>
+      </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A42" s="17" t="s">
@@ -4126,7 +4177,9 @@
       <c r="D42" s="17" t="s">
         <v>202</v>
       </c>
-      <c r="I42" s="7"/>
+      <c r="I42" s="23" t="s">
+        <v>273</v>
+      </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A43" s="17" t="s">
@@ -4141,7 +4194,9 @@
       <c r="D43" s="17" t="s">
         <v>202</v>
       </c>
-      <c r="I43" s="7"/>
+      <c r="I43" s="23" t="s">
+        <v>273</v>
+      </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A44" s="17" t="s">
@@ -4156,7 +4211,9 @@
       <c r="D44" s="17" t="s">
         <v>202</v>
       </c>
-      <c r="I44" s="7"/>
+      <c r="I44" s="23" t="s">
+        <v>273</v>
+      </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A45" t="s">
@@ -4177,6 +4234,7 @@
       <c r="F45">
         <v>80</v>
       </c>
+      <c r="I45" s="23"/>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A46" s="17" t="s">
@@ -4191,7 +4249,7 @@
       <c r="D46" s="17" t="s">
         <v>202</v>
       </c>
-      <c r="I46" s="7"/>
+      <c r="I46" s="23"/>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A47" s="17" t="s">
@@ -4206,7 +4264,7 @@
       <c r="D47" s="17" t="s">
         <v>202</v>
       </c>
-      <c r="I47" s="7"/>
+      <c r="I47" s="23"/>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A48" s="17" t="s">
@@ -4221,7 +4279,7 @@
       <c r="D48" s="17" t="s">
         <v>202</v>
       </c>
-      <c r="I48" s="7"/>
+      <c r="I48" s="23"/>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A49" s="17" t="s">
@@ -4236,7 +4294,7 @@
       <c r="D49" s="17" t="s">
         <v>202</v>
       </c>
-      <c r="I49" s="7"/>
+      <c r="I49" s="23"/>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A50" t="s">
@@ -4257,6 +4315,7 @@
       <c r="F50">
         <v>240</v>
       </c>
+      <c r="I50" s="23"/>
     </row>
     <row r="51" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A51" s="17" t="s">
@@ -4271,6 +4330,7 @@
       <c r="D51" s="17" t="s">
         <v>202</v>
       </c>
+      <c r="I51" s="23"/>
     </row>
     <row r="52" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A52" s="17" t="s">
@@ -4285,7 +4345,7 @@
       <c r="D52" s="17" t="s">
         <v>202</v>
       </c>
-      <c r="I52" s="7"/>
+      <c r="I52" s="23"/>
     </row>
     <row r="53" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A53" s="17" t="s">
@@ -4300,7 +4360,7 @@
       <c r="D53" s="17" t="s">
         <v>202</v>
       </c>
-      <c r="I53" s="7"/>
+      <c r="I53" s="23"/>
     </row>
     <row r="54" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A54" s="17" t="s">
@@ -4315,6 +4375,7 @@
       <c r="D54" s="17" t="s">
         <v>202</v>
       </c>
+      <c r="I54" s="23"/>
     </row>
     <row r="55" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A55" s="17" t="s">
@@ -4329,7 +4390,7 @@
       <c r="D55" s="17" t="s">
         <v>202</v>
       </c>
-      <c r="I55" s="7"/>
+      <c r="I55" s="23"/>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A56" s="17"/>

</xml_diff>

<commit_message>
Added Test/User Story 01 & 02
</commit_message>
<xml_diff>
--- a/Team2Report.xlsx
+++ b/Team2Report.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23127"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ztyle\Documents\SSW 555\SSW_555_Project_Sprint1\Agile_Methods_Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RedRo\OneDrive\Documents\Academic Texts\COOOOOOODE\Python Workspace\anaconda\Agile_Methods_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7254D44F-2F9C-4F9E-BDC2-6E484ED628B8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14ED2E0F-C8CA-4EBE-BDD4-733CE2D649CC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,6 @@
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -45,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="683" uniqueCount="281">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="694" uniqueCount="281">
   <si>
     <t>Date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -1106,11 +1105,11 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="66">
@@ -1388,7 +1387,7 @@
                   <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>34</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2282,16 +2281,16 @@
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.84375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.15234375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.4609375" customWidth="1"/>
-    <col min="4" max="4" width="22.84375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.4609375" customWidth="1"/>
+    <col min="1" max="1" width="7.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.453125" customWidth="1"/>
+    <col min="4" max="4" width="22.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>19</v>
       </c>
@@ -2308,7 +2307,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>180</v>
       </c>
@@ -2325,7 +2324,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>196</v>
       </c>
@@ -2342,7 +2341,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>190</v>
       </c>
@@ -2359,7 +2358,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>181</v>
       </c>
@@ -2376,7 +2375,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>186</v>
       </c>
@@ -2393,7 +2392,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D8" s="4" t="s">
         <v>34</v>
       </c>
@@ -2422,20 +2421,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J41"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" zoomScale="150" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12:E21"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="6.84375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.81640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="29" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.4609375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.4609375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>29</v>
       </c>
@@ -2453,7 +2452,7 @@
       </c>
       <c r="G1" s="18"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2470,7 +2469,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -2486,14 +2485,14 @@
       <c r="E3" s="17" t="s">
         <v>202</v>
       </c>
-      <c r="G3" s="23" t="s">
+      <c r="G3" s="24" t="s">
         <v>203</v>
       </c>
-      <c r="H3" s="23"/>
-      <c r="I3" s="23"/>
-      <c r="J3" s="23"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="H3" s="24"/>
+      <c r="I3" s="24"/>
+      <c r="J3" s="24"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1</v>
       </c>
@@ -2510,7 +2509,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1</v>
       </c>
@@ -2527,7 +2526,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>1</v>
       </c>
@@ -2544,7 +2543,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>1</v>
       </c>
@@ -2561,7 +2560,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>1</v>
       </c>
@@ -2578,7 +2577,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>1</v>
       </c>
@@ -2595,7 +2594,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>1</v>
       </c>
@@ -2612,7 +2611,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>1</v>
       </c>
@@ -2629,7 +2628,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>2</v>
       </c>
@@ -2646,7 +2645,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>2</v>
       </c>
@@ -2663,7 +2662,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>2</v>
       </c>
@@ -2680,7 +2679,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>2</v>
       </c>
@@ -2697,7 +2696,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>2</v>
       </c>
@@ -2714,7 +2713,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>2</v>
       </c>
@@ -2731,7 +2730,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>2</v>
       </c>
@@ -2748,7 +2747,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>2</v>
       </c>
@@ -2765,7 +2764,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>2</v>
       </c>
@@ -2782,7 +2781,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>2</v>
       </c>
@@ -2799,7 +2798,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>3</v>
       </c>
@@ -2816,7 +2815,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>3</v>
       </c>
@@ -2833,7 +2832,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>3</v>
       </c>
@@ -2850,7 +2849,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>3</v>
       </c>
@@ -2867,7 +2866,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>3</v>
       </c>
@@ -2884,7 +2883,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>3</v>
       </c>
@@ -2901,7 +2900,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>3</v>
       </c>
@@ -2918,7 +2917,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>3</v>
       </c>
@@ -2935,7 +2934,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>3</v>
       </c>
@@ -2952,7 +2951,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>3</v>
       </c>
@@ -2969,7 +2968,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>4</v>
       </c>
@@ -2986,7 +2985,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>4</v>
       </c>
@@ -3003,7 +3002,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>4</v>
       </c>
@@ -3020,7 +3019,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>4</v>
       </c>
@@ -3037,7 +3036,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>4</v>
       </c>
@@ -3054,7 +3053,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>4</v>
       </c>
@@ -3071,7 +3070,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>4</v>
       </c>
@@ -3088,7 +3087,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>4</v>
       </c>
@@ -3105,7 +3104,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>4</v>
       </c>
@@ -3122,7 +3121,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>4</v>
       </c>
@@ -3157,47 +3156,47 @@
       <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.84375" style="7"/>
-    <col min="2" max="2" width="10.15234375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.84375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.3046875" customWidth="1"/>
-    <col min="5" max="5" width="6.84375" customWidth="1"/>
-    <col min="6" max="6" width="12.4609375" style="9" customWidth="1"/>
+    <col min="1" max="1" width="10.81640625" style="7"/>
+    <col min="2" max="2" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.26953125" customWidth="1"/>
+    <col min="5" max="5" width="6.81640625" customWidth="1"/>
+    <col min="6" max="6" width="12.453125" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
         <v>161</v>
       </c>
@@ -3220,7 +3219,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>162</v>
       </c>
@@ -3236,7 +3235,7 @@
       <c r="F15" s="14"/>
       <c r="G15" s="9"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>163</v>
       </c>
@@ -3260,7 +3259,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="7" t="s">
         <v>164</v>
       </c>
@@ -3285,7 +3284,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="7" t="s">
         <v>165</v>
       </c>
@@ -3310,7 +3309,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="7" t="s">
         <v>166</v>
       </c>
@@ -3350,17 +3349,17 @@
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.84375" style="2"/>
-    <col min="2" max="2" width="16.69140625" customWidth="1"/>
-    <col min="3" max="3" width="12.4609375" customWidth="1"/>
-    <col min="4" max="4" width="7.15234375" customWidth="1"/>
-    <col min="5" max="5" width="6.84375" customWidth="1"/>
-    <col min="6" max="6" width="12.4609375" style="9" customWidth="1"/>
+    <col min="1" max="1" width="10.81640625" style="2"/>
+    <col min="2" max="2" width="16.7265625" customWidth="1"/>
+    <col min="3" max="3" width="12.453125" customWidth="1"/>
+    <col min="4" max="4" width="7.1796875" customWidth="1"/>
+    <col min="5" max="5" width="6.81640625" customWidth="1"/>
+    <col min="6" max="6" width="12.453125" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -3380,7 +3379,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="13">
         <v>42632</v>
       </c>
@@ -3391,42 +3390,42 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="13">
         <v>42647</v>
       </c>
       <c r="B3">
         <f>B2-COUNTIF(Sprint1!I2:I55, "Completed")</f>
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C3">
         <f>B2-B3</f>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D3">
         <f>Sprint1!G56</f>
-        <v>229</v>
+        <v>319</v>
       </c>
       <c r="E3">
         <f>Sprint1!H56</f>
-        <v>405</v>
+        <v>495</v>
       </c>
       <c r="F3" s="9">
         <f>(D3-D2)/E3*60</f>
-        <v>33.925925925925924</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+        <v>38.666666666666671</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="13">
         <v>42661</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="13">
         <v>42675</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="13">
         <v>42689</v>
       </c>
@@ -3443,23 +3442,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:I65"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="33" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.4609375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.4609375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.3046875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.69140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.4609375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.3046875" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.26953125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.7265625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.26953125" style="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
@@ -3488,7 +3487,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>114</v>
       </c>
@@ -3517,7 +3516,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="17" t="s">
         <v>204</v>
       </c>
@@ -3530,11 +3529,11 @@
       <c r="D3" s="17" t="s">
         <v>202</v>
       </c>
-      <c r="I3" s="24" t="s">
+      <c r="I3" s="23" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="17" t="s">
         <v>205</v>
       </c>
@@ -3547,11 +3546,11 @@
       <c r="D4" s="17" t="s">
         <v>202</v>
       </c>
-      <c r="I4" s="24" t="s">
+      <c r="I4" s="23" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="17" t="s">
         <v>206</v>
       </c>
@@ -3564,11 +3563,11 @@
       <c r="D5" s="17" t="s">
         <v>202</v>
       </c>
-      <c r="I5" s="24" t="s">
+      <c r="I5" s="23" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>115</v>
       </c>
@@ -3597,7 +3596,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="17" t="s">
         <v>209</v>
       </c>
@@ -3610,11 +3609,11 @@
       <c r="D7" s="17" t="s">
         <v>202</v>
       </c>
-      <c r="I7" s="24" t="s">
+      <c r="I7" s="23" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="17" t="s">
         <v>210</v>
       </c>
@@ -3627,11 +3626,11 @@
       <c r="D8" s="17" t="s">
         <v>202</v>
       </c>
-      <c r="I8" s="24" t="s">
+      <c r="I8" s="23" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="17" t="s">
         <v>211</v>
       </c>
@@ -3644,11 +3643,11 @@
       <c r="D9" s="17" t="s">
         <v>202</v>
       </c>
-      <c r="I9" s="24" t="s">
+      <c r="I9" s="23" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="17" t="s">
         <v>224</v>
       </c>
@@ -3661,11 +3660,11 @@
       <c r="D10" s="17" t="s">
         <v>202</v>
       </c>
-      <c r="I10" s="24" t="s">
+      <c r="I10" s="23" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>116</v>
       </c>
@@ -3684,9 +3683,17 @@
       <c r="F11">
         <v>100</v>
       </c>
-      <c r="I11" s="22"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="G11">
+        <v>45</v>
+      </c>
+      <c r="H11">
+        <v>60</v>
+      </c>
+      <c r="I11" s="23" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="17" t="s">
         <v>215</v>
       </c>
@@ -3699,9 +3706,11 @@
       <c r="D12" s="17" t="s">
         <v>202</v>
       </c>
-      <c r="I12" s="22"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I12" s="23" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="17" t="s">
         <v>216</v>
       </c>
@@ -3714,9 +3723,11 @@
       <c r="D13" s="17" t="s">
         <v>202</v>
       </c>
-      <c r="I13" s="22"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I13" s="23" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="17" t="s">
         <v>217</v>
       </c>
@@ -3729,9 +3740,11 @@
       <c r="D14" s="17" t="s">
         <v>202</v>
       </c>
-      <c r="I14" s="22"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I14" s="23" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="17" t="s">
         <v>236</v>
       </c>
@@ -3744,9 +3757,11 @@
       <c r="D15" s="17" t="s">
         <v>202</v>
       </c>
-      <c r="I15" s="22"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I15" s="23" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>117</v>
       </c>
@@ -3765,9 +3780,17 @@
       <c r="F16">
         <v>140</v>
       </c>
-      <c r="I16" s="22"/>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="G16">
+        <v>45</v>
+      </c>
+      <c r="H16">
+        <v>30</v>
+      </c>
+      <c r="I16" s="23" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="17" t="s">
         <v>220</v>
       </c>
@@ -3780,9 +3803,11 @@
       <c r="D17" s="17" t="s">
         <v>202</v>
       </c>
-      <c r="I17" s="22"/>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I17" s="23" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="17" t="s">
         <v>221</v>
       </c>
@@ -3795,9 +3820,11 @@
       <c r="D18" s="17" t="s">
         <v>202</v>
       </c>
-      <c r="I18" s="22"/>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I18" s="23" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="17" t="s">
         <v>222</v>
       </c>
@@ -3810,9 +3837,11 @@
       <c r="D19" s="17" t="s">
         <v>202</v>
       </c>
-      <c r="I19" s="22"/>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I19" s="23" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="17" t="s">
         <v>223</v>
       </c>
@@ -3825,9 +3854,11 @@
       <c r="D20" s="17" t="s">
         <v>202</v>
       </c>
-      <c r="I20" s="22"/>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I20" s="23" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" s="17" t="s">
         <v>237</v>
       </c>
@@ -3840,9 +3871,11 @@
       <c r="D21" s="17" t="s">
         <v>202</v>
       </c>
-      <c r="I21" s="22"/>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I21" s="23" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>118</v>
       </c>
@@ -3863,7 +3896,7 @@
       </c>
       <c r="I22" s="22"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" s="17" t="s">
         <v>229</v>
       </c>
@@ -3878,7 +3911,7 @@
       </c>
       <c r="I23" s="22"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" s="17" t="s">
         <v>230</v>
       </c>
@@ -3893,7 +3926,7 @@
       </c>
       <c r="I24" s="22"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" s="17" t="s">
         <v>231</v>
       </c>
@@ -3908,7 +3941,7 @@
       </c>
       <c r="I25" s="22"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" s="17" t="s">
         <v>232</v>
       </c>
@@ -3923,7 +3956,7 @@
       </c>
       <c r="I26" s="22"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" s="17" t="s">
         <v>233</v>
       </c>
@@ -3938,7 +3971,7 @@
       </c>
       <c r="I27" s="22"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>119</v>
       </c>
@@ -3959,7 +3992,7 @@
       </c>
       <c r="I28" s="22"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" s="17" t="s">
         <v>238</v>
       </c>
@@ -3974,7 +4007,7 @@
       </c>
       <c r="I29" s="22"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" s="17" t="s">
         <v>239</v>
       </c>
@@ -3989,7 +4022,7 @@
       </c>
       <c r="I30" s="22"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" s="17" t="s">
         <v>240</v>
       </c>
@@ -4004,7 +4037,7 @@
       </c>
       <c r="I31" s="22"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" s="17" t="s">
         <v>241</v>
       </c>
@@ -4019,7 +4052,7 @@
       </c>
       <c r="I32" s="22"/>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" s="17" t="s">
         <v>242</v>
       </c>
@@ -4034,7 +4067,7 @@
       </c>
       <c r="I33" s="22"/>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>120</v>
       </c>
@@ -4063,7 +4096,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" s="17" t="s">
         <v>244</v>
       </c>
@@ -4076,11 +4109,11 @@
       <c r="D35" s="17" t="s">
         <v>202</v>
       </c>
-      <c r="I35" s="24" t="s">
+      <c r="I35" s="23" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" s="17" t="s">
         <v>245</v>
       </c>
@@ -4093,11 +4126,11 @@
       <c r="D36" s="17" t="s">
         <v>202</v>
       </c>
-      <c r="I36" s="24" t="s">
+      <c r="I36" s="23" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" s="17" t="s">
         <v>246</v>
       </c>
@@ -4110,11 +4143,11 @@
       <c r="D37" s="17" t="s">
         <v>202</v>
       </c>
-      <c r="I37" s="24" t="s">
+      <c r="I37" s="23" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" s="17" t="s">
         <v>247</v>
       </c>
@@ -4127,11 +4160,11 @@
       <c r="D38" s="17" t="s">
         <v>202</v>
       </c>
-      <c r="I38" s="24" t="s">
+      <c r="I38" s="23" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39" s="17" t="s">
         <v>248</v>
       </c>
@@ -4144,11 +4177,11 @@
       <c r="D39" s="17" t="s">
         <v>202</v>
       </c>
-      <c r="I39" s="24" t="s">
+      <c r="I39" s="23" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40" s="17" t="s">
         <v>251</v>
       </c>
@@ -4161,11 +4194,11 @@
       <c r="D40" s="17" t="s">
         <v>202</v>
       </c>
-      <c r="I40" s="24" t="s">
+      <c r="I40" s="23" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>121</v>
       </c>
@@ -4194,7 +4227,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42" s="17" t="s">
         <v>254</v>
       </c>
@@ -4207,11 +4240,11 @@
       <c r="D42" s="17" t="s">
         <v>202</v>
       </c>
-      <c r="I42" s="24" t="s">
+      <c r="I42" s="23" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43" s="17" t="s">
         <v>255</v>
       </c>
@@ -4224,11 +4257,11 @@
       <c r="D43" s="17" t="s">
         <v>202</v>
       </c>
-      <c r="I43" s="24" t="s">
+      <c r="I43" s="23" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44" s="17" t="s">
         <v>256</v>
       </c>
@@ -4241,11 +4274,11 @@
       <c r="D44" s="17" t="s">
         <v>202</v>
       </c>
-      <c r="I44" s="24" t="s">
+      <c r="I44" s="23" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>122</v>
       </c>
@@ -4274,7 +4307,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A46" s="17" t="s">
         <v>257</v>
       </c>
@@ -4287,11 +4320,11 @@
       <c r="D46" s="17" t="s">
         <v>202</v>
       </c>
-      <c r="I46" s="24" t="s">
+      <c r="I46" s="23" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A47" s="17" t="s">
         <v>258</v>
       </c>
@@ -4304,11 +4337,11 @@
       <c r="D47" s="17" t="s">
         <v>202</v>
       </c>
-      <c r="I47" s="24" t="s">
+      <c r="I47" s="23" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A48" s="17" t="s">
         <v>259</v>
       </c>
@@ -4321,11 +4354,11 @@
       <c r="D48" s="17" t="s">
         <v>202</v>
       </c>
-      <c r="I48" s="24" t="s">
+      <c r="I48" s="23" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A49" s="17" t="s">
         <v>260</v>
       </c>
@@ -4338,11 +4371,11 @@
       <c r="D49" s="17" t="s">
         <v>202</v>
       </c>
-      <c r="I49" s="24" t="s">
+      <c r="I49" s="23" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>123</v>
       </c>
@@ -4371,7 +4404,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A51" s="17" t="s">
         <v>264</v>
       </c>
@@ -4384,11 +4417,11 @@
       <c r="D51" s="17" t="s">
         <v>202</v>
       </c>
-      <c r="I51" s="24" t="s">
+      <c r="I51" s="23" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A52" s="17" t="s">
         <v>266</v>
       </c>
@@ -4401,11 +4434,11 @@
       <c r="D52" s="17" t="s">
         <v>202</v>
       </c>
-      <c r="I52" s="24" t="s">
+      <c r="I52" s="23" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A53" s="17" t="s">
         <v>267</v>
       </c>
@@ -4418,11 +4451,11 @@
       <c r="D53" s="17" t="s">
         <v>202</v>
       </c>
-      <c r="I53" s="24" t="s">
+      <c r="I53" s="23" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A54" s="17" t="s">
         <v>268</v>
       </c>
@@ -4435,11 +4468,11 @@
       <c r="D54" s="17" t="s">
         <v>202</v>
       </c>
-      <c r="I54" s="24" t="s">
+      <c r="I54" s="23" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A55" s="17" t="s">
         <v>270</v>
       </c>
@@ -4452,11 +4485,11 @@
       <c r="D55" s="17" t="s">
         <v>202</v>
       </c>
-      <c r="I55" s="24" t="s">
+      <c r="I55" s="23" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A56" s="4" t="s">
         <v>279</v>
       </c>
@@ -4473,28 +4506,28 @@
       </c>
       <c r="G56">
         <f>SUM(G2:G55)</f>
-        <v>229</v>
+        <v>319</v>
       </c>
       <c r="H56">
         <f>SUM(H2:H55)</f>
-        <v>405</v>
+        <v>495</v>
       </c>
       <c r="I56" s="22"/>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A57" s="17"/>
       <c r="I57" s="7"/>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B58" s="5" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B59" s="5"/>
       <c r="I59" s="7"/>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B60" s="5" t="s">
         <v>31</v>
       </c>
@@ -4502,17 +4535,17 @@
         <v>274</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C61" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C62" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B64" s="5" t="s">
         <v>32</v>
       </c>
@@ -4520,7 +4553,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="65" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="65" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C65" t="s">
         <v>278</v>
       </c>
@@ -4536,16 +4569,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+    <sheetView zoomScale="150" workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="24.69140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
@@ -4574,7 +4607,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>124</v>
       </c>
@@ -4588,7 +4621,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>125</v>
       </c>
@@ -4602,7 +4635,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>126</v>
       </c>
@@ -4616,7 +4649,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>127</v>
       </c>
@@ -4630,7 +4663,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>128</v>
       </c>
@@ -4644,7 +4677,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>129</v>
       </c>
@@ -4658,7 +4691,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>130</v>
       </c>
@@ -4672,7 +4705,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>131</v>
       </c>
@@ -4686,7 +4719,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>132</v>
       </c>
@@ -4700,7 +4733,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>133</v>
       </c>
@@ -4729,9 +4762,9 @@
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
@@ -4774,9 +4807,9 @@
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
@@ -4819,13 +4852,13 @@
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="28.15234375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="49.4609375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="28.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="49.453125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>113</v>
       </c>
@@ -4836,7 +4869,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>114</v>
       </c>
@@ -4847,7 +4880,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>115</v>
       </c>
@@ -4858,7 +4891,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>116</v>
       </c>
@@ -4869,7 +4902,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>117</v>
       </c>
@@ -4880,7 +4913,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>118</v>
       </c>
@@ -4891,7 +4924,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>119</v>
       </c>
@@ -4902,7 +4935,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="45" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" ht="45" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>120</v>
       </c>
@@ -4913,7 +4946,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>121</v>
       </c>
@@ -4924,7 +4957,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>122</v>
       </c>
@@ -4935,7 +4968,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>123</v>
       </c>
@@ -4946,7 +4979,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>124</v>
       </c>
@@ -4957,7 +4990,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="45" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" ht="45" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>125</v>
       </c>
@@ -4968,7 +5001,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="45" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" ht="45" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>126</v>
       </c>
@@ -4979,7 +5012,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>127</v>
       </c>
@@ -4990,7 +5023,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>128</v>
       </c>
@@ -5001,7 +5034,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>129</v>
       </c>
@@ -5012,7 +5045,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>130</v>
       </c>
@@ -5023,7 +5056,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>131</v>
       </c>
@@ -5034,7 +5067,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>132</v>
       </c>
@@ -5045,7 +5078,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>133</v>
       </c>
@@ -5056,7 +5089,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>134</v>
       </c>
@@ -5067,7 +5100,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>135</v>
       </c>
@@ -5078,7 +5111,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>136</v>
       </c>
@@ -5089,7 +5122,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="45" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" ht="45" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>137</v>
       </c>
@@ -5100,7 +5133,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>138</v>
       </c>
@@ -5111,7 +5144,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="105" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" ht="105" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>139</v>
       </c>
@@ -5122,7 +5155,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>140</v>
       </c>
@@ -5133,7 +5166,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>141</v>
       </c>
@@ -5144,7 +5177,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>142</v>
       </c>
@@ -5155,7 +5188,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>143</v>
       </c>
@@ -5166,7 +5199,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>144</v>
       </c>
@@ -5177,7 +5210,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>145</v>
       </c>
@@ -5188,7 +5221,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>146</v>
       </c>
@@ -5199,7 +5232,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>147</v>
       </c>
@@ -5210,7 +5243,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>148</v>
       </c>
@@ -5221,7 +5254,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>149</v>
       </c>
@@ -5232,7 +5265,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>150</v>
       </c>
@@ -5243,7 +5276,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>151</v>
       </c>
@@ -5254,7 +5287,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>152</v>
       </c>
@@ -5265,7 +5298,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>153</v>
       </c>
@@ -5276,7 +5309,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>154</v>
       </c>
@@ -5287,7 +5320,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>155</v>
       </c>

</xml_diff>

<commit_message>
Changes to test_userStory09 and updates to my Sprint2 tab
</commit_message>
<xml_diff>
--- a/Team2Report.xlsx
+++ b/Team2Report.xlsx
@@ -5,12 +5,12 @@
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ztyle\Documents\SSW 555\SSW_555_Project_Sprint1\Agile_Methods_Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ztyle\Documents\SSW 555\SSW_555_Project_Master\Agile_Methods_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7254D44F-2F9C-4F9E-BDC2-6E484ED628B8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{661DDA39-7C37-4268-A442-0C0C0844D8C9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-8290" yWindow="3260" windowWidth="14400" windowHeight="7360" tabRatio="500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="683" uniqueCount="281">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="775" uniqueCount="325">
   <si>
     <t>Date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -918,6 +918,138 @@
   </si>
   <si>
     <t>Task finished</t>
+  </si>
+  <si>
+    <t>T19.01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Iterate through family </t>
+  </si>
+  <si>
+    <t>Store husband ID</t>
+  </si>
+  <si>
+    <t>Store wife ID</t>
+  </si>
+  <si>
+    <t>T19.02</t>
+  </si>
+  <si>
+    <t>T19.03</t>
+  </si>
+  <si>
+    <t>T19.04</t>
+  </si>
+  <si>
+    <t>T19.05</t>
+  </si>
+  <si>
+    <t>T19.06</t>
+  </si>
+  <si>
+    <t>T19.07</t>
+  </si>
+  <si>
+    <t>Store children</t>
+  </si>
+  <si>
+    <t>Iterate through individuals to find family ID through child</t>
+  </si>
+  <si>
+    <t>Store children through family ID</t>
+  </si>
+  <si>
+    <t>Store aunt and uncles as children through previous family ID</t>
+  </si>
+  <si>
+    <t>T20.01</t>
+  </si>
+  <si>
+    <t>T20.02</t>
+  </si>
+  <si>
+    <t>T20.03</t>
+  </si>
+  <si>
+    <t>T20.04</t>
+  </si>
+  <si>
+    <t>T20.05</t>
+  </si>
+  <si>
+    <t>T20.06</t>
+  </si>
+  <si>
+    <t>T20.07</t>
+  </si>
+  <si>
+    <t>Iterate through families</t>
+  </si>
+  <si>
+    <t>Find if there was a marriage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Find family ID of husband through child </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Find family ID of wife through child </t>
+  </si>
+  <si>
+    <t>Output an error if there is an overlap</t>
+  </si>
+  <si>
+    <t>T19.08</t>
+  </si>
+  <si>
+    <t>T19.09</t>
+  </si>
+  <si>
+    <t>T19.10</t>
+  </si>
+  <si>
+    <t>Find husband's father</t>
+  </si>
+  <si>
+    <t>Find husband's mother</t>
+  </si>
+  <si>
+    <t>Find wife's father</t>
+  </si>
+  <si>
+    <t>Find wife's mother</t>
+  </si>
+  <si>
+    <t>Find family ID of husband's father through child</t>
+  </si>
+  <si>
+    <t>Find family ID of husband's mother through child</t>
+  </si>
+  <si>
+    <t>Find family ID of wife's father through child</t>
+  </si>
+  <si>
+    <t>Find family ID of wife's mother through child</t>
+  </si>
+  <si>
+    <t>Find if family IDs of either parent of husband and wife are the same</t>
+  </si>
+  <si>
+    <t>T19.11</t>
+  </si>
+  <si>
+    <t>T19.12</t>
+  </si>
+  <si>
+    <t>T19.13</t>
+  </si>
+  <si>
+    <t>T19.14</t>
+  </si>
+  <si>
+    <t>T19.15</t>
+  </si>
+  <si>
+    <t>T19.16</t>
   </si>
 </sst>
 </file>
@@ -1106,11 +1238,11 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="66">
@@ -2486,12 +2618,12 @@
       <c r="E3" s="17" t="s">
         <v>202</v>
       </c>
-      <c r="G3" s="23" t="s">
+      <c r="G3" s="24" t="s">
         <v>203</v>
       </c>
-      <c r="H3" s="23"/>
-      <c r="I3" s="23"/>
-      <c r="J3" s="23"/>
+      <c r="H3" s="24"/>
+      <c r="I3" s="24"/>
+      <c r="J3" s="24"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4">
@@ -3530,7 +3662,7 @@
       <c r="D3" s="17" t="s">
         <v>202</v>
       </c>
-      <c r="I3" s="24" t="s">
+      <c r="I3" s="23" t="s">
         <v>280</v>
       </c>
     </row>
@@ -3547,7 +3679,7 @@
       <c r="D4" s="17" t="s">
         <v>202</v>
       </c>
-      <c r="I4" s="24" t="s">
+      <c r="I4" s="23" t="s">
         <v>280</v>
       </c>
     </row>
@@ -3564,7 +3696,7 @@
       <c r="D5" s="17" t="s">
         <v>202</v>
       </c>
-      <c r="I5" s="24" t="s">
+      <c r="I5" s="23" t="s">
         <v>280</v>
       </c>
     </row>
@@ -3610,7 +3742,7 @@
       <c r="D7" s="17" t="s">
         <v>202</v>
       </c>
-      <c r="I7" s="24" t="s">
+      <c r="I7" s="23" t="s">
         <v>280</v>
       </c>
     </row>
@@ -3627,7 +3759,7 @@
       <c r="D8" s="17" t="s">
         <v>202</v>
       </c>
-      <c r="I8" s="24" t="s">
+      <c r="I8" s="23" t="s">
         <v>280</v>
       </c>
     </row>
@@ -3644,7 +3776,7 @@
       <c r="D9" s="17" t="s">
         <v>202</v>
       </c>
-      <c r="I9" s="24" t="s">
+      <c r="I9" s="23" t="s">
         <v>280</v>
       </c>
     </row>
@@ -3661,7 +3793,7 @@
       <c r="D10" s="17" t="s">
         <v>202</v>
       </c>
-      <c r="I10" s="24" t="s">
+      <c r="I10" s="23" t="s">
         <v>280</v>
       </c>
     </row>
@@ -4076,7 +4208,7 @@
       <c r="D35" s="17" t="s">
         <v>202</v>
       </c>
-      <c r="I35" s="24" t="s">
+      <c r="I35" s="23" t="s">
         <v>280</v>
       </c>
     </row>
@@ -4093,7 +4225,7 @@
       <c r="D36" s="17" t="s">
         <v>202</v>
       </c>
-      <c r="I36" s="24" t="s">
+      <c r="I36" s="23" t="s">
         <v>280</v>
       </c>
     </row>
@@ -4110,7 +4242,7 @@
       <c r="D37" s="17" t="s">
         <v>202</v>
       </c>
-      <c r="I37" s="24" t="s">
+      <c r="I37" s="23" t="s">
         <v>280</v>
       </c>
     </row>
@@ -4127,7 +4259,7 @@
       <c r="D38" s="17" t="s">
         <v>202</v>
       </c>
-      <c r="I38" s="24" t="s">
+      <c r="I38" s="23" t="s">
         <v>280</v>
       </c>
     </row>
@@ -4144,7 +4276,7 @@
       <c r="D39" s="17" t="s">
         <v>202</v>
       </c>
-      <c r="I39" s="24" t="s">
+      <c r="I39" s="23" t="s">
         <v>280</v>
       </c>
     </row>
@@ -4161,7 +4293,7 @@
       <c r="D40" s="17" t="s">
         <v>202</v>
       </c>
-      <c r="I40" s="24" t="s">
+      <c r="I40" s="23" t="s">
         <v>280</v>
       </c>
     </row>
@@ -4207,7 +4339,7 @@
       <c r="D42" s="17" t="s">
         <v>202</v>
       </c>
-      <c r="I42" s="24" t="s">
+      <c r="I42" s="23" t="s">
         <v>280</v>
       </c>
     </row>
@@ -4224,7 +4356,7 @@
       <c r="D43" s="17" t="s">
         <v>202</v>
       </c>
-      <c r="I43" s="24" t="s">
+      <c r="I43" s="23" t="s">
         <v>280</v>
       </c>
     </row>
@@ -4241,7 +4373,7 @@
       <c r="D44" s="17" t="s">
         <v>202</v>
       </c>
-      <c r="I44" s="24" t="s">
+      <c r="I44" s="23" t="s">
         <v>280</v>
       </c>
     </row>
@@ -4287,7 +4419,7 @@
       <c r="D46" s="17" t="s">
         <v>202</v>
       </c>
-      <c r="I46" s="24" t="s">
+      <c r="I46" s="23" t="s">
         <v>280</v>
       </c>
     </row>
@@ -4304,7 +4436,7 @@
       <c r="D47" s="17" t="s">
         <v>202</v>
       </c>
-      <c r="I47" s="24" t="s">
+      <c r="I47" s="23" t="s">
         <v>280</v>
       </c>
     </row>
@@ -4321,7 +4453,7 @@
       <c r="D48" s="17" t="s">
         <v>202</v>
       </c>
-      <c r="I48" s="24" t="s">
+      <c r="I48" s="23" t="s">
         <v>280</v>
       </c>
     </row>
@@ -4338,7 +4470,7 @@
       <c r="D49" s="17" t="s">
         <v>202</v>
       </c>
-      <c r="I49" s="24" t="s">
+      <c r="I49" s="23" t="s">
         <v>280</v>
       </c>
     </row>
@@ -4384,7 +4516,7 @@
       <c r="D51" s="17" t="s">
         <v>202</v>
       </c>
-      <c r="I51" s="24" t="s">
+      <c r="I51" s="23" t="s">
         <v>280</v>
       </c>
     </row>
@@ -4401,7 +4533,7 @@
       <c r="D52" s="17" t="s">
         <v>202</v>
       </c>
-      <c r="I52" s="24" t="s">
+      <c r="I52" s="23" t="s">
         <v>280</v>
       </c>
     </row>
@@ -4418,7 +4550,7 @@
       <c r="D53" s="17" t="s">
         <v>202</v>
       </c>
-      <c r="I53" s="24" t="s">
+      <c r="I53" s="23" t="s">
         <v>280</v>
       </c>
     </row>
@@ -4435,7 +4567,7 @@
       <c r="D54" s="17" t="s">
         <v>202</v>
       </c>
-      <c r="I54" s="24" t="s">
+      <c r="I54" s="23" t="s">
         <v>280</v>
       </c>
     </row>
@@ -4452,7 +4584,7 @@
       <c r="D55" s="17" t="s">
         <v>202</v>
       </c>
-      <c r="I55" s="24" t="s">
+      <c r="I55" s="23" t="s">
         <v>280</v>
       </c>
     </row>
@@ -4534,15 +4666,15 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:I34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="24.69140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="54.61328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
@@ -4702,15 +4834,349 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>133</v>
+        <v>281</v>
       </c>
       <c r="B11" t="s">
-        <v>87</v>
+        <v>302</v>
       </c>
       <c r="C11" s="17" t="s">
         <v>186</v>
       </c>
       <c r="D11" s="17" t="s">
+        <v>202</v>
+      </c>
+      <c r="E11">
+        <v>65</v>
+      </c>
+      <c r="F11">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>285</v>
+      </c>
+      <c r="B12" t="s">
+        <v>303</v>
+      </c>
+      <c r="C12" s="17" t="s">
+        <v>186</v>
+      </c>
+      <c r="D12" s="17" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>286</v>
+      </c>
+      <c r="B13" t="s">
+        <v>283</v>
+      </c>
+      <c r="C13" s="17" t="s">
+        <v>186</v>
+      </c>
+      <c r="D13" s="17" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>287</v>
+      </c>
+      <c r="B14" t="s">
+        <v>284</v>
+      </c>
+      <c r="C14" s="17" t="s">
+        <v>186</v>
+      </c>
+      <c r="D14" s="17" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>288</v>
+      </c>
+      <c r="B15" t="s">
+        <v>304</v>
+      </c>
+      <c r="C15" s="17" t="s">
+        <v>186</v>
+      </c>
+      <c r="D15" s="17" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>289</v>
+      </c>
+      <c r="B16" t="s">
+        <v>305</v>
+      </c>
+      <c r="C16" s="17" t="s">
+        <v>186</v>
+      </c>
+      <c r="D16" s="17" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>290</v>
+      </c>
+      <c r="B17" t="s">
+        <v>310</v>
+      </c>
+      <c r="C17" s="17" t="s">
+        <v>186</v>
+      </c>
+      <c r="D17" s="17" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>307</v>
+      </c>
+      <c r="B18" t="s">
+        <v>311</v>
+      </c>
+      <c r="C18" s="17" t="s">
+        <v>186</v>
+      </c>
+      <c r="D18" s="17" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>308</v>
+      </c>
+      <c r="B19" t="s">
+        <v>312</v>
+      </c>
+      <c r="C19" s="17" t="s">
+        <v>186</v>
+      </c>
+      <c r="D19" s="17" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>309</v>
+      </c>
+      <c r="B20" t="s">
+        <v>313</v>
+      </c>
+      <c r="C20" s="17" t="s">
+        <v>186</v>
+      </c>
+      <c r="D20" s="17" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>319</v>
+      </c>
+      <c r="B21" t="s">
+        <v>314</v>
+      </c>
+      <c r="C21" s="17" t="s">
+        <v>186</v>
+      </c>
+      <c r="D21" s="17" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>320</v>
+      </c>
+      <c r="B22" t="s">
+        <v>315</v>
+      </c>
+      <c r="C22" s="17" t="s">
+        <v>186</v>
+      </c>
+      <c r="D22" s="17" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>321</v>
+      </c>
+      <c r="B23" t="s">
+        <v>316</v>
+      </c>
+      <c r="C23" s="17" t="s">
+        <v>186</v>
+      </c>
+      <c r="D23" s="17" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>322</v>
+      </c>
+      <c r="B24" t="s">
+        <v>317</v>
+      </c>
+      <c r="C24" s="17" t="s">
+        <v>186</v>
+      </c>
+      <c r="D24" s="17" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>323</v>
+      </c>
+      <c r="B25" t="s">
+        <v>318</v>
+      </c>
+      <c r="C25" s="17" t="s">
+        <v>186</v>
+      </c>
+      <c r="D25" s="17" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>324</v>
+      </c>
+      <c r="B26" t="s">
+        <v>306</v>
+      </c>
+      <c r="C26" s="17" t="s">
+        <v>186</v>
+      </c>
+      <c r="D26" s="17" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>133</v>
+      </c>
+      <c r="B27" t="s">
+        <v>87</v>
+      </c>
+      <c r="C27" s="17" t="s">
+        <v>186</v>
+      </c>
+      <c r="D27" s="17" t="s">
+        <v>202</v>
+      </c>
+      <c r="E27">
+        <v>50</v>
+      </c>
+      <c r="F27">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>295</v>
+      </c>
+      <c r="B28" t="s">
+        <v>282</v>
+      </c>
+      <c r="C28" s="17" t="s">
+        <v>186</v>
+      </c>
+      <c r="D28" s="17" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>296</v>
+      </c>
+      <c r="B29" t="s">
+        <v>291</v>
+      </c>
+      <c r="C29" s="17" t="s">
+        <v>186</v>
+      </c>
+      <c r="D29" s="17" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>297</v>
+      </c>
+      <c r="B30" t="s">
+        <v>283</v>
+      </c>
+      <c r="C30" s="17" t="s">
+        <v>186</v>
+      </c>
+      <c r="D30" s="17" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>298</v>
+      </c>
+      <c r="B31" t="s">
+        <v>284</v>
+      </c>
+      <c r="C31" s="17" t="s">
+        <v>186</v>
+      </c>
+      <c r="D31" s="17" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>299</v>
+      </c>
+      <c r="B32" t="s">
+        <v>292</v>
+      </c>
+      <c r="C32" s="17" t="s">
+        <v>186</v>
+      </c>
+      <c r="D32" s="17" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>300</v>
+      </c>
+      <c r="B33" t="s">
+        <v>293</v>
+      </c>
+      <c r="C33" s="17" t="s">
+        <v>186</v>
+      </c>
+      <c r="D33" s="17" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>301</v>
+      </c>
+      <c r="B34" t="s">
+        <v>294</v>
+      </c>
+      <c r="C34" s="17" t="s">
+        <v>186</v>
+      </c>
+      <c r="D34" s="17" t="s">
         <v>202</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added Sprint1 task completion
</commit_message>
<xml_diff>
--- a/Team2Report.xlsx
+++ b/Team2Report.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23127"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ztyle\Documents\SSW 555\SSW_555_Project_Master\Agile_Methods_Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RedRo\OneDrive\Documents\Academic Texts\COOOOOOODE\Python Workspace\anaconda\Agile_Methods_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{661DDA39-7C37-4268-A442-0C0C0844D8C9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B57A068-D39B-4AEF-8BD8-9B8CCF09081B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-8290" yWindow="3260" windowWidth="14400" windowHeight="7360" tabRatio="500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13236" yWindow="0" windowWidth="9804" windowHeight="8964" tabRatio="500" firstSheet="4" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,6 @@
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -45,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="775" uniqueCount="325">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="786" uniqueCount="325">
   <si>
     <t>Date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -1520,7 +1519,7 @@
                   <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>34</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2414,16 +2413,16 @@
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.84375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.15234375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.4609375" customWidth="1"/>
-    <col min="4" max="4" width="22.84375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.4609375" customWidth="1"/>
+    <col min="1" max="1" width="7.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.453125" customWidth="1"/>
+    <col min="4" max="4" width="22.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>19</v>
       </c>
@@ -2440,7 +2439,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>180</v>
       </c>
@@ -2457,7 +2456,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>196</v>
       </c>
@@ -2474,7 +2473,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>190</v>
       </c>
@@ -2491,7 +2490,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>181</v>
       </c>
@@ -2508,7 +2507,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>186</v>
       </c>
@@ -2525,7 +2524,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D8" s="4" t="s">
         <v>34</v>
       </c>
@@ -2558,16 +2557,16 @@
       <selection activeCell="B12" sqref="B12:E21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="6.84375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.81640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="29" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.4609375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.4609375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>29</v>
       </c>
@@ -2585,7 +2584,7 @@
       </c>
       <c r="G1" s="18"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2602,7 +2601,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -2625,7 +2624,7 @@
       <c r="I3" s="24"/>
       <c r="J3" s="24"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1</v>
       </c>
@@ -2642,7 +2641,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1</v>
       </c>
@@ -2659,7 +2658,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>1</v>
       </c>
@@ -2676,7 +2675,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>1</v>
       </c>
@@ -2693,7 +2692,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>1</v>
       </c>
@@ -2710,7 +2709,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>1</v>
       </c>
@@ -2727,7 +2726,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>1</v>
       </c>
@@ -2744,7 +2743,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>1</v>
       </c>
@@ -2761,7 +2760,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>2</v>
       </c>
@@ -2778,7 +2777,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>2</v>
       </c>
@@ -2795,7 +2794,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>2</v>
       </c>
@@ -2812,7 +2811,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>2</v>
       </c>
@@ -2829,7 +2828,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>2</v>
       </c>
@@ -2846,7 +2845,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>2</v>
       </c>
@@ -2863,7 +2862,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>2</v>
       </c>
@@ -2880,7 +2879,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>2</v>
       </c>
@@ -2897,7 +2896,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>2</v>
       </c>
@@ -2914,7 +2913,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>2</v>
       </c>
@@ -2931,7 +2930,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>3</v>
       </c>
@@ -2948,7 +2947,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>3</v>
       </c>
@@ -2965,7 +2964,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>3</v>
       </c>
@@ -2982,7 +2981,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>3</v>
       </c>
@@ -2999,7 +2998,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>3</v>
       </c>
@@ -3016,7 +3015,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>3</v>
       </c>
@@ -3033,7 +3032,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>3</v>
       </c>
@@ -3050,7 +3049,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>3</v>
       </c>
@@ -3067,7 +3066,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>3</v>
       </c>
@@ -3084,7 +3083,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>3</v>
       </c>
@@ -3101,7 +3100,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>4</v>
       </c>
@@ -3118,7 +3117,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>4</v>
       </c>
@@ -3135,7 +3134,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>4</v>
       </c>
@@ -3152,7 +3151,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>4</v>
       </c>
@@ -3169,7 +3168,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>4</v>
       </c>
@@ -3186,7 +3185,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>4</v>
       </c>
@@ -3203,7 +3202,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>4</v>
       </c>
@@ -3220,7 +3219,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>4</v>
       </c>
@@ -3237,7 +3236,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>4</v>
       </c>
@@ -3254,7 +3253,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>4</v>
       </c>
@@ -3289,47 +3288,47 @@
       <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.84375" style="7"/>
-    <col min="2" max="2" width="10.15234375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.84375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.3046875" customWidth="1"/>
-    <col min="5" max="5" width="6.84375" customWidth="1"/>
-    <col min="6" max="6" width="12.4609375" style="9" customWidth="1"/>
+    <col min="1" max="1" width="10.81640625" style="7"/>
+    <col min="2" max="2" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.26953125" customWidth="1"/>
+    <col min="5" max="5" width="6.81640625" customWidth="1"/>
+    <col min="6" max="6" width="12.453125" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
         <v>161</v>
       </c>
@@ -3352,7 +3351,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>162</v>
       </c>
@@ -3368,7 +3367,7 @@
       <c r="F15" s="14"/>
       <c r="G15" s="9"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>163</v>
       </c>
@@ -3392,7 +3391,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="7" t="s">
         <v>164</v>
       </c>
@@ -3417,7 +3416,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="7" t="s">
         <v>165</v>
       </c>
@@ -3442,7 +3441,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="7" t="s">
         <v>166</v>
       </c>
@@ -3482,17 +3481,17 @@
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.84375" style="2"/>
-    <col min="2" max="2" width="16.69140625" customWidth="1"/>
-    <col min="3" max="3" width="12.4609375" customWidth="1"/>
-    <col min="4" max="4" width="7.15234375" customWidth="1"/>
-    <col min="5" max="5" width="6.84375" customWidth="1"/>
-    <col min="6" max="6" width="12.4609375" style="9" customWidth="1"/>
+    <col min="1" max="1" width="10.81640625" style="2"/>
+    <col min="2" max="2" width="16.7265625" customWidth="1"/>
+    <col min="3" max="3" width="12.453125" customWidth="1"/>
+    <col min="4" max="4" width="7.1796875" customWidth="1"/>
+    <col min="5" max="5" width="6.81640625" customWidth="1"/>
+    <col min="6" max="6" width="12.453125" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -3512,7 +3511,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="13">
         <v>42632</v>
       </c>
@@ -3523,42 +3522,42 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="13">
         <v>42647</v>
       </c>
       <c r="B3">
         <f>B2-COUNTIF(Sprint1!I2:I55, "Completed")</f>
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C3">
         <f>B2-B3</f>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D3">
         <f>Sprint1!G56</f>
-        <v>229</v>
+        <v>319</v>
       </c>
       <c r="E3">
         <f>Sprint1!H56</f>
-        <v>405</v>
+        <v>570</v>
       </c>
       <c r="F3" s="9">
         <f>(D3-D2)/E3*60</f>
-        <v>33.925925925925924</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+        <v>33.578947368421048</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="13">
         <v>42661</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="13">
         <v>42675</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="13">
         <v>42689</v>
       </c>
@@ -3575,23 +3574,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:I65"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="33" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.4609375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.4609375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.3046875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.69140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.4609375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.3046875" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.26953125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.7265625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.26953125" style="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
@@ -3620,7 +3619,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>114</v>
       </c>
@@ -3649,7 +3648,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="17" t="s">
         <v>204</v>
       </c>
@@ -3666,7 +3665,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="17" t="s">
         <v>205</v>
       </c>
@@ -3683,7 +3682,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="17" t="s">
         <v>206</v>
       </c>
@@ -3700,7 +3699,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>115</v>
       </c>
@@ -3729,7 +3728,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="17" t="s">
         <v>209</v>
       </c>
@@ -3746,7 +3745,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="17" t="s">
         <v>210</v>
       </c>
@@ -3763,7 +3762,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="17" t="s">
         <v>211</v>
       </c>
@@ -3780,7 +3779,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="17" t="s">
         <v>224</v>
       </c>
@@ -3797,7 +3796,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>116</v>
       </c>
@@ -3816,9 +3815,17 @@
       <c r="F11">
         <v>100</v>
       </c>
-      <c r="I11" s="22"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="G11">
+        <v>45</v>
+      </c>
+      <c r="H11">
+        <v>120</v>
+      </c>
+      <c r="I11" s="22" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="17" t="s">
         <v>215</v>
       </c>
@@ -3831,9 +3838,11 @@
       <c r="D12" s="17" t="s">
         <v>202</v>
       </c>
-      <c r="I12" s="22"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I12" s="23" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="17" t="s">
         <v>216</v>
       </c>
@@ -3846,9 +3855,11 @@
       <c r="D13" s="17" t="s">
         <v>202</v>
       </c>
-      <c r="I13" s="22"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I13" s="23" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="17" t="s">
         <v>217</v>
       </c>
@@ -3861,9 +3872,11 @@
       <c r="D14" s="17" t="s">
         <v>202</v>
       </c>
-      <c r="I14" s="22"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I14" s="23" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="17" t="s">
         <v>236</v>
       </c>
@@ -3876,9 +3889,11 @@
       <c r="D15" s="17" t="s">
         <v>202</v>
       </c>
-      <c r="I15" s="22"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I15" s="23" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>117</v>
       </c>
@@ -3897,9 +3912,17 @@
       <c r="F16">
         <v>140</v>
       </c>
-      <c r="I16" s="22"/>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="G16">
+        <v>45</v>
+      </c>
+      <c r="H16">
+        <v>45</v>
+      </c>
+      <c r="I16" s="22" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="17" t="s">
         <v>220</v>
       </c>
@@ -3912,9 +3935,11 @@
       <c r="D17" s="17" t="s">
         <v>202</v>
       </c>
-      <c r="I17" s="22"/>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I17" s="23" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="17" t="s">
         <v>221</v>
       </c>
@@ -3927,9 +3952,11 @@
       <c r="D18" s="17" t="s">
         <v>202</v>
       </c>
-      <c r="I18" s="22"/>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I18" s="23" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="17" t="s">
         <v>222</v>
       </c>
@@ -3942,9 +3969,11 @@
       <c r="D19" s="17" t="s">
         <v>202</v>
       </c>
-      <c r="I19" s="22"/>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I19" s="23" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="17" t="s">
         <v>223</v>
       </c>
@@ -3957,9 +3986,11 @@
       <c r="D20" s="17" t="s">
         <v>202</v>
       </c>
-      <c r="I20" s="22"/>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I20" s="23" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" s="17" t="s">
         <v>237</v>
       </c>
@@ -3972,9 +4003,11 @@
       <c r="D21" s="17" t="s">
         <v>202</v>
       </c>
-      <c r="I21" s="22"/>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I21" s="23" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>118</v>
       </c>
@@ -3995,7 +4028,7 @@
       </c>
       <c r="I22" s="22"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" s="17" t="s">
         <v>229</v>
       </c>
@@ -4010,7 +4043,7 @@
       </c>
       <c r="I23" s="22"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" s="17" t="s">
         <v>230</v>
       </c>
@@ -4025,7 +4058,7 @@
       </c>
       <c r="I24" s="22"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" s="17" t="s">
         <v>231</v>
       </c>
@@ -4040,7 +4073,7 @@
       </c>
       <c r="I25" s="22"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" s="17" t="s">
         <v>232</v>
       </c>
@@ -4055,7 +4088,7 @@
       </c>
       <c r="I26" s="22"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" s="17" t="s">
         <v>233</v>
       </c>
@@ -4070,7 +4103,7 @@
       </c>
       <c r="I27" s="22"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>119</v>
       </c>
@@ -4091,7 +4124,7 @@
       </c>
       <c r="I28" s="22"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" s="17" t="s">
         <v>238</v>
       </c>
@@ -4106,7 +4139,7 @@
       </c>
       <c r="I29" s="22"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" s="17" t="s">
         <v>239</v>
       </c>
@@ -4121,7 +4154,7 @@
       </c>
       <c r="I30" s="22"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" s="17" t="s">
         <v>240</v>
       </c>
@@ -4136,7 +4169,7 @@
       </c>
       <c r="I31" s="22"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" s="17" t="s">
         <v>241</v>
       </c>
@@ -4151,7 +4184,7 @@
       </c>
       <c r="I32" s="22"/>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" s="17" t="s">
         <v>242</v>
       </c>
@@ -4166,7 +4199,7 @@
       </c>
       <c r="I33" s="22"/>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>120</v>
       </c>
@@ -4195,7 +4228,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" s="17" t="s">
         <v>244</v>
       </c>
@@ -4212,7 +4245,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" s="17" t="s">
         <v>245</v>
       </c>
@@ -4229,7 +4262,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" s="17" t="s">
         <v>246</v>
       </c>
@@ -4246,7 +4279,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" s="17" t="s">
         <v>247</v>
       </c>
@@ -4263,7 +4296,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39" s="17" t="s">
         <v>248</v>
       </c>
@@ -4280,7 +4313,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40" s="17" t="s">
         <v>251</v>
       </c>
@@ -4297,7 +4330,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>121</v>
       </c>
@@ -4326,7 +4359,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42" s="17" t="s">
         <v>254</v>
       </c>
@@ -4343,7 +4376,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43" s="17" t="s">
         <v>255</v>
       </c>
@@ -4360,7 +4393,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44" s="17" t="s">
         <v>256</v>
       </c>
@@ -4377,7 +4410,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>122</v>
       </c>
@@ -4406,7 +4439,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A46" s="17" t="s">
         <v>257</v>
       </c>
@@ -4423,7 +4456,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A47" s="17" t="s">
         <v>258</v>
       </c>
@@ -4440,7 +4473,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A48" s="17" t="s">
         <v>259</v>
       </c>
@@ -4457,7 +4490,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A49" s="17" t="s">
         <v>260</v>
       </c>
@@ -4474,7 +4507,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>123</v>
       </c>
@@ -4503,7 +4536,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A51" s="17" t="s">
         <v>264</v>
       </c>
@@ -4520,7 +4553,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A52" s="17" t="s">
         <v>266</v>
       </c>
@@ -4537,7 +4570,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A53" s="17" t="s">
         <v>267</v>
       </c>
@@ -4554,7 +4587,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A54" s="17" t="s">
         <v>268</v>
       </c>
@@ -4571,7 +4604,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A55" s="17" t="s">
         <v>270</v>
       </c>
@@ -4588,7 +4621,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A56" s="4" t="s">
         <v>279</v>
       </c>
@@ -4605,28 +4638,28 @@
       </c>
       <c r="G56">
         <f>SUM(G2:G55)</f>
-        <v>229</v>
+        <v>319</v>
       </c>
       <c r="H56">
         <f>SUM(H2:H55)</f>
-        <v>405</v>
+        <v>570</v>
       </c>
       <c r="I56" s="22"/>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A57" s="17"/>
       <c r="I57" s="7"/>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B58" s="5" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B59" s="5"/>
       <c r="I59" s="7"/>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B60" s="5" t="s">
         <v>31</v>
       </c>
@@ -4634,17 +4667,17 @@
         <v>274</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C61" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C62" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B64" s="5" t="s">
         <v>32</v>
       </c>
@@ -4652,7 +4685,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="65" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="65" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C65" t="s">
         <v>278</v>
       </c>
@@ -4668,16 +4701,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:I34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="54.61328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="54.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
@@ -4706,7 +4739,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>124</v>
       </c>
@@ -4720,7 +4753,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>125</v>
       </c>
@@ -4734,7 +4767,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>126</v>
       </c>
@@ -4748,7 +4781,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>127</v>
       </c>
@@ -4762,7 +4795,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>128</v>
       </c>
@@ -4776,7 +4809,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>129</v>
       </c>
@@ -4790,7 +4823,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>130</v>
       </c>
@@ -4804,7 +4837,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>131</v>
       </c>
@@ -4818,7 +4851,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>132</v>
       </c>
@@ -4832,7 +4865,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>281</v>
       </c>
@@ -4852,7 +4885,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>285</v>
       </c>
@@ -4866,7 +4899,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>286</v>
       </c>
@@ -4880,7 +4913,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>287</v>
       </c>
@@ -4894,7 +4927,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>288</v>
       </c>
@@ -4908,7 +4941,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>289</v>
       </c>
@@ -4922,7 +4955,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>290</v>
       </c>
@@ -4936,7 +4969,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>307</v>
       </c>
@@ -4950,7 +4983,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>308</v>
       </c>
@@ -4964,7 +4997,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>309</v>
       </c>
@@ -4978,7 +5011,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>319</v>
       </c>
@@ -4992,7 +5025,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>320</v>
       </c>
@@ -5006,7 +5039,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>321</v>
       </c>
@@ -5020,7 +5053,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>322</v>
       </c>
@@ -5034,7 +5067,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>323</v>
       </c>
@@ -5048,7 +5081,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>324</v>
       </c>
@@ -5062,7 +5095,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>133</v>
       </c>
@@ -5082,7 +5115,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>295</v>
       </c>
@@ -5096,7 +5129,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>296</v>
       </c>
@@ -5110,7 +5143,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>297</v>
       </c>
@@ -5124,7 +5157,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>298</v>
       </c>
@@ -5138,7 +5171,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>299</v>
       </c>
@@ -5152,7 +5185,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>300</v>
       </c>
@@ -5166,7 +5199,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>301</v>
       </c>
@@ -5195,9 +5228,9 @@
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
@@ -5240,9 +5273,9 @@
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
@@ -5285,13 +5318,13 @@
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="28.15234375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="49.4609375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="28.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="49.453125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>113</v>
       </c>
@@ -5302,7 +5335,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>114</v>
       </c>
@@ -5313,7 +5346,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>115</v>
       </c>
@@ -5324,7 +5357,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>116</v>
       </c>
@@ -5335,7 +5368,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>117</v>
       </c>
@@ -5346,7 +5379,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>118</v>
       </c>
@@ -5357,7 +5390,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>119</v>
       </c>
@@ -5368,7 +5401,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="45" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" ht="45" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>120</v>
       </c>
@@ -5379,7 +5412,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>121</v>
       </c>
@@ -5390,7 +5423,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>122</v>
       </c>
@@ -5401,7 +5434,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>123</v>
       </c>
@@ -5412,7 +5445,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>124</v>
       </c>
@@ -5423,7 +5456,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="45" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" ht="45" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>125</v>
       </c>
@@ -5434,7 +5467,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="45" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" ht="45" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>126</v>
       </c>
@@ -5445,7 +5478,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>127</v>
       </c>
@@ -5456,7 +5489,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>128</v>
       </c>
@@ -5467,7 +5500,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>129</v>
       </c>
@@ -5478,7 +5511,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>130</v>
       </c>
@@ -5489,7 +5522,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>131</v>
       </c>
@@ -5500,7 +5533,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>132</v>
       </c>
@@ -5511,7 +5544,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>133</v>
       </c>
@@ -5522,7 +5555,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>134</v>
       </c>
@@ -5533,7 +5566,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>135</v>
       </c>
@@ -5544,7 +5577,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>136</v>
       </c>
@@ -5555,7 +5588,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="45" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" ht="45" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>137</v>
       </c>
@@ -5566,7 +5599,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>138</v>
       </c>
@@ -5577,7 +5610,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="105" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" ht="105" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>139</v>
       </c>
@@ -5588,7 +5621,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>140</v>
       </c>
@@ -5599,7 +5632,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>141</v>
       </c>
@@ -5610,7 +5643,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>142</v>
       </c>
@@ -5621,7 +5654,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>143</v>
       </c>
@@ -5632,7 +5665,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>144</v>
       </c>
@@ -5643,7 +5676,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>145</v>
       </c>
@@ -5654,7 +5687,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>146</v>
       </c>
@@ -5665,7 +5698,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>147</v>
       </c>
@@ -5676,7 +5709,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>148</v>
       </c>
@@ -5687,7 +5720,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>149</v>
       </c>
@@ -5698,7 +5731,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>150</v>
       </c>
@@ -5709,7 +5742,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>151</v>
       </c>
@@ -5720,7 +5753,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>152</v>
       </c>
@@ -5731,7 +5764,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>153</v>
       </c>
@@ -5742,7 +5775,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>154</v>
       </c>
@@ -5753,7 +5786,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>155</v>
       </c>

</xml_diff>

<commit_message>
Added estimates for US13 & US14
</commit_message>
<xml_diff>
--- a/Team2Report.xlsx
+++ b/Team2Report.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23127"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RedRo\OneDrive\Documents\Academic Texts\COOOOOOODE\Python Workspace\anaconda\Agile_Methods_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="15" documentId="13_ncr:1_{AE5CA4A4-01C8-4A2A-9163-0272620C4B31}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{2755712C-E666-4E10-8D08-1EBE7E75A1FD}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{025FE077-6E90-4525-A095-6B67545ADA9E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13236" yWindow="0" windowWidth="9804" windowHeight="8964" tabRatio="500" firstSheet="5" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" firstSheet="3" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
     <sheet name="Sprint4" sheetId="6" r:id="rId8"/>
     <sheet name="Stories" sheetId="11" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="191028" calcCompleted="0"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -34,7 +34,6 @@
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -1020,7 +1019,7 @@
     <numFmt numFmtId="164" formatCode="m/d"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Verdana"/>
@@ -1281,7 +1280,7 @@
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
+  <c:date1904 val="1"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -1418,7 +1417,7 @@
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
+  <c:date1904 val="1"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -2367,16 +2366,16 @@
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.5" customWidth="1"/>
-    <col min="4" max="4" width="22.875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.5" customWidth="1"/>
+    <col min="1" max="1" width="7.90625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.08984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.453125" customWidth="1"/>
+    <col min="4" max="4" width="22.90625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="4" customFormat="1">
+    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -2393,7 +2392,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -2410,7 +2409,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -2427,7 +2426,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -2444,7 +2443,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -2461,7 +2460,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>25</v>
       </c>
@@ -2478,7 +2477,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D8" s="4" t="s">
         <v>30</v>
       </c>
@@ -2511,16 +2510,16 @@
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="6.875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.90625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="29" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="4" customFormat="1">
+    <row r="1" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>32</v>
       </c>
@@ -2537,7 +2536,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2554,7 +2553,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -2577,7 +2576,7 @@
       <c r="I3" s="23"/>
       <c r="J3" s="23"/>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1</v>
       </c>
@@ -2594,7 +2593,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1</v>
       </c>
@@ -2611,7 +2610,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>1</v>
       </c>
@@ -2628,7 +2627,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>1</v>
       </c>
@@ -2645,7 +2644,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>1</v>
       </c>
@@ -2662,7 +2661,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>1</v>
       </c>
@@ -2679,7 +2678,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>1</v>
       </c>
@@ -2696,7 +2695,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>1</v>
       </c>
@@ -2713,7 +2712,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>2</v>
       </c>
@@ -2730,7 +2729,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>2</v>
       </c>
@@ -2747,7 +2746,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>2</v>
       </c>
@@ -2764,7 +2763,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>2</v>
       </c>
@@ -2781,7 +2780,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>2</v>
       </c>
@@ -2798,7 +2797,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>2</v>
       </c>
@@ -2815,7 +2814,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>2</v>
       </c>
@@ -2832,7 +2831,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>2</v>
       </c>
@@ -2849,7 +2848,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>2</v>
       </c>
@@ -2866,7 +2865,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>2</v>
       </c>
@@ -2883,7 +2882,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>3</v>
       </c>
@@ -2900,7 +2899,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>3</v>
       </c>
@@ -2917,7 +2916,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>3</v>
       </c>
@@ -2934,7 +2933,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>3</v>
       </c>
@@ -2951,7 +2950,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>3</v>
       </c>
@@ -2968,7 +2967,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>3</v>
       </c>
@@ -2985,7 +2984,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="28" spans="1:5">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>3</v>
       </c>
@@ -3002,7 +3001,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="29" spans="1:5">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>3</v>
       </c>
@@ -3019,7 +3018,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="30" spans="1:5">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>3</v>
       </c>
@@ -3036,7 +3035,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="31" spans="1:5">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>3</v>
       </c>
@@ -3053,7 +3052,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="32" spans="1:5">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>4</v>
       </c>
@@ -3070,7 +3069,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="33" spans="1:5">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>4</v>
       </c>
@@ -3087,7 +3086,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="34" spans="1:5">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>4</v>
       </c>
@@ -3104,7 +3103,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="35" spans="1:5">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>4</v>
       </c>
@@ -3121,7 +3120,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="36" spans="1:5">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>4</v>
       </c>
@@ -3138,7 +3137,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="37" spans="1:5">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>4</v>
       </c>
@@ -3155,7 +3154,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="38" spans="1:5">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>4</v>
       </c>
@@ -3172,7 +3171,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="39" spans="1:5">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>4</v>
       </c>
@@ -3189,7 +3188,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="40" spans="1:5">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>4</v>
       </c>
@@ -3206,7 +3205,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="41" spans="1:5">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>4</v>
       </c>
@@ -3241,47 +3240,47 @@
       <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.875" style="7"/>
-    <col min="2" max="2" width="10.125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.25" customWidth="1"/>
-    <col min="5" max="5" width="6.875" customWidth="1"/>
-    <col min="6" max="6" width="12.5" style="9" customWidth="1"/>
+    <col min="1" max="1" width="10.90625" style="7"/>
+    <col min="2" max="2" width="10.08984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.90625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.26953125" customWidth="1"/>
+    <col min="5" max="5" width="6.90625" customWidth="1"/>
+    <col min="6" max="6" width="12.453125" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="4" customFormat="1">
+    <row r="14" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
         <v>125</v>
       </c>
@@ -3304,7 +3303,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>132</v>
       </c>
@@ -3320,7 +3319,7 @@
       <c r="F15" s="14"/>
       <c r="G15" s="9"/>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>133</v>
       </c>
@@ -3344,7 +3343,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="7" t="s">
         <v>134</v>
       </c>
@@ -3369,7 +3368,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="7" t="s">
         <v>135</v>
       </c>
@@ -3394,7 +3393,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="7" t="s">
         <v>136</v>
       </c>
@@ -3430,21 +3429,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView zoomScale="150" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.875" style="2"/>
-    <col min="2" max="2" width="16.75" customWidth="1"/>
-    <col min="3" max="3" width="12.5" customWidth="1"/>
-    <col min="4" max="4" width="7.125" customWidth="1"/>
-    <col min="5" max="5" width="6.875" customWidth="1"/>
-    <col min="6" max="6" width="12.5" style="9" customWidth="1"/>
+    <col min="1" max="1" width="10.90625" style="2"/>
+    <col min="2" max="2" width="16.7265625" customWidth="1"/>
+    <col min="3" max="3" width="12.453125" customWidth="1"/>
+    <col min="4" max="4" width="7.08984375" customWidth="1"/>
+    <col min="5" max="5" width="6.90625" customWidth="1"/>
+    <col min="6" max="6" width="12.453125" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="4" customFormat="1">
+    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>126</v>
       </c>
@@ -3464,7 +3463,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="13">
         <v>42632</v>
       </c>
@@ -3475,7 +3474,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="13">
         <v>42647</v>
       </c>
@@ -3499,17 +3498,17 @@
         <v>34.695652173913047</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="13">
         <v>42661</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="13">
         <v>42675</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="13">
         <v>42689</v>
       </c>
@@ -3526,23 +3525,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:I65"/>
   <sheetViews>
-    <sheetView topLeftCell="A38" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="K30" sqref="K30"/>
+    <sheetView topLeftCell="A41" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B63" sqref="B63"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="33" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.25" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.75" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.25" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.26953125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.7265625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.26953125" style="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>33</v>
       </c>
@@ -3571,7 +3570,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>37</v>
       </c>
@@ -3600,7 +3599,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="17" t="s">
         <v>143</v>
       </c>
@@ -3617,7 +3616,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="17" t="s">
         <v>146</v>
       </c>
@@ -3634,7 +3633,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="17" t="s">
         <v>148</v>
       </c>
@@ -3651,7 +3650,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>40</v>
       </c>
@@ -3680,7 +3679,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="17" t="s">
         <v>150</v>
       </c>
@@ -3697,7 +3696,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="17" t="s">
         <v>152</v>
       </c>
@@ -3714,7 +3713,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="17" t="s">
         <v>154</v>
       </c>
@@ -3731,7 +3730,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="17" t="s">
         <v>156</v>
       </c>
@@ -3748,7 +3747,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>43</v>
       </c>
@@ -3777,7 +3776,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="17" t="s">
         <v>158</v>
       </c>
@@ -3794,7 +3793,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="17" t="s">
         <v>160</v>
       </c>
@@ -3811,7 +3810,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="17" t="s">
         <v>161</v>
       </c>
@@ -3828,7 +3827,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="17" t="s">
         <v>163</v>
       </c>
@@ -3845,7 +3844,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>45</v>
       </c>
@@ -3874,7 +3873,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="17" spans="1:9">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="17" t="s">
         <v>165</v>
       </c>
@@ -3891,7 +3890,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="18" spans="1:9">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="17" t="s">
         <v>166</v>
       </c>
@@ -3908,7 +3907,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="19" spans="1:9">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="17" t="s">
         <v>168</v>
       </c>
@@ -3925,7 +3924,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="20" spans="1:9">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="17" t="s">
         <v>169</v>
       </c>
@@ -3942,7 +3941,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="21" spans="1:9">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" s="17" t="s">
         <v>171</v>
       </c>
@@ -3959,7 +3958,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="22" spans="1:9">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>47</v>
       </c>
@@ -3988,7 +3987,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="23" spans="1:9">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" s="17" t="s">
         <v>173</v>
       </c>
@@ -4005,7 +4004,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="24" spans="1:9">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" s="17" t="s">
         <v>174</v>
       </c>
@@ -4022,7 +4021,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="25" spans="1:9">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" s="17" t="s">
         <v>175</v>
       </c>
@@ -4039,7 +4038,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="26" spans="1:9">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" s="17" t="s">
         <v>176</v>
       </c>
@@ -4056,7 +4055,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="27" spans="1:9">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" s="17" t="s">
         <v>177</v>
       </c>
@@ -4073,7 +4072,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="28" spans="1:9">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>49</v>
       </c>
@@ -4102,7 +4101,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="29" spans="1:9">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" s="17" t="s">
         <v>179</v>
       </c>
@@ -4119,7 +4118,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="30" spans="1:9">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" s="17" t="s">
         <v>180</v>
       </c>
@@ -4136,7 +4135,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="31" spans="1:9">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" s="17" t="s">
         <v>181</v>
       </c>
@@ -4153,7 +4152,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="32" spans="1:9">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" s="17" t="s">
         <v>182</v>
       </c>
@@ -4170,7 +4169,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="33" spans="1:9">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" s="17" t="s">
         <v>183</v>
       </c>
@@ -4187,7 +4186,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="34" spans="1:9">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>51</v>
       </c>
@@ -4216,7 +4215,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="35" spans="1:9">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" s="17" t="s">
         <v>185</v>
       </c>
@@ -4233,7 +4232,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="36" spans="1:9">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" s="17" t="s">
         <v>186</v>
       </c>
@@ -4250,7 +4249,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="37" spans="1:9">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" s="17" t="s">
         <v>188</v>
       </c>
@@ -4267,7 +4266,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="38" spans="1:9">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" s="17" t="s">
         <v>190</v>
       </c>
@@ -4284,7 +4283,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="39" spans="1:9">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39" s="17" t="s">
         <v>191</v>
       </c>
@@ -4301,7 +4300,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="40" spans="1:9">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40" s="17" t="s">
         <v>193</v>
       </c>
@@ -4318,7 +4317,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="41" spans="1:9">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>53</v>
       </c>
@@ -4347,7 +4346,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="42" spans="1:9">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42" s="17" t="s">
         <v>195</v>
       </c>
@@ -4364,7 +4363,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="43" spans="1:9">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43" s="17" t="s">
         <v>196</v>
       </c>
@@ -4381,7 +4380,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="44" spans="1:9">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44" s="17" t="s">
         <v>197</v>
       </c>
@@ -4398,7 +4397,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="45" spans="1:9">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>55</v>
       </c>
@@ -4427,7 +4426,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="46" spans="1:9">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A46" s="17" t="s">
         <v>198</v>
       </c>
@@ -4444,7 +4443,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="47" spans="1:9">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A47" s="17" t="s">
         <v>200</v>
       </c>
@@ -4461,7 +4460,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="48" spans="1:9">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A48" s="17" t="s">
         <v>202</v>
       </c>
@@ -4478,7 +4477,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="49" spans="1:9">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A49" s="17" t="s">
         <v>203</v>
       </c>
@@ -4495,7 +4494,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="50" spans="1:9">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>57</v>
       </c>
@@ -4524,7 +4523,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="51" spans="1:9">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A51" s="17" t="s">
         <v>205</v>
       </c>
@@ -4541,7 +4540,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="52" spans="1:9">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A52" s="17" t="s">
         <v>207</v>
       </c>
@@ -4558,7 +4557,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="53" spans="1:9">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A53" s="17" t="s">
         <v>208</v>
       </c>
@@ -4575,7 +4574,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="54" spans="1:9">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A54" s="17" t="s">
         <v>209</v>
       </c>
@@ -4592,7 +4591,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="55" spans="1:9">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A55" s="17" t="s">
         <v>211</v>
       </c>
@@ -4609,7 +4608,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="56" spans="1:9">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A56" s="4" t="s">
         <v>213</v>
       </c>
@@ -4634,21 +4633,21 @@
       </c>
       <c r="I56" s="21"/>
     </row>
-    <row r="57" spans="1:9">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A57" s="17"/>
       <c r="I57" s="7"/>
     </row>
-    <row r="58" spans="1:9">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B58" s="5" t="s">
         <v>214</v>
       </c>
       <c r="I58" s="7"/>
     </row>
-    <row r="59" spans="1:9">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B59" s="5"/>
       <c r="I59" s="7"/>
     </row>
-    <row r="60" spans="1:9">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B60" s="5" t="s">
         <v>215</v>
       </c>
@@ -4657,19 +4656,19 @@
       </c>
       <c r="I60" s="7"/>
     </row>
-    <row r="61" spans="1:9">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C61" t="s">
         <v>217</v>
       </c>
       <c r="I61" s="7"/>
     </row>
-    <row r="62" spans="1:9">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C62" t="s">
         <v>218</v>
       </c>
       <c r="I62" s="7"/>
     </row>
-    <row r="64" spans="1:9">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B64" s="5" t="s">
         <v>219</v>
       </c>
@@ -4678,7 +4677,7 @@
       </c>
       <c r="I64" s="7"/>
     </row>
-    <row r="65" spans="3:3">
+    <row r="65" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C65" t="s">
         <v>221</v>
       </c>
@@ -4694,16 +4693,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:I34"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="54.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="54.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>33</v>
       </c>
@@ -4732,7 +4731,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>59</v>
       </c>
@@ -4746,7 +4745,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>61</v>
       </c>
@@ -4760,7 +4759,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>63</v>
       </c>
@@ -4773,8 +4772,14 @@
       <c r="D4" s="17" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="5" spans="1:9">
+      <c r="E4">
+        <v>50</v>
+      </c>
+      <c r="F4">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>65</v>
       </c>
@@ -4787,8 +4792,14 @@
       <c r="D5" s="17" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="6" spans="1:9">
+      <c r="E5">
+        <v>70</v>
+      </c>
+      <c r="F5">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>67</v>
       </c>
@@ -4808,7 +4819,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>69</v>
       </c>
@@ -4828,7 +4839,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>71</v>
       </c>
@@ -4842,7 +4853,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>73</v>
       </c>
@@ -4856,7 +4867,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>75</v>
       </c>
@@ -4870,7 +4881,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>222</v>
       </c>
@@ -4890,7 +4901,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>224</v>
       </c>
@@ -4904,7 +4915,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>226</v>
       </c>
@@ -4918,7 +4929,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>228</v>
       </c>
@@ -4932,7 +4943,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>230</v>
       </c>
@@ -4946,7 +4957,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>232</v>
       </c>
@@ -4960,7 +4971,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>234</v>
       </c>
@@ -4974,7 +4985,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>236</v>
       </c>
@@ -4988,7 +4999,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>238</v>
       </c>
@@ -5002,7 +5013,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>240</v>
       </c>
@@ -5016,7 +5027,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>242</v>
       </c>
@@ -5030,7 +5041,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>244</v>
       </c>
@@ -5044,7 +5055,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>246</v>
       </c>
@@ -5058,7 +5069,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>248</v>
       </c>
@@ -5072,7 +5083,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>250</v>
       </c>
@@ -5086,7 +5097,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>252</v>
       </c>
@@ -5100,7 +5111,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>77</v>
       </c>
@@ -5120,7 +5131,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="28" spans="1:6">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>254</v>
       </c>
@@ -5134,7 +5145,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="29" spans="1:6">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>256</v>
       </c>
@@ -5148,7 +5159,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="30" spans="1:6">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>258</v>
       </c>
@@ -5162,7 +5173,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="31" spans="1:6">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>259</v>
       </c>
@@ -5176,7 +5187,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="32" spans="1:6">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>260</v>
       </c>
@@ -5190,7 +5201,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="33" spans="1:4">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>262</v>
       </c>
@@ -5204,7 +5215,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="34" spans="1:4">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>264</v>
       </c>
@@ -5233,9 +5244,9 @@
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>33</v>
       </c>
@@ -5278,9 +5289,9 @@
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>33</v>
       </c>
@@ -5319,17 +5330,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:C43"/>
   <sheetViews>
-    <sheetView topLeftCell="B35" zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView topLeftCell="B10" zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="28.125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="49.5" style="1" customWidth="1"/>
+    <col min="2" max="2" width="28.08984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="49.453125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="4" customFormat="1">
+    <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>266</v>
       </c>
@@ -5340,7 +5351,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="30">
+    <row r="2" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>37</v>
       </c>
@@ -5351,7 +5362,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15">
+    <row r="3" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>40</v>
       </c>
@@ -5362,7 +5373,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15">
+    <row r="4" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>43</v>
       </c>
@@ -5373,7 +5384,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="30">
+    <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>45</v>
       </c>
@@ -5384,7 +5395,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="15">
+    <row r="6" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>47</v>
       </c>
@@ -5395,7 +5406,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="15">
+    <row r="7" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>49</v>
       </c>
@@ -5406,7 +5417,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="45">
+    <row r="8" spans="1:3" ht="45" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>51</v>
       </c>
@@ -5417,7 +5428,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="30">
+    <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>53</v>
       </c>
@@ -5428,7 +5439,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="30">
+    <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>55</v>
       </c>
@@ -5439,7 +5450,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="30">
+    <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>57</v>
       </c>
@@ -5450,7 +5461,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="30">
+    <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>59</v>
       </c>
@@ -5461,7 +5472,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="45">
+    <row r="13" spans="1:3" ht="45" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>61</v>
       </c>
@@ -5472,7 +5483,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="45">
+    <row r="14" spans="1:3" ht="45" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>63</v>
       </c>
@@ -5483,7 +5494,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="15">
+    <row r="15" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>65</v>
       </c>
@@ -5494,7 +5505,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="15">
+    <row r="16" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>67</v>
       </c>
@@ -5505,7 +5516,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="30">
+    <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>69</v>
       </c>
@@ -5516,7 +5527,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="15">
+    <row r="18" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>71</v>
       </c>
@@ -5527,7 +5538,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="15">
+    <row r="19" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>73</v>
       </c>
@@ -5538,7 +5549,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="15">
+    <row r="20" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>75</v>
       </c>
@@ -5549,7 +5560,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="15">
+    <row r="21" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>77</v>
       </c>
@@ -5560,7 +5571,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="30">
+    <row r="22" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>79</v>
       </c>
@@ -5571,7 +5582,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="30">
+    <row r="23" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>81</v>
       </c>
@@ -5582,7 +5593,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="30">
+    <row r="24" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>83</v>
       </c>
@@ -5593,7 +5604,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="45">
+    <row r="25" spans="1:3" ht="45" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>85</v>
       </c>
@@ -5604,7 +5615,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="30">
+    <row r="26" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>87</v>
       </c>
@@ -5615,7 +5626,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="105">
+    <row r="27" spans="1:3" ht="105" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>89</v>
       </c>
@@ -5626,7 +5637,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="15">
+    <row r="28" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>91</v>
       </c>
@@ -5637,7 +5648,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="30">
+    <row r="29" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>93</v>
       </c>
@@ -5648,7 +5659,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="15">
+    <row r="30" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>95</v>
       </c>
@@ -5659,7 +5670,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="15">
+    <row r="31" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>97</v>
       </c>
@@ -5670,7 +5681,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="30">
+    <row r="32" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>99</v>
       </c>
@@ -5681,7 +5692,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="15">
+    <row r="33" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>101</v>
       </c>
@@ -5692,7 +5703,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="30">
+    <row r="34" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>103</v>
       </c>
@@ -5703,7 +5714,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="30">
+    <row r="35" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>105</v>
       </c>
@@ -5714,7 +5725,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="30">
+    <row r="36" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>107</v>
       </c>
@@ -5725,7 +5736,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="15">
+    <row r="37" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>109</v>
       </c>
@@ -5736,7 +5747,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="30">
+    <row r="38" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>111</v>
       </c>
@@ -5747,7 +5758,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="30">
+    <row r="39" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>113</v>
       </c>
@@ -5758,7 +5769,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="30">
+    <row r="40" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>115</v>
       </c>
@@ -5769,7 +5780,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="30">
+    <row r="41" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>117</v>
       </c>
@@ -5780,7 +5791,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="30">
+    <row r="42" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>309</v>
       </c>
@@ -5791,7 +5802,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="30">
+    <row r="43" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>312</v>
       </c>

</xml_diff>

<commit_message>
Updated Team2 Report, sprint1AllTests.py and added test Results
Updated Team2 Report, sprint1AllTests.py and added test Results
</commit_message>
<xml_diff>
--- a/Team2Report.xlsx
+++ b/Team2Report.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10914"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Avaneesh/Desktop/CS 555/AgileMethodsProject/Agile_Methods_Project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/srikanth/Documenta/StevensInstitute/SoftwareEngg/SSW-555/SSW-555Project/Agile_Methods_Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="8" documentId="13_ncr:1_{CAD82888-E8C0-1741-A285-0C69E8134D77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{AE6CE610-402B-4DD1-A3F0-A7E16CFFE0F8}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BCE52E6-9655-3944-9A0E-B6A4DEF34B85}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25140" windowHeight="14640" tabRatio="500" firstSheet="3" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25140" windowHeight="14640" tabRatio="500" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -23,19 +23,10 @@
     <sheet name="Sprint4" sheetId="6" r:id="rId8"/>
     <sheet name="Stories" sheetId="11" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="191028" calcCompleted="0"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -45,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="798" uniqueCount="316">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="842" uniqueCount="334">
   <si>
     <t>Initials</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -1013,6 +1004,60 @@
   </si>
   <si>
     <t>All dates should be legitimate dates for the months specified (e.g., 2/30/2015 is not legitimate)</t>
+  </si>
+  <si>
+    <t>T17.01</t>
+  </si>
+  <si>
+    <t>T17.02</t>
+  </si>
+  <si>
+    <t>Find all the children in a family</t>
+  </si>
+  <si>
+    <t>T17.03</t>
+  </si>
+  <si>
+    <t>For each child check if the husband's ID is matching with any family members</t>
+  </si>
+  <si>
+    <t>T17.03.1</t>
+  </si>
+  <si>
+    <t>Output the error for descendants marriage</t>
+  </si>
+  <si>
+    <t>T17.04</t>
+  </si>
+  <si>
+    <t>For each child check if the wife's ID is matching with any family members</t>
+  </si>
+  <si>
+    <t>T17.04.1</t>
+  </si>
+  <si>
+    <t>T18.01</t>
+  </si>
+  <si>
+    <t>T18.02</t>
+  </si>
+  <si>
+    <t>T18.03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">For each child check if the child is married and fetch the spouse ID, </t>
+  </si>
+  <si>
+    <t>T18.04</t>
+  </si>
+  <si>
+    <t>Compare if a child's Spouse ID is matching with any of children in a family.</t>
+  </si>
+  <si>
+    <t>T18.04.1</t>
+  </si>
+  <si>
+    <t>Output the error for siblings marriage</t>
   </si>
 </sst>
 </file>
@@ -1023,7 +1068,7 @@
     <numFmt numFmtId="164" formatCode="m/d"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Verdana"/>
@@ -1078,12 +1123,27 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -1155,7 +1215,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1197,8 +1257,23 @@
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="66">
@@ -1284,7 +1359,7 @@
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
+  <c:date1904 val="1"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -1309,7 +1384,7 @@
             <c:numRef>
               <c:f>'Burndown README'!$B$15:$B$20</c:f>
               <c:numCache>
-                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:formatCode>m/d/yy</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>42632</c:v>
@@ -1380,7 +1455,7 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
+        <c:numFmt formatCode="m/d/yy" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1421,7 +1496,7 @@
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
+  <c:date1904 val="1"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -1446,7 +1521,7 @@
             <c:numRef>
               <c:f>Burndown!$A$2:$A$7</c:f>
               <c:numCache>
-                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:formatCode>m/d/yy</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>42632</c:v>
@@ -1476,16 +1551,7 @@
                   <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>40</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>40</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>40</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1517,7 +1583,7 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
+        <c:numFmt formatCode="m/d/yy" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2379,16 +2445,16 @@
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.95"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="7.875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.5" customWidth="1"/>
-    <col min="4" max="4" width="22.875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.83203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="20.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="4" customFormat="1">
+    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -2405,7 +2471,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -2422,7 +2488,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -2439,7 +2505,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -2456,7 +2522,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -2473,7 +2539,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>25</v>
       </c>
@@ -2490,7 +2556,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.15">
       <c r="D8" s="4" t="s">
         <v>30</v>
       </c>
@@ -2499,7 +2565,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D4">
+  <sortState ref="A2:D4">
     <sortCondition ref="C2:C4"/>
   </sortState>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -2519,20 +2585,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E11"/>
+    <sheetView zoomScale="150" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.95"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="6.875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="29" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="4" customFormat="1">
+    <row r="1" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>32</v>
       </c>
@@ -2549,7 +2615,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2566,7 +2632,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A3">
         <v>1</v>
       </c>
@@ -2582,14 +2648,14 @@
       <c r="E3" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="G3" s="23" t="s">
+      <c r="G3" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="H3" s="23"/>
-      <c r="I3" s="23"/>
-      <c r="J3" s="23"/>
-    </row>
-    <row r="4" spans="1:10">
+      <c r="H3" s="25"/>
+      <c r="I3" s="25"/>
+      <c r="J3" s="25"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A4">
         <v>1</v>
       </c>
@@ -2606,7 +2672,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A5">
         <v>1</v>
       </c>
@@ -2623,7 +2689,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A6">
         <v>1</v>
       </c>
@@ -2640,7 +2706,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A7">
         <v>1</v>
       </c>
@@ -2657,7 +2723,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A8">
         <v>1</v>
       </c>
@@ -2674,7 +2740,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A9">
         <v>1</v>
       </c>
@@ -2691,7 +2757,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A10">
         <v>1</v>
       </c>
@@ -2708,7 +2774,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A11">
         <v>1</v>
       </c>
@@ -2725,7 +2791,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A12">
         <v>2</v>
       </c>
@@ -2742,7 +2808,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A13">
         <v>2</v>
       </c>
@@ -2759,7 +2825,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A14">
         <v>2</v>
       </c>
@@ -2776,7 +2842,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A15">
         <v>2</v>
       </c>
@@ -2793,7 +2859,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A16">
         <v>2</v>
       </c>
@@ -2810,7 +2876,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A17">
         <v>2</v>
       </c>
@@ -2827,7 +2893,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A18">
         <v>2</v>
       </c>
@@ -2844,7 +2910,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A19">
         <v>2</v>
       </c>
@@ -2861,7 +2927,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A20">
         <v>2</v>
       </c>
@@ -2878,7 +2944,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A21">
         <v>2</v>
       </c>
@@ -2895,7 +2961,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A22">
         <v>3</v>
       </c>
@@ -2912,7 +2978,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A23">
         <v>3</v>
       </c>
@@ -2929,7 +2995,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A24">
         <v>3</v>
       </c>
@@ -2946,7 +3012,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A25">
         <v>3</v>
       </c>
@@ -2963,7 +3029,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A26">
         <v>3</v>
       </c>
@@ -2980,7 +3046,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A27">
         <v>3</v>
       </c>
@@ -2997,7 +3063,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="28" spans="1:5">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A28">
         <v>3</v>
       </c>
@@ -3014,7 +3080,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="29" spans="1:5">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A29">
         <v>3</v>
       </c>
@@ -3031,7 +3097,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="30" spans="1:5">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A30">
         <v>3</v>
       </c>
@@ -3048,7 +3114,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="31" spans="1:5">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A31">
         <v>3</v>
       </c>
@@ -3065,7 +3131,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="32" spans="1:5">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A32">
         <v>4</v>
       </c>
@@ -3082,7 +3148,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="33" spans="1:5">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A33">
         <v>4</v>
       </c>
@@ -3099,7 +3165,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="34" spans="1:5">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A34">
         <v>4</v>
       </c>
@@ -3116,7 +3182,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="35" spans="1:5">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A35">
         <v>4</v>
       </c>
@@ -3133,7 +3199,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="36" spans="1:5">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A36">
         <v>4</v>
       </c>
@@ -3150,7 +3216,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="37" spans="1:5">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A37">
         <v>4</v>
       </c>
@@ -3167,7 +3233,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="38" spans="1:5">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A38">
         <v>4</v>
       </c>
@@ -3184,7 +3250,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="39" spans="1:5">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A39">
         <v>4</v>
       </c>
@@ -3201,7 +3267,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="40" spans="1:5">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A40">
         <v>4</v>
       </c>
@@ -3218,7 +3284,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="41" spans="1:5">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A41">
         <v>4</v>
       </c>
@@ -3250,50 +3316,50 @@
   <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.95"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="10.875" style="7"/>
-    <col min="2" max="2" width="10.125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.375" customWidth="1"/>
-    <col min="5" max="5" width="6.875" customWidth="1"/>
+    <col min="1" max="1" width="10.83203125" style="7"/>
+    <col min="2" max="2" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.33203125" customWidth="1"/>
+    <col min="5" max="5" width="6.83203125" customWidth="1"/>
     <col min="6" max="6" width="12.5" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A1" s="7" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A2" s="7" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A3" s="7" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A5" s="7" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A6" s="7" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A8" s="7" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="4" customFormat="1">
+    <row r="14" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A14" s="4" t="s">
         <v>126</v>
       </c>
@@ -3316,7 +3382,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
         <v>133</v>
       </c>
@@ -3332,7 +3398,7 @@
       <c r="F15" s="14"/>
       <c r="G15" s="9"/>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
         <v>134</v>
       </c>
@@ -3356,7 +3422,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A17" s="7" t="s">
         <v>135</v>
       </c>
@@ -3381,7 +3447,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A18" s="7" t="s">
         <v>136</v>
       </c>
@@ -3406,7 +3472,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A19" s="7" t="s">
         <v>137</v>
       </c>
@@ -3442,21 +3508,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.95"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="10.875" style="2"/>
-    <col min="2" max="2" width="16.625" customWidth="1"/>
-    <col min="3" max="3" width="12.5" customWidth="1"/>
-    <col min="4" max="4" width="7.125" customWidth="1"/>
-    <col min="5" max="5" width="6.875" customWidth="1"/>
+    <col min="1" max="1" width="10.83203125" style="2"/>
+    <col min="2" max="2" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.1640625" customWidth="1"/>
+    <col min="5" max="5" width="6.83203125" customWidth="1"/>
     <col min="6" max="6" width="12.5" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="4" customFormat="1">
+    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="3" t="s">
         <v>127</v>
       </c>
@@ -3476,27 +3542,37 @@
         <v>132</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A2" s="13">
         <v>42632</v>
       </c>
       <c r="B2">
         <v>40</v>
       </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
       <c r="D2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:6">
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A3" s="13">
         <v>42647</v>
       </c>
       <c r="B3">
-        <v>0</v>
+        <f>B2-COUNTIF(Sprint1!$I$2:$I$55, "Completed")</f>
+        <v>30</v>
       </c>
       <c r="C3">
         <f>B2-B3</f>
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="D3">
         <f>Sprint1!G56</f>
@@ -3511,64 +3587,19 @@
         <v>34.695652173913047</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A4" s="13">
         <v>42661</v>
       </c>
-      <c r="B4">
-        <v>40</v>
-      </c>
-      <c r="C4">
-        <v>0</v>
-      </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-      <c r="E4">
-        <v>0</v>
-      </c>
-      <c r="F4" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A5" s="13">
         <v>42675</v>
       </c>
-      <c r="B5">
-        <v>40</v>
-      </c>
-      <c r="C5">
-        <v>0</v>
-      </c>
-      <c r="D5">
-        <v>0</v>
-      </c>
-      <c r="E5">
-        <v>0</v>
-      </c>
-      <c r="F5" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A6" s="13">
         <v>42689</v>
-      </c>
-      <c r="B6">
-        <v>40</v>
-      </c>
-      <c r="C6">
-        <v>0</v>
-      </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-      <c r="E6">
-        <v>0</v>
-      </c>
-      <c r="F6" s="9">
-        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -3584,22 +3615,22 @@
   <dimension ref="A1:I65"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="H68" sqref="H68"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.95"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="33" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.375" style="6" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.33203125" style="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="14.1">
+    <row r="1" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>33</v>
       </c>
@@ -3628,7 +3659,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>37</v>
       </c>
@@ -3657,7 +3688,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A3" s="17" t="s">
         <v>144</v>
       </c>
@@ -3674,7 +3705,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="14.1">
+    <row r="4" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A4" s="17" t="s">
         <v>147</v>
       </c>
@@ -3691,7 +3722,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A5" s="17" t="s">
         <v>149</v>
       </c>
@@ -3708,7 +3739,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>40</v>
       </c>
@@ -3737,7 +3768,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A7" s="17" t="s">
         <v>151</v>
       </c>
@@ -3754,7 +3785,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A8" s="17" t="s">
         <v>153</v>
       </c>
@@ -3771,7 +3802,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A9" s="17" t="s">
         <v>155</v>
       </c>
@@ -3788,7 +3819,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A10" s="17" t="s">
         <v>157</v>
       </c>
@@ -3805,7 +3836,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
         <v>43</v>
       </c>
@@ -3834,7 +3865,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A12" s="17" t="s">
         <v>159</v>
       </c>
@@ -3851,7 +3882,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A13" s="17" t="s">
         <v>161</v>
       </c>
@@ -3868,7 +3899,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A14" s="17" t="s">
         <v>162</v>
       </c>
@@ -3885,7 +3916,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A15" s="17" t="s">
         <v>164</v>
       </c>
@@ -3902,7 +3933,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
         <v>45</v>
       </c>
@@ -3931,7 +3962,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="17" spans="1:9">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A17" s="17" t="s">
         <v>166</v>
       </c>
@@ -3948,7 +3979,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="18" spans="1:9">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A18" s="17" t="s">
         <v>167</v>
       </c>
@@ -3965,7 +3996,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="19" spans="1:9">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A19" s="17" t="s">
         <v>169</v>
       </c>
@@ -3982,7 +4013,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="20" spans="1:9">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A20" s="17" t="s">
         <v>170</v>
       </c>
@@ -3999,7 +4030,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="21" spans="1:9">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A21" s="17" t="s">
         <v>172</v>
       </c>
@@ -4016,7 +4047,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="22" spans="1:9">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A22" t="s">
         <v>47</v>
       </c>
@@ -4045,7 +4076,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="23" spans="1:9">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A23" s="17" t="s">
         <v>174</v>
       </c>
@@ -4062,7 +4093,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="24" spans="1:9">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A24" s="17" t="s">
         <v>175</v>
       </c>
@@ -4079,7 +4110,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="25" spans="1:9">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A25" s="17" t="s">
         <v>176</v>
       </c>
@@ -4096,7 +4127,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="26" spans="1:9">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A26" s="17" t="s">
         <v>177</v>
       </c>
@@ -4113,7 +4144,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="27" spans="1:9">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A27" s="17" t="s">
         <v>178</v>
       </c>
@@ -4130,7 +4161,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="28" spans="1:9">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A28" t="s">
         <v>49</v>
       </c>
@@ -4159,7 +4190,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="29" spans="1:9">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A29" s="17" t="s">
         <v>180</v>
       </c>
@@ -4176,7 +4207,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="30" spans="1:9">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A30" s="17" t="s">
         <v>181</v>
       </c>
@@ -4193,7 +4224,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="31" spans="1:9">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A31" s="17" t="s">
         <v>182</v>
       </c>
@@ -4210,7 +4241,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="32" spans="1:9">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A32" s="17" t="s">
         <v>183</v>
       </c>
@@ -4227,7 +4258,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="33" spans="1:9">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A33" s="17" t="s">
         <v>184</v>
       </c>
@@ -4244,7 +4275,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="34" spans="1:9">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A34" t="s">
         <v>51</v>
       </c>
@@ -4273,7 +4304,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="35" spans="1:9">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A35" s="17" t="s">
         <v>186</v>
       </c>
@@ -4290,7 +4321,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="36" spans="1:9">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A36" s="17" t="s">
         <v>187</v>
       </c>
@@ -4307,7 +4338,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="37" spans="1:9">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A37" s="17" t="s">
         <v>189</v>
       </c>
@@ -4324,7 +4355,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="38" spans="1:9">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A38" s="17" t="s">
         <v>191</v>
       </c>
@@ -4341,7 +4372,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="39" spans="1:9">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A39" s="17" t="s">
         <v>192</v>
       </c>
@@ -4358,7 +4389,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="40" spans="1:9">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A40" s="17" t="s">
         <v>194</v>
       </c>
@@ -4375,7 +4406,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="41" spans="1:9">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A41" t="s">
         <v>53</v>
       </c>
@@ -4404,7 +4435,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="42" spans="1:9">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A42" s="17" t="s">
         <v>196</v>
       </c>
@@ -4421,7 +4452,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="43" spans="1:9">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A43" s="17" t="s">
         <v>197</v>
       </c>
@@ -4438,7 +4469,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="44" spans="1:9">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A44" s="17" t="s">
         <v>198</v>
       </c>
@@ -4455,7 +4486,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="45" spans="1:9">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A45" t="s">
         <v>55</v>
       </c>
@@ -4484,7 +4515,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="46" spans="1:9">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A46" s="17" t="s">
         <v>199</v>
       </c>
@@ -4501,7 +4532,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="47" spans="1:9">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A47" s="17" t="s">
         <v>201</v>
       </c>
@@ -4518,7 +4549,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="48" spans="1:9">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A48" s="17" t="s">
         <v>203</v>
       </c>
@@ -4535,7 +4566,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="49" spans="1:9">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A49" s="17" t="s">
         <v>204</v>
       </c>
@@ -4552,7 +4583,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="50" spans="1:9">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A50" t="s">
         <v>57</v>
       </c>
@@ -4581,7 +4612,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="51" spans="1:9" ht="14.1">
+    <row r="51" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A51" s="17" t="s">
         <v>206</v>
       </c>
@@ -4598,7 +4629,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="52" spans="1:9" ht="14.1">
+    <row r="52" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A52" s="17" t="s">
         <v>208</v>
       </c>
@@ -4615,7 +4646,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="53" spans="1:9" ht="14.1">
+    <row r="53" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A53" s="17" t="s">
         <v>209</v>
       </c>
@@ -4632,7 +4663,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="54" spans="1:9" ht="14.1">
+    <row r="54" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A54" s="17" t="s">
         <v>210</v>
       </c>
@@ -4649,7 +4680,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="55" spans="1:9" ht="14.1">
+    <row r="55" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A55" s="17" t="s">
         <v>212</v>
       </c>
@@ -4666,7 +4697,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="56" spans="1:9">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A56" s="4" t="s">
         <v>214</v>
       </c>
@@ -4691,56 +4722,85 @@
       </c>
       <c r="I56" s="21"/>
     </row>
-    <row r="57" spans="1:9">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A57" s="17"/>
       <c r="I57" s="7"/>
     </row>
-    <row r="58" spans="1:9" ht="14.1">
+    <row r="58" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="B58" s="5" t="s">
         <v>215</v>
       </c>
       <c r="I58" s="7"/>
     </row>
-    <row r="59" spans="1:9">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B59" s="5"/>
       <c r="I59" s="7"/>
     </row>
-    <row r="60" spans="1:9" ht="14.1">
+    <row r="60" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="B60" s="5" t="s">
         <v>216</v>
       </c>
-      <c r="C60" t="s">
+      <c r="C60" s="26" t="s">
         <v>217</v>
       </c>
+      <c r="D60" s="26"/>
+      <c r="E60" s="26"/>
+      <c r="F60" s="26"/>
       <c r="I60" s="7"/>
     </row>
-    <row r="61" spans="1:9">
-      <c r="C61" t="s">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="C61" s="26" t="s">
         <v>218</v>
       </c>
+      <c r="D61" s="26"/>
+      <c r="E61" s="26"/>
+      <c r="F61" s="26"/>
       <c r="I61" s="7"/>
     </row>
-    <row r="62" spans="1:9">
-      <c r="C62" t="s">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="C62" s="26" t="s">
         <v>219</v>
       </c>
+      <c r="D62" s="26"/>
+      <c r="E62" s="26"/>
+      <c r="F62" s="26"/>
       <c r="I62" s="7"/>
     </row>
-    <row r="64" spans="1:9" ht="14.1">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="C63" s="28"/>
+      <c r="D63" s="28"/>
+      <c r="E63" s="28"/>
+      <c r="F63" s="28"/>
+    </row>
+    <row r="64" spans="1:9" ht="27" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B64" s="5" t="s">
         <v>220</v>
       </c>
-      <c r="C64" t="s">
+      <c r="C64" s="27" t="s">
         <v>221</v>
       </c>
+      <c r="D64" s="27"/>
+      <c r="E64" s="27"/>
+      <c r="F64" s="27"/>
       <c r="I64" s="7"/>
     </row>
-    <row r="65" spans="3:3">
-      <c r="C65" t="s">
+    <row r="65" spans="3:6" ht="26" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C65" s="27" t="s">
         <v>222</v>
       </c>
+      <c r="D65" s="27"/>
+      <c r="E65" s="27"/>
+      <c r="F65" s="27"/>
     </row>
   </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="C60:F60"/>
+    <mergeCell ref="C61:F61"/>
+    <mergeCell ref="C62:F62"/>
+    <mergeCell ref="C64:F64"/>
+    <mergeCell ref="C65:F65"/>
+    <mergeCell ref="C63:F63"/>
+  </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
@@ -4749,18 +4809,18 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:I34"/>
+  <dimension ref="A1:I45"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.95"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="2" max="2" width="54.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="54.6640625" style="23" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="14.1">
+    <row r="1" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>33</v>
       </c>
@@ -4789,11 +4849,11 @@
         <v>142</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
-      <c r="A2" t="s">
+    <row r="2" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+      <c r="A2" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="23" t="s">
         <v>60</v>
       </c>
       <c r="C2" s="17" t="s">
@@ -4809,11 +4869,11 @@
         <v>90</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
-      <c r="A3" t="s">
+    <row r="3" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+      <c r="A3" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="23" t="s">
         <v>63</v>
       </c>
       <c r="C3" s="17" t="s">
@@ -4829,11 +4889,11 @@
         <v>120</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
-      <c r="A4" t="s">
+    <row r="4" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+      <c r="A4" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="23" t="s">
         <v>65</v>
       </c>
       <c r="C4" s="17" t="s">
@@ -4849,11 +4909,11 @@
         <v>90</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
-      <c r="A5" t="s">
+    <row r="5" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+      <c r="A5" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="23" t="s">
         <v>67</v>
       </c>
       <c r="C5" s="17" t="s">
@@ -4869,11 +4929,11 @@
         <v>120</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
-      <c r="A6" t="s">
+    <row r="6" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+      <c r="A6" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="23" t="s">
         <v>69</v>
       </c>
       <c r="C6" s="17" t="s">
@@ -4889,11 +4949,11 @@
         <v>90</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
-      <c r="A7" t="s">
+    <row r="7" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+      <c r="A7" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="23" t="s">
         <v>71</v>
       </c>
       <c r="C7" s="17" t="s">
@@ -4909,11 +4969,11 @@
         <v>90</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
-      <c r="A8" t="s">
+    <row r="8" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+      <c r="A8" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="23" t="s">
         <v>73</v>
       </c>
       <c r="C8" s="17" t="s">
@@ -4922,13 +4982,19 @@
       <c r="D8" s="17" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="9" spans="1:9">
+      <c r="E8">
+        <v>40</v>
+      </c>
+      <c r="F8">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
-        <v>74</v>
-      </c>
-      <c r="B9" t="s">
-        <v>75</v>
+        <v>316</v>
+      </c>
+      <c r="B9" s="23" t="s">
+        <v>224</v>
       </c>
       <c r="C9" s="17" t="s">
         <v>20</v>
@@ -4937,172 +5003,172 @@
         <v>61</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
+        <v>317</v>
+      </c>
+      <c r="B10" s="23" t="s">
+        <v>318</v>
+      </c>
+      <c r="C10" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" s="17" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="28" x14ac:dyDescent="0.15">
+      <c r="A11" t="s">
+        <v>319</v>
+      </c>
+      <c r="B11" s="23" t="s">
+        <v>320</v>
+      </c>
+      <c r="C11" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="D11" s="17" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+      <c r="A12" t="s">
+        <v>321</v>
+      </c>
+      <c r="B12" s="23" t="s">
+        <v>322</v>
+      </c>
+      <c r="C12" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="D12" s="17" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="28" x14ac:dyDescent="0.15">
+      <c r="A13" t="s">
+        <v>323</v>
+      </c>
+      <c r="B13" s="23" t="s">
+        <v>324</v>
+      </c>
+      <c r="C13" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="D13" s="17" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+      <c r="A14" t="s">
+        <v>325</v>
+      </c>
+      <c r="B14" s="23" t="s">
+        <v>322</v>
+      </c>
+      <c r="C14" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="D14" s="17" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+      <c r="A15" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B15" s="23" t="s">
+        <v>75</v>
+      </c>
+      <c r="C15" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="D15" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="E15">
+        <v>40</v>
+      </c>
+      <c r="F15">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+      <c r="A16" t="s">
+        <v>326</v>
+      </c>
+      <c r="B16" s="23" t="s">
+        <v>224</v>
+      </c>
+      <c r="C16" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="D16" s="17" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="14" x14ac:dyDescent="0.15">
+      <c r="A17" t="s">
+        <v>327</v>
+      </c>
+      <c r="B17" s="23" t="s">
+        <v>318</v>
+      </c>
+      <c r="C17" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="D17" s="17" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="28" x14ac:dyDescent="0.15">
+      <c r="A18" t="s">
+        <v>328</v>
+      </c>
+      <c r="B18" s="23" t="s">
+        <v>329</v>
+      </c>
+      <c r="C18" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="D18" s="17" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="28" x14ac:dyDescent="0.15">
+      <c r="A19" t="s">
+        <v>330</v>
+      </c>
+      <c r="B19" s="23" t="s">
+        <v>331</v>
+      </c>
+      <c r="C19" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="D19" s="17" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="14" x14ac:dyDescent="0.15">
+      <c r="A20" t="s">
+        <v>332</v>
+      </c>
+      <c r="B20" s="24" t="s">
+        <v>333</v>
+      </c>
+      <c r="C20" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="D20" s="17" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="14" x14ac:dyDescent="0.15">
+      <c r="A21" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B21" s="23" t="s">
         <v>77</v>
-      </c>
-      <c r="C10" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="D10" s="17" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9">
-      <c r="A11" t="s">
-        <v>223</v>
-      </c>
-      <c r="B11" t="s">
-        <v>224</v>
-      </c>
-      <c r="C11" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="D11" s="17" t="s">
-        <v>61</v>
-      </c>
-      <c r="E11">
-        <v>65</v>
-      </c>
-      <c r="F11">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9">
-      <c r="A12" t="s">
-        <v>225</v>
-      </c>
-      <c r="B12" t="s">
-        <v>226</v>
-      </c>
-      <c r="C12" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="D12" s="17" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9">
-      <c r="A13" t="s">
-        <v>227</v>
-      </c>
-      <c r="B13" t="s">
-        <v>228</v>
-      </c>
-      <c r="C13" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="D13" s="17" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9">
-      <c r="A14" t="s">
-        <v>229</v>
-      </c>
-      <c r="B14" t="s">
-        <v>230</v>
-      </c>
-      <c r="C14" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="D14" s="17" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9">
-      <c r="A15" t="s">
-        <v>231</v>
-      </c>
-      <c r="B15" t="s">
-        <v>232</v>
-      </c>
-      <c r="C15" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="D15" s="17" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9">
-      <c r="A16" t="s">
-        <v>233</v>
-      </c>
-      <c r="B16" t="s">
-        <v>234</v>
-      </c>
-      <c r="C16" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="D16" s="17" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6">
-      <c r="A17" t="s">
-        <v>235</v>
-      </c>
-      <c r="B17" t="s">
-        <v>236</v>
-      </c>
-      <c r="C17" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="D17" s="17" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6">
-      <c r="A18" t="s">
-        <v>237</v>
-      </c>
-      <c r="B18" t="s">
-        <v>238</v>
-      </c>
-      <c r="C18" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="D18" s="17" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6">
-      <c r="A19" t="s">
-        <v>239</v>
-      </c>
-      <c r="B19" t="s">
-        <v>240</v>
-      </c>
-      <c r="C19" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="D19" s="17" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6">
-      <c r="A20" t="s">
-        <v>241</v>
-      </c>
-      <c r="B20" t="s">
-        <v>242</v>
-      </c>
-      <c r="C20" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="D20" s="17" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6">
-      <c r="A21" t="s">
-        <v>243</v>
-      </c>
-      <c r="B21" t="s">
-        <v>244</v>
       </c>
       <c r="C21" s="17" t="s">
         <v>25</v>
@@ -5111,12 +5177,12 @@
         <v>61</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:6" ht="14" x14ac:dyDescent="0.15">
       <c r="A22" t="s">
-        <v>245</v>
-      </c>
-      <c r="B22" t="s">
-        <v>246</v>
+        <v>223</v>
+      </c>
+      <c r="B22" s="23" t="s">
+        <v>224</v>
       </c>
       <c r="C22" s="17" t="s">
         <v>25</v>
@@ -5124,13 +5190,19 @@
       <c r="D22" s="17" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="23" spans="1:6">
+      <c r="E22">
+        <v>65</v>
+      </c>
+      <c r="F22">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="14" x14ac:dyDescent="0.15">
       <c r="A23" t="s">
-        <v>247</v>
-      </c>
-      <c r="B23" t="s">
-        <v>248</v>
+        <v>225</v>
+      </c>
+      <c r="B23" s="23" t="s">
+        <v>226</v>
       </c>
       <c r="C23" s="17" t="s">
         <v>25</v>
@@ -5139,12 +5211,12 @@
         <v>61</v>
       </c>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:6" ht="14" x14ac:dyDescent="0.15">
       <c r="A24" t="s">
-        <v>249</v>
-      </c>
-      <c r="B24" t="s">
-        <v>250</v>
+        <v>227</v>
+      </c>
+      <c r="B24" s="23" t="s">
+        <v>228</v>
       </c>
       <c r="C24" s="17" t="s">
         <v>25</v>
@@ -5153,12 +5225,12 @@
         <v>61</v>
       </c>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:6" ht="14" x14ac:dyDescent="0.15">
       <c r="A25" t="s">
-        <v>251</v>
-      </c>
-      <c r="B25" t="s">
-        <v>252</v>
+        <v>229</v>
+      </c>
+      <c r="B25" s="23" t="s">
+        <v>230</v>
       </c>
       <c r="C25" s="17" t="s">
         <v>25</v>
@@ -5167,12 +5239,12 @@
         <v>61</v>
       </c>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:6" ht="14" x14ac:dyDescent="0.15">
       <c r="A26" t="s">
-        <v>253</v>
-      </c>
-      <c r="B26" t="s">
-        <v>254</v>
+        <v>231</v>
+      </c>
+      <c r="B26" s="23" t="s">
+        <v>232</v>
       </c>
       <c r="C26" s="17" t="s">
         <v>25</v>
@@ -5181,12 +5253,12 @@
         <v>61</v>
       </c>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27" spans="1:6" ht="14" x14ac:dyDescent="0.15">
       <c r="A27" t="s">
-        <v>78</v>
-      </c>
-      <c r="B27" t="s">
-        <v>79</v>
+        <v>233</v>
+      </c>
+      <c r="B27" s="23" t="s">
+        <v>234</v>
       </c>
       <c r="C27" s="17" t="s">
         <v>25</v>
@@ -5194,19 +5266,13 @@
       <c r="D27" s="17" t="s">
         <v>61</v>
       </c>
-      <c r="E27">
-        <v>50</v>
-      </c>
-      <c r="F27">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6">
+    </row>
+    <row r="28" spans="1:6" ht="14" x14ac:dyDescent="0.15">
       <c r="A28" t="s">
-        <v>255</v>
-      </c>
-      <c r="B28" t="s">
-        <v>256</v>
+        <v>235</v>
+      </c>
+      <c r="B28" s="23" t="s">
+        <v>236</v>
       </c>
       <c r="C28" s="17" t="s">
         <v>25</v>
@@ -5215,12 +5281,12 @@
         <v>61</v>
       </c>
     </row>
-    <row r="29" spans="1:6">
+    <row r="29" spans="1:6" ht="14" x14ac:dyDescent="0.15">
       <c r="A29" t="s">
-        <v>257</v>
-      </c>
-      <c r="B29" t="s">
-        <v>258</v>
+        <v>237</v>
+      </c>
+      <c r="B29" s="23" t="s">
+        <v>238</v>
       </c>
       <c r="C29" s="17" t="s">
         <v>25</v>
@@ -5229,12 +5295,12 @@
         <v>61</v>
       </c>
     </row>
-    <row r="30" spans="1:6">
+    <row r="30" spans="1:6" ht="14" x14ac:dyDescent="0.15">
       <c r="A30" t="s">
-        <v>259</v>
-      </c>
-      <c r="B30" t="s">
-        <v>228</v>
+        <v>239</v>
+      </c>
+      <c r="B30" s="23" t="s">
+        <v>240</v>
       </c>
       <c r="C30" s="17" t="s">
         <v>25</v>
@@ -5243,12 +5309,12 @@
         <v>61</v>
       </c>
     </row>
-    <row r="31" spans="1:6">
+    <row r="31" spans="1:6" ht="14" x14ac:dyDescent="0.15">
       <c r="A31" t="s">
-        <v>260</v>
-      </c>
-      <c r="B31" t="s">
-        <v>230</v>
+        <v>241</v>
+      </c>
+      <c r="B31" s="23" t="s">
+        <v>242</v>
       </c>
       <c r="C31" s="17" t="s">
         <v>25</v>
@@ -5257,12 +5323,12 @@
         <v>61</v>
       </c>
     </row>
-    <row r="32" spans="1:6">
+    <row r="32" spans="1:6" ht="14" x14ac:dyDescent="0.15">
       <c r="A32" t="s">
-        <v>261</v>
-      </c>
-      <c r="B32" t="s">
-        <v>262</v>
+        <v>243</v>
+      </c>
+      <c r="B32" s="23" t="s">
+        <v>244</v>
       </c>
       <c r="C32" s="17" t="s">
         <v>25</v>
@@ -5271,12 +5337,12 @@
         <v>61</v>
       </c>
     </row>
-    <row r="33" spans="1:4">
+    <row r="33" spans="1:6" ht="14" x14ac:dyDescent="0.15">
       <c r="A33" t="s">
-        <v>263</v>
-      </c>
-      <c r="B33" t="s">
-        <v>264</v>
+        <v>245</v>
+      </c>
+      <c r="B33" s="23" t="s">
+        <v>246</v>
       </c>
       <c r="C33" s="17" t="s">
         <v>25</v>
@@ -5285,17 +5351,177 @@
         <v>61</v>
       </c>
     </row>
-    <row r="34" spans="1:4">
+    <row r="34" spans="1:6" ht="14" x14ac:dyDescent="0.15">
       <c r="A34" t="s">
-        <v>265</v>
-      </c>
-      <c r="B34" t="s">
-        <v>266</v>
+        <v>247</v>
+      </c>
+      <c r="B34" s="23" t="s">
+        <v>248</v>
       </c>
       <c r="C34" s="17" t="s">
         <v>25</v>
       </c>
       <c r="D34" s="17" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="14" x14ac:dyDescent="0.15">
+      <c r="A35" t="s">
+        <v>249</v>
+      </c>
+      <c r="B35" s="23" t="s">
+        <v>250</v>
+      </c>
+      <c r="C35" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="D35" s="17" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="28" x14ac:dyDescent="0.15">
+      <c r="A36" t="s">
+        <v>251</v>
+      </c>
+      <c r="B36" s="23" t="s">
+        <v>252</v>
+      </c>
+      <c r="C36" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="D36" s="17" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" ht="14" x14ac:dyDescent="0.15">
+      <c r="A37" t="s">
+        <v>253</v>
+      </c>
+      <c r="B37" s="23" t="s">
+        <v>254</v>
+      </c>
+      <c r="C37" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="D37" s="17" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="14" x14ac:dyDescent="0.15">
+      <c r="A38" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="B38" s="23" t="s">
+        <v>79</v>
+      </c>
+      <c r="C38" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="D38" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="E38">
+        <v>50</v>
+      </c>
+      <c r="F38">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" ht="14" x14ac:dyDescent="0.15">
+      <c r="A39" t="s">
+        <v>255</v>
+      </c>
+      <c r="B39" s="23" t="s">
+        <v>256</v>
+      </c>
+      <c r="C39" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="D39" s="17" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" ht="14" x14ac:dyDescent="0.15">
+      <c r="A40" t="s">
+        <v>257</v>
+      </c>
+      <c r="B40" s="23" t="s">
+        <v>258</v>
+      </c>
+      <c r="C40" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="D40" s="17" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" ht="14" x14ac:dyDescent="0.15">
+      <c r="A41" t="s">
+        <v>259</v>
+      </c>
+      <c r="B41" s="23" t="s">
+        <v>228</v>
+      </c>
+      <c r="C41" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="D41" s="17" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" ht="14" x14ac:dyDescent="0.15">
+      <c r="A42" t="s">
+        <v>260</v>
+      </c>
+      <c r="B42" s="23" t="s">
+        <v>230</v>
+      </c>
+      <c r="C42" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="D42" s="17" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" ht="14" x14ac:dyDescent="0.15">
+      <c r="A43" t="s">
+        <v>261</v>
+      </c>
+      <c r="B43" s="23" t="s">
+        <v>262</v>
+      </c>
+      <c r="C43" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="D43" s="17" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" ht="14" x14ac:dyDescent="0.15">
+      <c r="A44" t="s">
+        <v>263</v>
+      </c>
+      <c r="B44" s="23" t="s">
+        <v>264</v>
+      </c>
+      <c r="C44" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="D44" s="17" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" ht="14" x14ac:dyDescent="0.15">
+      <c r="A45" t="s">
+        <v>265</v>
+      </c>
+      <c r="B45" s="23" t="s">
+        <v>266</v>
+      </c>
+      <c r="C45" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="D45" s="17" t="s">
         <v>61</v>
       </c>
     </row>
@@ -5314,9 +5540,9 @@
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.95"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:9" ht="27.95">
+    <row r="1" spans="1:9" ht="28" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>33</v>
       </c>
@@ -5359,9 +5585,9 @@
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.95"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:9" ht="27.95">
+    <row r="1" spans="1:9" ht="28" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>33</v>
       </c>
@@ -5404,13 +5630,13 @@
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.95"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="2" max="2" width="28.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="49.5" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="4" customFormat="1" ht="14.1">
+    <row r="1" spans="1:3" s="4" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>267</v>
       </c>
@@ -5421,7 +5647,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="33.950000000000003">
+    <row r="2" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>37</v>
       </c>
@@ -5432,7 +5658,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="17.100000000000001">
+    <row r="3" spans="1:3" ht="17" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>40</v>
       </c>
@@ -5443,7 +5669,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="17.100000000000001">
+    <row r="4" spans="1:3" ht="17" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>43</v>
       </c>
@@ -5454,7 +5680,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="33.950000000000003">
+    <row r="5" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>45</v>
       </c>
@@ -5465,7 +5691,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="33.950000000000003">
+    <row r="6" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>47</v>
       </c>
@@ -5476,7 +5702,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="17.100000000000001">
+    <row r="7" spans="1:3" ht="17" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
         <v>49</v>
       </c>
@@ -5487,7 +5713,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="51">
+    <row r="8" spans="1:3" ht="51" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>51</v>
       </c>
@@ -5498,7 +5724,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="33.950000000000003">
+    <row r="9" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
         <v>53</v>
       </c>
@@ -5509,7 +5735,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="33.950000000000003">
+    <row r="10" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>55</v>
       </c>
@@ -5520,7 +5746,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="51">
+    <row r="11" spans="1:3" ht="51" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
         <v>57</v>
       </c>
@@ -5531,7 +5757,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="33.950000000000003">
+    <row r="12" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
         <v>59</v>
       </c>
@@ -5542,7 +5768,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="51">
+    <row r="13" spans="1:3" ht="51" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
         <v>62</v>
       </c>
@@ -5553,7 +5779,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="68.099999999999994">
+    <row r="14" spans="1:3" ht="68" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
         <v>64</v>
       </c>
@@ -5564,7 +5790,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="33.950000000000003">
+    <row r="15" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
         <v>66</v>
       </c>
@@ -5575,7 +5801,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="17.100000000000001">
+    <row r="16" spans="1:3" ht="17" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
         <v>68</v>
       </c>
@@ -5586,7 +5812,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="33.950000000000003">
+    <row r="17" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
         <v>70</v>
       </c>
@@ -5597,7 +5823,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="17.100000000000001">
+    <row r="18" spans="1:3" ht="17" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
         <v>72</v>
       </c>
@@ -5608,7 +5834,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="17.100000000000001">
+    <row r="19" spans="1:3" ht="17" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
         <v>74</v>
       </c>
@@ -5619,7 +5845,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="17.100000000000001">
+    <row r="20" spans="1:3" ht="17" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
         <v>76</v>
       </c>
@@ -5630,7 +5856,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="33.950000000000003">
+    <row r="21" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
         <v>78</v>
       </c>
@@ -5641,7 +5867,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="33.950000000000003">
+    <row r="22" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A22" t="s">
         <v>80</v>
       </c>
@@ -5652,7 +5878,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="33.950000000000003">
+    <row r="23" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A23" t="s">
         <v>82</v>
       </c>
@@ -5663,7 +5889,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="33.950000000000003">
+    <row r="24" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A24" t="s">
         <v>84</v>
       </c>
@@ -5674,7 +5900,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="51">
+    <row r="25" spans="1:3" ht="51" x14ac:dyDescent="0.15">
       <c r="A25" t="s">
         <v>86</v>
       </c>
@@ -5685,7 +5911,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="33.950000000000003">
+    <row r="26" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A26" t="s">
         <v>88</v>
       </c>
@@ -5696,7 +5922,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="135.94999999999999">
+    <row r="27" spans="1:3" ht="136" x14ac:dyDescent="0.15">
       <c r="A27" t="s">
         <v>90</v>
       </c>
@@ -5707,7 +5933,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="33.950000000000003">
+    <row r="28" spans="1:3" ht="17" x14ac:dyDescent="0.15">
       <c r="A28" t="s">
         <v>92</v>
       </c>
@@ -5718,7 +5944,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="33.950000000000003">
+    <row r="29" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A29" t="s">
         <v>94</v>
       </c>
@@ -5729,7 +5955,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="17.100000000000001">
+    <row r="30" spans="1:3" ht="17" x14ac:dyDescent="0.15">
       <c r="A30" t="s">
         <v>96</v>
       </c>
@@ -5740,7 +5966,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="17.100000000000001">
+    <row r="31" spans="1:3" ht="17" x14ac:dyDescent="0.15">
       <c r="A31" t="s">
         <v>98</v>
       </c>
@@ -5751,7 +5977,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="33.950000000000003">
+    <row r="32" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A32" t="s">
         <v>100</v>
       </c>
@@ -5762,7 +5988,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="17.100000000000001">
+    <row r="33" spans="1:3" ht="17" x14ac:dyDescent="0.15">
       <c r="A33" t="s">
         <v>102</v>
       </c>
@@ -5773,7 +5999,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="33.950000000000003">
+    <row r="34" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A34" t="s">
         <v>104</v>
       </c>
@@ -5784,7 +6010,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="51">
+    <row r="35" spans="1:3" ht="51" x14ac:dyDescent="0.15">
       <c r="A35" t="s">
         <v>106</v>
       </c>
@@ -5795,7 +6021,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="33.950000000000003">
+    <row r="36" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A36" t="s">
         <v>108</v>
       </c>
@@ -5806,7 +6032,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="33.950000000000003">
+    <row r="37" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A37" t="s">
         <v>110</v>
       </c>
@@ -5817,7 +6043,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="33.950000000000003">
+    <row r="38" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A38" t="s">
         <v>112</v>
       </c>
@@ -5828,7 +6054,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="33.950000000000003">
+    <row r="39" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A39" t="s">
         <v>114</v>
       </c>
@@ -5839,7 +6065,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="33.950000000000003">
+    <row r="40" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A40" t="s">
         <v>116</v>
       </c>
@@ -5850,7 +6076,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="33.950000000000003">
+    <row r="41" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A41" t="s">
         <v>118</v>
       </c>
@@ -5861,7 +6087,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="33.950000000000003">
+    <row r="42" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A42" t="s">
         <v>310</v>
       </c>
@@ -5872,7 +6098,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="33.950000000000003">
+    <row r="43" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A43" t="s">
         <v>313</v>
       </c>

</xml_diff>

<commit_message>
Updated user story 20
</commit_message>
<xml_diff>
--- a/Team2Report.xlsx
+++ b/Team2Report.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10914"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23231"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/srikanth/Documenta/StevensInstitute/SoftwareEngg/SSW-555/SSW-555Project/Agile_Methods_Project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ztyle\Documents\SSW 555\SSW_555_Project_Master\Agile_Methods_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01300DA8-8214-FA42-9961-B50C852E5EE0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8ED33A7E-DCCB-40C4-B948-06AA2714FCEE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25140" windowHeight="14640" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -23,10 +23,19 @@
     <sheet name="Sprint4" sheetId="6" r:id="rId8"/>
     <sheet name="Stories" sheetId="11" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -36,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="876" uniqueCount="367">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="888" uniqueCount="370">
   <si>
     <t>Initials</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -832,9 +841,6 @@
     <t>T20.02</t>
   </si>
   <si>
-    <t>Store children</t>
-  </si>
-  <si>
     <t>T20.03</t>
   </si>
   <si>
@@ -844,21 +850,12 @@
     <t>T20.05</t>
   </si>
   <si>
-    <t>Iterate through individuals to find family ID through child</t>
-  </si>
-  <si>
     <t>T20.06</t>
   </si>
   <si>
-    <t>Store children through family ID</t>
-  </si>
-  <si>
     <t>T20.07</t>
   </si>
   <si>
-    <t>Store aunt and uncles as children through previous family ID</t>
-  </si>
-  <si>
     <t>Story ID</t>
   </si>
   <si>
@@ -1157,6 +1154,27 @@
   </si>
   <si>
     <t>T16.03</t>
+  </si>
+  <si>
+    <t>Find siblings of husband</t>
+  </si>
+  <si>
+    <t>Find siblings of wife</t>
+  </si>
+  <si>
+    <t>Find children of each sibling</t>
+  </si>
+  <si>
+    <t>Check if husband ID or wife ID is in children of each sibling</t>
+  </si>
+  <si>
+    <t>T20.08</t>
+  </si>
+  <si>
+    <t>T20.09</t>
+  </si>
+  <si>
+    <t>T20.10</t>
   </si>
 </sst>
 </file>
@@ -1483,7 +1501,7 @@
             <c:numRef>
               <c:f>'Burndown README'!$B$15:$B$20</c:f>
               <c:numCache>
-                <c:formatCode>m/d/yy</c:formatCode>
+                <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>42632</c:v>
@@ -1554,7 +1572,7 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="m/d/yy" sourceLinked="1"/>
+        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1620,7 +1638,7 @@
             <c:numRef>
               <c:f>Burndown!$A$2:$A$7</c:f>
               <c:numCache>
-                <c:formatCode>m/d/yy</c:formatCode>
+                <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>42632</c:v>
@@ -1682,7 +1700,7 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="m/d/yy" sourceLinked="1"/>
+        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2540,20 +2558,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+    <sheetView zoomScale="150" workbookViewId="0">
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.5" customWidth="1"/>
-    <col min="4" max="4" width="22.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.5" customWidth="1"/>
+    <col min="1" max="1" width="7.84375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.15234375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.4609375" customWidth="1"/>
+    <col min="4" max="4" width="22.84375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.4609375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -2570,7 +2588,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -2587,7 +2605,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -2604,7 +2622,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -2621,7 +2639,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -2638,7 +2656,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>25</v>
       </c>
@@ -2655,7 +2673,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D8" s="4" t="s">
         <v>30</v>
       </c>
@@ -2664,7 +2682,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:D4">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D4">
     <sortCondition ref="C2:C4"/>
   </sortState>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -2688,16 +2706,16 @@
       <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.84375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="29" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.4609375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.4609375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>32</v>
       </c>
@@ -2714,7 +2732,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2731,7 +2749,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -2754,7 +2772,7 @@
       <c r="I3" s="25"/>
       <c r="J3" s="25"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>1</v>
       </c>
@@ -2771,7 +2789,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>1</v>
       </c>
@@ -2788,7 +2806,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>1</v>
       </c>
@@ -2805,7 +2823,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>1</v>
       </c>
@@ -2822,7 +2840,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>1</v>
       </c>
@@ -2839,7 +2857,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>1</v>
       </c>
@@ -2856,7 +2874,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>1</v>
       </c>
@@ -2873,7 +2891,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>1</v>
       </c>
@@ -2890,7 +2908,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>2</v>
       </c>
@@ -2907,7 +2925,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>2</v>
       </c>
@@ -2924,7 +2942,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>2</v>
       </c>
@@ -2941,7 +2959,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>2</v>
       </c>
@@ -2958,7 +2976,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>2</v>
       </c>
@@ -2975,7 +2993,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>2</v>
       </c>
@@ -2992,7 +3010,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>2</v>
       </c>
@@ -3009,7 +3027,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>2</v>
       </c>
@@ -3026,7 +3044,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>2</v>
       </c>
@@ -3043,7 +3061,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>2</v>
       </c>
@@ -3060,7 +3078,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>3</v>
       </c>
@@ -3077,7 +3095,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>3</v>
       </c>
@@ -3094,7 +3112,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>3</v>
       </c>
@@ -3111,7 +3129,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>3</v>
       </c>
@@ -3128,7 +3146,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>3</v>
       </c>
@@ -3145,7 +3163,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>3</v>
       </c>
@@ -3162,7 +3180,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>3</v>
       </c>
@@ -3179,7 +3197,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>3</v>
       </c>
@@ -3196,7 +3214,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>3</v>
       </c>
@@ -3213,7 +3231,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>3</v>
       </c>
@@ -3230,7 +3248,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>4</v>
       </c>
@@ -3247,7 +3265,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>4</v>
       </c>
@@ -3264,7 +3282,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>4</v>
       </c>
@@ -3281,7 +3299,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>4</v>
       </c>
@@ -3298,7 +3316,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>4</v>
       </c>
@@ -3315,7 +3333,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>4</v>
       </c>
@@ -3332,7 +3350,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>4</v>
       </c>
@@ -3349,7 +3367,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>4</v>
       </c>
@@ -3366,7 +3384,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>4</v>
       </c>
@@ -3383,7 +3401,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>4</v>
       </c>
@@ -3418,47 +3436,47 @@
       <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="7"/>
-    <col min="2" max="2" width="10.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.33203125" customWidth="1"/>
-    <col min="5" max="5" width="6.83203125" customWidth="1"/>
-    <col min="6" max="6" width="12.5" style="9" customWidth="1"/>
+    <col min="1" max="1" width="10.84375" style="7"/>
+    <col min="2" max="2" width="10.15234375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.84375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.3046875" customWidth="1"/>
+    <col min="5" max="5" width="6.84375" customWidth="1"/>
+    <col min="6" max="6" width="12.4609375" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
         <v>126</v>
       </c>
@@ -3481,7 +3499,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>133</v>
       </c>
@@ -3497,7 +3515,7 @@
       <c r="F15" s="14"/>
       <c r="G15" s="9"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>134</v>
       </c>
@@ -3521,7 +3539,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
         <v>135</v>
       </c>
@@ -3546,7 +3564,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="7" t="s">
         <v>136</v>
       </c>
@@ -3571,7 +3589,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="7" t="s">
         <v>137</v>
       </c>
@@ -3611,17 +3629,17 @@
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="2"/>
-    <col min="2" max="2" width="18.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.1640625" customWidth="1"/>
-    <col min="5" max="5" width="6.83203125" customWidth="1"/>
-    <col min="6" max="6" width="12.5" style="9" customWidth="1"/>
+    <col min="1" max="1" width="10.84375" style="2"/>
+    <col min="2" max="2" width="18.4609375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.4609375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.15234375" customWidth="1"/>
+    <col min="5" max="5" width="6.84375" customWidth="1"/>
+    <col min="6" max="6" width="12.4609375" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>127</v>
       </c>
@@ -3641,7 +3659,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="13">
         <v>42632</v>
       </c>
@@ -3661,7 +3679,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="13">
         <v>42647</v>
       </c>
@@ -3686,17 +3704,17 @@
         <v>34.695652173913047</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="13">
         <v>42661</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="13">
         <v>42675</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="13">
         <v>42689</v>
       </c>
@@ -3717,19 +3735,19 @@
       <selection activeCell="A50" sqref="A50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="33" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.33203125" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.4609375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.4609375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.3046875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.69140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.4609375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.3046875" style="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>33</v>
       </c>
@@ -3758,7 +3776,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>37</v>
       </c>
@@ -3787,7 +3805,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="17" t="s">
         <v>144</v>
       </c>
@@ -3804,7 +3822,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="17" t="s">
         <v>147</v>
       </c>
@@ -3821,7 +3839,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="17" t="s">
         <v>149</v>
       </c>
@@ -3838,7 +3856,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>40</v>
       </c>
@@ -3867,7 +3885,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="17" t="s">
         <v>151</v>
       </c>
@@ -3884,7 +3902,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="17" t="s">
         <v>153</v>
       </c>
@@ -3901,7 +3919,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="17" t="s">
         <v>155</v>
       </c>
@@ -3918,7 +3936,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="17" t="s">
         <v>157</v>
       </c>
@@ -3935,7 +3953,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
         <v>43</v>
       </c>
@@ -3964,7 +3982,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="17" t="s">
         <v>159</v>
       </c>
@@ -3981,7 +3999,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="17" t="s">
         <v>161</v>
       </c>
@@ -3998,7 +4016,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="17" t="s">
         <v>162</v>
       </c>
@@ -4015,7 +4033,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="17" t="s">
         <v>164</v>
       </c>
@@ -4032,7 +4050,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
         <v>45</v>
       </c>
@@ -4061,7 +4079,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="17" t="s">
         <v>166</v>
       </c>
@@ -4078,7 +4096,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="17" t="s">
         <v>167</v>
       </c>
@@ -4095,7 +4113,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" s="17" t="s">
         <v>169</v>
       </c>
@@ -4112,7 +4130,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="17" t="s">
         <v>170</v>
       </c>
@@ -4129,7 +4147,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" s="17" t="s">
         <v>172</v>
       </c>
@@ -4146,7 +4164,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" s="4" t="s">
         <v>47</v>
       </c>
@@ -4175,7 +4193,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" s="17" t="s">
         <v>174</v>
       </c>
@@ -4192,7 +4210,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" s="17" t="s">
         <v>175</v>
       </c>
@@ -4209,7 +4227,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" s="17" t="s">
         <v>176</v>
       </c>
@@ -4226,7 +4244,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" s="17" t="s">
         <v>177</v>
       </c>
@@ -4243,7 +4261,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" s="17" t="s">
         <v>178</v>
       </c>
@@ -4260,7 +4278,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" s="4" t="s">
         <v>49</v>
       </c>
@@ -4289,7 +4307,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" s="17" t="s">
         <v>180</v>
       </c>
@@ -4306,7 +4324,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" s="17" t="s">
         <v>181</v>
       </c>
@@ -4323,7 +4341,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" s="17" t="s">
         <v>182</v>
       </c>
@@ -4340,7 +4358,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" s="17" t="s">
         <v>183</v>
       </c>
@@ -4357,7 +4375,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33" s="17" t="s">
         <v>184</v>
       </c>
@@ -4374,7 +4392,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34" s="4" t="s">
         <v>51</v>
       </c>
@@ -4403,7 +4421,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35" s="17" t="s">
         <v>186</v>
       </c>
@@ -4420,7 +4438,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A36" s="17" t="s">
         <v>187</v>
       </c>
@@ -4437,7 +4455,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A37" s="17" t="s">
         <v>189</v>
       </c>
@@ -4454,7 +4472,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A38" s="17" t="s">
         <v>191</v>
       </c>
@@ -4471,7 +4489,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A39" s="17" t="s">
         <v>192</v>
       </c>
@@ -4488,7 +4506,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A40" s="17" t="s">
         <v>194</v>
       </c>
@@ -4505,7 +4523,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A41" s="4" t="s">
         <v>53</v>
       </c>
@@ -4534,7 +4552,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A42" s="17" t="s">
         <v>196</v>
       </c>
@@ -4551,7 +4569,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A43" s="17" t="s">
         <v>197</v>
       </c>
@@ -4568,7 +4586,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A44" s="17" t="s">
         <v>198</v>
       </c>
@@ -4585,7 +4603,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A45" s="4" t="s">
         <v>55</v>
       </c>
@@ -4614,7 +4632,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A46" s="17" t="s">
         <v>199</v>
       </c>
@@ -4631,7 +4649,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A47" s="17" t="s">
         <v>201</v>
       </c>
@@ -4648,7 +4666,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A48" s="17" t="s">
         <v>203</v>
       </c>
@@ -4665,7 +4683,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A49" s="17" t="s">
         <v>204</v>
       </c>
@@ -4682,7 +4700,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A50" s="4" t="s">
         <v>57</v>
       </c>
@@ -4711,7 +4729,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="51" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A51" s="17" t="s">
         <v>206</v>
       </c>
@@ -4728,7 +4746,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="52" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A52" s="17" t="s">
         <v>208</v>
       </c>
@@ -4745,7 +4763,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="53" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A53" s="17" t="s">
         <v>209</v>
       </c>
@@ -4762,7 +4780,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="54" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A54" s="17" t="s">
         <v>210</v>
       </c>
@@ -4779,7 +4797,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="55" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A55" s="17" t="s">
         <v>212</v>
       </c>
@@ -4796,7 +4814,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A56" s="4" t="s">
         <v>214</v>
       </c>
@@ -4821,21 +4839,21 @@
       </c>
       <c r="I56" s="21"/>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A57" s="17"/>
       <c r="I57" s="7"/>
     </row>
-    <row r="58" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B58" s="5" t="s">
         <v>215</v>
       </c>
       <c r="I58" s="7"/>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B59" s="5"/>
       <c r="I59" s="7"/>
     </row>
-    <row r="60" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B60" s="5" t="s">
         <v>216</v>
       </c>
@@ -4847,7 +4865,7 @@
       <c r="F60" s="26"/>
       <c r="I60" s="7"/>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C61" s="26" t="s">
         <v>218</v>
       </c>
@@ -4856,7 +4874,7 @@
       <c r="F61" s="26"/>
       <c r="I61" s="7"/>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C62" s="26" t="s">
         <v>219</v>
       </c>
@@ -4865,13 +4883,13 @@
       <c r="F62" s="26"/>
       <c r="I62" s="7"/>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C63" s="28"/>
       <c r="D63" s="28"/>
       <c r="E63" s="28"/>
       <c r="F63" s="28"/>
     </row>
-    <row r="64" spans="1:9" ht="27" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="64" spans="1:9" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B64" s="5" t="s">
         <v>220</v>
       </c>
@@ -4883,7 +4901,7 @@
       <c r="F64" s="27"/>
       <c r="I64" s="7"/>
     </row>
-    <row r="65" spans="3:6" ht="26" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="65" spans="3:6" ht="26" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C65" s="27" t="s">
         <v>222</v>
       </c>
@@ -4908,18 +4926,18 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:I62"/>
+  <dimension ref="A1:I65"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B55" sqref="B55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="54.6640625" style="23" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="54.69140625" style="23" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>33</v>
       </c>
@@ -4948,7 +4966,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>59</v>
       </c>
@@ -4968,27 +4986,27 @@
         <v>90</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="17" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="B3" s="24" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="C3" s="17"/>
       <c r="D3" s="17"/>
     </row>
-    <row r="4" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="17" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B4" s="24" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
       <c r="C4" s="17"/>
       <c r="D4" s="17"/>
     </row>
-    <row r="5" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>62</v>
       </c>
@@ -5008,47 +5026,47 @@
         <v>120</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="17" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="B6" s="24" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="C6" s="17"/>
       <c r="D6" s="17"/>
     </row>
-    <row r="7" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="17" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
       <c r="B7" s="24" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="C7" s="17"/>
       <c r="D7" s="17"/>
     </row>
-    <row r="8" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="17" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="B8" s="24" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="C8" s="17"/>
       <c r="D8" s="17"/>
     </row>
-    <row r="9" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="17" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="B9" s="24" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="C9" s="17"/>
       <c r="D9" s="17"/>
     </row>
-    <row r="10" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>64</v>
       </c>
@@ -5068,37 +5086,37 @@
         <v>90</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="17" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
       <c r="B11" s="24" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="C11" s="17"/>
       <c r="D11" s="17"/>
     </row>
-    <row r="12" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="17" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
       <c r="B12" s="24" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
       <c r="C12" s="17"/>
       <c r="D12" s="17"/>
     </row>
-    <row r="13" spans="1:9" ht="28" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="17" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="B13" s="24" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="C13" s="17"/>
       <c r="D13" s="17"/>
     </row>
-    <row r="14" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
         <v>66</v>
       </c>
@@ -5118,37 +5136,37 @@
         <v>120</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="17" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="B15" s="24" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="C15" s="17"/>
       <c r="D15" s="17"/>
     </row>
-    <row r="16" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="17" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="B16" s="24" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
       <c r="C16" s="17"/>
       <c r="D16" s="17"/>
     </row>
-    <row r="17" spans="1:6" ht="14" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="17" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
       <c r="B17" s="24" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="C17" s="17"/>
       <c r="D17" s="17"/>
     </row>
-    <row r="18" spans="1:6" ht="14" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
         <v>68</v>
       </c>
@@ -5168,27 +5186,27 @@
         <v>90</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="14" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="17" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="B19" s="24" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="C19" s="17"/>
       <c r="D19" s="17"/>
     </row>
-    <row r="20" spans="1:6" ht="14" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="17" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="B20" s="24" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="C20" s="17"/>
       <c r="D20" s="17"/>
     </row>
-    <row r="21" spans="1:6" ht="14" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
         <v>70</v>
       </c>
@@ -5208,37 +5226,37 @@
         <v>90</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="14" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="17" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="B22" s="24" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="C22" s="17"/>
       <c r="D22" s="17"/>
     </row>
-    <row r="23" spans="1:6" ht="14" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="17" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
       <c r="B23" s="24" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="C23" s="17"/>
       <c r="D23" s="17"/>
     </row>
-    <row r="24" spans="1:6" ht="14" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="17" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="B24" s="24" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="C24" s="17"/>
       <c r="D24" s="17"/>
     </row>
-    <row r="25" spans="1:6" ht="14" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="4" t="s">
         <v>72</v>
       </c>
@@ -5258,9 +5276,9 @@
         <v>90</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="14" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="B26" s="23" t="s">
         <v>224</v>
@@ -5272,12 +5290,12 @@
         <v>61</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="14" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="B27" s="23" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="C27" s="17" t="s">
         <v>20</v>
@@ -5286,12 +5304,12 @@
         <v>61</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="28" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:6" ht="27" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="B28" s="23" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="C28" s="17" t="s">
         <v>20</v>
@@ -5300,12 +5318,12 @@
         <v>61</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="14" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="B29" s="23" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="C29" s="17" t="s">
         <v>20</v>
@@ -5314,12 +5332,12 @@
         <v>61</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="28" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:6" ht="27" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="B30" s="23" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="C30" s="17" t="s">
         <v>20</v>
@@ -5328,12 +5346,12 @@
         <v>61</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="14" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="B31" s="23" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="C31" s="17" t="s">
         <v>20</v>
@@ -5342,7 +5360,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="14" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" s="4" t="s">
         <v>74</v>
       </c>
@@ -5362,9 +5380,9 @@
         <v>90</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="14" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="B33" s="23" t="s">
         <v>224</v>
@@ -5376,12 +5394,12 @@
         <v>61</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="14" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="B34" s="23" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="C34" s="17" t="s">
         <v>20</v>
@@ -5390,12 +5408,12 @@
         <v>61</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="28" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="B35" s="23" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="C35" s="17" t="s">
         <v>20</v>
@@ -5404,12 +5422,12 @@
         <v>61</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="28" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:6" ht="27" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="B36" s="23" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="C36" s="17" t="s">
         <v>20</v>
@@ -5418,12 +5436,12 @@
         <v>61</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="14" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="B37" s="24" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="C37" s="17" t="s">
         <v>20</v>
@@ -5432,7 +5450,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="14" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" s="4" t="s">
         <v>76</v>
       </c>
@@ -5446,7 +5464,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="14" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>223</v>
       </c>
@@ -5466,7 +5484,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="14" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>225</v>
       </c>
@@ -5480,7 +5498,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="41" spans="1:6" ht="14" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>227</v>
       </c>
@@ -5494,7 +5512,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="42" spans="1:6" ht="14" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>229</v>
       </c>
@@ -5508,7 +5526,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="43" spans="1:6" ht="14" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>231</v>
       </c>
@@ -5522,7 +5540,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="44" spans="1:6" ht="14" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>233</v>
       </c>
@@ -5536,7 +5554,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="45" spans="1:6" ht="14" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>235</v>
       </c>
@@ -5550,7 +5568,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="46" spans="1:6" ht="14" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>237</v>
       </c>
@@ -5564,7 +5582,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="47" spans="1:6" ht="14" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>239</v>
       </c>
@@ -5578,7 +5596,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="48" spans="1:6" ht="14" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>241</v>
       </c>
@@ -5592,7 +5610,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="49" spans="1:6" ht="14" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>243</v>
       </c>
@@ -5606,7 +5624,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="50" spans="1:6" ht="14" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>245</v>
       </c>
@@ -5620,7 +5638,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="51" spans="1:6" ht="14" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>247</v>
       </c>
@@ -5634,7 +5652,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="52" spans="1:6" ht="14" x14ac:dyDescent="0.15">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>249</v>
       </c>
@@ -5648,7 +5666,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="53" spans="1:6" ht="28" x14ac:dyDescent="0.15">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>251</v>
       </c>
@@ -5662,7 +5680,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="54" spans="1:6" ht="14" x14ac:dyDescent="0.15">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>253</v>
       </c>
@@ -5676,7 +5694,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="55" spans="1:6" ht="14" x14ac:dyDescent="0.15">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A55" s="4" t="s">
         <v>78</v>
       </c>
@@ -5696,7 +5714,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="56" spans="1:6" ht="14" x14ac:dyDescent="0.15">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>255</v>
       </c>
@@ -5710,12 +5728,12 @@
         <v>61</v>
       </c>
     </row>
-    <row r="57" spans="1:6" ht="14" x14ac:dyDescent="0.15">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>257</v>
       </c>
       <c r="B57" s="23" t="s">
-        <v>258</v>
+        <v>207</v>
       </c>
       <c r="C57" s="17" t="s">
         <v>25</v>
@@ -5724,9 +5742,9 @@
         <v>61</v>
       </c>
     </row>
-    <row r="58" spans="1:6" ht="14" x14ac:dyDescent="0.15">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B58" s="23" t="s">
         <v>228</v>
@@ -5738,9 +5756,9 @@
         <v>61</v>
       </c>
     </row>
-    <row r="59" spans="1:6" ht="14" x14ac:dyDescent="0.15">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B59" s="23" t="s">
         <v>230</v>
@@ -5752,12 +5770,12 @@
         <v>61</v>
       </c>
     </row>
-    <row r="60" spans="1:6" ht="14" x14ac:dyDescent="0.15">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B60" s="23" t="s">
-        <v>262</v>
+        <v>232</v>
       </c>
       <c r="C60" s="17" t="s">
         <v>25</v>
@@ -5766,12 +5784,12 @@
         <v>61</v>
       </c>
     </row>
-    <row r="61" spans="1:6" ht="14" x14ac:dyDescent="0.15">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="B61" s="23" t="s">
-        <v>264</v>
+        <v>234</v>
       </c>
       <c r="C61" s="17" t="s">
         <v>25</v>
@@ -5780,17 +5798,59 @@
         <v>61</v>
       </c>
     </row>
-    <row r="62" spans="1:6" ht="14" x14ac:dyDescent="0.15">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="B62" s="23" t="s">
-        <v>266</v>
+        <v>363</v>
       </c>
       <c r="C62" s="17" t="s">
         <v>25</v>
       </c>
       <c r="D62" s="17" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
+        <v>367</v>
+      </c>
+      <c r="B63" s="23" t="s">
+        <v>364</v>
+      </c>
+      <c r="C63" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="D63" s="17" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
+        <v>368</v>
+      </c>
+      <c r="B64" s="23" t="s">
+        <v>365</v>
+      </c>
+      <c r="C64" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="D64" s="17" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
+        <v>369</v>
+      </c>
+      <c r="B65" s="23" t="s">
+        <v>366</v>
+      </c>
+      <c r="C65" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="D65" s="17" t="s">
         <v>61</v>
       </c>
     </row>
@@ -5809,9 +5869,9 @@
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:9" ht="28" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>33</v>
       </c>
@@ -5854,9 +5914,9 @@
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:9" ht="28" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>33</v>
       </c>
@@ -5899,24 +5959,24 @@
       <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="28.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="49.5" style="1" customWidth="1"/>
+    <col min="2" max="2" width="28.15234375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="49.4609375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="4" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>37</v>
       </c>
@@ -5924,10 +5984,10 @@
         <v>38</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>40</v>
       </c>
@@ -5935,10 +5995,10 @@
         <v>41</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>43</v>
       </c>
@@ -5946,10 +6006,10 @@
         <v>44</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>45</v>
       </c>
@@ -5957,10 +6017,10 @@
         <v>46</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>47</v>
       </c>
@@ -5968,10 +6028,10 @@
         <v>48</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>49</v>
       </c>
@@ -5979,10 +6039,10 @@
         <v>50</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="51" x14ac:dyDescent="0.15">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="45" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>51</v>
       </c>
@@ -5990,10 +6050,10 @@
         <v>52</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>53</v>
       </c>
@@ -6001,10 +6061,10 @@
         <v>54</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>55</v>
       </c>
@@ -6012,10 +6072,10 @@
         <v>56</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="51" x14ac:dyDescent="0.15">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>57</v>
       </c>
@@ -6023,10 +6083,10 @@
         <v>58</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>59</v>
       </c>
@@ -6034,10 +6094,10 @@
         <v>60</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="51" x14ac:dyDescent="0.15">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="45" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>62</v>
       </c>
@@ -6045,10 +6105,10 @@
         <v>63</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="68" x14ac:dyDescent="0.15">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="45" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>64</v>
       </c>
@@ -6056,10 +6116,10 @@
         <v>65</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>66</v>
       </c>
@@ -6067,10 +6127,10 @@
         <v>67</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>68</v>
       </c>
@@ -6078,10 +6138,10 @@
         <v>69</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>70</v>
       </c>
@@ -6089,10 +6149,10 @@
         <v>71</v>
       </c>
       <c r="C17" s="12" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>72</v>
       </c>
@@ -6100,10 +6160,10 @@
         <v>73</v>
       </c>
       <c r="C18" s="12" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>74</v>
       </c>
@@ -6111,10 +6171,10 @@
         <v>75</v>
       </c>
       <c r="C19" s="12" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>76</v>
       </c>
@@ -6122,10 +6182,10 @@
         <v>77</v>
       </c>
       <c r="C20" s="12" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>78</v>
       </c>
@@ -6133,10 +6193,10 @@
         <v>79</v>
       </c>
       <c r="C21" s="12" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>80</v>
       </c>
@@ -6144,10 +6204,10 @@
         <v>81</v>
       </c>
       <c r="C22" s="12" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>82</v>
       </c>
@@ -6155,10 +6215,10 @@
         <v>83</v>
       </c>
       <c r="C23" s="12" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>84</v>
       </c>
@@ -6166,10 +6226,10 @@
         <v>85</v>
       </c>
       <c r="C24" s="12" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" ht="51" x14ac:dyDescent="0.15">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="45" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>86</v>
       </c>
@@ -6177,10 +6237,10 @@
         <v>87</v>
       </c>
       <c r="C25" s="12" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>88</v>
       </c>
@@ -6188,10 +6248,10 @@
         <v>89</v>
       </c>
       <c r="C26" s="12" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" ht="136" x14ac:dyDescent="0.15">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="105" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>90</v>
       </c>
@@ -6199,10 +6259,10 @@
         <v>91</v>
       </c>
       <c r="C27" s="12" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>92</v>
       </c>
@@ -6210,10 +6270,10 @@
         <v>93</v>
       </c>
       <c r="C28" s="12" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>94</v>
       </c>
@@ -6221,10 +6281,10 @@
         <v>95</v>
       </c>
       <c r="C29" s="12" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>96</v>
       </c>
@@ -6232,10 +6292,10 @@
         <v>97</v>
       </c>
       <c r="C30" s="12" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>98</v>
       </c>
@@ -6243,10 +6303,10 @@
         <v>99</v>
       </c>
       <c r="C31" s="12" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>100</v>
       </c>
@@ -6254,10 +6314,10 @@
         <v>101</v>
       </c>
       <c r="C32" s="12" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>102</v>
       </c>
@@ -6265,10 +6325,10 @@
         <v>103</v>
       </c>
       <c r="C33" s="12" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>104</v>
       </c>
@@ -6276,10 +6336,10 @@
         <v>105</v>
       </c>
       <c r="C34" s="12" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" ht="51" x14ac:dyDescent="0.15">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>106</v>
       </c>
@@ -6287,10 +6347,10 @@
         <v>107</v>
       </c>
       <c r="C35" s="12" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>108</v>
       </c>
@@ -6298,10 +6358,10 @@
         <v>109</v>
       </c>
       <c r="C36" s="12" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>110</v>
       </c>
@@ -6309,10 +6369,10 @@
         <v>111</v>
       </c>
       <c r="C37" s="12" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>112</v>
       </c>
@@ -6320,10 +6380,10 @@
         <v>113</v>
       </c>
       <c r="C38" s="12" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>114</v>
       </c>
@@ -6331,10 +6391,10 @@
         <v>115</v>
       </c>
       <c r="C39" s="12" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>116</v>
       </c>
@@ -6342,10 +6402,10 @@
         <v>117</v>
       </c>
       <c r="C40" s="12" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>118</v>
       </c>
@@ -6353,29 +6413,29 @@
         <v>119</v>
       </c>
       <c r="C41" s="12" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>306</v>
+      </c>
+      <c r="B42" t="s">
+        <v>307</v>
+      </c>
+      <c r="C42" s="12" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
         <v>309</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" ht="34" x14ac:dyDescent="0.15">
-      <c r="A42" t="s">
+      <c r="B43" t="s">
         <v>310</v>
       </c>
-      <c r="B42" t="s">
+      <c r="C43" s="12" t="s">
         <v>311</v>
-      </c>
-      <c r="C42" s="12" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" ht="34" x14ac:dyDescent="0.15">
-      <c r="A43" t="s">
-        <v>313</v>
-      </c>
-      <c r="B43" t="s">
-        <v>314</v>
-      </c>
-      <c r="C43" s="12" t="s">
-        <v>315</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
test cases, updated spreadsheet, User Story 20 complete
</commit_message>
<xml_diff>
--- a/Team2Report.xlsx
+++ b/Team2Report.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ztyle\Documents\SSW 555\SSW_555_Project_Master\Agile_Methods_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8ED33A7E-DCCB-40C4-B948-06AA2714FCEE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40BE8232-3639-4746-A580-988E9D108DBA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4800" yWindow="1350" windowWidth="14400" windowHeight="7360" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="888" uniqueCount="370">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="900" uniqueCount="370">
   <si>
     <t>Initials</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -1647,10 +1647,10 @@
                   <c:v>42647</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>42661</c:v>
+                  <c:v>42668</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>42675</c:v>
+                  <c:v>42682</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>42689</c:v>
@@ -1669,6 +1669,9 @@
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>29</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3625,8 +3628,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
@@ -3706,12 +3709,32 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="13">
-        <v>42661</v>
+        <v>42668</v>
+      </c>
+      <c r="B4">
+        <f>B3-COUNTIF(Sprint2!$I$2:$I$65, "Completed")</f>
+        <v>29</v>
+      </c>
+      <c r="C4">
+        <f>B3-B4</f>
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <f>Sprint2!G66</f>
+        <v>55</v>
+      </c>
+      <c r="E4">
+        <f>Sprint2!H66</f>
+        <v>60</v>
+      </c>
+      <c r="F4" s="9">
+        <f>(D4-D3)/E4*60</f>
+        <v>-344</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="13">
-        <v>42675</v>
+        <v>42682</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
@@ -3731,8 +3754,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:I65"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A50" sqref="A50"/>
+    <sheetView topLeftCell="A46" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="F51" sqref="F51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
@@ -4926,10 +4949,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:I65"/>
+  <dimension ref="A1:I66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B55" sqref="B55"/>
+    <sheetView topLeftCell="B48" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I63" sqref="I63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
@@ -5610,7 +5633,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>243</v>
       </c>
@@ -5624,7 +5647,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>245</v>
       </c>
@@ -5638,7 +5661,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>247</v>
       </c>
@@ -5652,7 +5675,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>249</v>
       </c>
@@ -5666,7 +5689,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>251</v>
       </c>
@@ -5680,7 +5703,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>253</v>
       </c>
@@ -5694,7 +5717,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A55" s="4" t="s">
         <v>78</v>
       </c>
@@ -5713,8 +5736,17 @@
       <c r="F55">
         <v>80</v>
       </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G55">
+        <v>55</v>
+      </c>
+      <c r="H55">
+        <v>60</v>
+      </c>
+      <c r="I55" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>255</v>
       </c>
@@ -5727,8 +5759,11 @@
       <c r="D56" s="17" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I56" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>257</v>
       </c>
@@ -5741,8 +5776,11 @@
       <c r="D57" s="17" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I57" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>258</v>
       </c>
@@ -5755,8 +5793,11 @@
       <c r="D58" s="17" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I58" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>259</v>
       </c>
@@ -5769,8 +5810,11 @@
       <c r="D59" s="17" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I59" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>260</v>
       </c>
@@ -5783,8 +5827,11 @@
       <c r="D60" s="17" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I60" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>261</v>
       </c>
@@ -5797,8 +5844,11 @@
       <c r="D61" s="17" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I61" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>262</v>
       </c>
@@ -5811,8 +5861,11 @@
       <c r="D62" s="17" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I62" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>367</v>
       </c>
@@ -5825,8 +5878,11 @@
       <c r="D63" s="17" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I63" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>368</v>
       </c>
@@ -5839,8 +5895,11 @@
       <c r="D64" s="17" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="I64" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>369</v>
       </c>
@@ -5852,6 +5911,33 @@
       </c>
       <c r="D65" s="17" t="s">
         <v>61</v>
+      </c>
+      <c r="I65" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A66" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="B66" s="19"/>
+      <c r="C66" s="17"/>
+      <c r="D66" s="17"/>
+      <c r="E66">
+        <f t="shared" ref="E66:F66" si="0">SUM(E12:E65)</f>
+        <v>430</v>
+      </c>
+      <c r="F66">
+        <f t="shared" si="0"/>
+        <v>650</v>
+      </c>
+      <c r="G66">
+        <f>SUM(G12:G65)</f>
+        <v>55</v>
+      </c>
+      <c r="H66">
+        <f>SUM(H12:H65)</f>
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -6185,7 +6271,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>78</v>
       </c>

</xml_diff>

<commit_message>
completion of coding and testing of user story 19
</commit_message>
<xml_diff>
--- a/Team2Report.xlsx
+++ b/Team2Report.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ztyle\Documents\SSW 555\SSW_555_Project_Master\Agile_Methods_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40BE8232-3639-4746-A580-988E9D108DBA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94E55882-C48D-49D2-A168-C76EEEFD9492}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4800" yWindow="1350" windowWidth="14400" windowHeight="7360" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="900" uniqueCount="370">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="916" uniqueCount="370">
   <si>
     <t>Initials</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -1671,7 +1671,7 @@
                   <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>29</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3628,8 +3628,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="150" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
@@ -3713,23 +3713,23 @@
       </c>
       <c r="B4">
         <f>B3-COUNTIF(Sprint2!$I$2:$I$65, "Completed")</f>
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C4">
         <f>B3-B4</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D4">
         <f>Sprint2!G66</f>
-        <v>55</v>
+        <v>104</v>
       </c>
       <c r="E4">
         <f>Sprint2!H66</f>
-        <v>60</v>
+        <v>120</v>
       </c>
       <c r="F4" s="9">
         <f>(D4-D3)/E4*60</f>
-        <v>-344</v>
+        <v>-147.5</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -4951,8 +4951,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:I66"/>
   <sheetViews>
-    <sheetView topLeftCell="B48" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I63" sqref="I63"/>
+    <sheetView topLeftCell="A36" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G52" sqref="G52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
@@ -5403,7 +5403,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>322</v>
       </c>
@@ -5417,7 +5417,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>323</v>
       </c>
@@ -5431,7 +5431,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>324</v>
       </c>
@@ -5445,7 +5445,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="27" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:9" ht="27" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>326</v>
       </c>
@@ -5459,7 +5459,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>328</v>
       </c>
@@ -5473,7 +5473,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A38" s="4" t="s">
         <v>76</v>
       </c>
@@ -5487,7 +5487,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>223</v>
       </c>
@@ -5506,8 +5506,17 @@
       <c r="F39">
         <v>90</v>
       </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G39">
+        <v>49</v>
+      </c>
+      <c r="H39">
+        <v>60</v>
+      </c>
+      <c r="I39" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>225</v>
       </c>
@@ -5520,8 +5529,11 @@
       <c r="D40" s="17" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I40" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>227</v>
       </c>
@@ -5534,8 +5546,11 @@
       <c r="D41" s="17" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I41" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>229</v>
       </c>
@@ -5548,8 +5563,11 @@
       <c r="D42" s="17" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I42" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>231</v>
       </c>
@@ -5562,8 +5580,11 @@
       <c r="D43" s="17" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I43" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>233</v>
       </c>
@@ -5576,8 +5597,11 @@
       <c r="D44" s="17" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I44" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>235</v>
       </c>
@@ -5590,8 +5614,11 @@
       <c r="D45" s="17" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I45" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>237</v>
       </c>
@@ -5604,8 +5631,11 @@
       <c r="D46" s="17" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I46" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>239</v>
       </c>
@@ -5618,8 +5648,11 @@
       <c r="D47" s="17" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I47" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>241</v>
       </c>
@@ -5631,6 +5664,9 @@
       </c>
       <c r="D48" s="17" t="s">
         <v>61</v>
+      </c>
+      <c r="I48" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.3">
@@ -5646,6 +5682,9 @@
       <c r="D49" s="17" t="s">
         <v>61</v>
       </c>
+      <c r="I49" t="s">
+        <v>146</v>
+      </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
@@ -5660,6 +5699,9 @@
       <c r="D50" s="17" t="s">
         <v>61</v>
       </c>
+      <c r="I50" t="s">
+        <v>146</v>
+      </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
@@ -5674,6 +5716,9 @@
       <c r="D51" s="17" t="s">
         <v>61</v>
       </c>
+      <c r="I51" t="s">
+        <v>146</v>
+      </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
@@ -5688,6 +5733,9 @@
       <c r="D52" s="17" t="s">
         <v>61</v>
       </c>
+      <c r="I52" t="s">
+        <v>146</v>
+      </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
@@ -5702,6 +5750,9 @@
       <c r="D53" s="17" t="s">
         <v>61</v>
       </c>
+      <c r="I53" t="s">
+        <v>146</v>
+      </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
@@ -5715,6 +5766,9 @@
       </c>
       <c r="D54" s="17" t="s">
         <v>61</v>
+      </c>
+      <c r="I54" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.3">
@@ -5933,11 +5987,11 @@
       </c>
       <c r="G66">
         <f>SUM(G12:G65)</f>
-        <v>55</v>
+        <v>104</v>
       </c>
       <c r="H66">
         <f>SUM(H12:H65)</f>
-        <v>60</v>
+        <v>120</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated Sprint 2 Sheet
</commit_message>
<xml_diff>
--- a/Team2Report.xlsx
+++ b/Team2Report.xlsx
@@ -5,12 +5,12 @@
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ztyle\Documents\SSW 555\SSW_555_Project_Master\Agile_Methods_Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RedRo\OneDrive\Documents\Academic Texts\COOOOOOODE\Python Workspace\anaconda\Agile_Methods_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94E55882-C48D-49D2-A168-C76EEEFD9492}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C9E4643-E896-4547-B388-0D46639A59EE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" firstSheet="2" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="916" uniqueCount="370">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="924" uniqueCount="371">
   <si>
     <t>Initials</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -1175,6 +1175,9 @@
   </si>
   <si>
     <t>T20.10</t>
+  </si>
+  <si>
+    <t>Task Finished</t>
   </si>
 </sst>
 </file>
@@ -1671,7 +1674,7 @@
                   <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>28</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2565,16 +2568,16 @@
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.84375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.15234375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.4609375" customWidth="1"/>
-    <col min="4" max="4" width="22.84375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.4609375" customWidth="1"/>
+    <col min="1" max="1" width="7.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.453125" customWidth="1"/>
+    <col min="4" max="4" width="22.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -2591,7 +2594,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -2608,7 +2611,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -2625,7 +2628,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -2642,7 +2645,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -2659,7 +2662,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>25</v>
       </c>
@@ -2676,7 +2679,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D8" s="4" t="s">
         <v>30</v>
       </c>
@@ -2709,16 +2712,16 @@
       <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="6.84375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.81640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="29" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.4609375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.4609375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>32</v>
       </c>
@@ -2735,7 +2738,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2752,7 +2755,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -2775,7 +2778,7 @@
       <c r="I3" s="25"/>
       <c r="J3" s="25"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1</v>
       </c>
@@ -2792,7 +2795,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1</v>
       </c>
@@ -2809,7 +2812,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>1</v>
       </c>
@@ -2826,7 +2829,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>1</v>
       </c>
@@ -2843,7 +2846,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>1</v>
       </c>
@@ -2860,7 +2863,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>1</v>
       </c>
@@ -2877,7 +2880,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>1</v>
       </c>
@@ -2894,7 +2897,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>1</v>
       </c>
@@ -2911,7 +2914,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>2</v>
       </c>
@@ -2928,7 +2931,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>2</v>
       </c>
@@ -2945,7 +2948,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>2</v>
       </c>
@@ -2962,7 +2965,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>2</v>
       </c>
@@ -2979,7 +2982,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>2</v>
       </c>
@@ -2996,7 +2999,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>2</v>
       </c>
@@ -3013,7 +3016,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>2</v>
       </c>
@@ -3030,7 +3033,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>2</v>
       </c>
@@ -3047,7 +3050,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>2</v>
       </c>
@@ -3064,7 +3067,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>2</v>
       </c>
@@ -3081,7 +3084,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>3</v>
       </c>
@@ -3098,7 +3101,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>3</v>
       </c>
@@ -3115,7 +3118,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>3</v>
       </c>
@@ -3132,7 +3135,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>3</v>
       </c>
@@ -3149,7 +3152,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>3</v>
       </c>
@@ -3166,7 +3169,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>3</v>
       </c>
@@ -3183,7 +3186,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>3</v>
       </c>
@@ -3200,7 +3203,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>3</v>
       </c>
@@ -3217,7 +3220,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>3</v>
       </c>
@@ -3234,7 +3237,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>3</v>
       </c>
@@ -3251,7 +3254,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>4</v>
       </c>
@@ -3268,7 +3271,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>4</v>
       </c>
@@ -3285,7 +3288,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>4</v>
       </c>
@@ -3302,7 +3305,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>4</v>
       </c>
@@ -3319,7 +3322,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>4</v>
       </c>
@@ -3336,7 +3339,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>4</v>
       </c>
@@ -3353,7 +3356,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>4</v>
       </c>
@@ -3370,7 +3373,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>4</v>
       </c>
@@ -3387,7 +3390,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>4</v>
       </c>
@@ -3404,7 +3407,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>4</v>
       </c>
@@ -3439,47 +3442,47 @@
       <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.84375" style="7"/>
-    <col min="2" max="2" width="10.15234375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.84375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.3046875" customWidth="1"/>
-    <col min="5" max="5" width="6.84375" customWidth="1"/>
-    <col min="6" max="6" width="12.4609375" style="9" customWidth="1"/>
+    <col min="1" max="1" width="10.81640625" style="7"/>
+    <col min="2" max="2" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.26953125" customWidth="1"/>
+    <col min="5" max="5" width="6.81640625" customWidth="1"/>
+    <col min="6" max="6" width="12.453125" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
         <v>126</v>
       </c>
@@ -3502,7 +3505,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>133</v>
       </c>
@@ -3518,7 +3521,7 @@
       <c r="F15" s="14"/>
       <c r="G15" s="9"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>134</v>
       </c>
@@ -3542,7 +3545,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="7" t="s">
         <v>135</v>
       </c>
@@ -3567,7 +3570,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="7" t="s">
         <v>136</v>
       </c>
@@ -3592,7 +3595,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="7" t="s">
         <v>137</v>
       </c>
@@ -3628,21 +3631,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="150" workbookViewId="0">
+    <sheetView topLeftCell="A2" zoomScale="150" workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.84375" style="2"/>
-    <col min="2" max="2" width="18.4609375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.4609375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.15234375" customWidth="1"/>
-    <col min="5" max="5" width="6.84375" customWidth="1"/>
-    <col min="6" max="6" width="12.4609375" style="9" customWidth="1"/>
+    <col min="1" max="1" width="10.81640625" style="2"/>
+    <col min="2" max="2" width="18.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.1796875" customWidth="1"/>
+    <col min="5" max="5" width="6.81640625" customWidth="1"/>
+    <col min="6" max="6" width="12.453125" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>127</v>
       </c>
@@ -3662,7 +3665,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="13">
         <v>42632</v>
       </c>
@@ -3682,7 +3685,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="13">
         <v>42647</v>
       </c>
@@ -3707,17 +3710,17 @@
         <v>34.695652173913047</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="13">
         <v>42668</v>
       </c>
       <c r="B4">
         <f>B3-COUNTIF(Sprint2!$I$2:$I$65, "Completed")</f>
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C4">
         <f>B3-B4</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D4">
         <f>Sprint2!G66</f>
@@ -3732,12 +3735,12 @@
         <v>-147.5</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="13">
         <v>42682</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="13">
         <v>42689</v>
       </c>
@@ -3758,19 +3761,19 @@
       <selection activeCell="F51" sqref="F51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="33" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.4609375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.4609375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.3046875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.69140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.4609375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.3046875" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.26953125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.7265625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.26953125" style="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>33</v>
       </c>
@@ -3799,7 +3802,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>37</v>
       </c>
@@ -3828,7 +3831,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="17" t="s">
         <v>144</v>
       </c>
@@ -3845,7 +3848,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="17" t="s">
         <v>147</v>
       </c>
@@ -3862,7 +3865,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="17" t="s">
         <v>149</v>
       </c>
@@ -3879,7 +3882,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>40</v>
       </c>
@@ -3908,7 +3911,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="17" t="s">
         <v>151</v>
       </c>
@@ -3925,7 +3928,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="17" t="s">
         <v>153</v>
       </c>
@@ -3942,7 +3945,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="17" t="s">
         <v>155</v>
       </c>
@@ -3959,7 +3962,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="17" t="s">
         <v>157</v>
       </c>
@@ -3976,7 +3979,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
         <v>43</v>
       </c>
@@ -4005,7 +4008,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="17" t="s">
         <v>159</v>
       </c>
@@ -4022,7 +4025,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="17" t="s">
         <v>161</v>
       </c>
@@ -4039,7 +4042,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="17" t="s">
         <v>162</v>
       </c>
@@ -4056,7 +4059,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="17" t="s">
         <v>164</v>
       </c>
@@ -4073,7 +4076,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
         <v>45</v>
       </c>
@@ -4102,7 +4105,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="17" t="s">
         <v>166</v>
       </c>
@@ -4119,7 +4122,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="17" t="s">
         <v>167</v>
       </c>
@@ -4136,7 +4139,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="17" t="s">
         <v>169</v>
       </c>
@@ -4153,7 +4156,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="17" t="s">
         <v>170</v>
       </c>
@@ -4170,7 +4173,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" s="17" t="s">
         <v>172</v>
       </c>
@@ -4187,7 +4190,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
         <v>47</v>
       </c>
@@ -4216,7 +4219,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" s="17" t="s">
         <v>174</v>
       </c>
@@ -4233,7 +4236,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" s="17" t="s">
         <v>175</v>
       </c>
@@ -4250,7 +4253,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" s="17" t="s">
         <v>176</v>
       </c>
@@ -4267,7 +4270,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" s="17" t="s">
         <v>177</v>
       </c>
@@ -4284,7 +4287,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" s="17" t="s">
         <v>178</v>
       </c>
@@ -4301,7 +4304,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" s="4" t="s">
         <v>49</v>
       </c>
@@ -4330,7 +4333,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" s="17" t="s">
         <v>180</v>
       </c>
@@ -4347,7 +4350,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" s="17" t="s">
         <v>181</v>
       </c>
@@ -4364,7 +4367,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" s="17" t="s">
         <v>182</v>
       </c>
@@ -4381,7 +4384,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" s="17" t="s">
         <v>183</v>
       </c>
@@ -4398,7 +4401,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" s="17" t="s">
         <v>184</v>
       </c>
@@ -4415,7 +4418,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" s="4" t="s">
         <v>51</v>
       </c>
@@ -4444,7 +4447,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" s="17" t="s">
         <v>186</v>
       </c>
@@ -4461,7 +4464,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" s="17" t="s">
         <v>187</v>
       </c>
@@ -4478,7 +4481,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" s="17" t="s">
         <v>189</v>
       </c>
@@ -4495,7 +4498,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" s="17" t="s">
         <v>191</v>
       </c>
@@ -4512,7 +4515,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39" s="17" t="s">
         <v>192</v>
       </c>
@@ -4529,7 +4532,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40" s="17" t="s">
         <v>194</v>
       </c>
@@ -4546,7 +4549,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41" s="4" t="s">
         <v>53</v>
       </c>
@@ -4575,7 +4578,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42" s="17" t="s">
         <v>196</v>
       </c>
@@ -4592,7 +4595,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43" s="17" t="s">
         <v>197</v>
       </c>
@@ -4609,7 +4612,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44" s="17" t="s">
         <v>198</v>
       </c>
@@ -4626,7 +4629,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A45" s="4" t="s">
         <v>55</v>
       </c>
@@ -4655,7 +4658,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A46" s="17" t="s">
         <v>199</v>
       </c>
@@ -4672,7 +4675,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A47" s="17" t="s">
         <v>201</v>
       </c>
@@ -4689,7 +4692,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A48" s="17" t="s">
         <v>203</v>
       </c>
@@ -4706,7 +4709,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A49" s="17" t="s">
         <v>204</v>
       </c>
@@ -4723,7 +4726,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A50" s="4" t="s">
         <v>57</v>
       </c>
@@ -4752,7 +4755,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A51" s="17" t="s">
         <v>206</v>
       </c>
@@ -4769,7 +4772,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A52" s="17" t="s">
         <v>208</v>
       </c>
@@ -4786,7 +4789,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A53" s="17" t="s">
         <v>209</v>
       </c>
@@ -4803,7 +4806,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A54" s="17" t="s">
         <v>210</v>
       </c>
@@ -4820,7 +4823,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A55" s="17" t="s">
         <v>212</v>
       </c>
@@ -4837,7 +4840,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A56" s="4" t="s">
         <v>214</v>
       </c>
@@ -4862,21 +4865,21 @@
       </c>
       <c r="I56" s="21"/>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A57" s="17"/>
       <c r="I57" s="7"/>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B58" s="5" t="s">
         <v>215</v>
       </c>
       <c r="I58" s="7"/>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B59" s="5"/>
       <c r="I59" s="7"/>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B60" s="5" t="s">
         <v>216</v>
       </c>
@@ -4888,7 +4891,7 @@
       <c r="F60" s="26"/>
       <c r="I60" s="7"/>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C61" s="26" t="s">
         <v>218</v>
       </c>
@@ -4897,7 +4900,7 @@
       <c r="F61" s="26"/>
       <c r="I61" s="7"/>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C62" s="26" t="s">
         <v>219</v>
       </c>
@@ -4906,13 +4909,13 @@
       <c r="F62" s="26"/>
       <c r="I62" s="7"/>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C63" s="28"/>
       <c r="D63" s="28"/>
       <c r="E63" s="28"/>
       <c r="F63" s="28"/>
     </row>
-    <row r="64" spans="1:9" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:9" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B64" s="5" t="s">
         <v>220</v>
       </c>
@@ -4924,7 +4927,7 @@
       <c r="F64" s="27"/>
       <c r="I64" s="7"/>
     </row>
-    <row r="65" spans="3:6" ht="26" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="3:6" ht="25.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C65" s="27" t="s">
         <v>222</v>
       </c>
@@ -4951,16 +4954,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:I66"/>
   <sheetViews>
-    <sheetView topLeftCell="A36" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G52" sqref="G52"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I14" sqref="I14:I17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="54.69140625" style="23" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="54.7265625" style="23" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>33</v>
       </c>
@@ -4989,7 +4992,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>59</v>
       </c>
@@ -5009,7 +5012,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="17" t="s">
         <v>330</v>
       </c>
@@ -5019,7 +5022,7 @@
       <c r="C3" s="17"/>
       <c r="D3" s="17"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="17" t="s">
         <v>332</v>
       </c>
@@ -5029,7 +5032,7 @@
       <c r="C4" s="17"/>
       <c r="D4" s="17"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>62</v>
       </c>
@@ -5049,7 +5052,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="17" t="s">
         <v>337</v>
       </c>
@@ -5059,7 +5062,7 @@
       <c r="C6" s="17"/>
       <c r="D6" s="17"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="17" t="s">
         <v>338</v>
       </c>
@@ -5069,7 +5072,7 @@
       <c r="C7" s="17"/>
       <c r="D7" s="17"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="17" t="s">
         <v>339</v>
       </c>
@@ -5079,7 +5082,7 @@
       <c r="C8" s="17"/>
       <c r="D8" s="17"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="17" t="s">
         <v>340</v>
       </c>
@@ -5089,7 +5092,7 @@
       <c r="C9" s="17"/>
       <c r="D9" s="17"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>64</v>
       </c>
@@ -5108,8 +5111,11 @@
       <c r="F10">
         <v>90</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I10" s="17" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="17" t="s">
         <v>345</v>
       </c>
@@ -5118,8 +5124,11 @@
       </c>
       <c r="C11" s="17"/>
       <c r="D11" s="17"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I11" s="17" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="17" t="s">
         <v>346</v>
       </c>
@@ -5128,8 +5137,11 @@
       </c>
       <c r="C12" s="17"/>
       <c r="D12" s="17"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I12" s="17" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="17" t="s">
         <v>347</v>
       </c>
@@ -5138,8 +5150,11 @@
       </c>
       <c r="C13" s="17"/>
       <c r="D13" s="17"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I13" s="17" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
         <v>66</v>
       </c>
@@ -5158,8 +5173,11 @@
       <c r="F14">
         <v>120</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I14" s="17" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="17" t="s">
         <v>350</v>
       </c>
@@ -5168,8 +5186,11 @@
       </c>
       <c r="C15" s="17"/>
       <c r="D15" s="17"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I15" s="17" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="17" t="s">
         <v>351</v>
       </c>
@@ -5178,8 +5199,11 @@
       </c>
       <c r="C16" s="17"/>
       <c r="D16" s="17"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I16" s="17" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="17" t="s">
         <v>352</v>
       </c>
@@ -5188,8 +5212,11 @@
       </c>
       <c r="C17" s="17"/>
       <c r="D17" s="17"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I17" s="17" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
         <v>68</v>
       </c>
@@ -5209,7 +5236,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="17" t="s">
         <v>353</v>
       </c>
@@ -5219,7 +5246,7 @@
       <c r="C19" s="17"/>
       <c r="D19" s="17"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="17" t="s">
         <v>356</v>
       </c>
@@ -5229,7 +5256,7 @@
       <c r="C20" s="17"/>
       <c r="D20" s="17"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
         <v>70</v>
       </c>
@@ -5249,7 +5276,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" s="17" t="s">
         <v>357</v>
       </c>
@@ -5259,7 +5286,7 @@
       <c r="C22" s="17"/>
       <c r="D22" s="17"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" s="17" t="s">
         <v>361</v>
       </c>
@@ -5269,7 +5296,7 @@
       <c r="C23" s="17"/>
       <c r="D23" s="17"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" s="17" t="s">
         <v>362</v>
       </c>
@@ -5279,7 +5306,7 @@
       <c r="C24" s="17"/>
       <c r="D24" s="17"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
         <v>72</v>
       </c>
@@ -5299,7 +5326,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>312</v>
       </c>
@@ -5313,7 +5340,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>313</v>
       </c>
@@ -5327,7 +5354,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="27" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" ht="25.2" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>315</v>
       </c>
@@ -5341,7 +5368,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>317</v>
       </c>
@@ -5355,7 +5382,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="27" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" ht="25.2" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>319</v>
       </c>
@@ -5369,7 +5396,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>321</v>
       </c>
@@ -5383,7 +5410,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" s="4" t="s">
         <v>74</v>
       </c>
@@ -5403,7 +5430,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>322</v>
       </c>
@@ -5417,7 +5444,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>323</v>
       </c>
@@ -5431,7 +5458,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:9" ht="25.2" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>324</v>
       </c>
@@ -5445,7 +5472,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="36" spans="1:9" ht="27" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:9" ht="25.2" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>326</v>
       </c>
@@ -5459,7 +5486,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>328</v>
       </c>
@@ -5473,7 +5500,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" s="4" t="s">
         <v>76</v>
       </c>
@@ -5487,7 +5514,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>223</v>
       </c>
@@ -5516,7 +5543,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>225</v>
       </c>
@@ -5533,7 +5560,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>227</v>
       </c>
@@ -5550,7 +5577,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>229</v>
       </c>
@@ -5567,7 +5594,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>231</v>
       </c>
@@ -5584,7 +5611,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>233</v>
       </c>
@@ -5601,7 +5628,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>235</v>
       </c>
@@ -5618,7 +5645,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>237</v>
       </c>
@@ -5635,7 +5662,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>239</v>
       </c>
@@ -5652,7 +5679,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>241</v>
       </c>
@@ -5669,7 +5696,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>243</v>
       </c>
@@ -5686,7 +5713,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>245</v>
       </c>
@@ -5703,7 +5730,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>247</v>
       </c>
@@ -5720,7 +5747,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>249</v>
       </c>
@@ -5737,7 +5764,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:9" ht="25.2" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>251</v>
       </c>
@@ -5754,7 +5781,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>253</v>
       </c>
@@ -5771,7 +5798,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A55" s="4" t="s">
         <v>78</v>
       </c>
@@ -5800,7 +5827,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>255</v>
       </c>
@@ -5817,7 +5844,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>257</v>
       </c>
@@ -5834,7 +5861,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>258</v>
       </c>
@@ -5851,7 +5878,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>259</v>
       </c>
@@ -5868,7 +5895,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>260</v>
       </c>
@@ -5885,7 +5912,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>261</v>
       </c>
@@ -5902,7 +5929,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>262</v>
       </c>
@@ -5919,7 +5946,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>367</v>
       </c>
@@ -5936,7 +5963,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>368</v>
       </c>
@@ -5953,7 +5980,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>369</v>
       </c>
@@ -5970,7 +5997,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A66" s="4" t="s">
         <v>214</v>
       </c>
@@ -6009,9 +6036,9 @@
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>33</v>
       </c>
@@ -6054,9 +6081,9 @@
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>33</v>
       </c>
@@ -6099,13 +6126,13 @@
       <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="28.15234375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="49.4609375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="28.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="49.453125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>263</v>
       </c>
@@ -6116,7 +6143,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>37</v>
       </c>
@@ -6127,7 +6154,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>40</v>
       </c>
@@ -6138,7 +6165,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>43</v>
       </c>
@@ -6149,7 +6176,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>45</v>
       </c>
@@ -6160,7 +6187,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>47</v>
       </c>
@@ -6171,7 +6198,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>49</v>
       </c>
@@ -6182,7 +6209,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="45" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" ht="45" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>51</v>
       </c>
@@ -6193,7 +6220,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>53</v>
       </c>
@@ -6204,7 +6231,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>55</v>
       </c>
@@ -6215,7 +6242,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>57</v>
       </c>
@@ -6226,7 +6253,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>59</v>
       </c>
@@ -6237,7 +6264,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="45" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" ht="45" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>62</v>
       </c>
@@ -6248,7 +6275,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="45" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" ht="45" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>64</v>
       </c>
@@ -6259,7 +6286,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>66</v>
       </c>
@@ -6270,7 +6297,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>68</v>
       </c>
@@ -6281,7 +6308,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>70</v>
       </c>
@@ -6292,7 +6319,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>72</v>
       </c>
@@ -6303,7 +6330,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>74</v>
       </c>
@@ -6314,7 +6341,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>76</v>
       </c>
@@ -6325,7 +6352,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>78</v>
       </c>
@@ -6336,7 +6363,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>80</v>
       </c>
@@ -6347,7 +6374,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>82</v>
       </c>
@@ -6358,7 +6385,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>84</v>
       </c>
@@ -6369,7 +6396,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="45" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" ht="45" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>86</v>
       </c>
@@ -6380,7 +6407,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>88</v>
       </c>
@@ -6391,7 +6418,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="105" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" ht="105" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>90</v>
       </c>
@@ -6402,7 +6429,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>92</v>
       </c>
@@ -6413,7 +6440,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>94</v>
       </c>
@@ -6424,7 +6451,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>96</v>
       </c>
@@ -6435,7 +6462,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>98</v>
       </c>
@@ -6446,7 +6473,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>100</v>
       </c>
@@ -6457,7 +6484,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>102</v>
       </c>
@@ -6468,7 +6495,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>104</v>
       </c>
@@ -6479,7 +6506,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>106</v>
       </c>
@@ -6490,7 +6517,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>108</v>
       </c>
@@ -6501,7 +6528,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>110</v>
       </c>
@@ -6512,7 +6539,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>112</v>
       </c>
@@ -6523,7 +6550,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>114</v>
       </c>
@@ -6534,7 +6561,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>116</v>
       </c>
@@ -6545,7 +6572,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>118</v>
       </c>
@@ -6556,7 +6583,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>306</v>
       </c>
@@ -6567,7 +6594,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>309</v>
       </c>

</xml_diff>

<commit_message>
Sprint 2 Retrospective Updates
</commit_message>
<xml_diff>
--- a/Team2Report.xlsx
+++ b/Team2Report.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11012"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11011"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/srikanth/Documenta/StevensInstitute/SoftwareEngg/SSW-555/SSW-555Project/Agile_Methods_Project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Avaneesh/Desktop/CS 555/AgileProject/Agile_Methods_Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43412B8A-E6AD-784F-B596-DC4675C0D505}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4BABFE9-A35B-FB4C-96FA-D3991F9F3DC2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7620" yWindow="2060" windowWidth="23260" windowHeight="12580" tabRatio="500" firstSheet="2" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29080" yWindow="460" windowWidth="26440" windowHeight="19500" tabRatio="500" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -23,10 +23,19 @@
     <sheet name="Sprint4" sheetId="6" r:id="rId8"/>
     <sheet name="Stories" sheetId="11" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -36,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="940" uniqueCount="371">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1048" uniqueCount="412">
   <si>
     <t>Initials</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -1169,6 +1178,129 @@
   </si>
   <si>
     <t>Task Finished</t>
+  </si>
+  <si>
+    <t>2: One single branch</t>
+  </si>
+  <si>
+    <t>3: keep a modular approach</t>
+  </si>
+  <si>
+    <t>1: coding before pulling from github</t>
+  </si>
+  <si>
+    <t>2: keeping meeting off until the last minute</t>
+  </si>
+  <si>
+    <t>1: Constant communication with all team members</t>
+  </si>
+  <si>
+    <t>Not Started</t>
+  </si>
+  <si>
+    <t>Check gender with Husb or Wife</t>
+  </si>
+  <si>
+    <t>Store all ID's</t>
+  </si>
+  <si>
+    <t>T21.01</t>
+  </si>
+  <si>
+    <t>T22.01</t>
+  </si>
+  <si>
+    <t>T22.02</t>
+  </si>
+  <si>
+    <t>Check if all are unique, and return boolean</t>
+  </si>
+  <si>
+    <t>T23.01</t>
+  </si>
+  <si>
+    <t>T23.02</t>
+  </si>
+  <si>
+    <t>Store all name and dates</t>
+  </si>
+  <si>
+    <t>T24.01</t>
+  </si>
+  <si>
+    <t>T24.02</t>
+  </si>
+  <si>
+    <t>Find all spouses in each family</t>
+  </si>
+  <si>
+    <t>T25.01</t>
+  </si>
+  <si>
+    <t>T25.02</t>
+  </si>
+  <si>
+    <t>Find all families and grab first names</t>
+  </si>
+  <si>
+    <t>T26.01</t>
+  </si>
+  <si>
+    <t>T26.02</t>
+  </si>
+  <si>
+    <t>T27.01</t>
+  </si>
+  <si>
+    <t>T27.02</t>
+  </si>
+  <si>
+    <t>T28.01</t>
+  </si>
+  <si>
+    <t>T28.02</t>
+  </si>
+  <si>
+    <t>T29.01</t>
+  </si>
+  <si>
+    <t>T29.02</t>
+  </si>
+  <si>
+    <t>T30.01</t>
+  </si>
+  <si>
+    <t>T30.02</t>
+  </si>
+  <si>
+    <t>Grab all id's</t>
+  </si>
+  <si>
+    <t>Check that none have empty attributes</t>
+  </si>
+  <si>
+    <t>Grab all individuals</t>
+  </si>
+  <si>
+    <t>Find their own age</t>
+  </si>
+  <si>
+    <t>Find all siblings</t>
+  </si>
+  <si>
+    <t>Sort them by age</t>
+  </si>
+  <si>
+    <t>Find all individuals</t>
+  </si>
+  <si>
+    <t>Check if they died</t>
+  </si>
+  <si>
+    <t>Find all married couples</t>
+  </si>
+  <si>
+    <t>Check if they are living</t>
   </si>
 </sst>
 </file>
@@ -1665,7 +1797,7 @@
                   <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>24</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2679,7 +2811,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:D4">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D4">
     <sortCondition ref="C2:C4"/>
   </sortState>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -3430,7 +3562,7 @@
   <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -3622,8 +3754,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -3707,23 +3839,23 @@
       </c>
       <c r="B4">
         <f>B3-COUNTIF(Sprint2!$I$2:$I$65, "Completed")</f>
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C4">
         <f>B3-B4</f>
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D4">
         <f>Sprint2!G66</f>
-        <v>223</v>
+        <v>330</v>
       </c>
       <c r="E4">
         <f>Sprint2!H66</f>
-        <v>330</v>
+        <v>600</v>
       </c>
       <c r="F4" s="9">
         <f>(D4-D3)/E4*60</f>
-        <v>-32</v>
+        <v>-6.9</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.15">
@@ -3748,7 +3880,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:I65"/>
   <sheetViews>
-    <sheetView topLeftCell="A54" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="B58" sqref="B58:F65"/>
     </sheetView>
   </sheetViews>
@@ -4945,8 +5077,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:I79"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B80" sqref="B80"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -5002,6 +5134,15 @@
       <c r="F2">
         <v>90</v>
       </c>
+      <c r="G2">
+        <v>34</v>
+      </c>
+      <c r="H2">
+        <v>90</v>
+      </c>
+      <c r="I2" s="17" t="s">
+        <v>143</v>
+      </c>
     </row>
     <row r="3" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A3" s="17" t="s">
@@ -5012,6 +5153,9 @@
       </c>
       <c r="C3" s="17"/>
       <c r="D3" s="17"/>
+      <c r="I3" s="17" t="s">
+        <v>370</v>
+      </c>
     </row>
     <row r="4" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A4" s="17" t="s">
@@ -5022,6 +5166,9 @@
       </c>
       <c r="C4" s="17"/>
       <c r="D4" s="17"/>
+      <c r="I4" s="17" t="s">
+        <v>370</v>
+      </c>
     </row>
     <row r="5" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A5" s="4" t="s">
@@ -5042,6 +5189,15 @@
       <c r="F5">
         <v>120</v>
       </c>
+      <c r="G5">
+        <v>33</v>
+      </c>
+      <c r="H5">
+        <v>90</v>
+      </c>
+      <c r="I5" s="17" t="s">
+        <v>143</v>
+      </c>
     </row>
     <row r="6" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A6" s="17" t="s">
@@ -5052,6 +5208,9 @@
       </c>
       <c r="C6" s="17"/>
       <c r="D6" s="17"/>
+      <c r="I6" s="17" t="s">
+        <v>370</v>
+      </c>
     </row>
     <row r="7" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A7" s="17" t="s">
@@ -5062,6 +5221,9 @@
       </c>
       <c r="C7" s="17"/>
       <c r="D7" s="17"/>
+      <c r="I7" s="17" t="s">
+        <v>370</v>
+      </c>
     </row>
     <row r="8" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A8" s="17" t="s">
@@ -5072,6 +5234,9 @@
       </c>
       <c r="C8" s="17"/>
       <c r="D8" s="17"/>
+      <c r="I8" s="17" t="s">
+        <v>370</v>
+      </c>
     </row>
     <row r="9" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A9" s="17" t="s">
@@ -5082,6 +5247,9 @@
       </c>
       <c r="C9" s="17"/>
       <c r="D9" s="17"/>
+      <c r="I9" s="17" t="s">
+        <v>370</v>
+      </c>
     </row>
     <row r="10" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A10" s="4" t="s">
@@ -5100,6 +5268,12 @@
         <v>50</v>
       </c>
       <c r="F10">
+        <v>90</v>
+      </c>
+      <c r="G10">
+        <v>42</v>
+      </c>
+      <c r="H10">
         <v>90</v>
       </c>
       <c r="I10" s="17" t="s">
@@ -5164,6 +5338,12 @@
       <c r="F14">
         <v>120</v>
       </c>
+      <c r="G14">
+        <v>37</v>
+      </c>
+      <c r="H14">
+        <v>90</v>
+      </c>
       <c r="I14" s="17" t="s">
         <v>143</v>
       </c>
@@ -5226,6 +5406,15 @@
       <c r="F18">
         <v>90</v>
       </c>
+      <c r="G18">
+        <v>35</v>
+      </c>
+      <c r="H18">
+        <v>90</v>
+      </c>
+      <c r="I18" s="17" t="s">
+        <v>143</v>
+      </c>
     </row>
     <row r="19" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A19" s="17" t="s">
@@ -5236,6 +5425,9 @@
       </c>
       <c r="C19" s="17"/>
       <c r="D19" s="17"/>
+      <c r="I19" s="17" t="s">
+        <v>370</v>
+      </c>
     </row>
     <row r="20" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A20" s="17" t="s">
@@ -5246,6 +5438,9 @@
       </c>
       <c r="C20" s="17"/>
       <c r="D20" s="17"/>
+      <c r="I20" s="17" t="s">
+        <v>370</v>
+      </c>
     </row>
     <row r="21" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A21" s="4" t="s">
@@ -5266,6 +5461,15 @@
       <c r="F21">
         <v>90</v>
       </c>
+      <c r="G21">
+        <v>35</v>
+      </c>
+      <c r="H21">
+        <v>90</v>
+      </c>
+      <c r="I21" s="17" t="s">
+        <v>143</v>
+      </c>
     </row>
     <row r="22" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A22" s="17" t="s">
@@ -5276,6 +5480,9 @@
       </c>
       <c r="C22" s="17"/>
       <c r="D22" s="17"/>
+      <c r="I22" s="17" t="s">
+        <v>370</v>
+      </c>
     </row>
     <row r="23" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A23" s="17" t="s">
@@ -5286,6 +5493,9 @@
       </c>
       <c r="C23" s="17"/>
       <c r="D23" s="17"/>
+      <c r="I23" s="17" t="s">
+        <v>370</v>
+      </c>
     </row>
     <row r="24" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A24" s="17" t="s">
@@ -5296,6 +5506,9 @@
       </c>
       <c r="C24" s="17"/>
       <c r="D24" s="17"/>
+      <c r="I24" s="17" t="s">
+        <v>370</v>
+      </c>
     </row>
     <row r="25" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A25" s="4" t="s">
@@ -6056,11 +6269,11 @@
       </c>
       <c r="G66">
         <f>SUM(G12:G65)</f>
-        <v>223</v>
+        <v>330</v>
       </c>
       <c r="H66">
         <f>SUM(H12:H65)</f>
-        <v>330</v>
+        <v>600</v>
       </c>
     </row>
     <row r="72" spans="1:9" ht="14" x14ac:dyDescent="0.15">
@@ -6075,8 +6288,8 @@
       <c r="B74" s="5" t="s">
         <v>216</v>
       </c>
-      <c r="C74" s="26">
-        <v>1</v>
+      <c r="C74" s="26" t="s">
+        <v>375</v>
       </c>
       <c r="D74" s="26"/>
       <c r="E74" s="26"/>
@@ -6084,8 +6297,8 @@
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B75" s="1"/>
-      <c r="C75" s="26">
-        <v>2</v>
+      <c r="C75" s="26" t="s">
+        <v>371</v>
       </c>
       <c r="D75" s="26"/>
       <c r="E75" s="26"/>
@@ -6093,8 +6306,8 @@
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B76" s="1"/>
-      <c r="C76" s="26">
-        <v>3</v>
+      <c r="C76" s="26" t="s">
+        <v>372</v>
       </c>
       <c r="D76" s="26"/>
       <c r="E76" s="26"/>
@@ -6111,8 +6324,8 @@
       <c r="B78" s="5" t="s">
         <v>220</v>
       </c>
-      <c r="C78" s="27">
-        <v>1</v>
+      <c r="C78" s="27" t="s">
+        <v>373</v>
       </c>
       <c r="D78" s="27"/>
       <c r="E78" s="27"/>
@@ -6120,8 +6333,8 @@
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B79" s="1"/>
-      <c r="C79" s="27">
-        <v>2</v>
+      <c r="C79" s="27" t="s">
+        <v>374</v>
       </c>
       <c r="D79" s="27"/>
       <c r="E79" s="27"/>
@@ -6129,12 +6342,12 @@
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="C79:F79"/>
     <mergeCell ref="C74:F74"/>
     <mergeCell ref="C75:F75"/>
     <mergeCell ref="C76:F76"/>
     <mergeCell ref="C77:F77"/>
     <mergeCell ref="C78:F78"/>
-    <mergeCell ref="C79:F79"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -6144,13 +6357,16 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:I30"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView topLeftCell="A5" zoomScale="150" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="2" max="2" width="36.1640625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="28" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
@@ -6179,6 +6395,422 @@
       </c>
       <c r="I1" s="10" t="s">
         <v>142</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="17" x14ac:dyDescent="0.15">
+      <c r="A2" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="E2">
+        <v>20</v>
+      </c>
+      <c r="F2">
+        <v>30</v>
+      </c>
+      <c r="I2" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="16" x14ac:dyDescent="0.15">
+      <c r="A3" t="s">
+        <v>379</v>
+      </c>
+      <c r="B3" t="s">
+        <v>377</v>
+      </c>
+      <c r="C3" s="12"/>
+      <c r="D3" s="17"/>
+    </row>
+    <row r="4" spans="1:9" ht="17" x14ac:dyDescent="0.15">
+      <c r="A4" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="B4" t="s">
+        <v>83</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="E4">
+        <v>20</v>
+      </c>
+      <c r="F4">
+        <v>30</v>
+      </c>
+      <c r="I4" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="16" x14ac:dyDescent="0.15">
+      <c r="A5" t="s">
+        <v>380</v>
+      </c>
+      <c r="B5" t="s">
+        <v>378</v>
+      </c>
+      <c r="C5" s="12"/>
+      <c r="D5" s="17"/>
+    </row>
+    <row r="6" spans="1:9" ht="16" x14ac:dyDescent="0.15">
+      <c r="A6" t="s">
+        <v>381</v>
+      </c>
+      <c r="B6" t="s">
+        <v>382</v>
+      </c>
+      <c r="C6" s="12"/>
+      <c r="D6" s="17"/>
+    </row>
+    <row r="7" spans="1:9" ht="17" x14ac:dyDescent="0.15">
+      <c r="A7" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="B7" t="s">
+        <v>85</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="E7">
+        <v>30</v>
+      </c>
+      <c r="F7">
+        <v>90</v>
+      </c>
+      <c r="I7" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="16" x14ac:dyDescent="0.15">
+      <c r="A8" t="s">
+        <v>383</v>
+      </c>
+      <c r="B8" t="s">
+        <v>385</v>
+      </c>
+      <c r="C8" s="12"/>
+      <c r="D8" s="17"/>
+    </row>
+    <row r="9" spans="1:9" ht="16" x14ac:dyDescent="0.15">
+      <c r="A9" t="s">
+        <v>384</v>
+      </c>
+      <c r="B9" t="s">
+        <v>382</v>
+      </c>
+      <c r="C9" s="12"/>
+      <c r="D9" s="17"/>
+    </row>
+    <row r="10" spans="1:9" ht="17" x14ac:dyDescent="0.15">
+      <c r="A10" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="B10" t="s">
+        <v>87</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="E10">
+        <v>30</v>
+      </c>
+      <c r="F10">
+        <v>90</v>
+      </c>
+      <c r="I10" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="16" x14ac:dyDescent="0.15">
+      <c r="A11" t="s">
+        <v>386</v>
+      </c>
+      <c r="B11" t="s">
+        <v>388</v>
+      </c>
+      <c r="C11" s="12"/>
+      <c r="D11" s="17"/>
+    </row>
+    <row r="12" spans="1:9" ht="16" x14ac:dyDescent="0.15">
+      <c r="A12" t="s">
+        <v>387</v>
+      </c>
+      <c r="B12" t="s">
+        <v>382</v>
+      </c>
+      <c r="C12" s="12"/>
+      <c r="D12" s="17"/>
+    </row>
+    <row r="13" spans="1:9" ht="17" x14ac:dyDescent="0.15">
+      <c r="A13" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="B13" t="s">
+        <v>89</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="D13" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="E13">
+        <v>40</v>
+      </c>
+      <c r="F13">
+        <v>60</v>
+      </c>
+      <c r="I13" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="16" x14ac:dyDescent="0.15">
+      <c r="A14" t="s">
+        <v>389</v>
+      </c>
+      <c r="B14" t="s">
+        <v>391</v>
+      </c>
+      <c r="C14" s="12"/>
+      <c r="D14" s="17"/>
+    </row>
+    <row r="15" spans="1:9" ht="16" x14ac:dyDescent="0.15">
+      <c r="A15" t="s">
+        <v>390</v>
+      </c>
+      <c r="B15" t="s">
+        <v>382</v>
+      </c>
+      <c r="C15" s="12"/>
+      <c r="D15" s="17"/>
+    </row>
+    <row r="16" spans="1:9" ht="17" x14ac:dyDescent="0.15">
+      <c r="A16" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="B16" t="s">
+        <v>91</v>
+      </c>
+      <c r="C16" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="D16" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="E16">
+        <v>40</v>
+      </c>
+      <c r="F16">
+        <v>60</v>
+      </c>
+      <c r="I16" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="16" x14ac:dyDescent="0.15">
+      <c r="A17" t="s">
+        <v>392</v>
+      </c>
+      <c r="B17" t="s">
+        <v>402</v>
+      </c>
+      <c r="C17" s="12"/>
+      <c r="D17" s="17"/>
+    </row>
+    <row r="18" spans="1:9" ht="16" x14ac:dyDescent="0.15">
+      <c r="A18" t="s">
+        <v>393</v>
+      </c>
+      <c r="B18" t="s">
+        <v>403</v>
+      </c>
+      <c r="C18" s="12"/>
+      <c r="D18" s="17"/>
+    </row>
+    <row r="19" spans="1:9" ht="17" x14ac:dyDescent="0.15">
+      <c r="A19" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="B19" t="s">
+        <v>93</v>
+      </c>
+      <c r="C19" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="D19" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="E19">
+        <v>25</v>
+      </c>
+      <c r="F19">
+        <v>60</v>
+      </c>
+      <c r="I19" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="16" x14ac:dyDescent="0.15">
+      <c r="A20" t="s">
+        <v>394</v>
+      </c>
+      <c r="B20" t="s">
+        <v>404</v>
+      </c>
+      <c r="C20" s="12"/>
+      <c r="D20" s="17"/>
+    </row>
+    <row r="21" spans="1:9" ht="16" x14ac:dyDescent="0.15">
+      <c r="A21" t="s">
+        <v>395</v>
+      </c>
+      <c r="B21" t="s">
+        <v>405</v>
+      </c>
+      <c r="C21" s="12"/>
+      <c r="D21" s="17"/>
+    </row>
+    <row r="22" spans="1:9" ht="17" x14ac:dyDescent="0.15">
+      <c r="A22" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="B22" t="s">
+        <v>95</v>
+      </c>
+      <c r="C22" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="D22" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="E22">
+        <v>20</v>
+      </c>
+      <c r="F22">
+        <v>60</v>
+      </c>
+      <c r="I22" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="16" x14ac:dyDescent="0.15">
+      <c r="A23" t="s">
+        <v>396</v>
+      </c>
+      <c r="B23" t="s">
+        <v>406</v>
+      </c>
+      <c r="C23" s="12"/>
+      <c r="D23" s="17"/>
+    </row>
+    <row r="24" spans="1:9" ht="16" x14ac:dyDescent="0.15">
+      <c r="A24" t="s">
+        <v>397</v>
+      </c>
+      <c r="B24" t="s">
+        <v>407</v>
+      </c>
+      <c r="C24" s="12"/>
+      <c r="D24" s="17"/>
+    </row>
+    <row r="25" spans="1:9" ht="17" x14ac:dyDescent="0.15">
+      <c r="A25" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="B25" t="s">
+        <v>97</v>
+      </c>
+      <c r="C25" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="D25" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="E25">
+        <v>25</v>
+      </c>
+      <c r="F25">
+        <v>30</v>
+      </c>
+      <c r="I25" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="16" x14ac:dyDescent="0.15">
+      <c r="A26" t="s">
+        <v>398</v>
+      </c>
+      <c r="B26" t="s">
+        <v>408</v>
+      </c>
+      <c r="C26" s="12"/>
+      <c r="D26" s="17"/>
+    </row>
+    <row r="27" spans="1:9" ht="16" x14ac:dyDescent="0.15">
+      <c r="A27" t="s">
+        <v>399</v>
+      </c>
+      <c r="B27" t="s">
+        <v>409</v>
+      </c>
+      <c r="C27" s="12"/>
+      <c r="D27" s="17"/>
+    </row>
+    <row r="28" spans="1:9" ht="17" x14ac:dyDescent="0.15">
+      <c r="A28" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="B28" t="s">
+        <v>99</v>
+      </c>
+      <c r="C28" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="D28" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="E28">
+        <v>30</v>
+      </c>
+      <c r="F28">
+        <v>30</v>
+      </c>
+      <c r="I28" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A29" t="s">
+        <v>400</v>
+      </c>
+      <c r="B29" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A30" t="s">
+        <v>401</v>
+      </c>
+      <c r="B30" t="s">
+        <v>411</v>
       </c>
     </row>
   </sheetData>
@@ -6236,8 +6868,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:C43"/>
   <sheetViews>
-    <sheetView topLeftCell="A35" zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>

</xml_diff>

<commit_message>
Final Changes for Sprint2
Final Changes for Sprint2
</commit_message>
<xml_diff>
--- a/Team2Report.xlsx
+++ b/Team2Report.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11012"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Avaneesh/Desktop/CS 555/AgileProject/Agile_Methods_Project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/srikanth/Documenta/StevensInstitute/SoftwareEngg/SSW-555/SSW-555Project/Agile_Methods_Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4BABFE9-A35B-FB4C-96FA-D3991F9F3DC2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1186E06B-D3A8-5C43-85DA-881963B7F10F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29080" yWindow="460" windowWidth="26440" windowHeight="19500" tabRatio="500" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2360" yWindow="460" windowWidth="26440" windowHeight="16660" tabRatio="500" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -2811,7 +2811,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D4">
+  <sortState ref="A2:D4">
     <sortCondition ref="C2:C4"/>
   </sortState>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -3755,7 +3755,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -5077,7 +5077,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:I79"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScale="56" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
@@ -6359,7 +6359,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:I30"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" zoomScale="150" workbookViewId="0">
+    <sheetView zoomScale="87" workbookViewId="0">
       <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
@@ -6368,7 +6368,7 @@
     <col min="2" max="2" width="36.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="28" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>33</v>
       </c>
@@ -7175,7 +7175,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:3" ht="17" x14ac:dyDescent="0.15">
       <c r="A28" t="s">
         <v>92</v>
       </c>

</xml_diff>

<commit_message>
addition of userStory 30, associated test case, updates to other files, input files, and updates to spreadsheet report
</commit_message>
<xml_diff>
--- a/Team2Report.xlsx
+++ b/Team2Report.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23231"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Avaneesh/Desktop/CS 555/AgileProject/Agile_Methods_Project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ztyle\Documents\SSW 555\SSW_555_Project_Master\Agile_Methods_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26AAEF25-12D3-9B4B-91DD-55F2D9ADED1D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5CA2FC9-99BA-43CB-90D0-4AA60BBD91A7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14600" tabRatio="500" firstSheet="2" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1048" uniqueCount="412">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1053" uniqueCount="412">
   <si>
     <t>Initials</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -1627,7 +1627,7 @@
             <c:numRef>
               <c:f>'Burndown README'!$B$15:$B$20</c:f>
               <c:numCache>
-                <c:formatCode>m/d/yy</c:formatCode>
+                <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>42632</c:v>
@@ -1698,7 +1698,7 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="m/d/yy" sourceLinked="1"/>
+        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1764,7 +1764,7 @@
             <c:numRef>
               <c:f>Burndown!$A$2:$A$7</c:f>
               <c:numCache>
-                <c:formatCode>m/d/yy</c:formatCode>
+                <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>42632</c:v>
@@ -1799,6 +1799,9 @@
                 <c:pt idx="2">
                   <c:v>20</c:v>
                 </c:pt>
+                <c:pt idx="3">
+                  <c:v>10</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1829,7 +1832,7 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="m/d/yy" sourceLinked="1"/>
+        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2691,16 +2694,16 @@
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.5" customWidth="1"/>
-    <col min="4" max="4" width="22.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.5" customWidth="1"/>
+    <col min="1" max="1" width="7.84375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.15234375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.4609375" customWidth="1"/>
+    <col min="4" max="4" width="22.84375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.4609375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -2717,7 +2720,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -2734,7 +2737,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -2751,7 +2754,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -2768,7 +2771,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -2785,7 +2788,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>25</v>
       </c>
@@ -2802,7 +2805,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D8" s="4" t="s">
         <v>30</v>
       </c>
@@ -2835,16 +2838,16 @@
       <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.84375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="29" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.4609375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.4609375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>32</v>
       </c>
@@ -2861,7 +2864,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2878,7 +2881,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -2901,7 +2904,7 @@
       <c r="I3" s="25"/>
       <c r="J3" s="25"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>1</v>
       </c>
@@ -2918,7 +2921,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>1</v>
       </c>
@@ -2935,7 +2938,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>1</v>
       </c>
@@ -2952,7 +2955,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>1</v>
       </c>
@@ -2969,7 +2972,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>1</v>
       </c>
@@ -2986,7 +2989,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>1</v>
       </c>
@@ -3003,7 +3006,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>1</v>
       </c>
@@ -3020,7 +3023,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>1</v>
       </c>
@@ -3037,7 +3040,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>2</v>
       </c>
@@ -3054,7 +3057,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>2</v>
       </c>
@@ -3071,7 +3074,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>2</v>
       </c>
@@ -3088,7 +3091,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>2</v>
       </c>
@@ -3105,7 +3108,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>2</v>
       </c>
@@ -3122,7 +3125,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>2</v>
       </c>
@@ -3139,7 +3142,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>2</v>
       </c>
@@ -3156,7 +3159,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>2</v>
       </c>
@@ -3173,7 +3176,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>2</v>
       </c>
@@ -3190,7 +3193,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>2</v>
       </c>
@@ -3207,7 +3210,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>3</v>
       </c>
@@ -3224,7 +3227,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>3</v>
       </c>
@@ -3241,7 +3244,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>3</v>
       </c>
@@ -3258,7 +3261,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>3</v>
       </c>
@@ -3275,7 +3278,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>3</v>
       </c>
@@ -3292,7 +3295,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>3</v>
       </c>
@@ -3309,7 +3312,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>3</v>
       </c>
@@ -3326,7 +3329,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>3</v>
       </c>
@@ -3343,7 +3346,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>3</v>
       </c>
@@ -3360,7 +3363,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>3</v>
       </c>
@@ -3377,7 +3380,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>4</v>
       </c>
@@ -3394,7 +3397,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>4</v>
       </c>
@@ -3411,7 +3414,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>4</v>
       </c>
@@ -3428,7 +3431,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>4</v>
       </c>
@@ -3445,7 +3448,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>4</v>
       </c>
@@ -3462,7 +3465,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>4</v>
       </c>
@@ -3479,7 +3482,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>4</v>
       </c>
@@ -3496,7 +3499,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>4</v>
       </c>
@@ -3513,7 +3516,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>4</v>
       </c>
@@ -3530,7 +3533,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>4</v>
       </c>
@@ -3561,51 +3564,51 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
+    <sheetView topLeftCell="A10" zoomScale="150" workbookViewId="0">
       <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="7"/>
-    <col min="2" max="2" width="10.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.33203125" customWidth="1"/>
-    <col min="5" max="5" width="6.83203125" customWidth="1"/>
-    <col min="6" max="6" width="12.5" style="9" customWidth="1"/>
+    <col min="1" max="1" width="10.84375" style="7"/>
+    <col min="2" max="2" width="10.15234375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.84375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.3046875" customWidth="1"/>
+    <col min="5" max="5" width="6.84375" customWidth="1"/>
+    <col min="6" max="6" width="12.4609375" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
         <v>126</v>
       </c>
@@ -3628,7 +3631,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>133</v>
       </c>
@@ -3644,7 +3647,7 @@
       <c r="F15" s="14"/>
       <c r="G15" s="9"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>134</v>
       </c>
@@ -3668,7 +3671,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
         <v>135</v>
       </c>
@@ -3693,7 +3696,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="7" t="s">
         <v>136</v>
       </c>
@@ -3718,7 +3721,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="7" t="s">
         <v>137</v>
       </c>
@@ -3754,21 +3757,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="2"/>
-    <col min="2" max="2" width="18.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.1640625" customWidth="1"/>
-    <col min="5" max="5" width="6.83203125" customWidth="1"/>
-    <col min="6" max="6" width="12.5" style="9" customWidth="1"/>
+    <col min="1" max="1" width="10.84375" style="2"/>
+    <col min="2" max="2" width="18.4609375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.4609375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.15234375" customWidth="1"/>
+    <col min="5" max="5" width="6.84375" customWidth="1"/>
+    <col min="6" max="6" width="12.4609375" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>127</v>
       </c>
@@ -3788,7 +3791,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="13">
         <v>42632</v>
       </c>
@@ -3808,7 +3811,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="13">
         <v>42647</v>
       </c>
@@ -3833,7 +3836,7 @@
         <v>34.695652173913047</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="13">
         <v>42668</v>
       </c>
@@ -3858,12 +3861,31 @@
         <v>-6.9</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="13">
         <v>42682</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="B5">
+        <v>10</v>
+      </c>
+      <c r="C5">
+        <f>B4-B5</f>
+        <v>10</v>
+      </c>
+      <c r="D5">
+        <f>Sprint3!G31</f>
+        <v>36</v>
+      </c>
+      <c r="E5">
+        <f>Sprint3!H31</f>
+        <v>60</v>
+      </c>
+      <c r="F5" s="9">
+        <f>(D5-D4)/E5*60</f>
+        <v>-294</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="13">
         <v>42689</v>
       </c>
@@ -3880,23 +3902,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:I65"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B58" sqref="B58:F65"/>
+    <sheetView topLeftCell="A42" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="H55" sqref="H55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="33" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.33203125" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.4609375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.4609375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.3046875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.69140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.4609375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.3046875" style="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>33</v>
       </c>
@@ -3925,7 +3947,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>37</v>
       </c>
@@ -3954,7 +3976,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="17" t="s">
         <v>144</v>
       </c>
@@ -3971,7 +3993,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="17" t="s">
         <v>147</v>
       </c>
@@ -3988,7 +4010,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="17" t="s">
         <v>149</v>
       </c>
@@ -4005,7 +4027,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>40</v>
       </c>
@@ -4034,7 +4056,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="17" t="s">
         <v>151</v>
       </c>
@@ -4051,7 +4073,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="17" t="s">
         <v>153</v>
       </c>
@@ -4068,7 +4090,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="17" t="s">
         <v>155</v>
       </c>
@@ -4085,7 +4107,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="17" t="s">
         <v>157</v>
       </c>
@@ -4102,7 +4124,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
         <v>43</v>
       </c>
@@ -4131,7 +4153,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="17" t="s">
         <v>159</v>
       </c>
@@ -4148,7 +4170,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="17" t="s">
         <v>161</v>
       </c>
@@ -4165,7 +4187,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="17" t="s">
         <v>162</v>
       </c>
@@ -4182,7 +4204,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="17" t="s">
         <v>164</v>
       </c>
@@ -4199,7 +4221,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
         <v>45</v>
       </c>
@@ -4228,7 +4250,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="17" t="s">
         <v>166</v>
       </c>
@@ -4245,7 +4267,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="17" t="s">
         <v>167</v>
       </c>
@@ -4262,7 +4284,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" s="17" t="s">
         <v>169</v>
       </c>
@@ -4279,7 +4301,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="17" t="s">
         <v>170</v>
       </c>
@@ -4296,7 +4318,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" s="17" t="s">
         <v>172</v>
       </c>
@@ -4313,7 +4335,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" s="4" t="s">
         <v>47</v>
       </c>
@@ -4342,7 +4364,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" s="17" t="s">
         <v>174</v>
       </c>
@@ -4359,7 +4381,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" s="17" t="s">
         <v>175</v>
       </c>
@@ -4376,7 +4398,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" s="17" t="s">
         <v>176</v>
       </c>
@@ -4393,7 +4415,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" s="17" t="s">
         <v>177</v>
       </c>
@@ -4410,7 +4432,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" s="17" t="s">
         <v>178</v>
       </c>
@@ -4427,7 +4449,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" s="4" t="s">
         <v>49</v>
       </c>
@@ -4456,7 +4478,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" s="17" t="s">
         <v>180</v>
       </c>
@@ -4473,7 +4495,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" s="17" t="s">
         <v>181</v>
       </c>
@@ -4490,7 +4512,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" s="17" t="s">
         <v>182</v>
       </c>
@@ -4507,7 +4529,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" s="17" t="s">
         <v>183</v>
       </c>
@@ -4524,7 +4546,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33" s="17" t="s">
         <v>184</v>
       </c>
@@ -4541,7 +4563,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34" s="4" t="s">
         <v>51</v>
       </c>
@@ -4570,7 +4592,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35" s="17" t="s">
         <v>186</v>
       </c>
@@ -4587,7 +4609,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A36" s="17" t="s">
         <v>187</v>
       </c>
@@ -4604,7 +4626,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A37" s="17" t="s">
         <v>189</v>
       </c>
@@ -4621,7 +4643,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A38" s="17" t="s">
         <v>191</v>
       </c>
@@ -4638,7 +4660,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A39" s="17" t="s">
         <v>192</v>
       </c>
@@ -4655,7 +4677,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A40" s="17" t="s">
         <v>194</v>
       </c>
@@ -4672,7 +4694,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A41" s="4" t="s">
         <v>53</v>
       </c>
@@ -4701,7 +4723,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A42" s="17" t="s">
         <v>196</v>
       </c>
@@ -4718,7 +4740,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A43" s="17" t="s">
         <v>197</v>
       </c>
@@ -4735,7 +4757,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A44" s="17" t="s">
         <v>198</v>
       </c>
@@ -4752,7 +4774,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A45" s="4" t="s">
         <v>55</v>
       </c>
@@ -4781,7 +4803,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A46" s="17" t="s">
         <v>199</v>
       </c>
@@ -4798,7 +4820,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A47" s="17" t="s">
         <v>201</v>
       </c>
@@ -4815,7 +4837,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A48" s="17" t="s">
         <v>203</v>
       </c>
@@ -4832,7 +4854,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A49" s="17" t="s">
         <v>204</v>
       </c>
@@ -4849,7 +4871,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A50" s="4" t="s">
         <v>57</v>
       </c>
@@ -4878,7 +4900,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="51" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A51" s="17" t="s">
         <v>206</v>
       </c>
@@ -4895,7 +4917,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="52" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A52" s="17" t="s">
         <v>208</v>
       </c>
@@ -4912,7 +4934,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="53" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A53" s="17" t="s">
         <v>209</v>
       </c>
@@ -4929,7 +4951,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="54" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A54" s="17" t="s">
         <v>210</v>
       </c>
@@ -4946,7 +4968,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="55" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A55" s="17" t="s">
         <v>212</v>
       </c>
@@ -4963,7 +4985,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A56" s="4" t="s">
         <v>214</v>
       </c>
@@ -4988,21 +5010,21 @@
       </c>
       <c r="I56" s="21"/>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A57" s="17"/>
       <c r="I57" s="7"/>
     </row>
-    <row r="58" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B58" s="5" t="s">
         <v>215</v>
       </c>
       <c r="I58" s="7"/>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B59" s="5"/>
       <c r="I59" s="7"/>
     </row>
-    <row r="60" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B60" s="5" t="s">
         <v>216</v>
       </c>
@@ -5014,7 +5036,7 @@
       <c r="F60" s="26"/>
       <c r="I60" s="7"/>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C61" s="26" t="s">
         <v>218</v>
       </c>
@@ -5023,7 +5045,7 @@
       <c r="F61" s="26"/>
       <c r="I61" s="7"/>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C62" s="26" t="s">
         <v>219</v>
       </c>
@@ -5032,13 +5054,13 @@
       <c r="F62" s="26"/>
       <c r="I62" s="7"/>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C63" s="28"/>
       <c r="D63" s="28"/>
       <c r="E63" s="28"/>
       <c r="F63" s="28"/>
     </row>
-    <row r="64" spans="1:9" ht="27" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="64" spans="1:9" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B64" s="5" t="s">
         <v>220</v>
       </c>
@@ -5050,7 +5072,7 @@
       <c r="F64" s="27"/>
       <c r="I64" s="7"/>
     </row>
-    <row r="65" spans="3:6" ht="26" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="65" spans="3:6" ht="26" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C65" s="27" t="s">
         <v>222</v>
       </c>
@@ -5077,16 +5099,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:I79"/>
   <sheetViews>
-    <sheetView zoomScale="56" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView topLeftCell="A44" zoomScale="56" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E66" sqref="E66:H66"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="54.6640625" style="23" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="54.69140625" style="23" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>33</v>
       </c>
@@ -5115,7 +5137,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>59</v>
       </c>
@@ -5144,7 +5166,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="17" t="s">
         <v>330</v>
       </c>
@@ -5157,7 +5179,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="17" t="s">
         <v>332</v>
       </c>
@@ -5170,7 +5192,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>62</v>
       </c>
@@ -5199,7 +5221,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="17" t="s">
         <v>337</v>
       </c>
@@ -5212,7 +5234,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="17" t="s">
         <v>338</v>
       </c>
@@ -5225,7 +5247,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="17" t="s">
         <v>339</v>
       </c>
@@ -5238,7 +5260,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="17" t="s">
         <v>340</v>
       </c>
@@ -5251,7 +5273,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>64</v>
       </c>
@@ -5280,7 +5302,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="17" t="s">
         <v>345</v>
       </c>
@@ -5293,7 +5315,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="17" t="s">
         <v>346</v>
       </c>
@@ -5306,7 +5328,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="28" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="17" t="s">
         <v>347</v>
       </c>
@@ -5319,7 +5341,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
         <v>66</v>
       </c>
@@ -5348,7 +5370,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="17" t="s">
         <v>350</v>
       </c>
@@ -5361,7 +5383,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="17" t="s">
         <v>351</v>
       </c>
@@ -5374,7 +5396,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="17" t="s">
         <v>352</v>
       </c>
@@ -5387,7 +5409,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
         <v>68</v>
       </c>
@@ -5416,7 +5438,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" s="17" t="s">
         <v>353</v>
       </c>
@@ -5429,7 +5451,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="17" t="s">
         <v>356</v>
       </c>
@@ -5442,7 +5464,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
         <v>70</v>
       </c>
@@ -5471,7 +5493,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" s="17" t="s">
         <v>357</v>
       </c>
@@ -5484,7 +5506,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" s="17" t="s">
         <v>361</v>
       </c>
@@ -5497,7 +5519,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" s="17" t="s">
         <v>362</v>
       </c>
@@ -5510,7 +5532,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" s="4" t="s">
         <v>72</v>
       </c>
@@ -5539,7 +5561,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>312</v>
       </c>
@@ -5556,7 +5578,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="27" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>313</v>
       </c>
@@ -5573,7 +5595,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="28" spans="1:9" ht="28" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:9" ht="27" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>315</v>
       </c>
@@ -5590,7 +5612,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="29" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>317</v>
       </c>
@@ -5607,7 +5629,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="30" spans="1:9" ht="28" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:9" ht="27" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>319</v>
       </c>
@@ -5624,7 +5646,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="31" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>321</v>
       </c>
@@ -5641,7 +5663,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="32" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" s="4" t="s">
         <v>74</v>
       </c>
@@ -5670,7 +5692,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="33" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>322</v>
       </c>
@@ -5687,7 +5709,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="34" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>323</v>
       </c>
@@ -5704,7 +5726,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="35" spans="1:9" ht="28" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>324</v>
       </c>
@@ -5721,7 +5743,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="36" spans="1:9" ht="28" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:9" ht="27" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>326</v>
       </c>
@@ -5738,7 +5760,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="37" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>328</v>
       </c>
@@ -5755,7 +5777,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="38" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A38" s="4" t="s">
         <v>76</v>
       </c>
@@ -5769,7 +5791,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="39" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>223</v>
       </c>
@@ -5798,7 +5820,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="40" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>225</v>
       </c>
@@ -5815,7 +5837,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="41" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>227</v>
       </c>
@@ -5832,7 +5854,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="42" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>229</v>
       </c>
@@ -5849,7 +5871,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="43" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>231</v>
       </c>
@@ -5866,7 +5888,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="44" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>233</v>
       </c>
@@ -5883,7 +5905,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="45" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>235</v>
       </c>
@@ -5900,7 +5922,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="46" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>237</v>
       </c>
@@ -5917,7 +5939,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="47" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>239</v>
       </c>
@@ -5934,7 +5956,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="48" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>241</v>
       </c>
@@ -5951,7 +5973,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="49" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>243</v>
       </c>
@@ -5968,7 +5990,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="50" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>245</v>
       </c>
@@ -5985,7 +6007,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="51" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>247</v>
       </c>
@@ -6002,7 +6024,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="52" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>249</v>
       </c>
@@ -6019,7 +6041,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="53" spans="1:9" ht="28" x14ac:dyDescent="0.15">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>251</v>
       </c>
@@ -6036,7 +6058,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="54" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>253</v>
       </c>
@@ -6053,7 +6075,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="55" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A55" s="4" t="s">
         <v>78</v>
       </c>
@@ -6082,7 +6104,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="56" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>255</v>
       </c>
@@ -6099,7 +6121,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="57" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>257</v>
       </c>
@@ -6116,7 +6138,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="58" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>258</v>
       </c>
@@ -6133,7 +6155,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="59" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>259</v>
       </c>
@@ -6150,7 +6172,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="60" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>260</v>
       </c>
@@ -6167,7 +6189,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="61" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>261</v>
       </c>
@@ -6184,7 +6206,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="62" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>262</v>
       </c>
@@ -6201,7 +6223,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="63" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>367</v>
       </c>
@@ -6218,7 +6240,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="64" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>368</v>
       </c>
@@ -6235,7 +6257,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="65" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>369</v>
       </c>
@@ -6252,7 +6274,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A66" s="4" t="s">
         <v>214</v>
       </c>
@@ -6276,15 +6298,15 @@
         <v>600</v>
       </c>
     </row>
-    <row r="72" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B72" s="5" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B73" s="5"/>
     </row>
-    <row r="74" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B74" s="5" t="s">
         <v>216</v>
       </c>
@@ -6295,7 +6317,7 @@
       <c r="E74" s="26"/>
       <c r="F74" s="26"/>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B75" s="1"/>
       <c r="C75" s="26" t="s">
         <v>371</v>
@@ -6304,7 +6326,7 @@
       <c r="E75" s="26"/>
       <c r="F75" s="26"/>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B76" s="1"/>
       <c r="C76" s="26" t="s">
         <v>372</v>
@@ -6313,14 +6335,14 @@
       <c r="E76" s="26"/>
       <c r="F76" s="26"/>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B77" s="1"/>
       <c r="C77" s="28"/>
       <c r="D77" s="28"/>
       <c r="E77" s="28"/>
       <c r="F77" s="28"/>
     </row>
-    <row r="78" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B78" s="5" t="s">
         <v>220</v>
       </c>
@@ -6331,7 +6353,7 @@
       <c r="E78" s="27"/>
       <c r="F78" s="27"/>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B79" s="1"/>
       <c r="C79" s="27" t="s">
         <v>374</v>
@@ -6357,18 +6379,19 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:I30"/>
+  <dimension ref="A1:I31"/>
   <sheetViews>
-    <sheetView zoomScale="148" zoomScaleNormal="148" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="36.1640625" customWidth="1"/>
+    <col min="2" max="2" width="36.15234375" customWidth="1"/>
+    <col min="9" max="9" width="11.3828125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>33</v>
       </c>
@@ -6397,7 +6420,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="17" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:9" ht="15" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>80</v>
       </c>
@@ -6420,7 +6443,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="16" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:9" ht="15" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>379</v>
       </c>
@@ -6430,7 +6453,7 @@
       <c r="C3" s="12"/>
       <c r="D3" s="17"/>
     </row>
-    <row r="4" spans="1:9" ht="17" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:9" ht="15" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>82</v>
       </c>
@@ -6453,7 +6476,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="16" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:9" ht="15" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>380</v>
       </c>
@@ -6463,7 +6486,7 @@
       <c r="C5" s="12"/>
       <c r="D5" s="17"/>
     </row>
-    <row r="6" spans="1:9" ht="16" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:9" ht="15" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>381</v>
       </c>
@@ -6473,7 +6496,7 @@
       <c r="C6" s="12"/>
       <c r="D6" s="17"/>
     </row>
-    <row r="7" spans="1:9" ht="17" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:9" ht="15" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>84</v>
       </c>
@@ -6496,7 +6519,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="16" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:9" ht="15" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>383</v>
       </c>
@@ -6506,7 +6529,7 @@
       <c r="C8" s="12"/>
       <c r="D8" s="17"/>
     </row>
-    <row r="9" spans="1:9" ht="16" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:9" ht="15" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>384</v>
       </c>
@@ -6516,7 +6539,7 @@
       <c r="C9" s="12"/>
       <c r="D9" s="17"/>
     </row>
-    <row r="10" spans="1:9" ht="17" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:9" ht="15" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>86</v>
       </c>
@@ -6539,7 +6562,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="16" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:9" ht="15" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>386</v>
       </c>
@@ -6549,7 +6572,7 @@
       <c r="C11" s="12"/>
       <c r="D11" s="17"/>
     </row>
-    <row r="12" spans="1:9" ht="16" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:9" ht="15" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>387</v>
       </c>
@@ -6559,7 +6582,7 @@
       <c r="C12" s="12"/>
       <c r="D12" s="17"/>
     </row>
-    <row r="13" spans="1:9" ht="17" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:9" ht="15" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
         <v>88</v>
       </c>
@@ -6582,7 +6605,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="16" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:9" ht="15" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>389</v>
       </c>
@@ -6592,7 +6615,7 @@
       <c r="C14" s="12"/>
       <c r="D14" s="17"/>
     </row>
-    <row r="15" spans="1:9" ht="16" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:9" ht="15" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>390</v>
       </c>
@@ -6602,7 +6625,7 @@
       <c r="C15" s="12"/>
       <c r="D15" s="17"/>
     </row>
-    <row r="16" spans="1:9" ht="17" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:9" ht="15" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
         <v>90</v>
       </c>
@@ -6625,7 +6648,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="16" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:9" ht="15" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>392</v>
       </c>
@@ -6635,7 +6658,7 @@
       <c r="C17" s="12"/>
       <c r="D17" s="17"/>
     </row>
-    <row r="18" spans="1:9" ht="16" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:9" ht="15" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>393</v>
       </c>
@@ -6645,7 +6668,7 @@
       <c r="C18" s="12"/>
       <c r="D18" s="17"/>
     </row>
-    <row r="19" spans="1:9" ht="17" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:9" ht="15" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
         <v>92</v>
       </c>
@@ -6668,7 +6691,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="16" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:9" ht="15" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>394</v>
       </c>
@@ -6678,7 +6701,7 @@
       <c r="C20" s="12"/>
       <c r="D20" s="17"/>
     </row>
-    <row r="21" spans="1:9" ht="16" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:9" ht="15" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>395</v>
       </c>
@@ -6688,7 +6711,7 @@
       <c r="C21" s="12"/>
       <c r="D21" s="17"/>
     </row>
-    <row r="22" spans="1:9" ht="17" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:9" ht="15" x14ac:dyDescent="0.3">
       <c r="A22" s="4" t="s">
         <v>94</v>
       </c>
@@ -6711,7 +6734,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="16" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:9" ht="15" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>396</v>
       </c>
@@ -6721,7 +6744,7 @@
       <c r="C23" s="12"/>
       <c r="D23" s="17"/>
     </row>
-    <row r="24" spans="1:9" ht="16" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:9" ht="15" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>397</v>
       </c>
@@ -6731,7 +6754,7 @@
       <c r="C24" s="12"/>
       <c r="D24" s="17"/>
     </row>
-    <row r="25" spans="1:9" ht="17" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:9" ht="15" x14ac:dyDescent="0.3">
       <c r="A25" s="4" t="s">
         <v>96</v>
       </c>
@@ -6750,11 +6773,17 @@
       <c r="F25">
         <v>30</v>
       </c>
+      <c r="G25">
+        <v>15</v>
+      </c>
+      <c r="H25">
+        <v>30</v>
+      </c>
       <c r="I25" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" ht="16" x14ac:dyDescent="0.15">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="15" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>398</v>
       </c>
@@ -6763,8 +6792,11 @@
       </c>
       <c r="C26" s="12"/>
       <c r="D26" s="17"/>
-    </row>
-    <row r="27" spans="1:9" ht="16" x14ac:dyDescent="0.15">
+      <c r="I26" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="15" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>399</v>
       </c>
@@ -6773,8 +6805,11 @@
       </c>
       <c r="C27" s="12"/>
       <c r="D27" s="17"/>
-    </row>
-    <row r="28" spans="1:9" ht="17" x14ac:dyDescent="0.15">
+      <c r="I27" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="15" x14ac:dyDescent="0.3">
       <c r="A28" s="4" t="s">
         <v>98</v>
       </c>
@@ -6793,29 +6828,63 @@
       <c r="F28">
         <v>30</v>
       </c>
+      <c r="G28">
+        <v>21</v>
+      </c>
+      <c r="H28">
+        <v>30</v>
+      </c>
       <c r="I28" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.15">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>400</v>
       </c>
       <c r="B29" t="s">
         <v>410</v>
       </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="I29" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>401</v>
       </c>
       <c r="B30" t="s">
         <v>411</v>
+      </c>
+      <c r="I30" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A31" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="E31">
+        <f>SUM(E2:E30)</f>
+        <v>280</v>
+      </c>
+      <c r="F31">
+        <f t="shared" ref="F31:H31" si="0">SUM(F2:F30)</f>
+        <v>540</v>
+      </c>
+      <c r="G31">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+      <c r="H31">
+        <f t="shared" si="0"/>
+        <v>60</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -6827,9 +6896,9 @@
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:9" ht="28" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>33</v>
       </c>
@@ -6868,17 +6937,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:C43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="145" zoomScaleNormal="145" zoomScalePageLayoutView="150" workbookViewId="0">
+    <sheetView topLeftCell="A18" zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
       <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="28.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="49.5" style="1" customWidth="1"/>
+    <col min="2" max="2" width="28.15234375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="49.4609375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="4" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>263</v>
       </c>
@@ -6889,7 +6958,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>37</v>
       </c>
@@ -6900,7 +6969,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>40</v>
       </c>
@@ -6911,7 +6980,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>43</v>
       </c>
@@ -6922,7 +6991,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>45</v>
       </c>
@@ -6933,7 +7002,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>47</v>
       </c>
@@ -6944,7 +7013,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>49</v>
       </c>
@@ -6955,7 +7024,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="51" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:3" ht="45" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>51</v>
       </c>
@@ -6966,7 +7035,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>53</v>
       </c>
@@ -6977,7 +7046,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>55</v>
       </c>
@@ -6988,7 +7057,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="51" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>57</v>
       </c>
@@ -6999,7 +7068,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>59</v>
       </c>
@@ -7010,7 +7079,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="51" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:3" ht="45" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>62</v>
       </c>
@@ -7021,7 +7090,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="68" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:3" ht="45" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>64</v>
       </c>
@@ -7032,7 +7101,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>66</v>
       </c>
@@ -7043,7 +7112,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>68</v>
       </c>
@@ -7054,7 +7123,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>70</v>
       </c>
@@ -7065,7 +7134,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>72</v>
       </c>
@@ -7076,7 +7145,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>74</v>
       </c>
@@ -7087,7 +7156,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>76</v>
       </c>
@@ -7098,7 +7167,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>78</v>
       </c>
@@ -7109,7 +7178,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>80</v>
       </c>
@@ -7120,7 +7189,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>82</v>
       </c>
@@ -7131,7 +7200,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>84</v>
       </c>
@@ -7142,7 +7211,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="51" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:3" ht="45" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>86</v>
       </c>
@@ -7153,7 +7222,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>88</v>
       </c>
@@ -7164,7 +7233,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="136" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:3" ht="105" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>90</v>
       </c>
@@ -7175,7 +7244,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>92</v>
       </c>
@@ -7186,7 +7255,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>94</v>
       </c>
@@ -7197,7 +7266,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>96</v>
       </c>
@@ -7208,7 +7277,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>98</v>
       </c>
@@ -7219,7 +7288,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>100</v>
       </c>
@@ -7230,7 +7299,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>102</v>
       </c>
@@ -7241,7 +7310,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>104</v>
       </c>
@@ -7252,7 +7321,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="51" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>106</v>
       </c>
@@ -7263,7 +7332,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>108</v>
       </c>
@@ -7274,7 +7343,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>110</v>
       </c>
@@ -7285,7 +7354,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>112</v>
       </c>
@@ -7296,7 +7365,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>114</v>
       </c>
@@ -7307,7 +7376,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>116</v>
       </c>
@@ -7318,7 +7387,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>118</v>
       </c>
@@ -7329,7 +7398,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>306</v>
       </c>
@@ -7340,7 +7409,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>309</v>
       </c>

</xml_diff>

<commit_message>
Added userstories 27 and 28
Added userstories 27 and 28, and recreate all test reports
</commit_message>
<xml_diff>
--- a/Team2Report.xlsx
+++ b/Team2Report.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11012"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ztyle\Documents\SSW 555\SSW_555_Project_Master\Agile_Methods_Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/srikanth/Documenta/StevensInstitute/SoftwareEngg/SSW-555/SSW-555Project/Agile_Methods_Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5CA2FC9-99BA-43CB-90D0-4AA60BBD91A7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1996D1C6-096A-7140-B9C2-66E116EC7EC4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7900" yWindow="2660" windowWidth="26580" windowHeight="15900" tabRatio="500" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -23,19 +23,10 @@
     <sheet name="Sprint4" sheetId="6" r:id="rId8"/>
     <sheet name="Stories" sheetId="11" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -45,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1053" uniqueCount="412">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1057" uniqueCount="412">
   <si>
     <t>Initials</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -1627,7 +1618,7 @@
             <c:numRef>
               <c:f>'Burndown README'!$B$15:$B$20</c:f>
               <c:numCache>
-                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:formatCode>m/d/yy</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>42632</c:v>
@@ -1698,7 +1689,7 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
+        <c:numFmt formatCode="m/d/yy" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1764,7 +1755,7 @@
             <c:numRef>
               <c:f>Burndown!$A$2:$A$7</c:f>
               <c:numCache>
-                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:formatCode>m/d/yy</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>42632</c:v>
@@ -1832,7 +1823,7 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
+        <c:numFmt formatCode="m/d/yy" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2694,16 +2685,16 @@
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="7.84375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.15234375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.4609375" customWidth="1"/>
-    <col min="4" max="4" width="22.84375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.4609375" customWidth="1"/>
+    <col min="1" max="1" width="7.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.5" customWidth="1"/>
+    <col min="4" max="4" width="22.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -2720,7 +2711,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -2737,7 +2728,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -2754,7 +2745,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -2771,7 +2762,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -2788,7 +2779,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>25</v>
       </c>
@@ -2805,7 +2796,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.15">
       <c r="D8" s="4" t="s">
         <v>30</v>
       </c>
@@ -2814,7 +2805,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D4">
+  <sortState ref="A2:D4">
     <sortCondition ref="C2:C4"/>
   </sortState>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -2838,16 +2829,16 @@
       <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="6.84375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="29" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.4609375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.4609375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>32</v>
       </c>
@@ -2864,7 +2855,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2881,7 +2872,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A3">
         <v>1</v>
       </c>
@@ -2904,7 +2895,7 @@
       <c r="I3" s="25"/>
       <c r="J3" s="25"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A4">
         <v>1</v>
       </c>
@@ -2921,7 +2912,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A5">
         <v>1</v>
       </c>
@@ -2938,7 +2929,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A6">
         <v>1</v>
       </c>
@@ -2955,7 +2946,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A7">
         <v>1</v>
       </c>
@@ -2972,7 +2963,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A8">
         <v>1</v>
       </c>
@@ -2989,7 +2980,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A9">
         <v>1</v>
       </c>
@@ -3006,7 +2997,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A10">
         <v>1</v>
       </c>
@@ -3023,7 +3014,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A11">
         <v>1</v>
       </c>
@@ -3040,7 +3031,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A12">
         <v>2</v>
       </c>
@@ -3057,7 +3048,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A13">
         <v>2</v>
       </c>
@@ -3074,7 +3065,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A14">
         <v>2</v>
       </c>
@@ -3091,7 +3082,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A15">
         <v>2</v>
       </c>
@@ -3108,7 +3099,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A16">
         <v>2</v>
       </c>
@@ -3125,7 +3116,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A17">
         <v>2</v>
       </c>
@@ -3142,7 +3133,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A18">
         <v>2</v>
       </c>
@@ -3159,7 +3150,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A19">
         <v>2</v>
       </c>
@@ -3176,7 +3167,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A20">
         <v>2</v>
       </c>
@@ -3193,7 +3184,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A21">
         <v>2</v>
       </c>
@@ -3210,7 +3201,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A22">
         <v>3</v>
       </c>
@@ -3227,7 +3218,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A23">
         <v>3</v>
       </c>
@@ -3244,7 +3235,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A24">
         <v>3</v>
       </c>
@@ -3261,7 +3252,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A25">
         <v>3</v>
       </c>
@@ -3278,7 +3269,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A26">
         <v>3</v>
       </c>
@@ -3295,7 +3286,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A27">
         <v>3</v>
       </c>
@@ -3312,7 +3303,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A28">
         <v>3</v>
       </c>
@@ -3329,7 +3320,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A29">
         <v>3</v>
       </c>
@@ -3346,7 +3337,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A30">
         <v>3</v>
       </c>
@@ -3363,7 +3354,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A31">
         <v>3</v>
       </c>
@@ -3380,7 +3371,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A32">
         <v>4</v>
       </c>
@@ -3397,7 +3388,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A33">
         <v>4</v>
       </c>
@@ -3414,7 +3405,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A34">
         <v>4</v>
       </c>
@@ -3431,7 +3422,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A35">
         <v>4</v>
       </c>
@@ -3448,7 +3439,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A36">
         <v>4</v>
       </c>
@@ -3465,7 +3456,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A37">
         <v>4</v>
       </c>
@@ -3482,7 +3473,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A38">
         <v>4</v>
       </c>
@@ -3499,7 +3490,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A39">
         <v>4</v>
       </c>
@@ -3516,7 +3507,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A40">
         <v>4</v>
       </c>
@@ -3533,7 +3524,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A41">
         <v>4</v>
       </c>
@@ -3568,47 +3559,47 @@
       <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="10.84375" style="7"/>
-    <col min="2" max="2" width="10.15234375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.84375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.3046875" customWidth="1"/>
-    <col min="5" max="5" width="6.84375" customWidth="1"/>
-    <col min="6" max="6" width="12.4609375" style="9" customWidth="1"/>
+    <col min="1" max="1" width="10.83203125" style="7"/>
+    <col min="2" max="2" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.33203125" customWidth="1"/>
+    <col min="5" max="5" width="6.83203125" customWidth="1"/>
+    <col min="6" max="6" width="12.5" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A1" s="7" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A2" s="7" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A3" s="7" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A5" s="7" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A6" s="7" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A8" s="7" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A14" s="4" t="s">
         <v>126</v>
       </c>
@@ -3631,7 +3622,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
         <v>133</v>
       </c>
@@ -3647,7 +3638,7 @@
       <c r="F15" s="14"/>
       <c r="G15" s="9"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
         <v>134</v>
       </c>
@@ -3671,7 +3662,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A17" s="7" t="s">
         <v>135</v>
       </c>
@@ -3696,7 +3687,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A18" s="7" t="s">
         <v>136</v>
       </c>
@@ -3721,7 +3712,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A19" s="7" t="s">
         <v>137</v>
       </c>
@@ -3758,20 +3749,20 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="G34" sqref="G34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="10.84375" style="2"/>
-    <col min="2" max="2" width="18.4609375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.4609375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.15234375" customWidth="1"/>
-    <col min="5" max="5" width="6.84375" customWidth="1"/>
-    <col min="6" max="6" width="12.4609375" style="9" customWidth="1"/>
+    <col min="1" max="1" width="10.83203125" style="2"/>
+    <col min="2" max="2" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.1640625" customWidth="1"/>
+    <col min="5" max="5" width="6.83203125" customWidth="1"/>
+    <col min="6" max="6" width="12.5" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="3" t="s">
         <v>127</v>
       </c>
@@ -3791,7 +3782,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A2" s="13">
         <v>42632</v>
       </c>
@@ -3811,7 +3802,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A3" s="13">
         <v>42647</v>
       </c>
@@ -3836,7 +3827,7 @@
         <v>34.695652173913047</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A4" s="13">
         <v>42668</v>
       </c>
@@ -3861,7 +3852,7 @@
         <v>-6.9</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A5" s="13">
         <v>42682</v>
       </c>
@@ -3874,18 +3865,18 @@
       </c>
       <c r="D5">
         <f>Sprint3!G31</f>
-        <v>36</v>
+        <v>103</v>
       </c>
       <c r="E5">
         <f>Sprint3!H31</f>
-        <v>60</v>
+        <v>210</v>
       </c>
       <c r="F5" s="9">
         <f>(D5-D4)/E5*60</f>
-        <v>-294</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+        <v>-64.857142857142847</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A6" s="13">
         <v>42689</v>
       </c>
@@ -3902,23 +3893,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:I65"/>
   <sheetViews>
-    <sheetView topLeftCell="A42" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView zoomScale="109" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="H55" sqref="H55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="33" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.4609375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.4609375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.3046875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.69140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.4609375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.3046875" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.33203125" style="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>33</v>
       </c>
@@ -3947,7 +3938,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A2" s="4" t="s">
         <v>37</v>
       </c>
@@ -3976,7 +3967,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A3" s="17" t="s">
         <v>144</v>
       </c>
@@ -3993,7 +3984,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A4" s="17" t="s">
         <v>147</v>
       </c>
@@ -4010,7 +4001,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A5" s="17" t="s">
         <v>149</v>
       </c>
@@ -4027,7 +4018,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A6" s="4" t="s">
         <v>40</v>
       </c>
@@ -4056,7 +4047,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A7" s="17" t="s">
         <v>151</v>
       </c>
@@ -4073,7 +4064,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A8" s="17" t="s">
         <v>153</v>
       </c>
@@ -4090,7 +4081,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A9" s="17" t="s">
         <v>155</v>
       </c>
@@ -4107,7 +4098,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A10" s="17" t="s">
         <v>157</v>
       </c>
@@ -4124,7 +4115,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A11" s="4" t="s">
         <v>43</v>
       </c>
@@ -4153,7 +4144,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A12" s="17" t="s">
         <v>159</v>
       </c>
@@ -4170,7 +4161,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A13" s="17" t="s">
         <v>161</v>
       </c>
@@ -4187,7 +4178,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A14" s="17" t="s">
         <v>162</v>
       </c>
@@ -4204,7 +4195,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A15" s="17" t="s">
         <v>164</v>
       </c>
@@ -4221,7 +4212,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A16" s="4" t="s">
         <v>45</v>
       </c>
@@ -4250,7 +4241,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A17" s="17" t="s">
         <v>166</v>
       </c>
@@ -4267,7 +4258,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A18" s="17" t="s">
         <v>167</v>
       </c>
@@ -4284,7 +4275,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A19" s="17" t="s">
         <v>169</v>
       </c>
@@ -4301,7 +4292,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A20" s="17" t="s">
         <v>170</v>
       </c>
@@ -4318,7 +4309,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A21" s="17" t="s">
         <v>172</v>
       </c>
@@ -4335,7 +4326,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A22" s="4" t="s">
         <v>47</v>
       </c>
@@ -4364,7 +4355,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A23" s="17" t="s">
         <v>174</v>
       </c>
@@ -4381,7 +4372,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A24" s="17" t="s">
         <v>175</v>
       </c>
@@ -4398,7 +4389,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A25" s="17" t="s">
         <v>176</v>
       </c>
@@ -4415,7 +4406,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A26" s="17" t="s">
         <v>177</v>
       </c>
@@ -4432,7 +4423,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A27" s="17" t="s">
         <v>178</v>
       </c>
@@ -4449,7 +4440,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A28" s="4" t="s">
         <v>49</v>
       </c>
@@ -4478,7 +4469,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A29" s="17" t="s">
         <v>180</v>
       </c>
@@ -4495,7 +4486,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A30" s="17" t="s">
         <v>181</v>
       </c>
@@ -4512,7 +4503,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A31" s="17" t="s">
         <v>182</v>
       </c>
@@ -4529,7 +4520,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A32" s="17" t="s">
         <v>183</v>
       </c>
@@ -4546,7 +4537,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A33" s="17" t="s">
         <v>184</v>
       </c>
@@ -4563,7 +4554,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A34" s="4" t="s">
         <v>51</v>
       </c>
@@ -4592,7 +4583,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A35" s="17" t="s">
         <v>186</v>
       </c>
@@ -4609,7 +4600,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A36" s="17" t="s">
         <v>187</v>
       </c>
@@ -4626,7 +4617,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A37" s="17" t="s">
         <v>189</v>
       </c>
@@ -4643,7 +4634,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A38" s="17" t="s">
         <v>191</v>
       </c>
@@ -4660,7 +4651,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A39" s="17" t="s">
         <v>192</v>
       </c>
@@ -4677,7 +4668,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A40" s="17" t="s">
         <v>194</v>
       </c>
@@ -4694,7 +4685,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A41" s="4" t="s">
         <v>53</v>
       </c>
@@ -4723,7 +4714,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A42" s="17" t="s">
         <v>196</v>
       </c>
@@ -4740,7 +4731,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A43" s="17" t="s">
         <v>197</v>
       </c>
@@ -4757,7 +4748,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A44" s="17" t="s">
         <v>198</v>
       </c>
@@ -4774,7 +4765,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A45" s="4" t="s">
         <v>55</v>
       </c>
@@ -4803,7 +4794,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A46" s="17" t="s">
         <v>199</v>
       </c>
@@ -4820,7 +4811,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A47" s="17" t="s">
         <v>201</v>
       </c>
@@ -4837,7 +4828,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A48" s="17" t="s">
         <v>203</v>
       </c>
@@ -4854,7 +4845,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A49" s="17" t="s">
         <v>204</v>
       </c>
@@ -4871,7 +4862,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A50" s="4" t="s">
         <v>57</v>
       </c>
@@ -4900,7 +4891,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A51" s="17" t="s">
         <v>206</v>
       </c>
@@ -4917,7 +4908,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A52" s="17" t="s">
         <v>208</v>
       </c>
@@ -4934,7 +4925,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A53" s="17" t="s">
         <v>209</v>
       </c>
@@ -4951,7 +4942,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A54" s="17" t="s">
         <v>210</v>
       </c>
@@ -4968,7 +4959,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A55" s="17" t="s">
         <v>212</v>
       </c>
@@ -4985,7 +4976,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A56" s="4" t="s">
         <v>214</v>
       </c>
@@ -5010,21 +5001,21 @@
       </c>
       <c r="I56" s="21"/>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A57" s="17"/>
       <c r="I57" s="7"/>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="B58" s="5" t="s">
         <v>215</v>
       </c>
       <c r="I58" s="7"/>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B59" s="5"/>
       <c r="I59" s="7"/>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="B60" s="5" t="s">
         <v>216</v>
       </c>
@@ -5036,7 +5027,7 @@
       <c r="F60" s="26"/>
       <c r="I60" s="7"/>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C61" s="26" t="s">
         <v>218</v>
       </c>
@@ -5045,7 +5036,7 @@
       <c r="F61" s="26"/>
       <c r="I61" s="7"/>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C62" s="26" t="s">
         <v>219</v>
       </c>
@@ -5054,13 +5045,13 @@
       <c r="F62" s="26"/>
       <c r="I62" s="7"/>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C63" s="28"/>
       <c r="D63" s="28"/>
       <c r="E63" s="28"/>
       <c r="F63" s="28"/>
     </row>
-    <row r="64" spans="1:9" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:9" ht="27" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B64" s="5" t="s">
         <v>220</v>
       </c>
@@ -5072,7 +5063,7 @@
       <c r="F64" s="27"/>
       <c r="I64" s="7"/>
     </row>
-    <row r="65" spans="3:6" ht="26" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="3:6" ht="26" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C65" s="27" t="s">
         <v>222</v>
       </c>
@@ -5099,16 +5090,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:I79"/>
   <sheetViews>
-    <sheetView topLeftCell="A44" zoomScale="56" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A31" zoomScale="108" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E66" sqref="E66:H66"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="2" max="2" width="54.69140625" style="23" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="54.6640625" style="23" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>33</v>
       </c>
@@ -5137,7 +5128,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A2" s="4" t="s">
         <v>59</v>
       </c>
@@ -5166,7 +5157,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A3" s="17" t="s">
         <v>330</v>
       </c>
@@ -5179,7 +5170,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A4" s="17" t="s">
         <v>332</v>
       </c>
@@ -5192,7 +5183,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A5" s="4" t="s">
         <v>62</v>
       </c>
@@ -5221,7 +5212,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A6" s="17" t="s">
         <v>337</v>
       </c>
@@ -5234,7 +5225,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A7" s="17" t="s">
         <v>338</v>
       </c>
@@ -5247,7 +5238,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A8" s="17" t="s">
         <v>339</v>
       </c>
@@ -5260,7 +5251,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A9" s="17" t="s">
         <v>340</v>
       </c>
@@ -5273,7 +5264,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A10" s="4" t="s">
         <v>64</v>
       </c>
@@ -5302,7 +5293,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A11" s="17" t="s">
         <v>345</v>
       </c>
@@ -5315,7 +5306,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A12" s="17" t="s">
         <v>346</v>
       </c>
@@ -5328,7 +5319,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" ht="28" x14ac:dyDescent="0.15">
       <c r="A13" s="17" t="s">
         <v>347</v>
       </c>
@@ -5341,7 +5332,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A14" s="4" t="s">
         <v>66</v>
       </c>
@@ -5370,7 +5361,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A15" s="17" t="s">
         <v>350</v>
       </c>
@@ -5383,7 +5374,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A16" s="17" t="s">
         <v>351</v>
       </c>
@@ -5396,7 +5387,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A17" s="17" t="s">
         <v>352</v>
       </c>
@@ -5409,7 +5400,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A18" s="4" t="s">
         <v>68</v>
       </c>
@@ -5438,7 +5429,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A19" s="17" t="s">
         <v>353</v>
       </c>
@@ -5451,7 +5442,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A20" s="17" t="s">
         <v>356</v>
       </c>
@@ -5464,7 +5455,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A21" s="4" t="s">
         <v>70</v>
       </c>
@@ -5493,7 +5484,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A22" s="17" t="s">
         <v>357</v>
       </c>
@@ -5506,7 +5497,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A23" s="17" t="s">
         <v>361</v>
       </c>
@@ -5519,7 +5510,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A24" s="17" t="s">
         <v>362</v>
       </c>
@@ -5532,7 +5523,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A25" s="4" t="s">
         <v>72</v>
       </c>
@@ -5561,7 +5552,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A26" t="s">
         <v>312</v>
       </c>
@@ -5578,7 +5569,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A27" t="s">
         <v>313</v>
       </c>
@@ -5595,7 +5586,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="28" spans="1:9" ht="27" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" ht="28" x14ac:dyDescent="0.15">
       <c r="A28" t="s">
         <v>315</v>
       </c>
@@ -5612,7 +5603,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A29" t="s">
         <v>317</v>
       </c>
@@ -5629,7 +5620,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="30" spans="1:9" ht="27" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" ht="28" x14ac:dyDescent="0.15">
       <c r="A30" t="s">
         <v>319</v>
       </c>
@@ -5646,7 +5637,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A31" t="s">
         <v>321</v>
       </c>
@@ -5663,7 +5654,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A32" s="4" t="s">
         <v>74</v>
       </c>
@@ -5692,7 +5683,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A33" t="s">
         <v>322</v>
       </c>
@@ -5709,7 +5700,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A34" t="s">
         <v>323</v>
       </c>
@@ -5726,7 +5717,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:9" ht="28" x14ac:dyDescent="0.15">
       <c r="A35" t="s">
         <v>324</v>
       </c>
@@ -5743,7 +5734,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="36" spans="1:9" ht="27" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:9" ht="28" x14ac:dyDescent="0.15">
       <c r="A36" t="s">
         <v>326</v>
       </c>
@@ -5760,7 +5751,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A37" t="s">
         <v>328</v>
       </c>
@@ -5777,7 +5768,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A38" s="4" t="s">
         <v>76</v>
       </c>
@@ -5791,7 +5782,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A39" t="s">
         <v>223</v>
       </c>
@@ -5820,7 +5811,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A40" t="s">
         <v>225</v>
       </c>
@@ -5837,7 +5828,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A41" t="s">
         <v>227</v>
       </c>
@@ -5854,7 +5845,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A42" t="s">
         <v>229</v>
       </c>
@@ -5871,7 +5862,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A43" t="s">
         <v>231</v>
       </c>
@@ -5888,7 +5879,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A44" t="s">
         <v>233</v>
       </c>
@@ -5905,7 +5896,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A45" t="s">
         <v>235</v>
       </c>
@@ -5922,7 +5913,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A46" t="s">
         <v>237</v>
       </c>
@@ -5939,7 +5930,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A47" t="s">
         <v>239</v>
       </c>
@@ -5956,7 +5947,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A48" t="s">
         <v>241</v>
       </c>
@@ -5973,7 +5964,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A49" t="s">
         <v>243</v>
       </c>
@@ -5990,7 +5981,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A50" t="s">
         <v>245</v>
       </c>
@@ -6007,7 +5998,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A51" t="s">
         <v>247</v>
       </c>
@@ -6024,7 +6015,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A52" t="s">
         <v>249</v>
       </c>
@@ -6041,7 +6032,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:9" ht="28" x14ac:dyDescent="0.15">
       <c r="A53" t="s">
         <v>251</v>
       </c>
@@ -6058,7 +6049,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A54" t="s">
         <v>253</v>
       </c>
@@ -6075,7 +6066,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A55" s="4" t="s">
         <v>78</v>
       </c>
@@ -6104,7 +6095,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A56" t="s">
         <v>255</v>
       </c>
@@ -6121,7 +6112,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A57" t="s">
         <v>257</v>
       </c>
@@ -6138,7 +6129,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A58" t="s">
         <v>258</v>
       </c>
@@ -6155,7 +6146,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A59" t="s">
         <v>259</v>
       </c>
@@ -6172,7 +6163,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A60" t="s">
         <v>260</v>
       </c>
@@ -6189,7 +6180,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A61" t="s">
         <v>261</v>
       </c>
@@ -6206,7 +6197,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A62" t="s">
         <v>262</v>
       </c>
@@ -6223,7 +6214,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A63" t="s">
         <v>367</v>
       </c>
@@ -6240,7 +6231,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A64" t="s">
         <v>368</v>
       </c>
@@ -6257,7 +6248,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A65" t="s">
         <v>369</v>
       </c>
@@ -6274,7 +6265,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A66" s="4" t="s">
         <v>214</v>
       </c>
@@ -6298,15 +6289,15 @@
         <v>600</v>
       </c>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="B72" s="5" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B73" s="5"/>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="B74" s="5" t="s">
         <v>216</v>
       </c>
@@ -6317,7 +6308,7 @@
       <c r="E74" s="26"/>
       <c r="F74" s="26"/>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B75" s="1"/>
       <c r="C75" s="26" t="s">
         <v>371</v>
@@ -6326,7 +6317,7 @@
       <c r="E75" s="26"/>
       <c r="F75" s="26"/>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B76" s="1"/>
       <c r="C76" s="26" t="s">
         <v>372</v>
@@ -6335,14 +6326,14 @@
       <c r="E76" s="26"/>
       <c r="F76" s="26"/>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B77" s="1"/>
       <c r="C77" s="28"/>
       <c r="D77" s="28"/>
       <c r="E77" s="28"/>
       <c r="F77" s="28"/>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="B78" s="5" t="s">
         <v>220</v>
       </c>
@@ -6353,7 +6344,7 @@
       <c r="E78" s="27"/>
       <c r="F78" s="27"/>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B79" s="1"/>
       <c r="C79" s="27" t="s">
         <v>374</v>
@@ -6381,17 +6372,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:I31"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="2" max="2" width="36.15234375" customWidth="1"/>
-    <col min="9" max="9" width="11.3828125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="36.1640625" customWidth="1"/>
+    <col min="9" max="9" width="12.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>33</v>
       </c>
@@ -6420,7 +6411,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="15" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" ht="17" x14ac:dyDescent="0.15">
       <c r="A2" s="4" t="s">
         <v>80</v>
       </c>
@@ -6443,7 +6434,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="15" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" ht="16" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>379</v>
       </c>
@@ -6453,7 +6444,7 @@
       <c r="C3" s="12"/>
       <c r="D3" s="17"/>
     </row>
-    <row r="4" spans="1:9" ht="15" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" ht="17" x14ac:dyDescent="0.15">
       <c r="A4" s="4" t="s">
         <v>82</v>
       </c>
@@ -6476,7 +6467,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="15" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" ht="16" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>380</v>
       </c>
@@ -6486,7 +6477,7 @@
       <c r="C5" s="12"/>
       <c r="D5" s="17"/>
     </row>
-    <row r="6" spans="1:9" ht="15" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" ht="16" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>381</v>
       </c>
@@ -6496,7 +6487,7 @@
       <c r="C6" s="12"/>
       <c r="D6" s="17"/>
     </row>
-    <row r="7" spans="1:9" ht="15" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" ht="17" x14ac:dyDescent="0.15">
       <c r="A7" s="4" t="s">
         <v>84</v>
       </c>
@@ -6519,7 +6510,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="15" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" ht="16" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>383</v>
       </c>
@@ -6529,7 +6520,7 @@
       <c r="C8" s="12"/>
       <c r="D8" s="17"/>
     </row>
-    <row r="9" spans="1:9" ht="15" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" ht="16" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
         <v>384</v>
       </c>
@@ -6539,7 +6530,7 @@
       <c r="C9" s="12"/>
       <c r="D9" s="17"/>
     </row>
-    <row r="10" spans="1:9" ht="15" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" ht="17" x14ac:dyDescent="0.15">
       <c r="A10" s="4" t="s">
         <v>86</v>
       </c>
@@ -6562,7 +6553,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="15" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" ht="16" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
         <v>386</v>
       </c>
@@ -6572,7 +6563,7 @@
       <c r="C11" s="12"/>
       <c r="D11" s="17"/>
     </row>
-    <row r="12" spans="1:9" ht="15" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" ht="16" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
         <v>387</v>
       </c>
@@ -6582,7 +6573,7 @@
       <c r="C12" s="12"/>
       <c r="D12" s="17"/>
     </row>
-    <row r="13" spans="1:9" ht="15" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" ht="17" x14ac:dyDescent="0.15">
       <c r="A13" s="4" t="s">
         <v>88</v>
       </c>
@@ -6605,7 +6596,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="15" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" ht="16" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
         <v>389</v>
       </c>
@@ -6615,7 +6606,7 @@
       <c r="C14" s="12"/>
       <c r="D14" s="17"/>
     </row>
-    <row r="15" spans="1:9" ht="15" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" ht="16" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
         <v>390</v>
       </c>
@@ -6625,7 +6616,7 @@
       <c r="C15" s="12"/>
       <c r="D15" s="17"/>
     </row>
-    <row r="16" spans="1:9" ht="15" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" ht="17" x14ac:dyDescent="0.15">
       <c r="A16" s="4" t="s">
         <v>90</v>
       </c>
@@ -6648,7 +6639,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="15" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" ht="16" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
         <v>392</v>
       </c>
@@ -6658,7 +6649,7 @@
       <c r="C17" s="12"/>
       <c r="D17" s="17"/>
     </row>
-    <row r="18" spans="1:9" ht="15" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" ht="16" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
         <v>393</v>
       </c>
@@ -6668,7 +6659,7 @@
       <c r="C18" s="12"/>
       <c r="D18" s="17"/>
     </row>
-    <row r="19" spans="1:9" ht="15" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" ht="17" x14ac:dyDescent="0.15">
       <c r="A19" s="4" t="s">
         <v>92</v>
       </c>
@@ -6687,11 +6678,17 @@
       <c r="F19">
         <v>60</v>
       </c>
+      <c r="G19">
+        <v>23</v>
+      </c>
+      <c r="H19">
+        <v>60</v>
+      </c>
       <c r="I19" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" ht="15" x14ac:dyDescent="0.3">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="16" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
         <v>394</v>
       </c>
@@ -6700,8 +6697,11 @@
       </c>
       <c r="C20" s="12"/>
       <c r="D20" s="17"/>
-    </row>
-    <row r="21" spans="1:9" ht="15" x14ac:dyDescent="0.3">
+      <c r="I20" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="16" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
         <v>395</v>
       </c>
@@ -6710,8 +6710,11 @@
       </c>
       <c r="C21" s="12"/>
       <c r="D21" s="17"/>
-    </row>
-    <row r="22" spans="1:9" ht="15" x14ac:dyDescent="0.3">
+      <c r="I21" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="17" x14ac:dyDescent="0.15">
       <c r="A22" s="4" t="s">
         <v>94</v>
       </c>
@@ -6730,11 +6733,17 @@
       <c r="F22">
         <v>60</v>
       </c>
+      <c r="G22">
+        <v>44</v>
+      </c>
+      <c r="H22">
+        <v>90</v>
+      </c>
       <c r="I22" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" ht="15" x14ac:dyDescent="0.3">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="16" x14ac:dyDescent="0.15">
       <c r="A23" t="s">
         <v>396</v>
       </c>
@@ -6743,8 +6752,11 @@
       </c>
       <c r="C23" s="12"/>
       <c r="D23" s="17"/>
-    </row>
-    <row r="24" spans="1:9" ht="15" x14ac:dyDescent="0.3">
+      <c r="I23" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="16" x14ac:dyDescent="0.15">
       <c r="A24" t="s">
         <v>397</v>
       </c>
@@ -6753,8 +6765,11 @@
       </c>
       <c r="C24" s="12"/>
       <c r="D24" s="17"/>
-    </row>
-    <row r="25" spans="1:9" ht="15" x14ac:dyDescent="0.3">
+      <c r="I24" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="17" x14ac:dyDescent="0.15">
       <c r="A25" s="4" t="s">
         <v>96</v>
       </c>
@@ -6783,7 +6798,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="15" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" ht="16" x14ac:dyDescent="0.15">
       <c r="A26" t="s">
         <v>398</v>
       </c>
@@ -6796,7 +6811,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="27" spans="1:9" ht="15" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" ht="16" x14ac:dyDescent="0.15">
       <c r="A27" t="s">
         <v>399</v>
       </c>
@@ -6809,7 +6824,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="28" spans="1:9" ht="15" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" ht="17" x14ac:dyDescent="0.15">
       <c r="A28" s="4" t="s">
         <v>98</v>
       </c>
@@ -6838,7 +6853,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A29" t="s">
         <v>400</v>
       </c>
@@ -6849,7 +6864,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A30" t="s">
         <v>401</v>
       </c>
@@ -6860,7 +6875,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A31" s="4" t="s">
         <v>214</v>
       </c>
@@ -6874,11 +6889,11 @@
       </c>
       <c r="G31">
         <f t="shared" si="0"/>
-        <v>36</v>
+        <v>103</v>
       </c>
       <c r="H31">
         <f t="shared" si="0"/>
-        <v>60</v>
+        <v>210</v>
       </c>
     </row>
   </sheetData>
@@ -6896,9 +6911,9 @@
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="28" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>33</v>
       </c>
@@ -6937,17 +6952,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:C43"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView topLeftCell="A25" zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="2" max="2" width="28.15234375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="49.4609375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="28.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="49.5" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" s="4" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>263</v>
       </c>
@@ -6958,7 +6973,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>37</v>
       </c>
@@ -6969,7 +6984,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" ht="17" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>40</v>
       </c>
@@ -6980,7 +6995,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="17" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>43</v>
       </c>
@@ -6991,7 +7006,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>45</v>
       </c>
@@ -7002,7 +7017,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>47</v>
       </c>
@@ -7013,7 +7028,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" ht="17" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
         <v>49</v>
       </c>
@@ -7024,7 +7039,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="45" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" ht="51" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>51</v>
       </c>
@@ -7035,7 +7050,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
         <v>53</v>
       </c>
@@ -7046,7 +7061,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>55</v>
       </c>
@@ -7057,7 +7072,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" ht="51" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
         <v>57</v>
       </c>
@@ -7068,7 +7083,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
         <v>59</v>
       </c>
@@ -7079,7 +7094,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="45" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" ht="51" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
         <v>62</v>
       </c>
@@ -7090,7 +7105,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="45" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" ht="68" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
         <v>64</v>
       </c>
@@ -7101,7 +7116,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
         <v>66</v>
       </c>
@@ -7112,7 +7127,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" ht="17" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
         <v>68</v>
       </c>
@@ -7123,7 +7138,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
         <v>70</v>
       </c>
@@ -7134,7 +7149,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" ht="17" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
         <v>72</v>
       </c>
@@ -7145,7 +7160,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" ht="17" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
         <v>74</v>
       </c>
@@ -7156,7 +7171,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" ht="17" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
         <v>76</v>
       </c>
@@ -7167,7 +7182,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
         <v>78</v>
       </c>
@@ -7178,7 +7193,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A22" t="s">
         <v>80</v>
       </c>
@@ -7189,7 +7204,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A23" t="s">
         <v>82</v>
       </c>
@@ -7200,7 +7215,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A24" t="s">
         <v>84</v>
       </c>
@@ -7211,7 +7226,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="45" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" ht="51" x14ac:dyDescent="0.15">
       <c r="A25" t="s">
         <v>86</v>
       </c>
@@ -7222,7 +7237,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A26" t="s">
         <v>88</v>
       </c>
@@ -7233,7 +7248,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="105" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" ht="136" x14ac:dyDescent="0.15">
       <c r="A27" t="s">
         <v>90</v>
       </c>
@@ -7244,7 +7259,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A28" t="s">
         <v>92</v>
       </c>
@@ -7255,7 +7270,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A29" t="s">
         <v>94</v>
       </c>
@@ -7266,7 +7281,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" ht="17" x14ac:dyDescent="0.15">
       <c r="A30" t="s">
         <v>96</v>
       </c>
@@ -7277,7 +7292,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" ht="17" x14ac:dyDescent="0.15">
       <c r="A31" t="s">
         <v>98</v>
       </c>
@@ -7288,7 +7303,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A32" t="s">
         <v>100</v>
       </c>
@@ -7299,7 +7314,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" ht="17" x14ac:dyDescent="0.15">
       <c r="A33" t="s">
         <v>102</v>
       </c>
@@ -7310,7 +7325,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A34" t="s">
         <v>104</v>
       </c>
@@ -7321,7 +7336,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" ht="51" x14ac:dyDescent="0.15">
       <c r="A35" t="s">
         <v>106</v>
       </c>
@@ -7332,7 +7347,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A36" t="s">
         <v>108</v>
       </c>
@@ -7343,7 +7358,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A37" t="s">
         <v>110</v>
       </c>
@@ -7354,7 +7369,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A38" t="s">
         <v>112</v>
       </c>
@@ -7365,7 +7380,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A39" t="s">
         <v>114</v>
       </c>
@@ -7376,7 +7391,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A40" t="s">
         <v>116</v>
       </c>
@@ -7387,7 +7402,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A41" t="s">
         <v>118</v>
       </c>
@@ -7398,7 +7413,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A42" t="s">
         <v>306</v>
       </c>
@@ -7409,7 +7424,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A43" t="s">
         <v>309</v>
       </c>

</xml_diff>

<commit_message>
Added sprint3 retrospective and sprint4 planning
Added sprint3 retrospective and sprint4 planning
</commit_message>
<xml_diff>
--- a/Team2Report.xlsx
+++ b/Team2Report.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/srikanth/Documenta/StevensInstitute/SoftwareEngg/SSW-555/SSW-555Project/Agile_Methods_Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1996D1C6-096A-7140-B9C2-66E116EC7EC4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02CC102D-AFCA-0143-A502-15EEAFF6E2CD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7900" yWindow="2660" windowWidth="26580" windowHeight="15900" tabRatio="500" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1057" uniqueCount="412">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1169" uniqueCount="458">
   <si>
     <t>Initials</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -1292,6 +1292,144 @@
   </si>
   <si>
     <t>Check if they are living</t>
+  </si>
+  <si>
+    <t>1: Keep doing the code commits before the meetings</t>
+  </si>
+  <si>
+    <t>2: Make acceptance GED file prior to meetings</t>
+  </si>
+  <si>
+    <t>3: Review each others code</t>
+  </si>
+  <si>
+    <t>1: Avoid bad commenting</t>
+  </si>
+  <si>
+    <t>2: Avoid unused variables</t>
+  </si>
+  <si>
+    <t>T31.01</t>
+  </si>
+  <si>
+    <t>T31.02</t>
+  </si>
+  <si>
+    <t>Fecth individual age &amp; marriage</t>
+  </si>
+  <si>
+    <t>Print list of all living non married above 30yrs old</t>
+  </si>
+  <si>
+    <t>Fetch all children with in a family</t>
+  </si>
+  <si>
+    <t>Check if any child in a family has same birthday</t>
+  </si>
+  <si>
+    <t>T32.01</t>
+  </si>
+  <si>
+    <t>T33.01</t>
+  </si>
+  <si>
+    <t>Find all families with children</t>
+  </si>
+  <si>
+    <t>T33.02</t>
+  </si>
+  <si>
+    <t>Check if a child's parents are died</t>
+  </si>
+  <si>
+    <t>Get all families</t>
+  </si>
+  <si>
+    <t>Check if spouses have double ages</t>
+  </si>
+  <si>
+    <t>T34.01</t>
+  </si>
+  <si>
+    <t>T34.02</t>
+  </si>
+  <si>
+    <t>List the individuals</t>
+  </si>
+  <si>
+    <t>T35.01</t>
+  </si>
+  <si>
+    <t>T35.02</t>
+  </si>
+  <si>
+    <t>Check if an individual died</t>
+  </si>
+  <si>
+    <t>Check if deceased individual died within 30 days</t>
+  </si>
+  <si>
+    <t>T36.01</t>
+  </si>
+  <si>
+    <t>T36.02</t>
+  </si>
+  <si>
+    <t>T37.01</t>
+  </si>
+  <si>
+    <t>T37.02</t>
+  </si>
+  <si>
+    <t>T38.01</t>
+  </si>
+  <si>
+    <t>T38.02</t>
+  </si>
+  <si>
+    <t>Get all the Spouses of family</t>
+  </si>
+  <si>
+    <t>Check if a spouse is deceased within 30 days</t>
+  </si>
+  <si>
+    <t>T37.03</t>
+  </si>
+  <si>
+    <t>List all widows</t>
+  </si>
+  <si>
+    <t>Check if an individual's birth is within 30 days</t>
+  </si>
+  <si>
+    <t>Check if an individual's birthday is within 30 days</t>
+  </si>
+  <si>
+    <t>Check married families</t>
+  </si>
+  <si>
+    <t>Check if marriage anniversary is within 30 days</t>
+  </si>
+  <si>
+    <t>T39.01</t>
+  </si>
+  <si>
+    <t>T39.02</t>
+  </si>
+  <si>
+    <t>T40.01</t>
+  </si>
+  <si>
+    <t>T40.02</t>
+  </si>
+  <si>
+    <t>Insert the line number before reporting an error</t>
+  </si>
+  <si>
+    <t>Get the line number of a GED file</t>
+  </si>
+  <si>
+    <t>T32.02</t>
   </si>
 </sst>
 </file>
@@ -1357,7 +1495,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -1378,6 +1516,15 @@
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -1449,7 +1596,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1509,6 +1656,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="66">
     <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
@@ -3555,8 +3716,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="150" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+    <sheetView topLeftCell="A5" zoomScale="150" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -3749,7 +3910,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="G34" sqref="G34"/>
+      <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -3848,8 +4009,8 @@
         <v>600</v>
       </c>
       <c r="F4" s="9">
-        <f>(D4-D3)/E4*60</f>
-        <v>-6.9</v>
+        <f>((D3+D4)-D3)/E4*60</f>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.15">
@@ -3865,15 +4026,15 @@
       </c>
       <c r="D5">
         <f>Sprint3!G31</f>
-        <v>103</v>
+        <v>273</v>
       </c>
       <c r="E5">
         <f>Sprint3!H31</f>
-        <v>210</v>
+        <v>660</v>
       </c>
       <c r="F5" s="9">
-        <f>(D5-D4)/E5*60</f>
-        <v>-64.857142857142847</v>
+        <f>((D4+D5)-D4)/E5*60</f>
+        <v>24.818181818181817</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.15">
@@ -3893,7 +4054,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:I65"/>
   <sheetViews>
-    <sheetView zoomScale="109" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView topLeftCell="A36" zoomScale="109" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="H55" sqref="H55"/>
     </sheetView>
   </sheetViews>
@@ -5090,8 +5251,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:I79"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" zoomScale="108" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E66" sqref="E66:H66"/>
+    <sheetView topLeftCell="A56" zoomScale="108" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F87" sqref="F87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -6301,12 +6462,13 @@
       <c r="B74" s="5" t="s">
         <v>216</v>
       </c>
-      <c r="C74" s="26" t="s">
+      <c r="C74" s="33" t="s">
         <v>375</v>
       </c>
-      <c r="D74" s="26"/>
-      <c r="E74" s="26"/>
-      <c r="F74" s="26"/>
+      <c r="D74" s="34"/>
+      <c r="E74" s="34"/>
+      <c r="F74" s="34"/>
+      <c r="G74" s="34"/>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B75" s="1"/>
@@ -6354,9 +6516,8 @@
       <c r="F79" s="27"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="5">
     <mergeCell ref="C79:F79"/>
-    <mergeCell ref="C74:F74"/>
     <mergeCell ref="C75:F75"/>
     <mergeCell ref="C76:F76"/>
     <mergeCell ref="C77:F77"/>
@@ -6370,10 +6531,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:I31"/>
+  <dimension ref="A1:I45"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+    <sheetView topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E49" sqref="E49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -6430,8 +6591,14 @@
       <c r="F2">
         <v>30</v>
       </c>
+      <c r="G2">
+        <v>25</v>
+      </c>
+      <c r="H2">
+        <v>30</v>
+      </c>
       <c r="I2" t="s">
-        <v>376</v>
+        <v>143</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="16" x14ac:dyDescent="0.15">
@@ -6443,6 +6610,9 @@
       </c>
       <c r="C3" s="12"/>
       <c r="D3" s="17"/>
+      <c r="I3" t="s">
+        <v>370</v>
+      </c>
     </row>
     <row r="4" spans="1:9" ht="17" x14ac:dyDescent="0.15">
       <c r="A4" s="4" t="s">
@@ -6463,8 +6633,14 @@
       <c r="F4">
         <v>30</v>
       </c>
+      <c r="G4">
+        <v>29</v>
+      </c>
+      <c r="H4">
+        <v>30</v>
+      </c>
       <c r="I4" t="s">
-        <v>376</v>
+        <v>143</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="16" x14ac:dyDescent="0.15">
@@ -6476,6 +6652,9 @@
       </c>
       <c r="C5" s="12"/>
       <c r="D5" s="17"/>
+      <c r="I5" t="s">
+        <v>370</v>
+      </c>
     </row>
     <row r="6" spans="1:9" ht="16" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
@@ -6486,6 +6665,9 @@
       </c>
       <c r="C6" s="12"/>
       <c r="D6" s="17"/>
+      <c r="I6" t="s">
+        <v>370</v>
+      </c>
     </row>
     <row r="7" spans="1:9" ht="17" x14ac:dyDescent="0.15">
       <c r="A7" s="4" t="s">
@@ -6506,8 +6688,14 @@
       <c r="F7">
         <v>90</v>
       </c>
+      <c r="G7">
+        <v>27</v>
+      </c>
+      <c r="H7">
+        <v>120</v>
+      </c>
       <c r="I7" t="s">
-        <v>376</v>
+        <v>143</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="16" x14ac:dyDescent="0.15">
@@ -6519,6 +6707,9 @@
       </c>
       <c r="C8" s="12"/>
       <c r="D8" s="17"/>
+      <c r="I8" t="s">
+        <v>370</v>
+      </c>
     </row>
     <row r="9" spans="1:9" ht="16" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
@@ -6529,6 +6720,9 @@
       </c>
       <c r="C9" s="12"/>
       <c r="D9" s="17"/>
+      <c r="I9" t="s">
+        <v>370</v>
+      </c>
     </row>
     <row r="10" spans="1:9" ht="17" x14ac:dyDescent="0.15">
       <c r="A10" s="4" t="s">
@@ -6549,8 +6743,14 @@
       <c r="F10">
         <v>90</v>
       </c>
+      <c r="G10">
+        <v>28</v>
+      </c>
+      <c r="H10">
+        <v>60</v>
+      </c>
       <c r="I10" t="s">
-        <v>376</v>
+        <v>143</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="16" x14ac:dyDescent="0.15">
@@ -6562,6 +6762,9 @@
       </c>
       <c r="C11" s="12"/>
       <c r="D11" s="17"/>
+      <c r="I11" t="s">
+        <v>370</v>
+      </c>
     </row>
     <row r="12" spans="1:9" ht="16" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
@@ -6572,6 +6775,9 @@
       </c>
       <c r="C12" s="12"/>
       <c r="D12" s="17"/>
+      <c r="I12" t="s">
+        <v>370</v>
+      </c>
     </row>
     <row r="13" spans="1:9" ht="17" x14ac:dyDescent="0.15">
       <c r="A13" s="4" t="s">
@@ -6592,8 +6798,14 @@
       <c r="F13">
         <v>60</v>
       </c>
+      <c r="G13">
+        <v>22</v>
+      </c>
+      <c r="H13">
+        <v>60</v>
+      </c>
       <c r="I13" t="s">
-        <v>376</v>
+        <v>143</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="16" x14ac:dyDescent="0.15">
@@ -6605,6 +6817,9 @@
       </c>
       <c r="C14" s="12"/>
       <c r="D14" s="17"/>
+      <c r="I14" t="s">
+        <v>370</v>
+      </c>
     </row>
     <row r="15" spans="1:9" ht="16" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
@@ -6615,6 +6830,9 @@
       </c>
       <c r="C15" s="12"/>
       <c r="D15" s="17"/>
+      <c r="I15" t="s">
+        <v>370</v>
+      </c>
     </row>
     <row r="16" spans="1:9" ht="17" x14ac:dyDescent="0.15">
       <c r="A16" s="4" t="s">
@@ -6635,8 +6853,14 @@
       <c r="F16">
         <v>60</v>
       </c>
+      <c r="G16">
+        <v>39</v>
+      </c>
+      <c r="H16">
+        <v>150</v>
+      </c>
       <c r="I16" t="s">
-        <v>376</v>
+        <v>143</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="16" x14ac:dyDescent="0.15">
@@ -6648,6 +6872,9 @@
       </c>
       <c r="C17" s="12"/>
       <c r="D17" s="17"/>
+      <c r="I17" t="s">
+        <v>370</v>
+      </c>
     </row>
     <row r="18" spans="1:9" ht="16" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
@@ -6658,6 +6885,9 @@
       </c>
       <c r="C18" s="12"/>
       <c r="D18" s="17"/>
+      <c r="I18" t="s">
+        <v>370</v>
+      </c>
     </row>
     <row r="19" spans="1:9" ht="17" x14ac:dyDescent="0.15">
       <c r="A19" s="4" t="s">
@@ -6889,14 +7119,93 @@
       </c>
       <c r="G31">
         <f t="shared" si="0"/>
-        <v>103</v>
+        <v>273</v>
       </c>
       <c r="H31">
         <f t="shared" si="0"/>
-        <v>210</v>
-      </c>
+        <v>660</v>
+      </c>
+    </row>
+    <row r="37" spans="2:7" ht="14" x14ac:dyDescent="0.15">
+      <c r="B37" s="5" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="38" spans="2:7" x14ac:dyDescent="0.15">
+      <c r="B38" s="5"/>
+    </row>
+    <row r="39" spans="2:7" ht="14" x14ac:dyDescent="0.15">
+      <c r="B39" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="C39" s="26" t="s">
+        <v>412</v>
+      </c>
+      <c r="D39" s="26"/>
+      <c r="E39" s="26"/>
+      <c r="F39" s="26"/>
+      <c r="G39" s="26"/>
+    </row>
+    <row r="40" spans="2:7" x14ac:dyDescent="0.15">
+      <c r="B40" s="1"/>
+      <c r="C40" s="29" t="s">
+        <v>413</v>
+      </c>
+      <c r="D40" s="29"/>
+      <c r="E40" s="29"/>
+      <c r="F40" s="29"/>
+      <c r="G40" s="29"/>
+    </row>
+    <row r="41" spans="2:7" x14ac:dyDescent="0.15">
+      <c r="B41" s="1"/>
+      <c r="C41" s="29" t="s">
+        <v>414</v>
+      </c>
+      <c r="D41" s="29"/>
+      <c r="E41" s="29"/>
+      <c r="F41" s="29"/>
+      <c r="G41" s="29"/>
+    </row>
+    <row r="42" spans="2:7" x14ac:dyDescent="0.15">
+      <c r="B42" s="1"/>
+      <c r="C42" s="30"/>
+      <c r="D42" s="31"/>
+      <c r="E42" s="31"/>
+      <c r="F42" s="31"/>
+      <c r="G42" s="31"/>
+    </row>
+    <row r="43" spans="2:7" ht="14" x14ac:dyDescent="0.15">
+      <c r="B43" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="C43" s="27" t="s">
+        <v>415</v>
+      </c>
+      <c r="D43" s="27"/>
+      <c r="E43" s="27"/>
+      <c r="F43" s="27"/>
+    </row>
+    <row r="44" spans="2:7" x14ac:dyDescent="0.15">
+      <c r="B44" s="1"/>
+      <c r="C44" s="32" t="s">
+        <v>416</v>
+      </c>
+      <c r="D44" s="27"/>
+      <c r="E44" s="27"/>
+      <c r="F44" s="27"/>
+    </row>
+    <row r="45" spans="2:7" x14ac:dyDescent="0.15">
+      <c r="B45" s="23"/>
     </row>
   </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="C43:F43"/>
+    <mergeCell ref="C44:F44"/>
+    <mergeCell ref="C39:G39"/>
+    <mergeCell ref="C40:G40"/>
+    <mergeCell ref="C42:G42"/>
+    <mergeCell ref="C41:G41"/>
+  </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -6905,13 +7214,16 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:I33"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M20" sqref="M20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="2" max="2" width="28.5" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="28" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
@@ -6940,6 +7252,463 @@
       </c>
       <c r="I1" s="10" t="s">
         <v>142</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="17" x14ac:dyDescent="0.15">
+      <c r="A2" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="B2" s="23" t="s">
+        <v>101</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="E2">
+        <v>25</v>
+      </c>
+      <c r="F2">
+        <v>30</v>
+      </c>
+      <c r="I2" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="16" x14ac:dyDescent="0.15">
+      <c r="A3" t="s">
+        <v>417</v>
+      </c>
+      <c r="B3" s="23" t="s">
+        <v>419</v>
+      </c>
+      <c r="C3" s="12"/>
+      <c r="D3" s="17"/>
+    </row>
+    <row r="4" spans="1:9" ht="28" x14ac:dyDescent="0.15">
+      <c r="A4" t="s">
+        <v>418</v>
+      </c>
+      <c r="B4" s="23" t="s">
+        <v>420</v>
+      </c>
+      <c r="C4" s="12"/>
+      <c r="D4" s="17"/>
+    </row>
+    <row r="5" spans="1:9" ht="17" x14ac:dyDescent="0.15">
+      <c r="A5" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="B5" s="23" t="s">
+        <v>103</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="E5">
+        <v>25</v>
+      </c>
+      <c r="F5">
+        <v>30</v>
+      </c>
+      <c r="I5" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="28" x14ac:dyDescent="0.15">
+      <c r="A6" t="s">
+        <v>423</v>
+      </c>
+      <c r="B6" s="23" t="s">
+        <v>421</v>
+      </c>
+      <c r="C6" s="12"/>
+      <c r="D6" s="17"/>
+    </row>
+    <row r="7" spans="1:9" ht="28" x14ac:dyDescent="0.15">
+      <c r="A7" s="17" t="s">
+        <v>457</v>
+      </c>
+      <c r="B7" s="23" t="s">
+        <v>422</v>
+      </c>
+      <c r="C7" s="12"/>
+      <c r="D7" s="17"/>
+    </row>
+    <row r="8" spans="1:9" ht="17" x14ac:dyDescent="0.15">
+      <c r="A8" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="B8" s="23" t="s">
+        <v>105</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="E8">
+        <v>60</v>
+      </c>
+      <c r="F8">
+        <v>120</v>
+      </c>
+      <c r="I8" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="16" x14ac:dyDescent="0.15">
+      <c r="A9" t="s">
+        <v>424</v>
+      </c>
+      <c r="B9" s="23" t="s">
+        <v>425</v>
+      </c>
+      <c r="C9" s="12"/>
+      <c r="D9" s="17"/>
+    </row>
+    <row r="10" spans="1:9" ht="28" x14ac:dyDescent="0.15">
+      <c r="A10" t="s">
+        <v>426</v>
+      </c>
+      <c r="B10" s="23" t="s">
+        <v>427</v>
+      </c>
+      <c r="C10" s="12"/>
+      <c r="D10" s="17"/>
+    </row>
+    <row r="11" spans="1:9" ht="17" x14ac:dyDescent="0.15">
+      <c r="A11" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="B11" s="23" t="s">
+        <v>107</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="E11">
+        <v>60</v>
+      </c>
+      <c r="F11">
+        <v>60</v>
+      </c>
+      <c r="I11" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="16" x14ac:dyDescent="0.15">
+      <c r="A12" t="s">
+        <v>430</v>
+      </c>
+      <c r="B12" s="23" t="s">
+        <v>428</v>
+      </c>
+      <c r="C12" s="12"/>
+      <c r="D12" s="17"/>
+    </row>
+    <row r="13" spans="1:9" ht="28" x14ac:dyDescent="0.15">
+      <c r="A13" t="s">
+        <v>431</v>
+      </c>
+      <c r="B13" s="23" t="s">
+        <v>429</v>
+      </c>
+      <c r="C13" s="12"/>
+      <c r="D13" s="17"/>
+    </row>
+    <row r="14" spans="1:9" ht="17" x14ac:dyDescent="0.15">
+      <c r="A14" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="B14" s="23" t="s">
+        <v>109</v>
+      </c>
+      <c r="C14" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="D14" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="E14">
+        <v>45</v>
+      </c>
+      <c r="F14">
+        <v>60</v>
+      </c>
+      <c r="I14" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="28" x14ac:dyDescent="0.15">
+      <c r="A15" t="s">
+        <v>433</v>
+      </c>
+      <c r="B15" s="23" t="s">
+        <v>447</v>
+      </c>
+      <c r="C15" s="12"/>
+      <c r="D15" s="17"/>
+    </row>
+    <row r="16" spans="1:9" ht="16" x14ac:dyDescent="0.15">
+      <c r="A16" t="s">
+        <v>434</v>
+      </c>
+      <c r="B16" s="23" t="s">
+        <v>432</v>
+      </c>
+      <c r="C16" s="12"/>
+      <c r="D16" s="17"/>
+    </row>
+    <row r="17" spans="1:9" ht="17" x14ac:dyDescent="0.15">
+      <c r="A17" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="B17" s="23" t="s">
+        <v>111</v>
+      </c>
+      <c r="C17" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="D17" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="E17">
+        <v>45</v>
+      </c>
+      <c r="F17">
+        <v>60</v>
+      </c>
+      <c r="I17" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="16" x14ac:dyDescent="0.15">
+      <c r="A18" t="s">
+        <v>437</v>
+      </c>
+      <c r="B18" s="23" t="s">
+        <v>435</v>
+      </c>
+      <c r="C18" s="12"/>
+      <c r="D18" s="17"/>
+    </row>
+    <row r="19" spans="1:9" ht="28" x14ac:dyDescent="0.15">
+      <c r="A19" t="s">
+        <v>438</v>
+      </c>
+      <c r="B19" s="23" t="s">
+        <v>436</v>
+      </c>
+      <c r="C19" s="12"/>
+      <c r="D19" s="17"/>
+    </row>
+    <row r="20" spans="1:9" ht="17" x14ac:dyDescent="0.15">
+      <c r="A20" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="B20" s="23" t="s">
+        <v>113</v>
+      </c>
+      <c r="C20" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="D20" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="E20">
+        <v>45</v>
+      </c>
+      <c r="F20">
+        <v>90</v>
+      </c>
+      <c r="I20" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="16" x14ac:dyDescent="0.15">
+      <c r="A21" t="s">
+        <v>439</v>
+      </c>
+      <c r="B21" s="23" t="s">
+        <v>443</v>
+      </c>
+      <c r="C21" s="12"/>
+      <c r="D21" s="17"/>
+    </row>
+    <row r="22" spans="1:9" ht="28" x14ac:dyDescent="0.15">
+      <c r="A22" t="s">
+        <v>440</v>
+      </c>
+      <c r="B22" s="23" t="s">
+        <v>444</v>
+      </c>
+      <c r="C22" s="12"/>
+      <c r="D22" s="17"/>
+    </row>
+    <row r="23" spans="1:9" ht="16" x14ac:dyDescent="0.15">
+      <c r="A23" t="s">
+        <v>445</v>
+      </c>
+      <c r="B23" s="23" t="s">
+        <v>446</v>
+      </c>
+      <c r="C23" s="12"/>
+      <c r="D23" s="17"/>
+    </row>
+    <row r="24" spans="1:9" ht="17" x14ac:dyDescent="0.15">
+      <c r="A24" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="B24" s="23" t="s">
+        <v>115</v>
+      </c>
+      <c r="C24" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="D24" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="E24">
+        <v>50</v>
+      </c>
+      <c r="F24">
+        <v>90</v>
+      </c>
+      <c r="I24" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="28" x14ac:dyDescent="0.15">
+      <c r="A25" t="s">
+        <v>441</v>
+      </c>
+      <c r="B25" s="23" t="s">
+        <v>448</v>
+      </c>
+      <c r="C25" s="12"/>
+      <c r="D25" s="17"/>
+    </row>
+    <row r="26" spans="1:9" ht="16" x14ac:dyDescent="0.15">
+      <c r="A26" t="s">
+        <v>442</v>
+      </c>
+      <c r="B26" s="23" t="s">
+        <v>432</v>
+      </c>
+      <c r="C26" s="12"/>
+      <c r="D26" s="17"/>
+    </row>
+    <row r="27" spans="1:9" ht="17" x14ac:dyDescent="0.15">
+      <c r="A27" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="B27" s="23" t="s">
+        <v>117</v>
+      </c>
+      <c r="C27" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="D27" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="E27">
+        <v>20</v>
+      </c>
+      <c r="F27">
+        <v>30</v>
+      </c>
+      <c r="I27" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="16" x14ac:dyDescent="0.15">
+      <c r="A28" t="s">
+        <v>451</v>
+      </c>
+      <c r="B28" s="23" t="s">
+        <v>449</v>
+      </c>
+      <c r="C28" s="12"/>
+      <c r="D28" s="17"/>
+    </row>
+    <row r="29" spans="1:9" ht="28" x14ac:dyDescent="0.15">
+      <c r="A29" t="s">
+        <v>452</v>
+      </c>
+      <c r="B29" s="23" t="s">
+        <v>450</v>
+      </c>
+      <c r="C29" s="12"/>
+      <c r="D29" s="17"/>
+    </row>
+    <row r="30" spans="1:9" ht="17" x14ac:dyDescent="0.15">
+      <c r="A30" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="B30" s="23" t="s">
+        <v>119</v>
+      </c>
+      <c r="C30" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="D30" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="E30">
+        <v>55</v>
+      </c>
+      <c r="F30">
+        <v>80</v>
+      </c>
+      <c r="I30" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="28" x14ac:dyDescent="0.15">
+      <c r="A31" t="s">
+        <v>453</v>
+      </c>
+      <c r="B31" s="23" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" ht="28" x14ac:dyDescent="0.15">
+      <c r="A32" t="s">
+        <v>454</v>
+      </c>
+      <c r="B32" s="23" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A33" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="E33">
+        <f>SUM(E4:E32)</f>
+        <v>405</v>
+      </c>
+      <c r="F33">
+        <f t="shared" ref="F33:H33" si="0">SUM(F4:F32)</f>
+        <v>620</v>
+      </c>
+      <c r="G33">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H33">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -6952,8 +7721,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:C43"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView topLeftCell="A28" zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>

</xml_diff>

<commit_message>
updates to excel spreadsheet
</commit_message>
<xml_diff>
--- a/Team2Report.xlsx
+++ b/Team2Report.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11012"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23231"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/srikanth/Documenta/StevensInstitute/SoftwareEngg/SSW-555/SSW-555Project/Agile_Methods_Project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ztyle\Documents\SSW 555\SSW_555_Project_Master\Agile_Methods_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02CC102D-AFCA-0143-A502-15EEAFF6E2CD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB693E2D-2FC7-45EE-AB3F-9252597135E0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7900" yWindow="2660" windowWidth="26580" windowHeight="15900" tabRatio="500" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" firstSheet="2" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -23,10 +23,19 @@
     <sheet name="Sprint4" sheetId="6" r:id="rId8"/>
     <sheet name="Stories" sheetId="11" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -36,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1169" uniqueCount="458">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1173" uniqueCount="458">
   <si>
     <t>Initials</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -1644,6 +1653,8 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1657,6 +1668,9 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -1665,11 +1679,6 @@
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="66">
     <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
@@ -1779,7 +1788,7 @@
             <c:numRef>
               <c:f>'Burndown README'!$B$15:$B$20</c:f>
               <c:numCache>
-                <c:formatCode>m/d/yy</c:formatCode>
+                <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>42632</c:v>
@@ -1850,7 +1859,7 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="m/d/yy" sourceLinked="1"/>
+        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1916,7 +1925,7 @@
             <c:numRef>
               <c:f>Burndown!$A$2:$A$7</c:f>
               <c:numCache>
-                <c:formatCode>m/d/yy</c:formatCode>
+                <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>42632</c:v>
@@ -1954,6 +1963,9 @@
                 <c:pt idx="3">
                   <c:v>10</c:v>
                 </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1984,7 +1996,7 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="m/d/yy" sourceLinked="1"/>
+        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2846,16 +2858,16 @@
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.5" customWidth="1"/>
-    <col min="4" max="4" width="22.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.5" customWidth="1"/>
+    <col min="1" max="1" width="7.84375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.15234375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.4609375" customWidth="1"/>
+    <col min="4" max="4" width="22.84375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.4609375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -2872,7 +2884,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -2889,7 +2901,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -2906,7 +2918,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -2923,7 +2935,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -2940,7 +2952,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>25</v>
       </c>
@@ -2957,7 +2969,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D8" s="4" t="s">
         <v>30</v>
       </c>
@@ -2966,7 +2978,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:D4">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D4">
     <sortCondition ref="C2:C4"/>
   </sortState>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -2990,16 +3002,16 @@
       <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.84375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="29" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.4609375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.4609375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>32</v>
       </c>
@@ -3016,7 +3028,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -3033,7 +3045,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -3049,14 +3061,14 @@
       <c r="E3" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="G3" s="25" t="s">
+      <c r="G3" s="27" t="s">
         <v>42</v>
       </c>
-      <c r="H3" s="25"/>
-      <c r="I3" s="25"/>
-      <c r="J3" s="25"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="H3" s="27"/>
+      <c r="I3" s="27"/>
+      <c r="J3" s="27"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>1</v>
       </c>
@@ -3073,7 +3085,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>1</v>
       </c>
@@ -3090,7 +3102,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>1</v>
       </c>
@@ -3107,7 +3119,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>1</v>
       </c>
@@ -3124,7 +3136,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>1</v>
       </c>
@@ -3141,7 +3153,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>1</v>
       </c>
@@ -3158,7 +3170,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>1</v>
       </c>
@@ -3175,7 +3187,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>1</v>
       </c>
@@ -3192,7 +3204,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>2</v>
       </c>
@@ -3209,7 +3221,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>2</v>
       </c>
@@ -3226,7 +3238,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>2</v>
       </c>
@@ -3243,7 +3255,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>2</v>
       </c>
@@ -3260,7 +3272,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>2</v>
       </c>
@@ -3277,7 +3289,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>2</v>
       </c>
@@ -3294,7 +3306,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>2</v>
       </c>
@@ -3311,7 +3323,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>2</v>
       </c>
@@ -3328,7 +3340,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>2</v>
       </c>
@@ -3345,7 +3357,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>2</v>
       </c>
@@ -3362,7 +3374,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>3</v>
       </c>
@@ -3379,7 +3391,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>3</v>
       </c>
@@ -3396,7 +3408,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>3</v>
       </c>
@@ -3413,7 +3425,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>3</v>
       </c>
@@ -3430,7 +3442,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>3</v>
       </c>
@@ -3447,7 +3459,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>3</v>
       </c>
@@ -3464,7 +3476,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>3</v>
       </c>
@@ -3481,7 +3493,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>3</v>
       </c>
@@ -3498,7 +3510,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>3</v>
       </c>
@@ -3515,7 +3527,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>3</v>
       </c>
@@ -3532,7 +3544,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>4</v>
       </c>
@@ -3549,7 +3561,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>4</v>
       </c>
@@ -3566,7 +3578,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>4</v>
       </c>
@@ -3583,7 +3595,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>4</v>
       </c>
@@ -3600,7 +3612,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>4</v>
       </c>
@@ -3617,7 +3629,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>4</v>
       </c>
@@ -3634,7 +3646,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>4</v>
       </c>
@@ -3651,7 +3663,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>4</v>
       </c>
@@ -3668,7 +3680,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>4</v>
       </c>
@@ -3685,7 +3697,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>4</v>
       </c>
@@ -3720,47 +3732,47 @@
       <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="7"/>
-    <col min="2" max="2" width="10.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.33203125" customWidth="1"/>
-    <col min="5" max="5" width="6.83203125" customWidth="1"/>
-    <col min="6" max="6" width="12.5" style="9" customWidth="1"/>
+    <col min="1" max="1" width="10.84375" style="7"/>
+    <col min="2" max="2" width="10.15234375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.84375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.3046875" customWidth="1"/>
+    <col min="5" max="5" width="6.84375" customWidth="1"/>
+    <col min="6" max="6" width="12.4609375" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
         <v>126</v>
       </c>
@@ -3783,7 +3795,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>133</v>
       </c>
@@ -3799,7 +3811,7 @@
       <c r="F15" s="14"/>
       <c r="G15" s="9"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>134</v>
       </c>
@@ -3823,7 +3835,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
         <v>135</v>
       </c>
@@ -3848,7 +3860,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="7" t="s">
         <v>136</v>
       </c>
@@ -3873,7 +3885,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="7" t="s">
         <v>137</v>
       </c>
@@ -3909,21 +3921,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="E34" sqref="E34"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="2"/>
-    <col min="2" max="2" width="18.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.1640625" customWidth="1"/>
-    <col min="5" max="5" width="6.83203125" customWidth="1"/>
-    <col min="6" max="6" width="12.5" style="9" customWidth="1"/>
+    <col min="1" max="1" width="10.84375" style="2"/>
+    <col min="2" max="2" width="18.4609375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.4609375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.15234375" customWidth="1"/>
+    <col min="5" max="5" width="6.84375" customWidth="1"/>
+    <col min="6" max="6" width="12.4609375" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>127</v>
       </c>
@@ -3943,7 +3955,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="13">
         <v>42632</v>
       </c>
@@ -3963,7 +3975,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="13">
         <v>42647</v>
       </c>
@@ -3988,7 +4000,7 @@
         <v>34.695652173913047</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="13">
         <v>42668</v>
       </c>
@@ -4013,7 +4025,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="13">
         <v>42682</v>
       </c>
@@ -4037,9 +4049,27 @@
         <v>24.818181818181817</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="13">
         <v>42689</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>10</v>
+      </c>
+      <c r="D6">
+        <f>Sprint4!G33</f>
+        <v>101</v>
+      </c>
+      <c r="E6">
+        <f>Sprint4!H33</f>
+        <v>120</v>
+      </c>
+      <c r="F6" s="9">
+        <f>((D5+D6)-D5)/E6*60</f>
+        <v>50.5</v>
       </c>
     </row>
   </sheetData>
@@ -4058,19 +4088,19 @@
       <selection activeCell="H55" sqref="H55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="33" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.33203125" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.4609375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.4609375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.3046875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.69140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.4609375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.3046875" style="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>33</v>
       </c>
@@ -4099,7 +4129,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>37</v>
       </c>
@@ -4128,7 +4158,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="17" t="s">
         <v>144</v>
       </c>
@@ -4145,7 +4175,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="17" t="s">
         <v>147</v>
       </c>
@@ -4162,7 +4192,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="17" t="s">
         <v>149</v>
       </c>
@@ -4179,7 +4209,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>40</v>
       </c>
@@ -4208,7 +4238,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="17" t="s">
         <v>151</v>
       </c>
@@ -4225,7 +4255,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="17" t="s">
         <v>153</v>
       </c>
@@ -4242,7 +4272,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="17" t="s">
         <v>155</v>
       </c>
@@ -4259,7 +4289,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="17" t="s">
         <v>157</v>
       </c>
@@ -4276,7 +4306,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
         <v>43</v>
       </c>
@@ -4305,7 +4335,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="17" t="s">
         <v>159</v>
       </c>
@@ -4322,7 +4352,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="17" t="s">
         <v>161</v>
       </c>
@@ -4339,7 +4369,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="17" t="s">
         <v>162</v>
       </c>
@@ -4356,7 +4386,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="17" t="s">
         <v>164</v>
       </c>
@@ -4373,7 +4403,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
         <v>45</v>
       </c>
@@ -4402,7 +4432,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="17" t="s">
         <v>166</v>
       </c>
@@ -4419,7 +4449,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="17" t="s">
         <v>167</v>
       </c>
@@ -4436,7 +4466,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" s="17" t="s">
         <v>169</v>
       </c>
@@ -4453,7 +4483,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="17" t="s">
         <v>170</v>
       </c>
@@ -4470,7 +4500,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" s="17" t="s">
         <v>172</v>
       </c>
@@ -4487,7 +4517,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" s="4" t="s">
         <v>47</v>
       </c>
@@ -4516,7 +4546,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" s="17" t="s">
         <v>174</v>
       </c>
@@ -4533,7 +4563,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" s="17" t="s">
         <v>175</v>
       </c>
@@ -4550,7 +4580,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" s="17" t="s">
         <v>176</v>
       </c>
@@ -4567,7 +4597,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" s="17" t="s">
         <v>177</v>
       </c>
@@ -4584,7 +4614,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" s="17" t="s">
         <v>178</v>
       </c>
@@ -4601,7 +4631,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" s="4" t="s">
         <v>49</v>
       </c>
@@ -4630,7 +4660,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" s="17" t="s">
         <v>180</v>
       </c>
@@ -4647,7 +4677,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" s="17" t="s">
         <v>181</v>
       </c>
@@ -4664,7 +4694,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" s="17" t="s">
         <v>182</v>
       </c>
@@ -4681,7 +4711,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" s="17" t="s">
         <v>183</v>
       </c>
@@ -4698,7 +4728,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33" s="17" t="s">
         <v>184</v>
       </c>
@@ -4715,7 +4745,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34" s="4" t="s">
         <v>51</v>
       </c>
@@ -4744,7 +4774,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35" s="17" t="s">
         <v>186</v>
       </c>
@@ -4761,7 +4791,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A36" s="17" t="s">
         <v>187</v>
       </c>
@@ -4778,7 +4808,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A37" s="17" t="s">
         <v>189</v>
       </c>
@@ -4795,7 +4825,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A38" s="17" t="s">
         <v>191</v>
       </c>
@@ -4812,7 +4842,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A39" s="17" t="s">
         <v>192</v>
       </c>
@@ -4829,7 +4859,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A40" s="17" t="s">
         <v>194</v>
       </c>
@@ -4846,7 +4876,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A41" s="4" t="s">
         <v>53</v>
       </c>
@@ -4875,7 +4905,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A42" s="17" t="s">
         <v>196</v>
       </c>
@@ -4892,7 +4922,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A43" s="17" t="s">
         <v>197</v>
       </c>
@@ -4909,7 +4939,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A44" s="17" t="s">
         <v>198</v>
       </c>
@@ -4926,7 +4956,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A45" s="4" t="s">
         <v>55</v>
       </c>
@@ -4955,7 +4985,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A46" s="17" t="s">
         <v>199</v>
       </c>
@@ -4972,7 +5002,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A47" s="17" t="s">
         <v>201</v>
       </c>
@@ -4989,7 +5019,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A48" s="17" t="s">
         <v>203</v>
       </c>
@@ -5006,7 +5036,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A49" s="17" t="s">
         <v>204</v>
       </c>
@@ -5023,7 +5053,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A50" s="4" t="s">
         <v>57</v>
       </c>
@@ -5052,7 +5082,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="51" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A51" s="17" t="s">
         <v>206</v>
       </c>
@@ -5069,7 +5099,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="52" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A52" s="17" t="s">
         <v>208</v>
       </c>
@@ -5086,7 +5116,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="53" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A53" s="17" t="s">
         <v>209</v>
       </c>
@@ -5103,7 +5133,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="54" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A54" s="17" t="s">
         <v>210</v>
       </c>
@@ -5120,7 +5150,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="55" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A55" s="17" t="s">
         <v>212</v>
       </c>
@@ -5137,7 +5167,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A56" s="4" t="s">
         <v>214</v>
       </c>
@@ -5162,75 +5192,75 @@
       </c>
       <c r="I56" s="21"/>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A57" s="17"/>
       <c r="I57" s="7"/>
     </row>
-    <row r="58" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B58" s="5" t="s">
         <v>215</v>
       </c>
       <c r="I58" s="7"/>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B59" s="5"/>
       <c r="I59" s="7"/>
     </row>
-    <row r="60" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B60" s="5" t="s">
         <v>216</v>
       </c>
-      <c r="C60" s="26" t="s">
+      <c r="C60" s="28" t="s">
         <v>217</v>
       </c>
-      <c r="D60" s="26"/>
-      <c r="E60" s="26"/>
-      <c r="F60" s="26"/>
+      <c r="D60" s="28"/>
+      <c r="E60" s="28"/>
+      <c r="F60" s="28"/>
       <c r="I60" s="7"/>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="C61" s="26" t="s">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C61" s="28" t="s">
         <v>218</v>
       </c>
-      <c r="D61" s="26"/>
-      <c r="E61" s="26"/>
-      <c r="F61" s="26"/>
+      <c r="D61" s="28"/>
+      <c r="E61" s="28"/>
+      <c r="F61" s="28"/>
       <c r="I61" s="7"/>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="C62" s="26" t="s">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C62" s="28" t="s">
         <v>219</v>
       </c>
-      <c r="D62" s="26"/>
-      <c r="E62" s="26"/>
-      <c r="F62" s="26"/>
+      <c r="D62" s="28"/>
+      <c r="E62" s="28"/>
+      <c r="F62" s="28"/>
       <c r="I62" s="7"/>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="C63" s="28"/>
-      <c r="D63" s="28"/>
-      <c r="E63" s="28"/>
-      <c r="F63" s="28"/>
-    </row>
-    <row r="64" spans="1:9" ht="27" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C63" s="30"/>
+      <c r="D63" s="30"/>
+      <c r="E63" s="30"/>
+      <c r="F63" s="30"/>
+    </row>
+    <row r="64" spans="1:9" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B64" s="5" t="s">
         <v>220</v>
       </c>
-      <c r="C64" s="27" t="s">
+      <c r="C64" s="29" t="s">
         <v>221</v>
       </c>
-      <c r="D64" s="27"/>
-      <c r="E64" s="27"/>
-      <c r="F64" s="27"/>
+      <c r="D64" s="29"/>
+      <c r="E64" s="29"/>
+      <c r="F64" s="29"/>
       <c r="I64" s="7"/>
     </row>
-    <row r="65" spans="3:6" ht="26" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C65" s="27" t="s">
+    <row r="65" spans="3:6" ht="26" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C65" s="29" t="s">
         <v>222</v>
       </c>
-      <c r="D65" s="27"/>
-      <c r="E65" s="27"/>
-      <c r="F65" s="27"/>
+      <c r="D65" s="29"/>
+      <c r="E65" s="29"/>
+      <c r="F65" s="29"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -5255,12 +5285,12 @@
       <selection activeCell="F87" sqref="F87"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="54.6640625" style="23" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="54.69140625" style="23" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>33</v>
       </c>
@@ -5289,7 +5319,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>59</v>
       </c>
@@ -5318,7 +5348,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="17" t="s">
         <v>330</v>
       </c>
@@ -5331,7 +5361,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="17" t="s">
         <v>332</v>
       </c>
@@ -5344,7 +5374,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>62</v>
       </c>
@@ -5373,7 +5403,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="17" t="s">
         <v>337</v>
       </c>
@@ -5386,7 +5416,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="17" t="s">
         <v>338</v>
       </c>
@@ -5399,7 +5429,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="17" t="s">
         <v>339</v>
       </c>
@@ -5412,7 +5442,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="17" t="s">
         <v>340</v>
       </c>
@@ -5425,7 +5455,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>64</v>
       </c>
@@ -5454,7 +5484,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="17" t="s">
         <v>345</v>
       </c>
@@ -5467,7 +5497,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="17" t="s">
         <v>346</v>
       </c>
@@ -5480,7 +5510,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="28" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="17" t="s">
         <v>347</v>
       </c>
@@ -5493,7 +5523,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
         <v>66</v>
       </c>
@@ -5522,7 +5552,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="17" t="s">
         <v>350</v>
       </c>
@@ -5535,7 +5565,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="17" t="s">
         <v>351</v>
       </c>
@@ -5548,7 +5578,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="17" t="s">
         <v>352</v>
       </c>
@@ -5561,7 +5591,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
         <v>68</v>
       </c>
@@ -5590,7 +5620,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" s="17" t="s">
         <v>353</v>
       </c>
@@ -5603,7 +5633,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="17" t="s">
         <v>356</v>
       </c>
@@ -5616,7 +5646,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
         <v>70</v>
       </c>
@@ -5645,7 +5675,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" s="17" t="s">
         <v>357</v>
       </c>
@@ -5658,7 +5688,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" s="17" t="s">
         <v>361</v>
       </c>
@@ -5671,7 +5701,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" s="17" t="s">
         <v>362</v>
       </c>
@@ -5684,7 +5714,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" s="4" t="s">
         <v>72</v>
       </c>
@@ -5713,7 +5743,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>312</v>
       </c>
@@ -5730,7 +5760,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="27" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>313</v>
       </c>
@@ -5747,7 +5777,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="28" spans="1:9" ht="28" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:9" ht="27" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>315</v>
       </c>
@@ -5764,7 +5794,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="29" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>317</v>
       </c>
@@ -5781,7 +5811,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="30" spans="1:9" ht="28" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:9" ht="27" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>319</v>
       </c>
@@ -5798,7 +5828,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="31" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>321</v>
       </c>
@@ -5815,7 +5845,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="32" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" s="4" t="s">
         <v>74</v>
       </c>
@@ -5844,7 +5874,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="33" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>322</v>
       </c>
@@ -5861,7 +5891,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="34" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>323</v>
       </c>
@@ -5878,7 +5908,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="35" spans="1:9" ht="28" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>324</v>
       </c>
@@ -5895,7 +5925,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="36" spans="1:9" ht="28" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:9" ht="27" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>326</v>
       </c>
@@ -5912,7 +5942,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="37" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>328</v>
       </c>
@@ -5929,7 +5959,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="38" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A38" s="4" t="s">
         <v>76</v>
       </c>
@@ -5943,7 +5973,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="39" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>223</v>
       </c>
@@ -5972,7 +6002,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="40" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>225</v>
       </c>
@@ -5989,7 +6019,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="41" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>227</v>
       </c>
@@ -6006,7 +6036,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="42" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>229</v>
       </c>
@@ -6023,7 +6053,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="43" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>231</v>
       </c>
@@ -6040,7 +6070,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="44" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>233</v>
       </c>
@@ -6057,7 +6087,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="45" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>235</v>
       </c>
@@ -6074,7 +6104,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="46" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>237</v>
       </c>
@@ -6091,7 +6121,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="47" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>239</v>
       </c>
@@ -6108,7 +6138,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="48" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>241</v>
       </c>
@@ -6125,7 +6155,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="49" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>243</v>
       </c>
@@ -6142,7 +6172,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="50" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>245</v>
       </c>
@@ -6159,7 +6189,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="51" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>247</v>
       </c>
@@ -6176,7 +6206,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="52" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>249</v>
       </c>
@@ -6193,7 +6223,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="53" spans="1:9" ht="28" x14ac:dyDescent="0.15">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>251</v>
       </c>
@@ -6210,7 +6240,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="54" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>253</v>
       </c>
@@ -6227,7 +6257,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="55" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A55" s="4" t="s">
         <v>78</v>
       </c>
@@ -6256,7 +6286,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="56" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>255</v>
       </c>
@@ -6273,7 +6303,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="57" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>257</v>
       </c>
@@ -6290,7 +6320,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="58" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>258</v>
       </c>
@@ -6307,7 +6337,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="59" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>259</v>
       </c>
@@ -6324,7 +6354,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="60" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>260</v>
       </c>
@@ -6341,7 +6371,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="61" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>261</v>
       </c>
@@ -6358,7 +6388,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="62" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>262</v>
       </c>
@@ -6375,7 +6405,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="63" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>367</v>
       </c>
@@ -6392,7 +6422,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="64" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>368</v>
       </c>
@@ -6409,7 +6439,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="65" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>369</v>
       </c>
@@ -6426,7 +6456,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A66" s="4" t="s">
         <v>214</v>
       </c>
@@ -6450,70 +6480,70 @@
         <v>600</v>
       </c>
     </row>
-    <row r="72" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B72" s="5" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B73" s="5"/>
     </row>
-    <row r="74" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B74" s="5" t="s">
         <v>216</v>
       </c>
-      <c r="C74" s="33" t="s">
+      <c r="C74" s="25" t="s">
         <v>375</v>
       </c>
-      <c r="D74" s="34"/>
-      <c r="E74" s="34"/>
-      <c r="F74" s="34"/>
-      <c r="G74" s="34"/>
-    </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="D74" s="26"/>
+      <c r="E74" s="26"/>
+      <c r="F74" s="26"/>
+      <c r="G74" s="26"/>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B75" s="1"/>
-      <c r="C75" s="26" t="s">
+      <c r="C75" s="28" t="s">
         <v>371</v>
       </c>
-      <c r="D75" s="26"/>
-      <c r="E75" s="26"/>
-      <c r="F75" s="26"/>
-    </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="D75" s="28"/>
+      <c r="E75" s="28"/>
+      <c r="F75" s="28"/>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B76" s="1"/>
-      <c r="C76" s="26" t="s">
+      <c r="C76" s="28" t="s">
         <v>372</v>
       </c>
-      <c r="D76" s="26"/>
-      <c r="E76" s="26"/>
-      <c r="F76" s="26"/>
-    </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="D76" s="28"/>
+      <c r="E76" s="28"/>
+      <c r="F76" s="28"/>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B77" s="1"/>
-      <c r="C77" s="28"/>
-      <c r="D77" s="28"/>
-      <c r="E77" s="28"/>
-      <c r="F77" s="28"/>
-    </row>
-    <row r="78" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+      <c r="C77" s="30"/>
+      <c r="D77" s="30"/>
+      <c r="E77" s="30"/>
+      <c r="F77" s="30"/>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B78" s="5" t="s">
         <v>220</v>
       </c>
-      <c r="C78" s="27" t="s">
+      <c r="C78" s="29" t="s">
         <v>373</v>
       </c>
-      <c r="D78" s="27"/>
-      <c r="E78" s="27"/>
-      <c r="F78" s="27"/>
-    </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="D78" s="29"/>
+      <c r="E78" s="29"/>
+      <c r="F78" s="29"/>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B79" s="1"/>
-      <c r="C79" s="27" t="s">
+      <c r="C79" s="29" t="s">
         <v>374</v>
       </c>
-      <c r="D79" s="27"/>
-      <c r="E79" s="27"/>
-      <c r="F79" s="27"/>
+      <c r="D79" s="29"/>
+      <c r="E79" s="29"/>
+      <c r="F79" s="29"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -6537,13 +6567,13 @@
       <selection activeCell="E49" sqref="E49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="36.1640625" customWidth="1"/>
-    <col min="9" max="9" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="36.15234375" customWidth="1"/>
+    <col min="9" max="9" width="12.4609375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>33</v>
       </c>
@@ -6572,7 +6602,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="17" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:9" ht="15" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>80</v>
       </c>
@@ -6601,7 +6631,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="16" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:9" ht="15" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>379</v>
       </c>
@@ -6614,7 +6644,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="17" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:9" ht="15" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>82</v>
       </c>
@@ -6643,7 +6673,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="16" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:9" ht="15" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>380</v>
       </c>
@@ -6656,7 +6686,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="16" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:9" ht="15" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>381</v>
       </c>
@@ -6669,7 +6699,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="17" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:9" ht="15" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>84</v>
       </c>
@@ -6698,7 +6728,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="16" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:9" ht="15" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>383</v>
       </c>
@@ -6711,7 +6741,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="16" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:9" ht="15" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>384</v>
       </c>
@@ -6724,7 +6754,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="17" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:9" ht="15" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>86</v>
       </c>
@@ -6753,7 +6783,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="16" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:9" ht="15" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>386</v>
       </c>
@@ -6766,7 +6796,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="16" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:9" ht="15" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>387</v>
       </c>
@@ -6779,7 +6809,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="17" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:9" ht="15" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
         <v>88</v>
       </c>
@@ -6808,7 +6838,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="16" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:9" ht="15" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>389</v>
       </c>
@@ -6821,7 +6851,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="16" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:9" ht="15" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>390</v>
       </c>
@@ -6834,7 +6864,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="17" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:9" ht="15" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
         <v>90</v>
       </c>
@@ -6863,7 +6893,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="16" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:9" ht="15" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>392</v>
       </c>
@@ -6876,7 +6906,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="16" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:9" ht="15" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>393</v>
       </c>
@@ -6889,7 +6919,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="17" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:9" ht="15" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
         <v>92</v>
       </c>
@@ -6918,7 +6948,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="16" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:9" ht="15" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>394</v>
       </c>
@@ -6931,7 +6961,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="16" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:9" ht="15" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>395</v>
       </c>
@@ -6944,7 +6974,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="17" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:9" ht="15" x14ac:dyDescent="0.3">
       <c r="A22" s="4" t="s">
         <v>94</v>
       </c>
@@ -6973,7 +7003,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="16" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:9" ht="15" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>396</v>
       </c>
@@ -6986,7 +7016,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="16" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:9" ht="15" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>397</v>
       </c>
@@ -6999,7 +7029,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="17" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:9" ht="15" x14ac:dyDescent="0.3">
       <c r="A25" s="4" t="s">
         <v>96</v>
       </c>
@@ -7028,7 +7058,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="16" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:9" ht="15" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>398</v>
       </c>
@@ -7041,7 +7071,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="27" spans="1:9" ht="16" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:9" ht="15" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>399</v>
       </c>
@@ -7054,7 +7084,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="28" spans="1:9" ht="17" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:9" ht="15" x14ac:dyDescent="0.3">
       <c r="A28" s="4" t="s">
         <v>98</v>
       </c>
@@ -7083,7 +7113,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>400</v>
       </c>
@@ -7094,7 +7124,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>401</v>
       </c>
@@ -7105,7 +7135,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" s="4" t="s">
         <v>214</v>
       </c>
@@ -7126,75 +7156,75 @@
         <v>660</v>
       </c>
     </row>
-    <row r="37" spans="2:7" ht="14" x14ac:dyDescent="0.15">
+    <row r="37" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B37" s="5" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="38" spans="2:7" x14ac:dyDescent="0.15">
+    <row r="38" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B38" s="5"/>
     </row>
-    <row r="39" spans="2:7" ht="14" x14ac:dyDescent="0.15">
+    <row r="39" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B39" s="5" t="s">
         <v>216</v>
       </c>
-      <c r="C39" s="26" t="s">
+      <c r="C39" s="28" t="s">
         <v>412</v>
       </c>
-      <c r="D39" s="26"/>
-      <c r="E39" s="26"/>
-      <c r="F39" s="26"/>
-      <c r="G39" s="26"/>
-    </row>
-    <row r="40" spans="2:7" x14ac:dyDescent="0.15">
+      <c r="D39" s="28"/>
+      <c r="E39" s="28"/>
+      <c r="F39" s="28"/>
+      <c r="G39" s="28"/>
+    </row>
+    <row r="40" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B40" s="1"/>
-      <c r="C40" s="29" t="s">
+      <c r="C40" s="32" t="s">
         <v>413</v>
       </c>
-      <c r="D40" s="29"/>
-      <c r="E40" s="29"/>
-      <c r="F40" s="29"/>
-      <c r="G40" s="29"/>
-    </row>
-    <row r="41" spans="2:7" x14ac:dyDescent="0.15">
+      <c r="D40" s="32"/>
+      <c r="E40" s="32"/>
+      <c r="F40" s="32"/>
+      <c r="G40" s="32"/>
+    </row>
+    <row r="41" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B41" s="1"/>
-      <c r="C41" s="29" t="s">
+      <c r="C41" s="32" t="s">
         <v>414</v>
       </c>
-      <c r="D41" s="29"/>
-      <c r="E41" s="29"/>
-      <c r="F41" s="29"/>
-      <c r="G41" s="29"/>
-    </row>
-    <row r="42" spans="2:7" x14ac:dyDescent="0.15">
+      <c r="D41" s="32"/>
+      <c r="E41" s="32"/>
+      <c r="F41" s="32"/>
+      <c r="G41" s="32"/>
+    </row>
+    <row r="42" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B42" s="1"/>
-      <c r="C42" s="30"/>
-      <c r="D42" s="31"/>
-      <c r="E42" s="31"/>
-      <c r="F42" s="31"/>
-      <c r="G42" s="31"/>
-    </row>
-    <row r="43" spans="2:7" ht="14" x14ac:dyDescent="0.15">
+      <c r="C42" s="33"/>
+      <c r="D42" s="34"/>
+      <c r="E42" s="34"/>
+      <c r="F42" s="34"/>
+      <c r="G42" s="34"/>
+    </row>
+    <row r="43" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B43" s="5" t="s">
         <v>220</v>
       </c>
-      <c r="C43" s="27" t="s">
+      <c r="C43" s="29" t="s">
         <v>415</v>
       </c>
-      <c r="D43" s="27"/>
-      <c r="E43" s="27"/>
-      <c r="F43" s="27"/>
-    </row>
-    <row r="44" spans="2:7" x14ac:dyDescent="0.15">
+      <c r="D43" s="29"/>
+      <c r="E43" s="29"/>
+      <c r="F43" s="29"/>
+    </row>
+    <row r="44" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B44" s="1"/>
-      <c r="C44" s="32" t="s">
+      <c r="C44" s="31" t="s">
         <v>416</v>
       </c>
-      <c r="D44" s="27"/>
-      <c r="E44" s="27"/>
-      <c r="F44" s="27"/>
-    </row>
-    <row r="45" spans="2:7" x14ac:dyDescent="0.15">
+      <c r="D44" s="29"/>
+      <c r="E44" s="29"/>
+      <c r="F44" s="29"/>
+    </row>
+    <row r="45" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B45" s="23"/>
     </row>
   </sheetData>
@@ -7216,16 +7246,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:I33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M20" sqref="M20"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="28.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.4609375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.3828125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="28" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>33</v>
       </c>
@@ -7254,7 +7285,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="17" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:9" ht="15" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>100</v>
       </c>
@@ -7277,7 +7308,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="16" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:9" ht="15" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>417</v>
       </c>
@@ -7287,7 +7318,7 @@
       <c r="C3" s="12"/>
       <c r="D3" s="17"/>
     </row>
-    <row r="4" spans="1:9" ht="28" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:9" ht="27" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>418</v>
       </c>
@@ -7297,7 +7328,7 @@
       <c r="C4" s="12"/>
       <c r="D4" s="17"/>
     </row>
-    <row r="5" spans="1:9" ht="17" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:9" ht="15" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>102</v>
       </c>
@@ -7320,7 +7351,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="28" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:9" ht="15" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>423</v>
       </c>
@@ -7330,7 +7361,7 @@
       <c r="C6" s="12"/>
       <c r="D6" s="17"/>
     </row>
-    <row r="7" spans="1:9" ht="28" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:9" ht="27" x14ac:dyDescent="0.3">
       <c r="A7" s="17" t="s">
         <v>457</v>
       </c>
@@ -7340,7 +7371,7 @@
       <c r="C7" s="12"/>
       <c r="D7" s="17"/>
     </row>
-    <row r="8" spans="1:9" ht="17" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:9" ht="15" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>104</v>
       </c>
@@ -7363,7 +7394,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="16" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:9" ht="15" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>424</v>
       </c>
@@ -7373,7 +7404,7 @@
       <c r="C9" s="12"/>
       <c r="D9" s="17"/>
     </row>
-    <row r="10" spans="1:9" ht="28" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:9" ht="15" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>426</v>
       </c>
@@ -7383,7 +7414,7 @@
       <c r="C10" s="12"/>
       <c r="D10" s="17"/>
     </row>
-    <row r="11" spans="1:9" ht="17" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:9" ht="15" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
         <v>106</v>
       </c>
@@ -7406,7 +7437,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="16" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:9" ht="15" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>430</v>
       </c>
@@ -7416,7 +7447,7 @@
       <c r="C12" s="12"/>
       <c r="D12" s="17"/>
     </row>
-    <row r="13" spans="1:9" ht="28" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:9" ht="15" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>431</v>
       </c>
@@ -7426,7 +7457,7 @@
       <c r="C13" s="12"/>
       <c r="D13" s="17"/>
     </row>
-    <row r="14" spans="1:9" ht="17" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:9" ht="15" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
         <v>108</v>
       </c>
@@ -7449,7 +7480,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="28" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:9" ht="27" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>433</v>
       </c>
@@ -7459,7 +7490,7 @@
       <c r="C15" s="12"/>
       <c r="D15" s="17"/>
     </row>
-    <row r="16" spans="1:9" ht="16" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:9" ht="15" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>434</v>
       </c>
@@ -7469,7 +7500,7 @@
       <c r="C16" s="12"/>
       <c r="D16" s="17"/>
     </row>
-    <row r="17" spans="1:9" ht="17" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:9" ht="15" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
         <v>110</v>
       </c>
@@ -7492,7 +7523,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="16" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:9" ht="15" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>437</v>
       </c>
@@ -7502,7 +7533,7 @@
       <c r="C18" s="12"/>
       <c r="D18" s="17"/>
     </row>
-    <row r="19" spans="1:9" ht="28" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:9" ht="27" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>438</v>
       </c>
@@ -7512,7 +7543,7 @@
       <c r="C19" s="12"/>
       <c r="D19" s="17"/>
     </row>
-    <row r="20" spans="1:9" ht="17" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:9" ht="15" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
         <v>112</v>
       </c>
@@ -7535,7 +7566,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="16" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:9" ht="15" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>439</v>
       </c>
@@ -7545,7 +7576,7 @@
       <c r="C21" s="12"/>
       <c r="D21" s="17"/>
     </row>
-    <row r="22" spans="1:9" ht="28" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:9" ht="27" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>440</v>
       </c>
@@ -7555,7 +7586,7 @@
       <c r="C22" s="12"/>
       <c r="D22" s="17"/>
     </row>
-    <row r="23" spans="1:9" ht="16" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:9" ht="15" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>445</v>
       </c>
@@ -7565,7 +7596,7 @@
       <c r="C23" s="12"/>
       <c r="D23" s="17"/>
     </row>
-    <row r="24" spans="1:9" ht="17" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:9" ht="15" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="s">
         <v>114</v>
       </c>
@@ -7588,7 +7619,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="28" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:9" ht="27" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>441</v>
       </c>
@@ -7598,7 +7629,7 @@
       <c r="C25" s="12"/>
       <c r="D25" s="17"/>
     </row>
-    <row r="26" spans="1:9" ht="16" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:9" ht="15" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>442</v>
       </c>
@@ -7608,7 +7639,7 @@
       <c r="C26" s="12"/>
       <c r="D26" s="17"/>
     </row>
-    <row r="27" spans="1:9" ht="17" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:9" ht="15" x14ac:dyDescent="0.3">
       <c r="A27" s="4" t="s">
         <v>116</v>
       </c>
@@ -7627,11 +7658,17 @@
       <c r="F27">
         <v>30</v>
       </c>
+      <c r="G27">
+        <v>23</v>
+      </c>
+      <c r="H27">
+        <v>30</v>
+      </c>
       <c r="I27" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" ht="16" x14ac:dyDescent="0.15">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="15" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>451</v>
       </c>
@@ -7640,8 +7677,11 @@
       </c>
       <c r="C28" s="12"/>
       <c r="D28" s="17"/>
-    </row>
-    <row r="29" spans="1:9" ht="28" x14ac:dyDescent="0.15">
+      <c r="I28" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="27" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>452</v>
       </c>
@@ -7650,8 +7690,11 @@
       </c>
       <c r="C29" s="12"/>
       <c r="D29" s="17"/>
-    </row>
-    <row r="30" spans="1:9" ht="17" x14ac:dyDescent="0.15">
+      <c r="I29" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="15" x14ac:dyDescent="0.3">
       <c r="A30" s="4" t="s">
         <v>118</v>
       </c>
@@ -7670,27 +7713,39 @@
       <c r="F30">
         <v>80</v>
       </c>
+      <c r="G30">
+        <v>78</v>
+      </c>
+      <c r="H30">
+        <v>90</v>
+      </c>
       <c r="I30" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" ht="28" x14ac:dyDescent="0.15">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>453</v>
       </c>
       <c r="B31" s="23" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="32" spans="1:9" ht="28" x14ac:dyDescent="0.15">
+      <c r="I31" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" ht="27" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>454</v>
       </c>
       <c r="B32" s="23" t="s">
         <v>455</v>
       </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="I32" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33" s="4" t="s">
         <v>214</v>
       </c>
@@ -7704,11 +7759,11 @@
       </c>
       <c r="G33">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>101</v>
       </c>
       <c r="H33">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>120</v>
       </c>
     </row>
   </sheetData>
@@ -7725,13 +7780,13 @@
       <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="28.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="49.5" style="1" customWidth="1"/>
+    <col min="2" max="2" width="28.15234375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="49.4609375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="4" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>263</v>
       </c>
@@ -7742,7 +7797,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>37</v>
       </c>
@@ -7753,7 +7808,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>40</v>
       </c>
@@ -7764,7 +7819,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>43</v>
       </c>
@@ -7775,7 +7830,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>45</v>
       </c>
@@ -7786,7 +7841,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>47</v>
       </c>
@@ -7797,7 +7852,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>49</v>
       </c>
@@ -7808,7 +7863,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="51" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:3" ht="45" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>51</v>
       </c>
@@ -7819,7 +7874,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>53</v>
       </c>
@@ -7830,7 +7885,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>55</v>
       </c>
@@ -7841,7 +7896,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="51" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>57</v>
       </c>
@@ -7852,7 +7907,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>59</v>
       </c>
@@ -7863,7 +7918,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="51" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:3" ht="45" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>62</v>
       </c>
@@ -7874,7 +7929,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="68" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:3" ht="45" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>64</v>
       </c>
@@ -7885,7 +7940,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>66</v>
       </c>
@@ -7896,7 +7951,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>68</v>
       </c>
@@ -7907,7 +7962,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>70</v>
       </c>
@@ -7918,7 +7973,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>72</v>
       </c>
@@ -7929,7 +7984,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>74</v>
       </c>
@@ -7940,7 +7995,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>76</v>
       </c>
@@ -7951,7 +8006,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>78</v>
       </c>
@@ -7962,7 +8017,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>80</v>
       </c>
@@ -7973,7 +8028,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>82</v>
       </c>
@@ -7984,7 +8039,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>84</v>
       </c>
@@ -7995,7 +8050,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="51" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:3" ht="45" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>86</v>
       </c>
@@ -8006,7 +8061,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>88</v>
       </c>
@@ -8017,7 +8072,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="136" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:3" ht="105" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>90</v>
       </c>
@@ -8028,7 +8083,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>92</v>
       </c>
@@ -8039,7 +8094,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>94</v>
       </c>
@@ -8050,7 +8105,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>96</v>
       </c>
@@ -8061,7 +8116,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>98</v>
       </c>
@@ -8072,7 +8127,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>100</v>
       </c>
@@ -8083,7 +8138,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>102</v>
       </c>
@@ -8094,7 +8149,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>104</v>
       </c>
@@ -8105,7 +8160,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="51" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>106</v>
       </c>
@@ -8116,7 +8171,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>108</v>
       </c>
@@ -8127,7 +8182,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>110</v>
       </c>
@@ -8138,7 +8193,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>112</v>
       </c>
@@ -8149,7 +8204,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>114</v>
       </c>
@@ -8160,7 +8215,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>116</v>
       </c>
@@ -8171,7 +8226,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>118</v>
       </c>
@@ -8182,7 +8237,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>306</v>
       </c>
@@ -8193,7 +8248,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>309</v>
       </c>

</xml_diff>

<commit_message>
Added UserStory 37 and 38 with test files
Added UserStory 37 and 38 with test files and commneted out all print outs statements internal to all userstories.
</commit_message>
<xml_diff>
--- a/Team2Report.xlsx
+++ b/Team2Report.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11012"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ztyle\Documents\SSW 555\SSW_555_Project_Master\Agile_Methods_Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/srikanth/Documenta/StevensInstitute/SoftwareEngg/SSW-555/SSW-555Project/Agile_Methods_Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB693E2D-2FC7-45EE-AB3F-9252597135E0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF344955-0744-2D42-941B-104B1E06FC3F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" firstSheet="2" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="24340" windowHeight="14140" tabRatio="500" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -23,19 +23,10 @@
     <sheet name="Sprint4" sheetId="6" r:id="rId8"/>
     <sheet name="Stories" sheetId="11" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -45,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1173" uniqueCount="458">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1186" uniqueCount="461">
   <si>
     <t>Initials</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -1439,6 +1430,15 @@
   </si>
   <si>
     <t>T32.02</t>
+  </si>
+  <si>
+    <t>1: ??</t>
+  </si>
+  <si>
+    <t>2: ??</t>
+  </si>
+  <si>
+    <t>3: ??</t>
   </si>
 </sst>
 </file>
@@ -1605,7 +1605,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1653,7 +1653,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1678,6 +1677,18 @@
     </xf>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="20" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="66">
@@ -1788,7 +1799,7 @@
             <c:numRef>
               <c:f>'Burndown README'!$B$15:$B$20</c:f>
               <c:numCache>
-                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:formatCode>m/d/yy</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>42632</c:v>
@@ -1859,7 +1870,7 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
+        <c:numFmt formatCode="m/d/yy" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1925,10 +1936,10 @@
             <c:numRef>
               <c:f>Burndown!$A$2:$A$7</c:f>
               <c:numCache>
-                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:formatCode>m/d/yy</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>42632</c:v>
+                  <c:v>42633</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>42647</c:v>
@@ -1940,7 +1951,7 @@
                   <c:v>42682</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>42689</c:v>
+                  <c:v>42703</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1964,7 +1975,7 @@
                   <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1996,7 +2007,7 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
+        <c:numFmt formatCode="m/d/yy" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2858,16 +2869,16 @@
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="7.84375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.15234375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.4609375" customWidth="1"/>
-    <col min="4" max="4" width="22.84375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.4609375" customWidth="1"/>
+    <col min="1" max="1" width="7.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.5" customWidth="1"/>
+    <col min="4" max="4" width="22.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -2884,7 +2895,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -2901,7 +2912,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -2918,7 +2929,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -2935,7 +2946,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -2952,7 +2963,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>25</v>
       </c>
@@ -2969,7 +2980,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.15">
       <c r="D8" s="4" t="s">
         <v>30</v>
       </c>
@@ -2978,7 +2989,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D4">
+  <sortState ref="A2:D4">
     <sortCondition ref="C2:C4"/>
   </sortState>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -3002,16 +3013,16 @@
       <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="6.84375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="29" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.4609375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.4609375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>32</v>
       </c>
@@ -3028,7 +3039,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A2">
         <v>1</v>
       </c>
@@ -3045,7 +3056,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A3">
         <v>1</v>
       </c>
@@ -3061,14 +3072,14 @@
       <c r="E3" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="G3" s="27" t="s">
+      <c r="G3" s="26" t="s">
         <v>42</v>
       </c>
-      <c r="H3" s="27"/>
-      <c r="I3" s="27"/>
-      <c r="J3" s="27"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="H3" s="26"/>
+      <c r="I3" s="26"/>
+      <c r="J3" s="26"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A4">
         <v>1</v>
       </c>
@@ -3085,7 +3096,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A5">
         <v>1</v>
       </c>
@@ -3102,7 +3113,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A6">
         <v>1</v>
       </c>
@@ -3119,7 +3130,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A7">
         <v>1</v>
       </c>
@@ -3136,7 +3147,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A8">
         <v>1</v>
       </c>
@@ -3153,7 +3164,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A9">
         <v>1</v>
       </c>
@@ -3170,7 +3181,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A10">
         <v>1</v>
       </c>
@@ -3187,7 +3198,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A11">
         <v>1</v>
       </c>
@@ -3204,7 +3215,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A12">
         <v>2</v>
       </c>
@@ -3221,7 +3232,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A13">
         <v>2</v>
       </c>
@@ -3238,7 +3249,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A14">
         <v>2</v>
       </c>
@@ -3255,7 +3266,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A15">
         <v>2</v>
       </c>
@@ -3272,7 +3283,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A16">
         <v>2</v>
       </c>
@@ -3289,7 +3300,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A17">
         <v>2</v>
       </c>
@@ -3306,7 +3317,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A18">
         <v>2</v>
       </c>
@@ -3323,7 +3334,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A19">
         <v>2</v>
       </c>
@@ -3340,7 +3351,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A20">
         <v>2</v>
       </c>
@@ -3357,7 +3368,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A21">
         <v>2</v>
       </c>
@@ -3374,7 +3385,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A22">
         <v>3</v>
       </c>
@@ -3391,7 +3402,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A23">
         <v>3</v>
       </c>
@@ -3408,7 +3419,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A24">
         <v>3</v>
       </c>
@@ -3425,7 +3436,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A25">
         <v>3</v>
       </c>
@@ -3442,7 +3453,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A26">
         <v>3</v>
       </c>
@@ -3459,7 +3470,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A27">
         <v>3</v>
       </c>
@@ -3476,7 +3487,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A28">
         <v>3</v>
       </c>
@@ -3493,7 +3504,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A29">
         <v>3</v>
       </c>
@@ -3510,7 +3521,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A30">
         <v>3</v>
       </c>
@@ -3527,7 +3538,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A31">
         <v>3</v>
       </c>
@@ -3544,7 +3555,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A32">
         <v>4</v>
       </c>
@@ -3561,7 +3572,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A33">
         <v>4</v>
       </c>
@@ -3578,7 +3589,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A34">
         <v>4</v>
       </c>
@@ -3595,7 +3606,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A35">
         <v>4</v>
       </c>
@@ -3612,7 +3623,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A36">
         <v>4</v>
       </c>
@@ -3629,7 +3640,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A37">
         <v>4</v>
       </c>
@@ -3646,7 +3657,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A38">
         <v>4</v>
       </c>
@@ -3663,7 +3674,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A39">
         <v>4</v>
       </c>
@@ -3680,7 +3691,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A40">
         <v>4</v>
       </c>
@@ -3697,7 +3708,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A41">
         <v>4</v>
       </c>
@@ -3732,47 +3743,47 @@
       <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="10.84375" style="7"/>
-    <col min="2" max="2" width="10.15234375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.84375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.3046875" customWidth="1"/>
-    <col min="5" max="5" width="6.84375" customWidth="1"/>
-    <col min="6" max="6" width="12.4609375" style="9" customWidth="1"/>
+    <col min="1" max="1" width="10.83203125" style="7"/>
+    <col min="2" max="2" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.33203125" customWidth="1"/>
+    <col min="5" max="5" width="6.83203125" customWidth="1"/>
+    <col min="6" max="6" width="12.5" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A1" s="7" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A2" s="7" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A3" s="7" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A5" s="7" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A6" s="7" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A8" s="7" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A14" s="4" t="s">
         <v>126</v>
       </c>
@@ -3795,7 +3806,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
         <v>133</v>
       </c>
@@ -3811,7 +3822,7 @@
       <c r="F15" s="14"/>
       <c r="G15" s="9"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
         <v>134</v>
       </c>
@@ -3835,7 +3846,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A17" s="7" t="s">
         <v>135</v>
       </c>
@@ -3860,7 +3871,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A18" s="7" t="s">
         <v>136</v>
       </c>
@@ -3885,7 +3896,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A19" s="7" t="s">
         <v>137</v>
       </c>
@@ -3921,21 +3932,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="10.84375" style="2"/>
-    <col min="2" max="2" width="18.4609375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.4609375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.15234375" customWidth="1"/>
-    <col min="5" max="5" width="6.84375" customWidth="1"/>
-    <col min="6" max="6" width="12.4609375" style="9" customWidth="1"/>
+    <col min="1" max="1" width="10.83203125" style="2"/>
+    <col min="2" max="2" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.1640625" customWidth="1"/>
+    <col min="5" max="5" width="6.83203125" customWidth="1"/>
+    <col min="6" max="6" width="12.5" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="3" t="s">
         <v>127</v>
       </c>
@@ -3955,9 +3966,9 @@
         <v>132</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A2" s="13">
-        <v>42632</v>
+        <v>42633</v>
       </c>
       <c r="B2">
         <v>40</v>
@@ -3975,7 +3986,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A3" s="13">
         <v>42647</v>
       </c>
@@ -4000,7 +4011,7 @@
         <v>34.695652173913047</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A4" s="13">
         <v>42668</v>
       </c>
@@ -4025,11 +4036,12 @@
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A5" s="13">
         <v>42682</v>
       </c>
       <c r="B5">
+        <f>B4-COUNTIF(Sprint3!$I$2:$I$65, "Completed")</f>
         <v>10</v>
       </c>
       <c r="C5">
@@ -4049,27 +4061,29 @@
         <v>24.818181818181817</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A6" s="13">
-        <v>42689</v>
+        <v>42703</v>
       </c>
       <c r="B6">
-        <v>0</v>
+        <f>B5-COUNTIF(Sprint4!$I$2:$I$65, "Completed")</f>
+        <v>6</v>
       </c>
       <c r="C6">
-        <v>10</v>
+        <f>B5-B6</f>
+        <v>4</v>
       </c>
       <c r="D6">
         <f>Sprint4!G33</f>
-        <v>101</v>
+        <v>219</v>
       </c>
       <c r="E6">
         <f>Sprint4!H33</f>
-        <v>120</v>
+        <v>330</v>
       </c>
       <c r="F6" s="9">
         <f>((D5+D6)-D5)/E6*60</f>
-        <v>50.5</v>
+        <v>39.81818181818182</v>
       </c>
     </row>
   </sheetData>
@@ -4088,19 +4102,19 @@
       <selection activeCell="H55" sqref="H55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="33" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.4609375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.4609375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.3046875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.69140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.4609375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.3046875" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.33203125" style="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>33</v>
       </c>
@@ -4129,7 +4143,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A2" s="4" t="s">
         <v>37</v>
       </c>
@@ -4158,7 +4172,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A3" s="17" t="s">
         <v>144</v>
       </c>
@@ -4175,7 +4189,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A4" s="17" t="s">
         <v>147</v>
       </c>
@@ -4192,7 +4206,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A5" s="17" t="s">
         <v>149</v>
       </c>
@@ -4209,7 +4223,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A6" s="4" t="s">
         <v>40</v>
       </c>
@@ -4238,7 +4252,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A7" s="17" t="s">
         <v>151</v>
       </c>
@@ -4255,7 +4269,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A8" s="17" t="s">
         <v>153</v>
       </c>
@@ -4272,7 +4286,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A9" s="17" t="s">
         <v>155</v>
       </c>
@@ -4289,7 +4303,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A10" s="17" t="s">
         <v>157</v>
       </c>
@@ -4306,7 +4320,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A11" s="4" t="s">
         <v>43</v>
       </c>
@@ -4335,7 +4349,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A12" s="17" t="s">
         <v>159</v>
       </c>
@@ -4352,7 +4366,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A13" s="17" t="s">
         <v>161</v>
       </c>
@@ -4369,7 +4383,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A14" s="17" t="s">
         <v>162</v>
       </c>
@@ -4386,7 +4400,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A15" s="17" t="s">
         <v>164</v>
       </c>
@@ -4403,7 +4417,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A16" s="4" t="s">
         <v>45</v>
       </c>
@@ -4432,7 +4446,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A17" s="17" t="s">
         <v>166</v>
       </c>
@@ -4449,7 +4463,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A18" s="17" t="s">
         <v>167</v>
       </c>
@@ -4466,7 +4480,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A19" s="17" t="s">
         <v>169</v>
       </c>
@@ -4483,7 +4497,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A20" s="17" t="s">
         <v>170</v>
       </c>
@@ -4500,7 +4514,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A21" s="17" t="s">
         <v>172</v>
       </c>
@@ -4517,7 +4531,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A22" s="4" t="s">
         <v>47</v>
       </c>
@@ -4546,7 +4560,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A23" s="17" t="s">
         <v>174</v>
       </c>
@@ -4563,7 +4577,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A24" s="17" t="s">
         <v>175</v>
       </c>
@@ -4580,7 +4594,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A25" s="17" t="s">
         <v>176</v>
       </c>
@@ -4597,7 +4611,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A26" s="17" t="s">
         <v>177</v>
       </c>
@@ -4614,7 +4628,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A27" s="17" t="s">
         <v>178</v>
       </c>
@@ -4631,7 +4645,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A28" s="4" t="s">
         <v>49</v>
       </c>
@@ -4660,7 +4674,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A29" s="17" t="s">
         <v>180</v>
       </c>
@@ -4677,7 +4691,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A30" s="17" t="s">
         <v>181</v>
       </c>
@@ -4694,7 +4708,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A31" s="17" t="s">
         <v>182</v>
       </c>
@@ -4711,7 +4725,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A32" s="17" t="s">
         <v>183</v>
       </c>
@@ -4728,7 +4742,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A33" s="17" t="s">
         <v>184</v>
       </c>
@@ -4745,7 +4759,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A34" s="4" t="s">
         <v>51</v>
       </c>
@@ -4774,7 +4788,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A35" s="17" t="s">
         <v>186</v>
       </c>
@@ -4791,7 +4805,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A36" s="17" t="s">
         <v>187</v>
       </c>
@@ -4808,7 +4822,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A37" s="17" t="s">
         <v>189</v>
       </c>
@@ -4825,7 +4839,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A38" s="17" t="s">
         <v>191</v>
       </c>
@@ -4842,7 +4856,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A39" s="17" t="s">
         <v>192</v>
       </c>
@@ -4859,7 +4873,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A40" s="17" t="s">
         <v>194</v>
       </c>
@@ -4876,7 +4890,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A41" s="4" t="s">
         <v>53</v>
       </c>
@@ -4905,7 +4919,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A42" s="17" t="s">
         <v>196</v>
       </c>
@@ -4922,7 +4936,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A43" s="17" t="s">
         <v>197</v>
       </c>
@@ -4939,7 +4953,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A44" s="17" t="s">
         <v>198</v>
       </c>
@@ -4956,7 +4970,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A45" s="4" t="s">
         <v>55</v>
       </c>
@@ -4985,7 +4999,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A46" s="17" t="s">
         <v>199</v>
       </c>
@@ -5002,7 +5016,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A47" s="17" t="s">
         <v>201</v>
       </c>
@@ -5019,7 +5033,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A48" s="17" t="s">
         <v>203</v>
       </c>
@@ -5036,7 +5050,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A49" s="17" t="s">
         <v>204</v>
       </c>
@@ -5053,7 +5067,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A50" s="4" t="s">
         <v>57</v>
       </c>
@@ -5082,7 +5096,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A51" s="17" t="s">
         <v>206</v>
       </c>
@@ -5099,7 +5113,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A52" s="17" t="s">
         <v>208</v>
       </c>
@@ -5116,7 +5130,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A53" s="17" t="s">
         <v>209</v>
       </c>
@@ -5133,7 +5147,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A54" s="17" t="s">
         <v>210</v>
       </c>
@@ -5150,7 +5164,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A55" s="17" t="s">
         <v>212</v>
       </c>
@@ -5167,7 +5181,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A56" s="4" t="s">
         <v>214</v>
       </c>
@@ -5192,75 +5206,75 @@
       </c>
       <c r="I56" s="21"/>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A57" s="17"/>
       <c r="I57" s="7"/>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="B58" s="5" t="s">
         <v>215</v>
       </c>
       <c r="I58" s="7"/>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B59" s="5"/>
       <c r="I59" s="7"/>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="B60" s="5" t="s">
         <v>216</v>
       </c>
-      <c r="C60" s="28" t="s">
+      <c r="C60" s="27" t="s">
         <v>217</v>
       </c>
-      <c r="D60" s="28"/>
-      <c r="E60" s="28"/>
-      <c r="F60" s="28"/>
+      <c r="D60" s="27"/>
+      <c r="E60" s="27"/>
+      <c r="F60" s="27"/>
       <c r="I60" s="7"/>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="C61" s="28" t="s">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="C61" s="27" t="s">
         <v>218</v>
       </c>
-      <c r="D61" s="28"/>
-      <c r="E61" s="28"/>
-      <c r="F61" s="28"/>
+      <c r="D61" s="27"/>
+      <c r="E61" s="27"/>
+      <c r="F61" s="27"/>
       <c r="I61" s="7"/>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="C62" s="28" t="s">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="C62" s="27" t="s">
         <v>219</v>
       </c>
-      <c r="D62" s="28"/>
-      <c r="E62" s="28"/>
-      <c r="F62" s="28"/>
+      <c r="D62" s="27"/>
+      <c r="E62" s="27"/>
+      <c r="F62" s="27"/>
       <c r="I62" s="7"/>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="C63" s="30"/>
-      <c r="D63" s="30"/>
-      <c r="E63" s="30"/>
-      <c r="F63" s="30"/>
-    </row>
-    <row r="64" spans="1:9" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="C63" s="29"/>
+      <c r="D63" s="29"/>
+      <c r="E63" s="29"/>
+      <c r="F63" s="29"/>
+    </row>
+    <row r="64" spans="1:9" ht="27" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B64" s="5" t="s">
         <v>220</v>
       </c>
-      <c r="C64" s="29" t="s">
+      <c r="C64" s="28" t="s">
         <v>221</v>
       </c>
-      <c r="D64" s="29"/>
-      <c r="E64" s="29"/>
-      <c r="F64" s="29"/>
+      <c r="D64" s="28"/>
+      <c r="E64" s="28"/>
+      <c r="F64" s="28"/>
       <c r="I64" s="7"/>
     </row>
-    <row r="65" spans="3:6" ht="26" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C65" s="29" t="s">
+    <row r="65" spans="3:6" ht="26" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C65" s="28" t="s">
         <v>222</v>
       </c>
-      <c r="D65" s="29"/>
-      <c r="E65" s="29"/>
-      <c r="F65" s="29"/>
+      <c r="D65" s="28"/>
+      <c r="E65" s="28"/>
+      <c r="F65" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -5282,15 +5296,15 @@
   <dimension ref="A1:I79"/>
   <sheetViews>
     <sheetView topLeftCell="A56" zoomScale="108" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F87" sqref="F87"/>
+      <selection activeCell="H76" sqref="H76"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="2" max="2" width="54.69140625" style="23" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="54.6640625" style="23" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>33</v>
       </c>
@@ -5319,7 +5333,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A2" s="4" t="s">
         <v>59</v>
       </c>
@@ -5348,7 +5362,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A3" s="17" t="s">
         <v>330</v>
       </c>
@@ -5361,7 +5375,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A4" s="17" t="s">
         <v>332</v>
       </c>
@@ -5374,7 +5388,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A5" s="4" t="s">
         <v>62</v>
       </c>
@@ -5403,7 +5417,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A6" s="17" t="s">
         <v>337</v>
       </c>
@@ -5416,7 +5430,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A7" s="17" t="s">
         <v>338</v>
       </c>
@@ -5429,7 +5443,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A8" s="17" t="s">
         <v>339</v>
       </c>
@@ -5442,7 +5456,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A9" s="17" t="s">
         <v>340</v>
       </c>
@@ -5455,7 +5469,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A10" s="4" t="s">
         <v>64</v>
       </c>
@@ -5484,7 +5498,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A11" s="17" t="s">
         <v>345</v>
       </c>
@@ -5497,7 +5511,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A12" s="17" t="s">
         <v>346</v>
       </c>
@@ -5510,7 +5524,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" ht="28" x14ac:dyDescent="0.15">
       <c r="A13" s="17" t="s">
         <v>347</v>
       </c>
@@ -5523,7 +5537,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A14" s="4" t="s">
         <v>66</v>
       </c>
@@ -5552,7 +5566,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A15" s="17" t="s">
         <v>350</v>
       </c>
@@ -5565,7 +5579,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A16" s="17" t="s">
         <v>351</v>
       </c>
@@ -5578,7 +5592,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A17" s="17" t="s">
         <v>352</v>
       </c>
@@ -5591,7 +5605,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A18" s="4" t="s">
         <v>68</v>
       </c>
@@ -5620,7 +5634,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A19" s="17" t="s">
         <v>353</v>
       </c>
@@ -5633,7 +5647,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A20" s="17" t="s">
         <v>356</v>
       </c>
@@ -5646,7 +5660,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A21" s="4" t="s">
         <v>70</v>
       </c>
@@ -5675,7 +5689,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A22" s="17" t="s">
         <v>357</v>
       </c>
@@ -5688,7 +5702,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A23" s="17" t="s">
         <v>361</v>
       </c>
@@ -5701,7 +5715,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A24" s="17" t="s">
         <v>362</v>
       </c>
@@ -5714,7 +5728,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A25" s="4" t="s">
         <v>72</v>
       </c>
@@ -5743,7 +5757,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A26" t="s">
         <v>312</v>
       </c>
@@ -5760,7 +5774,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A27" t="s">
         <v>313</v>
       </c>
@@ -5777,7 +5791,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="28" spans="1:9" ht="27" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" ht="28" x14ac:dyDescent="0.15">
       <c r="A28" t="s">
         <v>315</v>
       </c>
@@ -5794,7 +5808,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A29" t="s">
         <v>317</v>
       </c>
@@ -5811,7 +5825,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="30" spans="1:9" ht="27" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" ht="28" x14ac:dyDescent="0.15">
       <c r="A30" t="s">
         <v>319</v>
       </c>
@@ -5828,7 +5842,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A31" t="s">
         <v>321</v>
       </c>
@@ -5845,7 +5859,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A32" s="4" t="s">
         <v>74</v>
       </c>
@@ -5874,7 +5888,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A33" t="s">
         <v>322</v>
       </c>
@@ -5891,7 +5905,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A34" t="s">
         <v>323</v>
       </c>
@@ -5908,7 +5922,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:9" ht="28" x14ac:dyDescent="0.15">
       <c r="A35" t="s">
         <v>324</v>
       </c>
@@ -5925,7 +5939,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="36" spans="1:9" ht="27" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:9" ht="28" x14ac:dyDescent="0.15">
       <c r="A36" t="s">
         <v>326</v>
       </c>
@@ -5942,7 +5956,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A37" t="s">
         <v>328</v>
       </c>
@@ -5959,7 +5973,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A38" s="4" t="s">
         <v>76</v>
       </c>
@@ -5973,7 +5987,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A39" t="s">
         <v>223</v>
       </c>
@@ -6002,7 +6016,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A40" t="s">
         <v>225</v>
       </c>
@@ -6019,7 +6033,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A41" t="s">
         <v>227</v>
       </c>
@@ -6036,7 +6050,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A42" t="s">
         <v>229</v>
       </c>
@@ -6053,7 +6067,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A43" t="s">
         <v>231</v>
       </c>
@@ -6070,7 +6084,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A44" t="s">
         <v>233</v>
       </c>
@@ -6087,7 +6101,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A45" t="s">
         <v>235</v>
       </c>
@@ -6104,7 +6118,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A46" t="s">
         <v>237</v>
       </c>
@@ -6121,7 +6135,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A47" t="s">
         <v>239</v>
       </c>
@@ -6138,7 +6152,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A48" t="s">
         <v>241</v>
       </c>
@@ -6155,7 +6169,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A49" t="s">
         <v>243</v>
       </c>
@@ -6172,7 +6186,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A50" t="s">
         <v>245</v>
       </c>
@@ -6189,7 +6203,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A51" t="s">
         <v>247</v>
       </c>
@@ -6206,7 +6220,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A52" t="s">
         <v>249</v>
       </c>
@@ -6223,7 +6237,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:9" ht="28" x14ac:dyDescent="0.15">
       <c r="A53" t="s">
         <v>251</v>
       </c>
@@ -6240,7 +6254,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A54" t="s">
         <v>253</v>
       </c>
@@ -6257,7 +6271,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A55" s="4" t="s">
         <v>78</v>
       </c>
@@ -6286,7 +6300,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A56" t="s">
         <v>255</v>
       </c>
@@ -6303,7 +6317,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A57" t="s">
         <v>257</v>
       </c>
@@ -6320,7 +6334,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A58" t="s">
         <v>258</v>
       </c>
@@ -6337,7 +6351,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A59" t="s">
         <v>259</v>
       </c>
@@ -6354,7 +6368,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A60" t="s">
         <v>260</v>
       </c>
@@ -6371,7 +6385,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A61" t="s">
         <v>261</v>
       </c>
@@ -6388,7 +6402,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A62" t="s">
         <v>262</v>
       </c>
@@ -6405,7 +6419,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A63" t="s">
         <v>367</v>
       </c>
@@ -6422,7 +6436,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A64" t="s">
         <v>368</v>
       </c>
@@ -6439,7 +6453,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A65" t="s">
         <v>369</v>
       </c>
@@ -6456,7 +6470,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A66" s="4" t="s">
         <v>214</v>
       </c>
@@ -6480,73 +6494,74 @@
         <v>600</v>
       </c>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="B72" s="5" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B73" s="5"/>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B74" s="5" t="s">
         <v>216</v>
       </c>
-      <c r="C74" s="25" t="s">
+      <c r="C74" s="28" t="s">
         <v>375</v>
       </c>
-      <c r="D74" s="26"/>
-      <c r="E74" s="26"/>
-      <c r="F74" s="26"/>
-      <c r="G74" s="26"/>
-    </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="D74" s="28"/>
+      <c r="E74" s="28"/>
+      <c r="F74" s="28"/>
+      <c r="G74" s="25"/>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B75" s="1"/>
-      <c r="C75" s="28" t="s">
+      <c r="C75" s="27" t="s">
         <v>371</v>
       </c>
-      <c r="D75" s="28"/>
-      <c r="E75" s="28"/>
-      <c r="F75" s="28"/>
-    </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="D75" s="27"/>
+      <c r="E75" s="27"/>
+      <c r="F75" s="27"/>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B76" s="1"/>
-      <c r="C76" s="28" t="s">
+      <c r="C76" s="27" t="s">
         <v>372</v>
       </c>
-      <c r="D76" s="28"/>
-      <c r="E76" s="28"/>
-      <c r="F76" s="28"/>
-    </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="D76" s="27"/>
+      <c r="E76" s="27"/>
+      <c r="F76" s="27"/>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B77" s="1"/>
-      <c r="C77" s="30"/>
-      <c r="D77" s="30"/>
-      <c r="E77" s="30"/>
-      <c r="F77" s="30"/>
-    </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C77" s="29"/>
+      <c r="D77" s="29"/>
+      <c r="E77" s="29"/>
+      <c r="F77" s="29"/>
+    </row>
+    <row r="78" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="B78" s="5" t="s">
         <v>220</v>
       </c>
-      <c r="C78" s="29" t="s">
+      <c r="C78" s="28" t="s">
         <v>373</v>
       </c>
-      <c r="D78" s="29"/>
-      <c r="E78" s="29"/>
-      <c r="F78" s="29"/>
-    </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="D78" s="28"/>
+      <c r="E78" s="28"/>
+      <c r="F78" s="28"/>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B79" s="1"/>
-      <c r="C79" s="29" t="s">
+      <c r="C79" s="28" t="s">
         <v>374</v>
       </c>
-      <c r="D79" s="29"/>
-      <c r="E79" s="29"/>
-      <c r="F79" s="29"/>
+      <c r="D79" s="28"/>
+      <c r="E79" s="28"/>
+      <c r="F79" s="28"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="6">
+    <mergeCell ref="C74:F74"/>
     <mergeCell ref="C79:F79"/>
     <mergeCell ref="C75:F75"/>
     <mergeCell ref="C76:F76"/>
@@ -6564,16 +6579,16 @@
   <dimension ref="A1:I45"/>
   <sheetViews>
     <sheetView topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E49" sqref="E49"/>
+      <selection activeCell="F49" sqref="F49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="2" max="2" width="36.15234375" customWidth="1"/>
-    <col min="9" max="9" width="12.4609375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="36.1640625" customWidth="1"/>
+    <col min="9" max="9" width="12.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>33</v>
       </c>
@@ -6602,7 +6617,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="15" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" ht="17" x14ac:dyDescent="0.15">
       <c r="A2" s="4" t="s">
         <v>80</v>
       </c>
@@ -6631,7 +6646,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="15" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" ht="16" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>379</v>
       </c>
@@ -6644,7 +6659,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="15" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" ht="17" x14ac:dyDescent="0.15">
       <c r="A4" s="4" t="s">
         <v>82</v>
       </c>
@@ -6673,7 +6688,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="15" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" ht="16" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>380</v>
       </c>
@@ -6686,7 +6701,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="15" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" ht="16" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>381</v>
       </c>
@@ -6699,7 +6714,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="15" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" ht="17" x14ac:dyDescent="0.15">
       <c r="A7" s="4" t="s">
         <v>84</v>
       </c>
@@ -6728,7 +6743,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="15" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" ht="16" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>383</v>
       </c>
@@ -6741,7 +6756,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="15" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" ht="16" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
         <v>384</v>
       </c>
@@ -6754,7 +6769,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="15" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" ht="17" x14ac:dyDescent="0.15">
       <c r="A10" s="4" t="s">
         <v>86</v>
       </c>
@@ -6783,7 +6798,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="15" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" ht="16" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
         <v>386</v>
       </c>
@@ -6796,7 +6811,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="15" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" ht="16" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
         <v>387</v>
       </c>
@@ -6809,7 +6824,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="15" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" ht="17" x14ac:dyDescent="0.15">
       <c r="A13" s="4" t="s">
         <v>88</v>
       </c>
@@ -6838,7 +6853,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="15" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" ht="16" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
         <v>389</v>
       </c>
@@ -6851,7 +6866,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="15" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" ht="16" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
         <v>390</v>
       </c>
@@ -6864,7 +6879,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="15" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" ht="17" x14ac:dyDescent="0.15">
       <c r="A16" s="4" t="s">
         <v>90</v>
       </c>
@@ -6893,7 +6908,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="15" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" ht="16" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
         <v>392</v>
       </c>
@@ -6906,7 +6921,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="15" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" ht="16" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
         <v>393</v>
       </c>
@@ -6919,7 +6934,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="15" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" ht="17" x14ac:dyDescent="0.15">
       <c r="A19" s="4" t="s">
         <v>92</v>
       </c>
@@ -6948,7 +6963,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="15" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" ht="16" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
         <v>394</v>
       </c>
@@ -6961,7 +6976,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="15" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" ht="16" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
         <v>395</v>
       </c>
@@ -6974,7 +6989,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="15" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" ht="17" x14ac:dyDescent="0.15">
       <c r="A22" s="4" t="s">
         <v>94</v>
       </c>
@@ -7003,7 +7018,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="15" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" ht="16" x14ac:dyDescent="0.15">
       <c r="A23" t="s">
         <v>396</v>
       </c>
@@ -7016,7 +7031,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="15" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" ht="16" x14ac:dyDescent="0.15">
       <c r="A24" t="s">
         <v>397</v>
       </c>
@@ -7029,7 +7044,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="15" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" ht="17" x14ac:dyDescent="0.15">
       <c r="A25" s="4" t="s">
         <v>96</v>
       </c>
@@ -7058,7 +7073,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="15" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" ht="16" x14ac:dyDescent="0.15">
       <c r="A26" t="s">
         <v>398</v>
       </c>
@@ -7071,7 +7086,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="27" spans="1:9" ht="15" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" ht="16" x14ac:dyDescent="0.15">
       <c r="A27" t="s">
         <v>399</v>
       </c>
@@ -7084,7 +7099,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="28" spans="1:9" ht="15" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" ht="17" x14ac:dyDescent="0.15">
       <c r="A28" s="4" t="s">
         <v>98</v>
       </c>
@@ -7113,7 +7128,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A29" t="s">
         <v>400</v>
       </c>
@@ -7124,7 +7139,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A30" t="s">
         <v>401</v>
       </c>
@@ -7135,7 +7150,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A31" s="4" t="s">
         <v>214</v>
       </c>
@@ -7156,75 +7171,75 @@
         <v>660</v>
       </c>
     </row>
-    <row r="37" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:7" ht="14" x14ac:dyDescent="0.15">
       <c r="B37" s="5" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="38" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:7" x14ac:dyDescent="0.15">
       <c r="B38" s="5"/>
     </row>
-    <row r="39" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:7" ht="14" x14ac:dyDescent="0.15">
       <c r="B39" s="5" t="s">
         <v>216</v>
       </c>
-      <c r="C39" s="28" t="s">
+      <c r="C39" s="27" t="s">
         <v>412</v>
       </c>
-      <c r="D39" s="28"/>
-      <c r="E39" s="28"/>
-      <c r="F39" s="28"/>
-      <c r="G39" s="28"/>
-    </row>
-    <row r="40" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="D39" s="27"/>
+      <c r="E39" s="27"/>
+      <c r="F39" s="27"/>
+      <c r="G39" s="27"/>
+    </row>
+    <row r="40" spans="2:7" x14ac:dyDescent="0.15">
       <c r="B40" s="1"/>
-      <c r="C40" s="32" t="s">
+      <c r="C40" s="31" t="s">
         <v>413</v>
       </c>
-      <c r="D40" s="32"/>
-      <c r="E40" s="32"/>
-      <c r="F40" s="32"/>
-      <c r="G40" s="32"/>
-    </row>
-    <row r="41" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="D40" s="31"/>
+      <c r="E40" s="31"/>
+      <c r="F40" s="31"/>
+      <c r="G40" s="31"/>
+    </row>
+    <row r="41" spans="2:7" x14ac:dyDescent="0.15">
       <c r="B41" s="1"/>
-      <c r="C41" s="32" t="s">
+      <c r="C41" s="31" t="s">
         <v>414</v>
       </c>
-      <c r="D41" s="32"/>
-      <c r="E41" s="32"/>
-      <c r="F41" s="32"/>
-      <c r="G41" s="32"/>
-    </row>
-    <row r="42" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="D41" s="31"/>
+      <c r="E41" s="31"/>
+      <c r="F41" s="31"/>
+      <c r="G41" s="31"/>
+    </row>
+    <row r="42" spans="2:7" x14ac:dyDescent="0.15">
       <c r="B42" s="1"/>
-      <c r="C42" s="33"/>
-      <c r="D42" s="34"/>
-      <c r="E42" s="34"/>
-      <c r="F42" s="34"/>
-      <c r="G42" s="34"/>
-    </row>
-    <row r="43" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="C42" s="32"/>
+      <c r="D42" s="33"/>
+      <c r="E42" s="33"/>
+      <c r="F42" s="33"/>
+      <c r="G42" s="33"/>
+    </row>
+    <row r="43" spans="2:7" ht="14" x14ac:dyDescent="0.15">
       <c r="B43" s="5" t="s">
         <v>220</v>
       </c>
-      <c r="C43" s="29" t="s">
+      <c r="C43" s="28" t="s">
         <v>415</v>
       </c>
-      <c r="D43" s="29"/>
-      <c r="E43" s="29"/>
-      <c r="F43" s="29"/>
-    </row>
-    <row r="44" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="D43" s="28"/>
+      <c r="E43" s="28"/>
+      <c r="F43" s="28"/>
+    </row>
+    <row r="44" spans="2:7" x14ac:dyDescent="0.15">
       <c r="B44" s="1"/>
-      <c r="C44" s="31" t="s">
+      <c r="C44" s="30" t="s">
         <v>416</v>
       </c>
-      <c r="D44" s="29"/>
-      <c r="E44" s="29"/>
-      <c r="F44" s="29"/>
-    </row>
-    <row r="45" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="D44" s="28"/>
+      <c r="E44" s="28"/>
+      <c r="F44" s="28"/>
+    </row>
+    <row r="45" spans="2:7" x14ac:dyDescent="0.15">
       <c r="B45" s="23"/>
     </row>
   </sheetData>
@@ -7244,19 +7259,19 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:I33"/>
+  <dimension ref="A1:I46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="G31" sqref="G31"/>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="F51" sqref="F51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="2" max="2" width="28.4609375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.3828125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>33</v>
       </c>
@@ -7285,7 +7300,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="15" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" ht="17" x14ac:dyDescent="0.15">
       <c r="A2" s="4" t="s">
         <v>100</v>
       </c>
@@ -7308,7 +7323,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="15" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" ht="16" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>417</v>
       </c>
@@ -7318,7 +7333,7 @@
       <c r="C3" s="12"/>
       <c r="D3" s="17"/>
     </row>
-    <row r="4" spans="1:9" ht="27" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" ht="28" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>418</v>
       </c>
@@ -7328,7 +7343,7 @@
       <c r="C4" s="12"/>
       <c r="D4" s="17"/>
     </row>
-    <row r="5" spans="1:9" ht="15" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" ht="17" x14ac:dyDescent="0.15">
       <c r="A5" s="4" t="s">
         <v>102</v>
       </c>
@@ -7351,7 +7366,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="15" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" ht="28" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>423</v>
       </c>
@@ -7361,7 +7376,7 @@
       <c r="C6" s="12"/>
       <c r="D6" s="17"/>
     </row>
-    <row r="7" spans="1:9" ht="27" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" ht="28" x14ac:dyDescent="0.15">
       <c r="A7" s="17" t="s">
         <v>457</v>
       </c>
@@ -7371,7 +7386,7 @@
       <c r="C7" s="12"/>
       <c r="D7" s="17"/>
     </row>
-    <row r="8" spans="1:9" ht="15" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" ht="17" x14ac:dyDescent="0.15">
       <c r="A8" s="4" t="s">
         <v>104</v>
       </c>
@@ -7394,7 +7409,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="15" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" ht="16" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
         <v>424</v>
       </c>
@@ -7404,7 +7419,7 @@
       <c r="C9" s="12"/>
       <c r="D9" s="17"/>
     </row>
-    <row r="10" spans="1:9" ht="15" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" ht="28" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>426</v>
       </c>
@@ -7414,7 +7429,7 @@
       <c r="C10" s="12"/>
       <c r="D10" s="17"/>
     </row>
-    <row r="11" spans="1:9" ht="15" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" ht="17" x14ac:dyDescent="0.15">
       <c r="A11" s="4" t="s">
         <v>106</v>
       </c>
@@ -7437,7 +7452,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="15" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" ht="16" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
         <v>430</v>
       </c>
@@ -7447,7 +7462,7 @@
       <c r="C12" s="12"/>
       <c r="D12" s="17"/>
     </row>
-    <row r="13" spans="1:9" ht="15" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" ht="28" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
         <v>431</v>
       </c>
@@ -7457,7 +7472,7 @@
       <c r="C13" s="12"/>
       <c r="D13" s="17"/>
     </row>
-    <row r="14" spans="1:9" ht="15" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" ht="17" x14ac:dyDescent="0.15">
       <c r="A14" s="4" t="s">
         <v>108</v>
       </c>
@@ -7480,7 +7495,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="27" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" ht="28" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
         <v>433</v>
       </c>
@@ -7490,7 +7505,7 @@
       <c r="C15" s="12"/>
       <c r="D15" s="17"/>
     </row>
-    <row r="16" spans="1:9" ht="15" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" ht="16" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
         <v>434</v>
       </c>
@@ -7500,7 +7515,7 @@
       <c r="C16" s="12"/>
       <c r="D16" s="17"/>
     </row>
-    <row r="17" spans="1:9" ht="15" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" ht="17" x14ac:dyDescent="0.15">
       <c r="A17" s="4" t="s">
         <v>110</v>
       </c>
@@ -7523,7 +7538,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="15" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" ht="16" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
         <v>437</v>
       </c>
@@ -7533,7 +7548,7 @@
       <c r="C18" s="12"/>
       <c r="D18" s="17"/>
     </row>
-    <row r="19" spans="1:9" ht="27" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" ht="28" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
         <v>438</v>
       </c>
@@ -7543,7 +7558,7 @@
       <c r="C19" s="12"/>
       <c r="D19" s="17"/>
     </row>
-    <row r="20" spans="1:9" ht="15" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" ht="17" x14ac:dyDescent="0.15">
       <c r="A20" s="4" t="s">
         <v>112</v>
       </c>
@@ -7562,11 +7577,17 @@
       <c r="F20">
         <v>90</v>
       </c>
+      <c r="G20">
+        <v>69</v>
+      </c>
+      <c r="H20">
+        <v>120</v>
+      </c>
       <c r="I20" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" ht="15" x14ac:dyDescent="0.3">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="16" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
         <v>439</v>
       </c>
@@ -7575,8 +7596,11 @@
       </c>
       <c r="C21" s="12"/>
       <c r="D21" s="17"/>
-    </row>
-    <row r="22" spans="1:9" ht="27" x14ac:dyDescent="0.3">
+      <c r="I21" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="28" x14ac:dyDescent="0.15">
       <c r="A22" t="s">
         <v>440</v>
       </c>
@@ -7585,8 +7609,11 @@
       </c>
       <c r="C22" s="12"/>
       <c r="D22" s="17"/>
-    </row>
-    <row r="23" spans="1:9" ht="15" x14ac:dyDescent="0.3">
+      <c r="I22" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="16" x14ac:dyDescent="0.15">
       <c r="A23" t="s">
         <v>445</v>
       </c>
@@ -7595,8 +7622,11 @@
       </c>
       <c r="C23" s="12"/>
       <c r="D23" s="17"/>
-    </row>
-    <row r="24" spans="1:9" ht="15" x14ac:dyDescent="0.3">
+      <c r="I23" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="17" x14ac:dyDescent="0.15">
       <c r="A24" s="4" t="s">
         <v>114</v>
       </c>
@@ -7615,11 +7645,17 @@
       <c r="F24">
         <v>90</v>
       </c>
+      <c r="G24">
+        <v>49</v>
+      </c>
+      <c r="H24">
+        <v>90</v>
+      </c>
       <c r="I24" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" ht="27" x14ac:dyDescent="0.3">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="28" x14ac:dyDescent="0.15">
       <c r="A25" t="s">
         <v>441</v>
       </c>
@@ -7628,8 +7664,11 @@
       </c>
       <c r="C25" s="12"/>
       <c r="D25" s="17"/>
-    </row>
-    <row r="26" spans="1:9" ht="15" x14ac:dyDescent="0.3">
+      <c r="I25" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="16" x14ac:dyDescent="0.15">
       <c r="A26" t="s">
         <v>442</v>
       </c>
@@ -7638,8 +7677,11 @@
       </c>
       <c r="C26" s="12"/>
       <c r="D26" s="17"/>
-    </row>
-    <row r="27" spans="1:9" ht="15" x14ac:dyDescent="0.3">
+      <c r="I26" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="17" x14ac:dyDescent="0.15">
       <c r="A27" s="4" t="s">
         <v>116</v>
       </c>
@@ -7668,7 +7710,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="28" spans="1:9" ht="15" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" ht="16" x14ac:dyDescent="0.15">
       <c r="A28" t="s">
         <v>451</v>
       </c>
@@ -7681,7 +7723,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="29" spans="1:9" ht="27" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" ht="28" x14ac:dyDescent="0.15">
       <c r="A29" t="s">
         <v>452</v>
       </c>
@@ -7694,7 +7736,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="30" spans="1:9" ht="15" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" ht="17" x14ac:dyDescent="0.15">
       <c r="A30" s="4" t="s">
         <v>118</v>
       </c>
@@ -7723,7 +7765,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" ht="28" x14ac:dyDescent="0.15">
       <c r="A31" t="s">
         <v>453</v>
       </c>
@@ -7734,7 +7776,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="32" spans="1:9" ht="27" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:9" ht="28" x14ac:dyDescent="0.15">
       <c r="A32" t="s">
         <v>454</v>
       </c>
@@ -7745,7 +7787,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A33" s="4" t="s">
         <v>214</v>
       </c>
@@ -7759,14 +7801,90 @@
       </c>
       <c r="G33">
         <f t="shared" si="0"/>
-        <v>101</v>
+        <v>219</v>
       </c>
       <c r="H33">
         <f t="shared" si="0"/>
-        <v>120</v>
-      </c>
+        <v>330</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" ht="14" x14ac:dyDescent="0.15">
+      <c r="B39" s="5" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="B40" s="5"/>
+    </row>
+    <row r="41" spans="1:8" ht="14" x14ac:dyDescent="0.15">
+      <c r="B41" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="C41" s="34" t="s">
+        <v>458</v>
+      </c>
+      <c r="D41" s="27"/>
+      <c r="E41" s="27"/>
+      <c r="F41" s="27"/>
+      <c r="G41" s="27"/>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="B42" s="1"/>
+      <c r="C42" s="35" t="s">
+        <v>459</v>
+      </c>
+      <c r="D42" s="31"/>
+      <c r="E42" s="31"/>
+      <c r="F42" s="31"/>
+      <c r="G42" s="31"/>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="B43" s="1"/>
+      <c r="C43" s="35" t="s">
+        <v>460</v>
+      </c>
+      <c r="D43" s="31"/>
+      <c r="E43" s="31"/>
+      <c r="F43" s="31"/>
+      <c r="G43" s="31"/>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="B44" s="1"/>
+      <c r="C44" s="32"/>
+      <c r="D44" s="33"/>
+      <c r="E44" s="33"/>
+      <c r="F44" s="33"/>
+      <c r="G44" s="33"/>
+    </row>
+    <row r="45" spans="1:8" ht="14" x14ac:dyDescent="0.15">
+      <c r="B45" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="C45" s="36" t="s">
+        <v>458</v>
+      </c>
+      <c r="D45" s="28"/>
+      <c r="E45" s="28"/>
+      <c r="F45" s="28"/>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="B46" s="1"/>
+      <c r="C46" s="37" t="s">
+        <v>459</v>
+      </c>
+      <c r="D46" s="28"/>
+      <c r="E46" s="28"/>
+      <c r="F46" s="28"/>
     </row>
   </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="C41:G41"/>
+    <mergeCell ref="C42:G42"/>
+    <mergeCell ref="C43:G43"/>
+    <mergeCell ref="C44:G44"/>
+    <mergeCell ref="C45:F45"/>
+    <mergeCell ref="C46:F46"/>
+  </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -7776,17 +7894,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:C43"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
+    <sheetView topLeftCell="A32" zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
       <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="2" max="2" width="28.15234375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="49.4609375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="28.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="49.5" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" s="4" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>263</v>
       </c>
@@ -7797,7 +7915,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>37</v>
       </c>
@@ -7808,7 +7926,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" ht="17" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>40</v>
       </c>
@@ -7819,7 +7937,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="17" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>43</v>
       </c>
@@ -7830,7 +7948,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>45</v>
       </c>
@@ -7841,7 +7959,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>47</v>
       </c>
@@ -7852,7 +7970,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" ht="17" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
         <v>49</v>
       </c>
@@ -7863,7 +7981,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="45" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" ht="51" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>51</v>
       </c>
@@ -7874,7 +7992,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
         <v>53</v>
       </c>
@@ -7885,7 +8003,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>55</v>
       </c>
@@ -7896,7 +8014,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" ht="51" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
         <v>57</v>
       </c>
@@ -7907,7 +8025,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
         <v>59</v>
       </c>
@@ -7918,7 +8036,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="45" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" ht="51" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
         <v>62</v>
       </c>
@@ -7929,7 +8047,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="45" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" ht="68" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
         <v>64</v>
       </c>
@@ -7940,7 +8058,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
         <v>66</v>
       </c>
@@ -7951,7 +8069,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" ht="17" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
         <v>68</v>
       </c>
@@ -7962,7 +8080,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
         <v>70</v>
       </c>
@@ -7973,7 +8091,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" ht="17" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
         <v>72</v>
       </c>
@@ -7984,7 +8102,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" ht="17" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
         <v>74</v>
       </c>
@@ -7995,7 +8113,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" ht="17" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
         <v>76</v>
       </c>
@@ -8006,7 +8124,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
         <v>78</v>
       </c>
@@ -8017,7 +8135,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A22" t="s">
         <v>80</v>
       </c>
@@ -8028,7 +8146,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A23" t="s">
         <v>82</v>
       </c>
@@ -8039,7 +8157,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A24" t="s">
         <v>84</v>
       </c>
@@ -8050,7 +8168,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="45" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" ht="51" x14ac:dyDescent="0.15">
       <c r="A25" t="s">
         <v>86</v>
       </c>
@@ -8061,7 +8179,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A26" t="s">
         <v>88</v>
       </c>
@@ -8072,7 +8190,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="105" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" ht="136" x14ac:dyDescent="0.15">
       <c r="A27" t="s">
         <v>90</v>
       </c>
@@ -8083,7 +8201,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A28" t="s">
         <v>92</v>
       </c>
@@ -8094,7 +8212,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A29" t="s">
         <v>94</v>
       </c>
@@ -8105,7 +8223,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" ht="17" x14ac:dyDescent="0.15">
       <c r="A30" t="s">
         <v>96</v>
       </c>
@@ -8116,7 +8234,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" ht="17" x14ac:dyDescent="0.15">
       <c r="A31" t="s">
         <v>98</v>
       </c>
@@ -8127,7 +8245,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A32" t="s">
         <v>100</v>
       </c>
@@ -8138,7 +8256,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" ht="17" x14ac:dyDescent="0.15">
       <c r="A33" t="s">
         <v>102</v>
       </c>
@@ -8149,7 +8267,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A34" t="s">
         <v>104</v>
       </c>
@@ -8160,7 +8278,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" ht="51" x14ac:dyDescent="0.15">
       <c r="A35" t="s">
         <v>106</v>
       </c>
@@ -8171,7 +8289,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A36" t="s">
         <v>108</v>
       </c>
@@ -8182,7 +8300,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A37" t="s">
         <v>110</v>
       </c>
@@ -8193,7 +8311,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A38" t="s">
         <v>112</v>
       </c>
@@ -8204,7 +8322,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A39" t="s">
         <v>114</v>
       </c>
@@ -8215,7 +8333,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A40" t="s">
         <v>116</v>
       </c>
@@ -8226,7 +8344,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A41" t="s">
         <v>118</v>
       </c>
@@ -8237,7 +8355,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A42" t="s">
         <v>306</v>
       </c>
@@ -8248,7 +8366,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A43" t="s">
         <v>309</v>
       </c>

</xml_diff>